<commit_message>
p: process function array argumenting
</commit_message>
<xml_diff>
--- a/OOMII.xlsx
+++ b/OOMII.xlsx
@@ -346,7 +346,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:OR3"/>
+  <dimension ref="A1:OR5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2402,12 +2402,6 @@
           <t>type01</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
           <t>0.0625</t>
@@ -2438,9 +2432,6 @@
           <t>25.0</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr"/>
-      <c r="P2" t="inlineStr"/>
       <c r="Q2" t="inlineStr">
         <is>
           <t>3.22</t>
@@ -2451,7 +2442,6 @@
           <t>3.03</t>
         </is>
       </c>
-      <c r="S2" t="inlineStr"/>
       <c r="T2" t="inlineStr">
         <is>
           <t>3.00</t>
@@ -2482,23 +2472,11 @@
           <t>2.75</t>
         </is>
       </c>
-      <c r="Z2" t="inlineStr"/>
-      <c r="AA2" t="inlineStr"/>
-      <c r="AB2" t="inlineStr"/>
-      <c r="AC2" t="inlineStr"/>
-      <c r="AD2" t="inlineStr"/>
-      <c r="AE2" t="inlineStr"/>
-      <c r="AF2" t="inlineStr"/>
-      <c r="AG2" t="inlineStr"/>
-      <c r="AH2" t="inlineStr"/>
-      <c r="AI2" t="inlineStr"/>
-      <c r="AJ2" t="inlineStr"/>
       <c r="AK2" t="inlineStr">
         <is>
           <t>94</t>
         </is>
       </c>
-      <c r="AL2" t="inlineStr"/>
       <c r="AM2" t="inlineStr">
         <is>
           <t>93</t>
@@ -2529,10 +2507,6 @@
           <t>35</t>
         </is>
       </c>
-      <c r="AS2" t="inlineStr"/>
-      <c r="AT2" t="inlineStr"/>
-      <c r="AU2" t="inlineStr"/>
-      <c r="AV2" t="inlineStr"/>
       <c r="AW2" t="inlineStr">
         <is>
           <t>.1</t>
@@ -2563,18 +2537,6 @@
           <t>.9</t>
         </is>
       </c>
-      <c r="BC2" t="inlineStr"/>
-      <c r="BD2" t="inlineStr"/>
-      <c r="BE2" t="inlineStr"/>
-      <c r="BF2" t="inlineStr"/>
-      <c r="BG2" t="inlineStr"/>
-      <c r="BH2" t="inlineStr"/>
-      <c r="BI2" t="inlineStr"/>
-      <c r="BJ2" t="inlineStr"/>
-      <c r="BK2" t="inlineStr"/>
-      <c r="BL2" t="inlineStr"/>
-      <c r="BM2" t="inlineStr"/>
-      <c r="BN2" t="inlineStr"/>
       <c r="BO2" t="inlineStr">
         <is>
           <t>0.0625</t>
@@ -2605,9 +2567,6 @@
           <t>25.0</t>
         </is>
       </c>
-      <c r="BU2" t="inlineStr"/>
-      <c r="BV2" t="inlineStr"/>
-      <c r="BW2" t="inlineStr"/>
       <c r="BX2" t="inlineStr">
         <is>
           <t>2.51</t>
@@ -2618,7 +2577,6 @@
           <t>2.20</t>
         </is>
       </c>
-      <c r="BZ2" t="inlineStr"/>
       <c r="CA2" t="inlineStr">
         <is>
           <t>2.23</t>
@@ -2649,23 +2607,11 @@
           <t>1.99</t>
         </is>
       </c>
-      <c r="CG2" t="inlineStr"/>
-      <c r="CH2" t="inlineStr"/>
-      <c r="CI2" t="inlineStr"/>
-      <c r="CJ2" t="inlineStr"/>
-      <c r="CK2" t="inlineStr"/>
-      <c r="CL2" t="inlineStr"/>
-      <c r="CM2" t="inlineStr"/>
-      <c r="CN2" t="inlineStr"/>
-      <c r="CO2" t="inlineStr"/>
-      <c r="CP2" t="inlineStr"/>
-      <c r="CQ2" t="inlineStr"/>
       <c r="CR2" t="inlineStr">
         <is>
           <t>91</t>
         </is>
       </c>
-      <c r="CS2" t="inlineStr"/>
       <c r="CT2" t="inlineStr">
         <is>
           <t>39</t>
@@ -2696,10 +2642,6 @@
           <t>79</t>
         </is>
       </c>
-      <c r="CZ2" t="inlineStr"/>
-      <c r="DA2" t="inlineStr"/>
-      <c r="DB2" t="inlineStr"/>
-      <c r="DC2" t="inlineStr"/>
       <c r="DD2" t="inlineStr">
         <is>
           <t>.2</t>
@@ -2730,36 +2672,11 @@
           <t>.13</t>
         </is>
       </c>
-      <c r="DJ2" t="inlineStr"/>
-      <c r="DK2" t="inlineStr"/>
-      <c r="DL2" t="inlineStr"/>
-      <c r="DM2" t="inlineStr"/>
-      <c r="DN2" t="inlineStr"/>
-      <c r="DO2" t="inlineStr"/>
       <c r="DP2" t="inlineStr">
         <is>
           <t>220</t>
         </is>
       </c>
-      <c r="DQ2" t="inlineStr"/>
-      <c r="DR2" t="inlineStr"/>
-      <c r="DS2" t="inlineStr"/>
-      <c r="DT2" t="inlineStr"/>
-      <c r="DU2" t="inlineStr"/>
-      <c r="DV2" t="inlineStr"/>
-      <c r="DW2" t="inlineStr"/>
-      <c r="DX2" t="inlineStr"/>
-      <c r="DY2" t="inlineStr"/>
-      <c r="DZ2" t="inlineStr"/>
-      <c r="EA2" t="inlineStr"/>
-      <c r="EB2" t="inlineStr"/>
-      <c r="EC2" t="inlineStr"/>
-      <c r="ED2" t="inlineStr"/>
-      <c r="EE2" t="inlineStr"/>
-      <c r="EF2" t="inlineStr"/>
-      <c r="EG2" t="inlineStr"/>
-      <c r="EH2" t="inlineStr"/>
-      <c r="EI2" t="inlineStr"/>
       <c r="EJ2" t="inlineStr">
         <is>
           <t>2.57</t>
@@ -2790,16 +2707,11 @@
           <t>1.69</t>
         </is>
       </c>
-      <c r="EP2" t="inlineStr"/>
-      <c r="EQ2" t="inlineStr"/>
-      <c r="ER2" t="inlineStr"/>
-      <c r="ES2" t="inlineStr"/>
       <c r="ET2" t="inlineStr">
         <is>
           <t>68</t>
         </is>
       </c>
-      <c r="EU2" t="inlineStr"/>
       <c r="EV2" t="inlineStr">
         <is>
           <t>55</t>
@@ -2830,29 +2742,6 @@
           <t>51</t>
         </is>
       </c>
-      <c r="FB2" t="inlineStr"/>
-      <c r="FC2" t="inlineStr"/>
-      <c r="FD2" t="inlineStr"/>
-      <c r="FE2" t="inlineStr"/>
-      <c r="FF2" t="inlineStr"/>
-      <c r="FG2" t="inlineStr"/>
-      <c r="FH2" t="inlineStr"/>
-      <c r="FI2" t="inlineStr"/>
-      <c r="FJ2" t="inlineStr"/>
-      <c r="FK2" t="inlineStr"/>
-      <c r="FL2" t="inlineStr"/>
-      <c r="FM2" t="inlineStr"/>
-      <c r="FN2" t="inlineStr"/>
-      <c r="FO2" t="inlineStr"/>
-      <c r="FP2" t="inlineStr"/>
-      <c r="FQ2" t="inlineStr"/>
-      <c r="FR2" t="inlineStr"/>
-      <c r="FS2" t="inlineStr"/>
-      <c r="FT2" t="inlineStr"/>
-      <c r="FU2" t="inlineStr"/>
-      <c r="FV2" t="inlineStr"/>
-      <c r="FW2" t="inlineStr"/>
-      <c r="FX2" t="inlineStr"/>
       <c r="FY2" t="inlineStr">
         <is>
           <t>.4</t>
@@ -2883,51 +2772,6 @@
           <t>.24</t>
         </is>
       </c>
-      <c r="GE2" t="inlineStr"/>
-      <c r="GF2" t="inlineStr"/>
-      <c r="GG2" t="inlineStr"/>
-      <c r="GH2" t="inlineStr"/>
-      <c r="GI2" t="inlineStr"/>
-      <c r="GJ2" t="inlineStr"/>
-      <c r="GK2" t="inlineStr"/>
-      <c r="GL2" t="inlineStr"/>
-      <c r="GM2" t="inlineStr"/>
-      <c r="GN2" t="inlineStr"/>
-      <c r="GO2" t="inlineStr"/>
-      <c r="GP2" t="inlineStr"/>
-      <c r="GQ2" t="inlineStr"/>
-      <c r="GR2" t="inlineStr"/>
-      <c r="GS2" t="inlineStr"/>
-      <c r="GT2" t="inlineStr"/>
-      <c r="GU2" t="inlineStr"/>
-      <c r="GV2" t="inlineStr"/>
-      <c r="GW2" t="inlineStr"/>
-      <c r="GX2" t="inlineStr"/>
-      <c r="GY2" t="inlineStr"/>
-      <c r="GZ2" t="inlineStr"/>
-      <c r="HA2" t="inlineStr"/>
-      <c r="HB2" t="inlineStr"/>
-      <c r="HC2" t="inlineStr"/>
-      <c r="HD2" t="inlineStr"/>
-      <c r="HE2" t="inlineStr"/>
-      <c r="HF2" t="inlineStr"/>
-      <c r="HG2" t="inlineStr"/>
-      <c r="HH2" t="inlineStr"/>
-      <c r="HI2" t="inlineStr"/>
-      <c r="HJ2" t="inlineStr"/>
-      <c r="HK2" t="inlineStr"/>
-      <c r="HL2" t="inlineStr"/>
-      <c r="HM2" t="inlineStr"/>
-      <c r="HN2" t="inlineStr"/>
-      <c r="HO2" t="inlineStr"/>
-      <c r="HP2" t="inlineStr"/>
-      <c r="HQ2" t="inlineStr"/>
-      <c r="HR2" t="inlineStr"/>
-      <c r="HS2" t="inlineStr"/>
-      <c r="HT2" t="inlineStr"/>
-      <c r="HU2" t="inlineStr"/>
-      <c r="HV2" t="inlineStr"/>
-      <c r="HW2" t="inlineStr"/>
       <c r="HX2" t="inlineStr">
         <is>
           <t>0.0625</t>
@@ -2958,9 +2802,6 @@
           <t>25.0</t>
         </is>
       </c>
-      <c r="ID2" t="inlineStr"/>
-      <c r="IE2" t="inlineStr"/>
-      <c r="IF2" t="inlineStr"/>
       <c r="IG2" t="inlineStr">
         <is>
           <t>5.45</t>
@@ -2971,7 +2812,6 @@
           <t>9.33</t>
         </is>
       </c>
-      <c r="II2" t="inlineStr"/>
       <c r="IJ2" t="inlineStr">
         <is>
           <t>7.32</t>
@@ -3002,23 +2842,11 @@
           <t>7.31</t>
         </is>
       </c>
-      <c r="IP2" t="inlineStr"/>
-      <c r="IQ2" t="inlineStr"/>
-      <c r="IR2" t="inlineStr"/>
-      <c r="IS2" t="inlineStr"/>
-      <c r="IT2" t="inlineStr"/>
-      <c r="IU2" t="inlineStr"/>
-      <c r="IV2" t="inlineStr"/>
-      <c r="IW2" t="inlineStr"/>
-      <c r="IX2" t="inlineStr"/>
-      <c r="IY2" t="inlineStr"/>
-      <c r="IZ2" t="inlineStr"/>
       <c r="JA2" t="inlineStr">
         <is>
           <t>153</t>
         </is>
       </c>
-      <c r="JB2" t="inlineStr"/>
       <c r="JC2" t="inlineStr">
         <is>
           <t>143</t>
@@ -3049,10 +2877,6 @@
           <t>134</t>
         </is>
       </c>
-      <c r="JI2" t="inlineStr"/>
-      <c r="JJ2" t="inlineStr"/>
-      <c r="JK2" t="inlineStr"/>
-      <c r="JL2" t="inlineStr"/>
       <c r="JM2" t="inlineStr">
         <is>
           <t>.9</t>
@@ -3083,136 +2907,6 @@
           <t>.15</t>
         </is>
       </c>
-      <c r="JS2" t="inlineStr"/>
-      <c r="JT2" t="inlineStr"/>
-      <c r="JU2" t="inlineStr"/>
-      <c r="JV2" t="inlineStr"/>
-      <c r="JW2" t="inlineStr"/>
-      <c r="JX2" t="inlineStr"/>
-      <c r="JY2" t="inlineStr"/>
-      <c r="JZ2" t="inlineStr"/>
-      <c r="KA2" t="inlineStr"/>
-      <c r="KB2" t="inlineStr"/>
-      <c r="KC2" t="inlineStr"/>
-      <c r="KD2" t="inlineStr"/>
-      <c r="KE2" t="inlineStr"/>
-      <c r="KF2" t="inlineStr"/>
-      <c r="KG2" t="inlineStr"/>
-      <c r="KH2" t="inlineStr"/>
-      <c r="KI2" t="inlineStr"/>
-      <c r="KJ2" t="inlineStr"/>
-      <c r="KK2" t="inlineStr"/>
-      <c r="KL2" t="inlineStr"/>
-      <c r="KM2" t="inlineStr"/>
-      <c r="KN2" t="inlineStr"/>
-      <c r="KO2" t="inlineStr"/>
-      <c r="KP2" t="inlineStr"/>
-      <c r="KQ2" t="inlineStr"/>
-      <c r="KR2" t="inlineStr"/>
-      <c r="KS2" t="inlineStr"/>
-      <c r="KT2" t="inlineStr"/>
-      <c r="KU2" t="inlineStr"/>
-      <c r="KV2" t="inlineStr"/>
-      <c r="KW2" t="inlineStr"/>
-      <c r="KX2" t="inlineStr"/>
-      <c r="KY2" t="inlineStr"/>
-      <c r="KZ2" t="inlineStr"/>
-      <c r="LA2" t="inlineStr"/>
-      <c r="LB2" t="inlineStr"/>
-      <c r="LC2" t="inlineStr"/>
-      <c r="LD2" t="inlineStr"/>
-      <c r="LE2" t="inlineStr"/>
-      <c r="LF2" t="inlineStr"/>
-      <c r="LG2" t="inlineStr"/>
-      <c r="LH2" t="inlineStr"/>
-      <c r="LI2" t="inlineStr"/>
-      <c r="LJ2" t="inlineStr"/>
-      <c r="LK2" t="inlineStr"/>
-      <c r="LL2" t="inlineStr"/>
-      <c r="LM2" t="inlineStr"/>
-      <c r="LN2" t="inlineStr"/>
-      <c r="LO2" t="inlineStr"/>
-      <c r="LP2" t="inlineStr"/>
-      <c r="LQ2" t="inlineStr"/>
-      <c r="LR2" t="inlineStr"/>
-      <c r="LS2" t="inlineStr"/>
-      <c r="LT2" t="inlineStr"/>
-      <c r="LU2" t="inlineStr"/>
-      <c r="LV2" t="inlineStr"/>
-      <c r="LW2" t="inlineStr"/>
-      <c r="LX2" t="inlineStr"/>
-      <c r="LY2" t="inlineStr"/>
-      <c r="LZ2" t="inlineStr"/>
-      <c r="MA2" t="inlineStr"/>
-      <c r="MB2" t="inlineStr"/>
-      <c r="MC2" t="inlineStr"/>
-      <c r="MD2" t="inlineStr"/>
-      <c r="ME2" t="inlineStr"/>
-      <c r="MF2" t="inlineStr"/>
-      <c r="MG2" t="inlineStr"/>
-      <c r="MH2" t="inlineStr"/>
-      <c r="MI2" t="inlineStr"/>
-      <c r="MJ2" t="inlineStr"/>
-      <c r="MK2" t="inlineStr"/>
-      <c r="ML2" t="inlineStr"/>
-      <c r="MM2" t="inlineStr"/>
-      <c r="MN2" t="inlineStr"/>
-      <c r="MO2" t="inlineStr"/>
-      <c r="MP2" t="inlineStr"/>
-      <c r="MQ2" t="inlineStr"/>
-      <c r="MR2" t="inlineStr"/>
-      <c r="MS2" t="inlineStr"/>
-      <c r="MT2" t="inlineStr"/>
-      <c r="MU2" t="inlineStr"/>
-      <c r="MV2" t="inlineStr"/>
-      <c r="MW2" t="inlineStr"/>
-      <c r="MX2" t="inlineStr"/>
-      <c r="MY2" t="inlineStr"/>
-      <c r="MZ2" t="inlineStr"/>
-      <c r="NA2" t="inlineStr"/>
-      <c r="NB2" t="inlineStr"/>
-      <c r="NC2" t="inlineStr"/>
-      <c r="ND2" t="inlineStr"/>
-      <c r="NE2" t="inlineStr"/>
-      <c r="NF2" t="inlineStr"/>
-      <c r="NG2" t="inlineStr"/>
-      <c r="NH2" t="inlineStr"/>
-      <c r="NI2" t="inlineStr"/>
-      <c r="NJ2" t="inlineStr"/>
-      <c r="NK2" t="inlineStr"/>
-      <c r="NL2" t="inlineStr"/>
-      <c r="NM2" t="inlineStr"/>
-      <c r="NN2" t="inlineStr"/>
-      <c r="NO2" t="inlineStr"/>
-      <c r="NP2" t="inlineStr"/>
-      <c r="NQ2" t="inlineStr"/>
-      <c r="NR2" t="inlineStr"/>
-      <c r="NS2" t="inlineStr"/>
-      <c r="NT2" t="inlineStr"/>
-      <c r="NU2" t="inlineStr"/>
-      <c r="NV2" t="inlineStr"/>
-      <c r="NW2" t="inlineStr"/>
-      <c r="NX2" t="inlineStr"/>
-      <c r="NY2" t="inlineStr"/>
-      <c r="NZ2" t="inlineStr"/>
-      <c r="OA2" t="inlineStr"/>
-      <c r="OB2" t="inlineStr"/>
-      <c r="OC2" t="inlineStr"/>
-      <c r="OD2" t="inlineStr"/>
-      <c r="OE2" t="inlineStr"/>
-      <c r="OF2" t="inlineStr"/>
-      <c r="OG2" t="inlineStr"/>
-      <c r="OH2" t="inlineStr"/>
-      <c r="OI2" t="inlineStr"/>
-      <c r="OJ2" t="inlineStr"/>
-      <c r="OK2" t="inlineStr"/>
-      <c r="OL2" t="inlineStr"/>
-      <c r="OM2" t="inlineStr"/>
-      <c r="ON2" t="inlineStr"/>
-      <c r="OO2" t="inlineStr"/>
-      <c r="OP2" t="inlineStr"/>
-      <c r="OQ2" t="inlineStr"/>
-      <c r="OR2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -3220,12 +2914,6 @@
           <t>type01</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr">
         <is>
           <t>0.0625</t>
@@ -3256,9 +2944,6 @@
           <t>25.0</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
-      <c r="P3" t="inlineStr"/>
       <c r="Q3" t="inlineStr">
         <is>
           <t>4.39</t>
@@ -3269,7 +2954,6 @@
           <t>2.88</t>
         </is>
       </c>
-      <c r="S3" t="inlineStr"/>
       <c r="T3" t="inlineStr">
         <is>
           <t>2.92</t>
@@ -3300,23 +2984,11 @@
           <t>2.90</t>
         </is>
       </c>
-      <c r="Z3" t="inlineStr"/>
-      <c r="AA3" t="inlineStr"/>
-      <c r="AB3" t="inlineStr"/>
-      <c r="AC3" t="inlineStr"/>
-      <c r="AD3" t="inlineStr"/>
-      <c r="AE3" t="inlineStr"/>
-      <c r="AF3" t="inlineStr"/>
-      <c r="AG3" t="inlineStr"/>
-      <c r="AH3" t="inlineStr"/>
-      <c r="AI3" t="inlineStr"/>
-      <c r="AJ3" t="inlineStr"/>
       <c r="AK3" t="inlineStr">
         <is>
           <t>6</t>
         </is>
       </c>
-      <c r="AL3" t="inlineStr"/>
       <c r="AM3" t="inlineStr">
         <is>
           <t>67</t>
@@ -3347,10 +3019,6 @@
           <t>66</t>
         </is>
       </c>
-      <c r="AS3" t="inlineStr"/>
-      <c r="AT3" t="inlineStr"/>
-      <c r="AU3" t="inlineStr"/>
-      <c r="AV3" t="inlineStr"/>
       <c r="AW3" t="inlineStr">
         <is>
           <t>-1</t>
@@ -3381,18 +3049,6 @@
           <t>-1</t>
         </is>
       </c>
-      <c r="BC3" t="inlineStr"/>
-      <c r="BD3" t="inlineStr"/>
-      <c r="BE3" t="inlineStr"/>
-      <c r="BF3" t="inlineStr"/>
-      <c r="BG3" t="inlineStr"/>
-      <c r="BH3" t="inlineStr"/>
-      <c r="BI3" t="inlineStr"/>
-      <c r="BJ3" t="inlineStr"/>
-      <c r="BK3" t="inlineStr"/>
-      <c r="BL3" t="inlineStr"/>
-      <c r="BM3" t="inlineStr"/>
-      <c r="BN3" t="inlineStr"/>
       <c r="BO3" t="inlineStr">
         <is>
           <t>0.0625</t>
@@ -3423,9 +3079,6 @@
           <t>25.0</t>
         </is>
       </c>
-      <c r="BU3" t="inlineStr"/>
-      <c r="BV3" t="inlineStr"/>
-      <c r="BW3" t="inlineStr"/>
       <c r="BX3" t="inlineStr">
         <is>
           <t>3.06</t>
@@ -3436,7 +3089,6 @@
           <t>2.17</t>
         </is>
       </c>
-      <c r="BZ3" t="inlineStr"/>
       <c r="CA3" t="inlineStr">
         <is>
           <t>225</t>
@@ -3467,23 +3119,11 @@
           <t>2.16</t>
         </is>
       </c>
-      <c r="CG3" t="inlineStr"/>
-      <c r="CH3" t="inlineStr"/>
-      <c r="CI3" t="inlineStr"/>
-      <c r="CJ3" t="inlineStr"/>
-      <c r="CK3" t="inlineStr"/>
-      <c r="CL3" t="inlineStr"/>
-      <c r="CM3" t="inlineStr"/>
-      <c r="CN3" t="inlineStr"/>
-      <c r="CO3" t="inlineStr"/>
-      <c r="CP3" t="inlineStr"/>
-      <c r="CQ3" t="inlineStr"/>
       <c r="CR3" t="inlineStr">
         <is>
           <t>71</t>
         </is>
       </c>
-      <c r="CS3" t="inlineStr"/>
       <c r="CT3" t="inlineStr">
         <is>
           <t>74</t>
@@ -3514,10 +3154,6 @@
           <t>71</t>
         </is>
       </c>
-      <c r="CZ3" t="inlineStr"/>
-      <c r="DA3" t="inlineStr"/>
-      <c r="DB3" t="inlineStr"/>
-      <c r="DC3" t="inlineStr"/>
       <c r="DD3" t="inlineStr">
         <is>
           <t>0</t>
@@ -3548,36 +3184,11 @@
           <t>4</t>
         </is>
       </c>
-      <c r="DJ3" t="inlineStr"/>
-      <c r="DK3" t="inlineStr"/>
-      <c r="DL3" t="inlineStr"/>
-      <c r="DM3" t="inlineStr"/>
-      <c r="DN3" t="inlineStr"/>
-      <c r="DO3" t="inlineStr"/>
       <c r="DP3" t="inlineStr">
         <is>
           <t>20</t>
         </is>
       </c>
-      <c r="DQ3" t="inlineStr"/>
-      <c r="DR3" t="inlineStr"/>
-      <c r="DS3" t="inlineStr"/>
-      <c r="DT3" t="inlineStr"/>
-      <c r="DU3" t="inlineStr"/>
-      <c r="DV3" t="inlineStr"/>
-      <c r="DW3" t="inlineStr"/>
-      <c r="DX3" t="inlineStr"/>
-      <c r="DY3" t="inlineStr"/>
-      <c r="DZ3" t="inlineStr"/>
-      <c r="EA3" t="inlineStr"/>
-      <c r="EB3" t="inlineStr"/>
-      <c r="EC3" t="inlineStr"/>
-      <c r="ED3" t="inlineStr"/>
-      <c r="EE3" t="inlineStr"/>
-      <c r="EF3" t="inlineStr"/>
-      <c r="EG3" t="inlineStr"/>
-      <c r="EH3" t="inlineStr"/>
-      <c r="EI3" t="inlineStr"/>
       <c r="EJ3" t="inlineStr">
         <is>
           <t>2.60</t>
@@ -3608,16 +3219,11 @@
           <t>1.75</t>
         </is>
       </c>
-      <c r="EP3" t="inlineStr"/>
-      <c r="EQ3" t="inlineStr"/>
-      <c r="ER3" t="inlineStr"/>
-      <c r="ES3" t="inlineStr"/>
       <c r="ET3" t="inlineStr">
         <is>
           <t>66</t>
         </is>
       </c>
-      <c r="EU3" t="inlineStr"/>
       <c r="EV3" t="inlineStr">
         <is>
           <t>73</t>
@@ -3648,29 +3254,6 @@
           <t>61</t>
         </is>
       </c>
-      <c r="FB3" t="inlineStr"/>
-      <c r="FC3" t="inlineStr"/>
-      <c r="FD3" t="inlineStr"/>
-      <c r="FE3" t="inlineStr"/>
-      <c r="FF3" t="inlineStr"/>
-      <c r="FG3" t="inlineStr"/>
-      <c r="FH3" t="inlineStr"/>
-      <c r="FI3" t="inlineStr"/>
-      <c r="FJ3" t="inlineStr"/>
-      <c r="FK3" t="inlineStr"/>
-      <c r="FL3" t="inlineStr"/>
-      <c r="FM3" t="inlineStr"/>
-      <c r="FN3" t="inlineStr"/>
-      <c r="FO3" t="inlineStr"/>
-      <c r="FP3" t="inlineStr"/>
-      <c r="FQ3" t="inlineStr"/>
-      <c r="FR3" t="inlineStr"/>
-      <c r="FS3" t="inlineStr"/>
-      <c r="FT3" t="inlineStr"/>
-      <c r="FU3" t="inlineStr"/>
-      <c r="FV3" t="inlineStr"/>
-      <c r="FW3" t="inlineStr"/>
-      <c r="FX3" t="inlineStr"/>
       <c r="FY3" t="inlineStr">
         <is>
           <t>2</t>
@@ -3701,51 +3284,6 @@
           <t>-15</t>
         </is>
       </c>
-      <c r="GE3" t="inlineStr"/>
-      <c r="GF3" t="inlineStr"/>
-      <c r="GG3" t="inlineStr"/>
-      <c r="GH3" t="inlineStr"/>
-      <c r="GI3" t="inlineStr"/>
-      <c r="GJ3" t="inlineStr"/>
-      <c r="GK3" t="inlineStr"/>
-      <c r="GL3" t="inlineStr"/>
-      <c r="GM3" t="inlineStr"/>
-      <c r="GN3" t="inlineStr"/>
-      <c r="GO3" t="inlineStr"/>
-      <c r="GP3" t="inlineStr"/>
-      <c r="GQ3" t="inlineStr"/>
-      <c r="GR3" t="inlineStr"/>
-      <c r="GS3" t="inlineStr"/>
-      <c r="GT3" t="inlineStr"/>
-      <c r="GU3" t="inlineStr"/>
-      <c r="GV3" t="inlineStr"/>
-      <c r="GW3" t="inlineStr"/>
-      <c r="GX3" t="inlineStr"/>
-      <c r="GY3" t="inlineStr"/>
-      <c r="GZ3" t="inlineStr"/>
-      <c r="HA3" t="inlineStr"/>
-      <c r="HB3" t="inlineStr"/>
-      <c r="HC3" t="inlineStr"/>
-      <c r="HD3" t="inlineStr"/>
-      <c r="HE3" t="inlineStr"/>
-      <c r="HF3" t="inlineStr"/>
-      <c r="HG3" t="inlineStr"/>
-      <c r="HH3" t="inlineStr"/>
-      <c r="HI3" t="inlineStr"/>
-      <c r="HJ3" t="inlineStr"/>
-      <c r="HK3" t="inlineStr"/>
-      <c r="HL3" t="inlineStr"/>
-      <c r="HM3" t="inlineStr"/>
-      <c r="HN3" t="inlineStr"/>
-      <c r="HO3" t="inlineStr"/>
-      <c r="HP3" t="inlineStr"/>
-      <c r="HQ3" t="inlineStr"/>
-      <c r="HR3" t="inlineStr"/>
-      <c r="HS3" t="inlineStr"/>
-      <c r="HT3" t="inlineStr"/>
-      <c r="HU3" t="inlineStr"/>
-      <c r="HV3" t="inlineStr"/>
-      <c r="HW3" t="inlineStr"/>
       <c r="HX3" t="inlineStr">
         <is>
           <t>0.0625</t>
@@ -3776,9 +3314,6 @@
           <t>25.0</t>
         </is>
       </c>
-      <c r="ID3" t="inlineStr"/>
-      <c r="IE3" t="inlineStr"/>
-      <c r="IF3" t="inlineStr"/>
       <c r="IG3" t="inlineStr">
         <is>
           <t>7.21</t>
@@ -3789,7 +3324,6 @@
           <t>7.63</t>
         </is>
       </c>
-      <c r="II3" t="inlineStr"/>
       <c r="IJ3" t="inlineStr">
         <is>
           <t>8.01</t>
@@ -3820,23 +3354,11 @@
           <t>8.58</t>
         </is>
       </c>
-      <c r="IP3" t="inlineStr"/>
-      <c r="IQ3" t="inlineStr"/>
-      <c r="IR3" t="inlineStr"/>
-      <c r="IS3" t="inlineStr"/>
-      <c r="IT3" t="inlineStr"/>
-      <c r="IU3" t="inlineStr"/>
-      <c r="IV3" t="inlineStr"/>
-      <c r="IW3" t="inlineStr"/>
-      <c r="IX3" t="inlineStr"/>
-      <c r="IY3" t="inlineStr"/>
-      <c r="IZ3" t="inlineStr"/>
       <c r="JA3" t="inlineStr">
         <is>
           <t>106</t>
         </is>
       </c>
-      <c r="JB3" t="inlineStr"/>
       <c r="JC3" t="inlineStr">
         <is>
           <t>111</t>
@@ -3867,10 +3389,6 @@
           <t>119</t>
         </is>
       </c>
-      <c r="JI3" t="inlineStr"/>
-      <c r="JJ3" t="inlineStr"/>
-      <c r="JK3" t="inlineStr"/>
-      <c r="JL3" t="inlineStr"/>
       <c r="JM3" t="inlineStr">
         <is>
           <t>-3</t>
@@ -3901,136 +3419,1336 @@
           <t>4</t>
         </is>
       </c>
-      <c r="JS3" t="inlineStr"/>
-      <c r="JT3" t="inlineStr"/>
-      <c r="JU3" t="inlineStr"/>
-      <c r="JV3" t="inlineStr"/>
-      <c r="JW3" t="inlineStr"/>
-      <c r="JX3" t="inlineStr"/>
-      <c r="JY3" t="inlineStr"/>
-      <c r="JZ3" t="inlineStr"/>
-      <c r="KA3" t="inlineStr"/>
-      <c r="KB3" t="inlineStr"/>
-      <c r="KC3" t="inlineStr"/>
-      <c r="KD3" t="inlineStr"/>
-      <c r="KE3" t="inlineStr"/>
-      <c r="KF3" t="inlineStr"/>
-      <c r="KG3" t="inlineStr"/>
-      <c r="KH3" t="inlineStr"/>
-      <c r="KI3" t="inlineStr"/>
-      <c r="KJ3" t="inlineStr"/>
-      <c r="KK3" t="inlineStr"/>
-      <c r="KL3" t="inlineStr"/>
-      <c r="KM3" t="inlineStr"/>
-      <c r="KN3" t="inlineStr"/>
-      <c r="KO3" t="inlineStr"/>
-      <c r="KP3" t="inlineStr"/>
-      <c r="KQ3" t="inlineStr"/>
-      <c r="KR3" t="inlineStr"/>
-      <c r="KS3" t="inlineStr"/>
-      <c r="KT3" t="inlineStr"/>
-      <c r="KU3" t="inlineStr"/>
-      <c r="KV3" t="inlineStr"/>
-      <c r="KW3" t="inlineStr"/>
-      <c r="KX3" t="inlineStr"/>
-      <c r="KY3" t="inlineStr"/>
-      <c r="KZ3" t="inlineStr"/>
-      <c r="LA3" t="inlineStr"/>
-      <c r="LB3" t="inlineStr"/>
-      <c r="LC3" t="inlineStr"/>
-      <c r="LD3" t="inlineStr"/>
-      <c r="LE3" t="inlineStr"/>
-      <c r="LF3" t="inlineStr"/>
-      <c r="LG3" t="inlineStr"/>
-      <c r="LH3" t="inlineStr"/>
-      <c r="LI3" t="inlineStr"/>
-      <c r="LJ3" t="inlineStr"/>
-      <c r="LK3" t="inlineStr"/>
-      <c r="LL3" t="inlineStr"/>
-      <c r="LM3" t="inlineStr"/>
-      <c r="LN3" t="inlineStr"/>
-      <c r="LO3" t="inlineStr"/>
-      <c r="LP3" t="inlineStr"/>
-      <c r="LQ3" t="inlineStr"/>
-      <c r="LR3" t="inlineStr"/>
-      <c r="LS3" t="inlineStr"/>
-      <c r="LT3" t="inlineStr"/>
-      <c r="LU3" t="inlineStr"/>
-      <c r="LV3" t="inlineStr"/>
-      <c r="LW3" t="inlineStr"/>
-      <c r="LX3" t="inlineStr"/>
-      <c r="LY3" t="inlineStr"/>
-      <c r="LZ3" t="inlineStr"/>
-      <c r="MA3" t="inlineStr"/>
-      <c r="MB3" t="inlineStr"/>
-      <c r="MC3" t="inlineStr"/>
-      <c r="MD3" t="inlineStr"/>
-      <c r="ME3" t="inlineStr"/>
-      <c r="MF3" t="inlineStr"/>
-      <c r="MG3" t="inlineStr"/>
-      <c r="MH3" t="inlineStr"/>
-      <c r="MI3" t="inlineStr"/>
-      <c r="MJ3" t="inlineStr"/>
-      <c r="MK3" t="inlineStr"/>
-      <c r="ML3" t="inlineStr"/>
-      <c r="MM3" t="inlineStr"/>
-      <c r="MN3" t="inlineStr"/>
-      <c r="MO3" t="inlineStr"/>
-      <c r="MP3" t="inlineStr"/>
-      <c r="MQ3" t="inlineStr"/>
-      <c r="MR3" t="inlineStr"/>
-      <c r="MS3" t="inlineStr"/>
-      <c r="MT3" t="inlineStr"/>
-      <c r="MU3" t="inlineStr"/>
-      <c r="MV3" t="inlineStr"/>
-      <c r="MW3" t="inlineStr"/>
-      <c r="MX3" t="inlineStr"/>
-      <c r="MY3" t="inlineStr"/>
-      <c r="MZ3" t="inlineStr"/>
-      <c r="NA3" t="inlineStr"/>
-      <c r="NB3" t="inlineStr"/>
-      <c r="NC3" t="inlineStr"/>
-      <c r="ND3" t="inlineStr"/>
-      <c r="NE3" t="inlineStr"/>
-      <c r="NF3" t="inlineStr"/>
-      <c r="NG3" t="inlineStr"/>
-      <c r="NH3" t="inlineStr"/>
-      <c r="NI3" t="inlineStr"/>
-      <c r="NJ3" t="inlineStr"/>
-      <c r="NK3" t="inlineStr"/>
-      <c r="NL3" t="inlineStr"/>
-      <c r="NM3" t="inlineStr"/>
-      <c r="NN3" t="inlineStr"/>
-      <c r="NO3" t="inlineStr"/>
-      <c r="NP3" t="inlineStr"/>
-      <c r="NQ3" t="inlineStr"/>
-      <c r="NR3" t="inlineStr"/>
-      <c r="NS3" t="inlineStr"/>
-      <c r="NT3" t="inlineStr"/>
-      <c r="NU3" t="inlineStr"/>
-      <c r="NV3" t="inlineStr"/>
-      <c r="NW3" t="inlineStr"/>
-      <c r="NX3" t="inlineStr"/>
-      <c r="NY3" t="inlineStr"/>
-      <c r="NZ3" t="inlineStr"/>
-      <c r="OA3" t="inlineStr"/>
-      <c r="OB3" t="inlineStr"/>
-      <c r="OC3" t="inlineStr"/>
-      <c r="OD3" t="inlineStr"/>
-      <c r="OE3" t="inlineStr"/>
-      <c r="OF3" t="inlineStr"/>
-      <c r="OG3" t="inlineStr"/>
-      <c r="OH3" t="inlineStr"/>
-      <c r="OI3" t="inlineStr"/>
-      <c r="OJ3" t="inlineStr"/>
-      <c r="OK3" t="inlineStr"/>
-      <c r="OL3" t="inlineStr"/>
-      <c r="OM3" t="inlineStr"/>
-      <c r="ON3" t="inlineStr"/>
-      <c r="OO3" t="inlineStr"/>
-      <c r="OP3" t="inlineStr"/>
-      <c r="OQ3" t="inlineStr"/>
-      <c r="OR3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>type01</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>16.0</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>3.22</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>3.03</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>3.00</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>2.97</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>3.01</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>2.93</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>2.31</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>2.75</t>
+        </is>
+      </c>
+      <c r="AK4" t="inlineStr">
+        <is>
+          <t>94</t>
+        </is>
+      </c>
+      <c r="AM4" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="AN4" t="inlineStr">
+        <is>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="AO4" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="AP4" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="AQ4" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="AR4" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="AW4" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="AX4" t="inlineStr">
+        <is>
+          <t>.2</t>
+        </is>
+      </c>
+      <c r="AY4" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="AZ4" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="BA4" t="inlineStr">
+        <is>
+          <t>.7</t>
+        </is>
+      </c>
+      <c r="BB4" t="inlineStr">
+        <is>
+          <t>.9</t>
+        </is>
+      </c>
+      <c r="BO4" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="BP4" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="BQ4" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="BR4" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="BS4" t="inlineStr">
+        <is>
+          <t>15.0</t>
+        </is>
+      </c>
+      <c r="BT4" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="BX4" t="inlineStr">
+        <is>
+          <t>2.51</t>
+        </is>
+      </c>
+      <c r="BY4" t="inlineStr">
+        <is>
+          <t>2.20</t>
+        </is>
+      </c>
+      <c r="CA4" t="inlineStr">
+        <is>
+          <t>2.23</t>
+        </is>
+      </c>
+      <c r="CB4" t="inlineStr">
+        <is>
+          <t>2.25</t>
+        </is>
+      </c>
+      <c r="CC4" t="inlineStr">
+        <is>
+          <t>2.27</t>
+        </is>
+      </c>
+      <c r="CD4" t="inlineStr">
+        <is>
+          <t>2.20</t>
+        </is>
+      </c>
+      <c r="CE4" t="inlineStr">
+        <is>
+          <t>2.10</t>
+        </is>
+      </c>
+      <c r="CF4" t="inlineStr">
+        <is>
+          <t>1.99</t>
+        </is>
+      </c>
+      <c r="CR4" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="CT4" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="CU4" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="CV4" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="CW4" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="CX4" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="CY4" t="inlineStr">
+        <is>
+          <t>79</t>
+        </is>
+      </c>
+      <c r="DD4" t="inlineStr">
+        <is>
+          <t>.2</t>
+        </is>
+      </c>
+      <c r="DE4" t="inlineStr">
+        <is>
+          <t>.2</t>
+        </is>
+      </c>
+      <c r="DF4" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="DG4" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="DH4" t="inlineStr">
+        <is>
+          <t>.3</t>
+        </is>
+      </c>
+      <c r="DI4" t="inlineStr">
+        <is>
+          <t>.13</t>
+        </is>
+      </c>
+      <c r="DP4" t="inlineStr">
+        <is>
+          <t>220</t>
+        </is>
+      </c>
+      <c r="EJ4" t="inlineStr">
+        <is>
+          <t>2.57</t>
+        </is>
+      </c>
+      <c r="EK4" t="inlineStr">
+        <is>
+          <t>1.75</t>
+        </is>
+      </c>
+      <c r="EL4" t="inlineStr">
+        <is>
+          <t>1.67</t>
+        </is>
+      </c>
+      <c r="EM4" t="inlineStr">
+        <is>
+          <t>1.69</t>
+        </is>
+      </c>
+      <c r="EN4" t="inlineStr">
+        <is>
+          <t>1.73</t>
+        </is>
+      </c>
+      <c r="EO4" t="inlineStr">
+        <is>
+          <t>1.69</t>
+        </is>
+      </c>
+      <c r="ET4" t="inlineStr">
+        <is>
+          <t>68</t>
+        </is>
+      </c>
+      <c r="EV4" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="EW4" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="EX4" t="inlineStr">
+        <is>
+          <t>63</t>
+        </is>
+      </c>
+      <c r="EY4" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="EZ4" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="FA4" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="FY4" t="inlineStr">
+        <is>
+          <t>.4</t>
+        </is>
+      </c>
+      <c r="FZ4" t="inlineStr">
+        <is>
+          <t>.3</t>
+        </is>
+      </c>
+      <c r="GA4" t="inlineStr">
+        <is>
+          <t>.0</t>
+        </is>
+      </c>
+      <c r="GB4" t="inlineStr">
+        <is>
+          <t>.3</t>
+        </is>
+      </c>
+      <c r="GC4" t="inlineStr">
+        <is>
+          <t>.11</t>
+        </is>
+      </c>
+      <c r="GD4" t="inlineStr">
+        <is>
+          <t>.24</t>
+        </is>
+      </c>
+      <c r="HX4" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="HY4" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="HZ4" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="IA4" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="IB4" t="inlineStr">
+        <is>
+          <t>16.0</t>
+        </is>
+      </c>
+      <c r="IC4" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="IG4" t="inlineStr">
+        <is>
+          <t>5.45</t>
+        </is>
+      </c>
+      <c r="IH4" t="inlineStr">
+        <is>
+          <t>9.33</t>
+        </is>
+      </c>
+      <c r="IJ4" t="inlineStr">
+        <is>
+          <t>7.32</t>
+        </is>
+      </c>
+      <c r="IK4" t="inlineStr">
+        <is>
+          <t>0.47</t>
+        </is>
+      </c>
+      <c r="IL4" t="inlineStr">
+        <is>
+          <t>7.99</t>
+        </is>
+      </c>
+      <c r="IM4" t="inlineStr">
+        <is>
+          <t>7.64</t>
+        </is>
+      </c>
+      <c r="IN4" t="inlineStr">
+        <is>
+          <t>3.12</t>
+        </is>
+      </c>
+      <c r="IO4" t="inlineStr">
+        <is>
+          <t>7.31</t>
+        </is>
+      </c>
+      <c r="JA4" t="inlineStr">
+        <is>
+          <t>153</t>
+        </is>
+      </c>
+      <c r="JC4" t="inlineStr">
+        <is>
+          <t>143</t>
+        </is>
+      </c>
+      <c r="JD4" t="inlineStr">
+        <is>
+          <t>155</t>
+        </is>
+      </c>
+      <c r="JE4" t="inlineStr">
+        <is>
+          <t>147</t>
+        </is>
+      </c>
+      <c r="JF4" t="inlineStr">
+        <is>
+          <t>140</t>
+        </is>
+      </c>
+      <c r="JG4" t="inlineStr">
+        <is>
+          <t>149</t>
+        </is>
+      </c>
+      <c r="JH4" t="inlineStr">
+        <is>
+          <t>134</t>
+        </is>
+      </c>
+      <c r="JM4" t="inlineStr">
+        <is>
+          <t>.9</t>
+        </is>
+      </c>
+      <c r="JN4" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="JO4" t="inlineStr">
+        <is>
+          <t>.7</t>
+        </is>
+      </c>
+      <c r="JP4" t="inlineStr">
+        <is>
+          <t>.11</t>
+        </is>
+      </c>
+      <c r="JQ4" t="inlineStr">
+        <is>
+          <t>.5</t>
+        </is>
+      </c>
+      <c r="JR4" t="inlineStr">
+        <is>
+          <t>.15</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>type01</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>16.0</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>3.22</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>3.03</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr"/>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>3.00</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>2.97</t>
+        </is>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>3.01</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>2.93</t>
+        </is>
+      </c>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>2.31</t>
+        </is>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>2.75</t>
+        </is>
+      </c>
+      <c r="Z5" t="inlineStr"/>
+      <c r="AA5" t="inlineStr"/>
+      <c r="AB5" t="inlineStr"/>
+      <c r="AC5" t="inlineStr"/>
+      <c r="AD5" t="inlineStr"/>
+      <c r="AE5" t="inlineStr"/>
+      <c r="AF5" t="inlineStr"/>
+      <c r="AG5" t="inlineStr"/>
+      <c r="AH5" t="inlineStr"/>
+      <c r="AI5" t="inlineStr"/>
+      <c r="AJ5" t="inlineStr"/>
+      <c r="AK5" t="inlineStr">
+        <is>
+          <t>94</t>
+        </is>
+      </c>
+      <c r="AL5" t="inlineStr"/>
+      <c r="AM5" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="AN5" t="inlineStr">
+        <is>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="AO5" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="AP5" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="AQ5" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="AR5" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="AS5" t="inlineStr"/>
+      <c r="AT5" t="inlineStr"/>
+      <c r="AU5" t="inlineStr"/>
+      <c r="AV5" t="inlineStr"/>
+      <c r="AW5" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="AX5" t="inlineStr">
+        <is>
+          <t>.2</t>
+        </is>
+      </c>
+      <c r="AY5" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="AZ5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="BA5" t="inlineStr">
+        <is>
+          <t>.7</t>
+        </is>
+      </c>
+      <c r="BB5" t="inlineStr">
+        <is>
+          <t>.9</t>
+        </is>
+      </c>
+      <c r="BC5" t="inlineStr"/>
+      <c r="BD5" t="inlineStr"/>
+      <c r="BE5" t="inlineStr"/>
+      <c r="BF5" t="inlineStr"/>
+      <c r="BG5" t="inlineStr"/>
+      <c r="BH5" t="inlineStr"/>
+      <c r="BI5" t="inlineStr"/>
+      <c r="BJ5" t="inlineStr"/>
+      <c r="BK5" t="inlineStr"/>
+      <c r="BL5" t="inlineStr"/>
+      <c r="BM5" t="inlineStr"/>
+      <c r="BN5" t="inlineStr"/>
+      <c r="BO5" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="BP5" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="BQ5" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="BR5" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="BS5" t="inlineStr">
+        <is>
+          <t>15.0</t>
+        </is>
+      </c>
+      <c r="BT5" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="BU5" t="inlineStr"/>
+      <c r="BV5" t="inlineStr"/>
+      <c r="BW5" t="inlineStr"/>
+      <c r="BX5" t="inlineStr">
+        <is>
+          <t>2.51</t>
+        </is>
+      </c>
+      <c r="BY5" t="inlineStr">
+        <is>
+          <t>2.20</t>
+        </is>
+      </c>
+      <c r="BZ5" t="inlineStr"/>
+      <c r="CA5" t="inlineStr">
+        <is>
+          <t>2.23</t>
+        </is>
+      </c>
+      <c r="CB5" t="inlineStr">
+        <is>
+          <t>2.25</t>
+        </is>
+      </c>
+      <c r="CC5" t="inlineStr">
+        <is>
+          <t>2.27</t>
+        </is>
+      </c>
+      <c r="CD5" t="inlineStr">
+        <is>
+          <t>2.20</t>
+        </is>
+      </c>
+      <c r="CE5" t="inlineStr">
+        <is>
+          <t>2.10</t>
+        </is>
+      </c>
+      <c r="CF5" t="inlineStr">
+        <is>
+          <t>1.99</t>
+        </is>
+      </c>
+      <c r="CG5" t="inlineStr"/>
+      <c r="CH5" t="inlineStr"/>
+      <c r="CI5" t="inlineStr"/>
+      <c r="CJ5" t="inlineStr"/>
+      <c r="CK5" t="inlineStr"/>
+      <c r="CL5" t="inlineStr"/>
+      <c r="CM5" t="inlineStr"/>
+      <c r="CN5" t="inlineStr"/>
+      <c r="CO5" t="inlineStr"/>
+      <c r="CP5" t="inlineStr"/>
+      <c r="CQ5" t="inlineStr"/>
+      <c r="CR5" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="CS5" t="inlineStr"/>
+      <c r="CT5" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="CU5" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="CV5" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="CW5" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="CX5" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="CY5" t="inlineStr">
+        <is>
+          <t>79</t>
+        </is>
+      </c>
+      <c r="CZ5" t="inlineStr"/>
+      <c r="DA5" t="inlineStr"/>
+      <c r="DB5" t="inlineStr"/>
+      <c r="DC5" t="inlineStr"/>
+      <c r="DD5" t="inlineStr">
+        <is>
+          <t>.2</t>
+        </is>
+      </c>
+      <c r="DE5" t="inlineStr">
+        <is>
+          <t>.2</t>
+        </is>
+      </c>
+      <c r="DF5" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="DG5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="DH5" t="inlineStr">
+        <is>
+          <t>.3</t>
+        </is>
+      </c>
+      <c r="DI5" t="inlineStr">
+        <is>
+          <t>.13</t>
+        </is>
+      </c>
+      <c r="DJ5" t="inlineStr"/>
+      <c r="DK5" t="inlineStr"/>
+      <c r="DL5" t="inlineStr"/>
+      <c r="DM5" t="inlineStr"/>
+      <c r="DN5" t="inlineStr"/>
+      <c r="DO5" t="inlineStr"/>
+      <c r="DP5" t="inlineStr">
+        <is>
+          <t>220</t>
+        </is>
+      </c>
+      <c r="DQ5" t="inlineStr"/>
+      <c r="DR5" t="inlineStr"/>
+      <c r="DS5" t="inlineStr"/>
+      <c r="DT5" t="inlineStr"/>
+      <c r="DU5" t="inlineStr"/>
+      <c r="DV5" t="inlineStr"/>
+      <c r="DW5" t="inlineStr"/>
+      <c r="DX5" t="inlineStr"/>
+      <c r="DY5" t="inlineStr"/>
+      <c r="DZ5" t="inlineStr"/>
+      <c r="EA5" t="inlineStr"/>
+      <c r="EB5" t="inlineStr"/>
+      <c r="EC5" t="inlineStr"/>
+      <c r="ED5" t="inlineStr"/>
+      <c r="EE5" t="inlineStr"/>
+      <c r="EF5" t="inlineStr"/>
+      <c r="EG5" t="inlineStr"/>
+      <c r="EH5" t="inlineStr"/>
+      <c r="EI5" t="inlineStr"/>
+      <c r="EJ5" t="inlineStr">
+        <is>
+          <t>2.57</t>
+        </is>
+      </c>
+      <c r="EK5" t="inlineStr">
+        <is>
+          <t>1.75</t>
+        </is>
+      </c>
+      <c r="EL5" t="inlineStr">
+        <is>
+          <t>1.67</t>
+        </is>
+      </c>
+      <c r="EM5" t="inlineStr">
+        <is>
+          <t>1.69</t>
+        </is>
+      </c>
+      <c r="EN5" t="inlineStr">
+        <is>
+          <t>1.73</t>
+        </is>
+      </c>
+      <c r="EO5" t="inlineStr">
+        <is>
+          <t>1.69</t>
+        </is>
+      </c>
+      <c r="EP5" t="inlineStr"/>
+      <c r="EQ5" t="inlineStr"/>
+      <c r="ER5" t="inlineStr"/>
+      <c r="ES5" t="inlineStr"/>
+      <c r="ET5" t="inlineStr">
+        <is>
+          <t>68</t>
+        </is>
+      </c>
+      <c r="EU5" t="inlineStr"/>
+      <c r="EV5" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="EW5" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="EX5" t="inlineStr">
+        <is>
+          <t>63</t>
+        </is>
+      </c>
+      <c r="EY5" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="EZ5" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="FA5" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="FB5" t="inlineStr"/>
+      <c r="FC5" t="inlineStr"/>
+      <c r="FD5" t="inlineStr"/>
+      <c r="FE5" t="inlineStr"/>
+      <c r="FF5" t="inlineStr"/>
+      <c r="FG5" t="inlineStr"/>
+      <c r="FH5" t="inlineStr"/>
+      <c r="FI5" t="inlineStr"/>
+      <c r="FJ5" t="inlineStr"/>
+      <c r="FK5" t="inlineStr"/>
+      <c r="FL5" t="inlineStr"/>
+      <c r="FM5" t="inlineStr"/>
+      <c r="FN5" t="inlineStr"/>
+      <c r="FO5" t="inlineStr"/>
+      <c r="FP5" t="inlineStr"/>
+      <c r="FQ5" t="inlineStr"/>
+      <c r="FR5" t="inlineStr"/>
+      <c r="FS5" t="inlineStr"/>
+      <c r="FT5" t="inlineStr"/>
+      <c r="FU5" t="inlineStr"/>
+      <c r="FV5" t="inlineStr"/>
+      <c r="FW5" t="inlineStr"/>
+      <c r="FX5" t="inlineStr"/>
+      <c r="FY5" t="inlineStr">
+        <is>
+          <t>.4</t>
+        </is>
+      </c>
+      <c r="FZ5" t="inlineStr">
+        <is>
+          <t>.3</t>
+        </is>
+      </c>
+      <c r="GA5" t="inlineStr">
+        <is>
+          <t>.0</t>
+        </is>
+      </c>
+      <c r="GB5" t="inlineStr">
+        <is>
+          <t>.3</t>
+        </is>
+      </c>
+      <c r="GC5" t="inlineStr">
+        <is>
+          <t>.11</t>
+        </is>
+      </c>
+      <c r="GD5" t="inlineStr">
+        <is>
+          <t>.24</t>
+        </is>
+      </c>
+      <c r="GE5" t="inlineStr"/>
+      <c r="GF5" t="inlineStr"/>
+      <c r="GG5" t="inlineStr"/>
+      <c r="GH5" t="inlineStr"/>
+      <c r="GI5" t="inlineStr"/>
+      <c r="GJ5" t="inlineStr"/>
+      <c r="GK5" t="inlineStr"/>
+      <c r="GL5" t="inlineStr"/>
+      <c r="GM5" t="inlineStr"/>
+      <c r="GN5" t="inlineStr"/>
+      <c r="GO5" t="inlineStr"/>
+      <c r="GP5" t="inlineStr"/>
+      <c r="GQ5" t="inlineStr"/>
+      <c r="GR5" t="inlineStr"/>
+      <c r="GS5" t="inlineStr"/>
+      <c r="GT5" t="inlineStr"/>
+      <c r="GU5" t="inlineStr"/>
+      <c r="GV5" t="inlineStr"/>
+      <c r="GW5" t="inlineStr"/>
+      <c r="GX5" t="inlineStr"/>
+      <c r="GY5" t="inlineStr"/>
+      <c r="GZ5" t="inlineStr"/>
+      <c r="HA5" t="inlineStr"/>
+      <c r="HB5" t="inlineStr"/>
+      <c r="HC5" t="inlineStr"/>
+      <c r="HD5" t="inlineStr"/>
+      <c r="HE5" t="inlineStr"/>
+      <c r="HF5" t="inlineStr"/>
+      <c r="HG5" t="inlineStr"/>
+      <c r="HH5" t="inlineStr"/>
+      <c r="HI5" t="inlineStr"/>
+      <c r="HJ5" t="inlineStr"/>
+      <c r="HK5" t="inlineStr"/>
+      <c r="HL5" t="inlineStr"/>
+      <c r="HM5" t="inlineStr"/>
+      <c r="HN5" t="inlineStr"/>
+      <c r="HO5" t="inlineStr"/>
+      <c r="HP5" t="inlineStr"/>
+      <c r="HQ5" t="inlineStr"/>
+      <c r="HR5" t="inlineStr"/>
+      <c r="HS5" t="inlineStr"/>
+      <c r="HT5" t="inlineStr"/>
+      <c r="HU5" t="inlineStr"/>
+      <c r="HV5" t="inlineStr"/>
+      <c r="HW5" t="inlineStr"/>
+      <c r="HX5" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="HY5" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="HZ5" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="IA5" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="IB5" t="inlineStr">
+        <is>
+          <t>16.0</t>
+        </is>
+      </c>
+      <c r="IC5" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="ID5" t="inlineStr"/>
+      <c r="IE5" t="inlineStr"/>
+      <c r="IF5" t="inlineStr"/>
+      <c r="IG5" t="inlineStr">
+        <is>
+          <t>5.45</t>
+        </is>
+      </c>
+      <c r="IH5" t="inlineStr">
+        <is>
+          <t>9.33</t>
+        </is>
+      </c>
+      <c r="II5" t="inlineStr"/>
+      <c r="IJ5" t="inlineStr">
+        <is>
+          <t>7.32</t>
+        </is>
+      </c>
+      <c r="IK5" t="inlineStr">
+        <is>
+          <t>0.47</t>
+        </is>
+      </c>
+      <c r="IL5" t="inlineStr">
+        <is>
+          <t>7.99</t>
+        </is>
+      </c>
+      <c r="IM5" t="inlineStr">
+        <is>
+          <t>7.64</t>
+        </is>
+      </c>
+      <c r="IN5" t="inlineStr">
+        <is>
+          <t>3.12</t>
+        </is>
+      </c>
+      <c r="IO5" t="inlineStr">
+        <is>
+          <t>7.31</t>
+        </is>
+      </c>
+      <c r="IP5" t="inlineStr"/>
+      <c r="IQ5" t="inlineStr"/>
+      <c r="IR5" t="inlineStr"/>
+      <c r="IS5" t="inlineStr"/>
+      <c r="IT5" t="inlineStr"/>
+      <c r="IU5" t="inlineStr"/>
+      <c r="IV5" t="inlineStr"/>
+      <c r="IW5" t="inlineStr"/>
+      <c r="IX5" t="inlineStr"/>
+      <c r="IY5" t="inlineStr"/>
+      <c r="IZ5" t="inlineStr"/>
+      <c r="JA5" t="inlineStr">
+        <is>
+          <t>153</t>
+        </is>
+      </c>
+      <c r="JB5" t="inlineStr"/>
+      <c r="JC5" t="inlineStr">
+        <is>
+          <t>143</t>
+        </is>
+      </c>
+      <c r="JD5" t="inlineStr">
+        <is>
+          <t>155</t>
+        </is>
+      </c>
+      <c r="JE5" t="inlineStr">
+        <is>
+          <t>147</t>
+        </is>
+      </c>
+      <c r="JF5" t="inlineStr">
+        <is>
+          <t>140</t>
+        </is>
+      </c>
+      <c r="JG5" t="inlineStr">
+        <is>
+          <t>149</t>
+        </is>
+      </c>
+      <c r="JH5" t="inlineStr">
+        <is>
+          <t>134</t>
+        </is>
+      </c>
+      <c r="JI5" t="inlineStr"/>
+      <c r="JJ5" t="inlineStr"/>
+      <c r="JK5" t="inlineStr"/>
+      <c r="JL5" t="inlineStr"/>
+      <c r="JM5" t="inlineStr">
+        <is>
+          <t>.9</t>
+        </is>
+      </c>
+      <c r="JN5" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="JO5" t="inlineStr">
+        <is>
+          <t>.7</t>
+        </is>
+      </c>
+      <c r="JP5" t="inlineStr">
+        <is>
+          <t>.11</t>
+        </is>
+      </c>
+      <c r="JQ5" t="inlineStr">
+        <is>
+          <t>.5</t>
+        </is>
+      </c>
+      <c r="JR5" t="inlineStr">
+        <is>
+          <t>.15</t>
+        </is>
+      </c>
+      <c r="JS5" t="inlineStr"/>
+      <c r="JT5" t="inlineStr"/>
+      <c r="JU5" t="inlineStr"/>
+      <c r="JV5" t="inlineStr"/>
+      <c r="JW5" t="inlineStr"/>
+      <c r="JX5" t="inlineStr"/>
+      <c r="JY5" t="inlineStr"/>
+      <c r="JZ5" t="inlineStr"/>
+      <c r="KA5" t="inlineStr"/>
+      <c r="KB5" t="inlineStr"/>
+      <c r="KC5" t="inlineStr"/>
+      <c r="KD5" t="inlineStr"/>
+      <c r="KE5" t="inlineStr"/>
+      <c r="KF5" t="inlineStr"/>
+      <c r="KG5" t="inlineStr"/>
+      <c r="KH5" t="inlineStr"/>
+      <c r="KI5" t="inlineStr"/>
+      <c r="KJ5" t="inlineStr"/>
+      <c r="KK5" t="inlineStr"/>
+      <c r="KL5" t="inlineStr"/>
+      <c r="KM5" t="inlineStr"/>
+      <c r="KN5" t="inlineStr"/>
+      <c r="KO5" t="inlineStr"/>
+      <c r="KP5" t="inlineStr"/>
+      <c r="KQ5" t="inlineStr"/>
+      <c r="KR5" t="inlineStr"/>
+      <c r="KS5" t="inlineStr"/>
+      <c r="KT5" t="inlineStr"/>
+      <c r="KU5" t="inlineStr"/>
+      <c r="KV5" t="inlineStr"/>
+      <c r="KW5" t="inlineStr"/>
+      <c r="KX5" t="inlineStr"/>
+      <c r="KY5" t="inlineStr"/>
+      <c r="KZ5" t="inlineStr"/>
+      <c r="LA5" t="inlineStr"/>
+      <c r="LB5" t="inlineStr"/>
+      <c r="LC5" t="inlineStr"/>
+      <c r="LD5" t="inlineStr"/>
+      <c r="LE5" t="inlineStr"/>
+      <c r="LF5" t="inlineStr"/>
+      <c r="LG5" t="inlineStr"/>
+      <c r="LH5" t="inlineStr"/>
+      <c r="LI5" t="inlineStr"/>
+      <c r="LJ5" t="inlineStr"/>
+      <c r="LK5" t="inlineStr"/>
+      <c r="LL5" t="inlineStr"/>
+      <c r="LM5" t="inlineStr"/>
+      <c r="LN5" t="inlineStr"/>
+      <c r="LO5" t="inlineStr"/>
+      <c r="LP5" t="inlineStr"/>
+      <c r="LQ5" t="inlineStr"/>
+      <c r="LR5" t="inlineStr"/>
+      <c r="LS5" t="inlineStr"/>
+      <c r="LT5" t="inlineStr"/>
+      <c r="LU5" t="inlineStr"/>
+      <c r="LV5" t="inlineStr"/>
+      <c r="LW5" t="inlineStr"/>
+      <c r="LX5" t="inlineStr"/>
+      <c r="LY5" t="inlineStr"/>
+      <c r="LZ5" t="inlineStr"/>
+      <c r="MA5" t="inlineStr"/>
+      <c r="MB5" t="inlineStr"/>
+      <c r="MC5" t="inlineStr"/>
+      <c r="MD5" t="inlineStr"/>
+      <c r="ME5" t="inlineStr"/>
+      <c r="MF5" t="inlineStr"/>
+      <c r="MG5" t="inlineStr"/>
+      <c r="MH5" t="inlineStr"/>
+      <c r="MI5" t="inlineStr"/>
+      <c r="MJ5" t="inlineStr"/>
+      <c r="MK5" t="inlineStr"/>
+      <c r="ML5" t="inlineStr"/>
+      <c r="MM5" t="inlineStr"/>
+      <c r="MN5" t="inlineStr"/>
+      <c r="MO5" t="inlineStr"/>
+      <c r="MP5" t="inlineStr"/>
+      <c r="MQ5" t="inlineStr"/>
+      <c r="MR5" t="inlineStr"/>
+      <c r="MS5" t="inlineStr"/>
+      <c r="MT5" t="inlineStr"/>
+      <c r="MU5" t="inlineStr"/>
+      <c r="MV5" t="inlineStr"/>
+      <c r="MW5" t="inlineStr"/>
+      <c r="MX5" t="inlineStr"/>
+      <c r="MY5" t="inlineStr"/>
+      <c r="MZ5" t="inlineStr"/>
+      <c r="NA5" t="inlineStr"/>
+      <c r="NB5" t="inlineStr"/>
+      <c r="NC5" t="inlineStr"/>
+      <c r="ND5" t="inlineStr"/>
+      <c r="NE5" t="inlineStr"/>
+      <c r="NF5" t="inlineStr"/>
+      <c r="NG5" t="inlineStr"/>
+      <c r="NH5" t="inlineStr"/>
+      <c r="NI5" t="inlineStr"/>
+      <c r="NJ5" t="inlineStr"/>
+      <c r="NK5" t="inlineStr"/>
+      <c r="NL5" t="inlineStr"/>
+      <c r="NM5" t="inlineStr"/>
+      <c r="NN5" t="inlineStr"/>
+      <c r="NO5" t="inlineStr"/>
+      <c r="NP5" t="inlineStr"/>
+      <c r="NQ5" t="inlineStr"/>
+      <c r="NR5" t="inlineStr"/>
+      <c r="NS5" t="inlineStr"/>
+      <c r="NT5" t="inlineStr"/>
+      <c r="NU5" t="inlineStr"/>
+      <c r="NV5" t="inlineStr"/>
+      <c r="NW5" t="inlineStr"/>
+      <c r="NX5" t="inlineStr"/>
+      <c r="NY5" t="inlineStr"/>
+      <c r="NZ5" t="inlineStr"/>
+      <c r="OA5" t="inlineStr"/>
+      <c r="OB5" t="inlineStr"/>
+      <c r="OC5" t="inlineStr"/>
+      <c r="OD5" t="inlineStr"/>
+      <c r="OE5" t="inlineStr"/>
+      <c r="OF5" t="inlineStr"/>
+      <c r="OG5" t="inlineStr"/>
+      <c r="OH5" t="inlineStr"/>
+      <c r="OI5" t="inlineStr"/>
+      <c r="OJ5" t="inlineStr"/>
+      <c r="OK5" t="inlineStr"/>
+      <c r="OL5" t="inlineStr"/>
+      <c r="OM5" t="inlineStr"/>
+      <c r="ON5" t="inlineStr"/>
+      <c r="OO5" t="inlineStr"/>
+      <c r="OP5" t="inlineStr"/>
+      <c r="OQ5" t="inlineStr"/>
+      <c r="OR5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
c: main argument arr
</commit_message>
<xml_diff>
--- a/OOMII.xlsx
+++ b/OOMII.xlsx
@@ -346,7 +346,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:OR5"/>
+  <dimension ref="A1:OR9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3938,12 +3938,6 @@
           <t>type01</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr">
         <is>
           <t>0.0625</t>
@@ -3974,9 +3968,6 @@
           <t>25.0</t>
         </is>
       </c>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
-      <c r="P5" t="inlineStr"/>
       <c r="Q5" t="inlineStr">
         <is>
           <t>3.22</t>
@@ -3987,7 +3978,6 @@
           <t>3.03</t>
         </is>
       </c>
-      <c r="S5" t="inlineStr"/>
       <c r="T5" t="inlineStr">
         <is>
           <t>3.00</t>
@@ -4018,23 +4008,11 @@
           <t>2.75</t>
         </is>
       </c>
-      <c r="Z5" t="inlineStr"/>
-      <c r="AA5" t="inlineStr"/>
-      <c r="AB5" t="inlineStr"/>
-      <c r="AC5" t="inlineStr"/>
-      <c r="AD5" t="inlineStr"/>
-      <c r="AE5" t="inlineStr"/>
-      <c r="AF5" t="inlineStr"/>
-      <c r="AG5" t="inlineStr"/>
-      <c r="AH5" t="inlineStr"/>
-      <c r="AI5" t="inlineStr"/>
-      <c r="AJ5" t="inlineStr"/>
       <c r="AK5" t="inlineStr">
         <is>
           <t>94</t>
         </is>
       </c>
-      <c r="AL5" t="inlineStr"/>
       <c r="AM5" t="inlineStr">
         <is>
           <t>93</t>
@@ -4065,10 +4043,6 @@
           <t>35</t>
         </is>
       </c>
-      <c r="AS5" t="inlineStr"/>
-      <c r="AT5" t="inlineStr"/>
-      <c r="AU5" t="inlineStr"/>
-      <c r="AV5" t="inlineStr"/>
       <c r="AW5" t="inlineStr">
         <is>
           <t>.1</t>
@@ -4099,18 +4073,6 @@
           <t>.9</t>
         </is>
       </c>
-      <c r="BC5" t="inlineStr"/>
-      <c r="BD5" t="inlineStr"/>
-      <c r="BE5" t="inlineStr"/>
-      <c r="BF5" t="inlineStr"/>
-      <c r="BG5" t="inlineStr"/>
-      <c r="BH5" t="inlineStr"/>
-      <c r="BI5" t="inlineStr"/>
-      <c r="BJ5" t="inlineStr"/>
-      <c r="BK5" t="inlineStr"/>
-      <c r="BL5" t="inlineStr"/>
-      <c r="BM5" t="inlineStr"/>
-      <c r="BN5" t="inlineStr"/>
       <c r="BO5" t="inlineStr">
         <is>
           <t>0.0625</t>
@@ -4141,9 +4103,6 @@
           <t>25.0</t>
         </is>
       </c>
-      <c r="BU5" t="inlineStr"/>
-      <c r="BV5" t="inlineStr"/>
-      <c r="BW5" t="inlineStr"/>
       <c r="BX5" t="inlineStr">
         <is>
           <t>2.51</t>
@@ -4154,7 +4113,6 @@
           <t>2.20</t>
         </is>
       </c>
-      <c r="BZ5" t="inlineStr"/>
       <c r="CA5" t="inlineStr">
         <is>
           <t>2.23</t>
@@ -4185,23 +4143,11 @@
           <t>1.99</t>
         </is>
       </c>
-      <c r="CG5" t="inlineStr"/>
-      <c r="CH5" t="inlineStr"/>
-      <c r="CI5" t="inlineStr"/>
-      <c r="CJ5" t="inlineStr"/>
-      <c r="CK5" t="inlineStr"/>
-      <c r="CL5" t="inlineStr"/>
-      <c r="CM5" t="inlineStr"/>
-      <c r="CN5" t="inlineStr"/>
-      <c r="CO5" t="inlineStr"/>
-      <c r="CP5" t="inlineStr"/>
-      <c r="CQ5" t="inlineStr"/>
       <c r="CR5" t="inlineStr">
         <is>
           <t>91</t>
         </is>
       </c>
-      <c r="CS5" t="inlineStr"/>
       <c r="CT5" t="inlineStr">
         <is>
           <t>39</t>
@@ -4232,10 +4178,6 @@
           <t>79</t>
         </is>
       </c>
-      <c r="CZ5" t="inlineStr"/>
-      <c r="DA5" t="inlineStr"/>
-      <c r="DB5" t="inlineStr"/>
-      <c r="DC5" t="inlineStr"/>
       <c r="DD5" t="inlineStr">
         <is>
           <t>.2</t>
@@ -4266,36 +4208,11 @@
           <t>.13</t>
         </is>
       </c>
-      <c r="DJ5" t="inlineStr"/>
-      <c r="DK5" t="inlineStr"/>
-      <c r="DL5" t="inlineStr"/>
-      <c r="DM5" t="inlineStr"/>
-      <c r="DN5" t="inlineStr"/>
-      <c r="DO5" t="inlineStr"/>
       <c r="DP5" t="inlineStr">
         <is>
           <t>220</t>
         </is>
       </c>
-      <c r="DQ5" t="inlineStr"/>
-      <c r="DR5" t="inlineStr"/>
-      <c r="DS5" t="inlineStr"/>
-      <c r="DT5" t="inlineStr"/>
-      <c r="DU5" t="inlineStr"/>
-      <c r="DV5" t="inlineStr"/>
-      <c r="DW5" t="inlineStr"/>
-      <c r="DX5" t="inlineStr"/>
-      <c r="DY5" t="inlineStr"/>
-      <c r="DZ5" t="inlineStr"/>
-      <c r="EA5" t="inlineStr"/>
-      <c r="EB5" t="inlineStr"/>
-      <c r="EC5" t="inlineStr"/>
-      <c r="ED5" t="inlineStr"/>
-      <c r="EE5" t="inlineStr"/>
-      <c r="EF5" t="inlineStr"/>
-      <c r="EG5" t="inlineStr"/>
-      <c r="EH5" t="inlineStr"/>
-      <c r="EI5" t="inlineStr"/>
       <c r="EJ5" t="inlineStr">
         <is>
           <t>2.57</t>
@@ -4326,16 +4243,11 @@
           <t>1.69</t>
         </is>
       </c>
-      <c r="EP5" t="inlineStr"/>
-      <c r="EQ5" t="inlineStr"/>
-      <c r="ER5" t="inlineStr"/>
-      <c r="ES5" t="inlineStr"/>
       <c r="ET5" t="inlineStr">
         <is>
           <t>68</t>
         </is>
       </c>
-      <c r="EU5" t="inlineStr"/>
       <c r="EV5" t="inlineStr">
         <is>
           <t>55</t>
@@ -4366,29 +4278,6 @@
           <t>51</t>
         </is>
       </c>
-      <c r="FB5" t="inlineStr"/>
-      <c r="FC5" t="inlineStr"/>
-      <c r="FD5" t="inlineStr"/>
-      <c r="FE5" t="inlineStr"/>
-      <c r="FF5" t="inlineStr"/>
-      <c r="FG5" t="inlineStr"/>
-      <c r="FH5" t="inlineStr"/>
-      <c r="FI5" t="inlineStr"/>
-      <c r="FJ5" t="inlineStr"/>
-      <c r="FK5" t="inlineStr"/>
-      <c r="FL5" t="inlineStr"/>
-      <c r="FM5" t="inlineStr"/>
-      <c r="FN5" t="inlineStr"/>
-      <c r="FO5" t="inlineStr"/>
-      <c r="FP5" t="inlineStr"/>
-      <c r="FQ5" t="inlineStr"/>
-      <c r="FR5" t="inlineStr"/>
-      <c r="FS5" t="inlineStr"/>
-      <c r="FT5" t="inlineStr"/>
-      <c r="FU5" t="inlineStr"/>
-      <c r="FV5" t="inlineStr"/>
-      <c r="FW5" t="inlineStr"/>
-      <c r="FX5" t="inlineStr"/>
       <c r="FY5" t="inlineStr">
         <is>
           <t>.4</t>
@@ -4419,51 +4308,6 @@
           <t>.24</t>
         </is>
       </c>
-      <c r="GE5" t="inlineStr"/>
-      <c r="GF5" t="inlineStr"/>
-      <c r="GG5" t="inlineStr"/>
-      <c r="GH5" t="inlineStr"/>
-      <c r="GI5" t="inlineStr"/>
-      <c r="GJ5" t="inlineStr"/>
-      <c r="GK5" t="inlineStr"/>
-      <c r="GL5" t="inlineStr"/>
-      <c r="GM5" t="inlineStr"/>
-      <c r="GN5" t="inlineStr"/>
-      <c r="GO5" t="inlineStr"/>
-      <c r="GP5" t="inlineStr"/>
-      <c r="GQ5" t="inlineStr"/>
-      <c r="GR5" t="inlineStr"/>
-      <c r="GS5" t="inlineStr"/>
-      <c r="GT5" t="inlineStr"/>
-      <c r="GU5" t="inlineStr"/>
-      <c r="GV5" t="inlineStr"/>
-      <c r="GW5" t="inlineStr"/>
-      <c r="GX5" t="inlineStr"/>
-      <c r="GY5" t="inlineStr"/>
-      <c r="GZ5" t="inlineStr"/>
-      <c r="HA5" t="inlineStr"/>
-      <c r="HB5" t="inlineStr"/>
-      <c r="HC5" t="inlineStr"/>
-      <c r="HD5" t="inlineStr"/>
-      <c r="HE5" t="inlineStr"/>
-      <c r="HF5" t="inlineStr"/>
-      <c r="HG5" t="inlineStr"/>
-      <c r="HH5" t="inlineStr"/>
-      <c r="HI5" t="inlineStr"/>
-      <c r="HJ5" t="inlineStr"/>
-      <c r="HK5" t="inlineStr"/>
-      <c r="HL5" t="inlineStr"/>
-      <c r="HM5" t="inlineStr"/>
-      <c r="HN5" t="inlineStr"/>
-      <c r="HO5" t="inlineStr"/>
-      <c r="HP5" t="inlineStr"/>
-      <c r="HQ5" t="inlineStr"/>
-      <c r="HR5" t="inlineStr"/>
-      <c r="HS5" t="inlineStr"/>
-      <c r="HT5" t="inlineStr"/>
-      <c r="HU5" t="inlineStr"/>
-      <c r="HV5" t="inlineStr"/>
-      <c r="HW5" t="inlineStr"/>
       <c r="HX5" t="inlineStr">
         <is>
           <t>0.0625</t>
@@ -4494,9 +4338,6 @@
           <t>25.0</t>
         </is>
       </c>
-      <c r="ID5" t="inlineStr"/>
-      <c r="IE5" t="inlineStr"/>
-      <c r="IF5" t="inlineStr"/>
       <c r="IG5" t="inlineStr">
         <is>
           <t>5.45</t>
@@ -4507,7 +4348,6 @@
           <t>9.33</t>
         </is>
       </c>
-      <c r="II5" t="inlineStr"/>
       <c r="IJ5" t="inlineStr">
         <is>
           <t>7.32</t>
@@ -4538,23 +4378,11 @@
           <t>7.31</t>
         </is>
       </c>
-      <c r="IP5" t="inlineStr"/>
-      <c r="IQ5" t="inlineStr"/>
-      <c r="IR5" t="inlineStr"/>
-      <c r="IS5" t="inlineStr"/>
-      <c r="IT5" t="inlineStr"/>
-      <c r="IU5" t="inlineStr"/>
-      <c r="IV5" t="inlineStr"/>
-      <c r="IW5" t="inlineStr"/>
-      <c r="IX5" t="inlineStr"/>
-      <c r="IY5" t="inlineStr"/>
-      <c r="IZ5" t="inlineStr"/>
       <c r="JA5" t="inlineStr">
         <is>
           <t>153</t>
         </is>
       </c>
-      <c r="JB5" t="inlineStr"/>
       <c r="JC5" t="inlineStr">
         <is>
           <t>143</t>
@@ -4585,10 +4413,6 @@
           <t>134</t>
         </is>
       </c>
-      <c r="JI5" t="inlineStr"/>
-      <c r="JJ5" t="inlineStr"/>
-      <c r="JK5" t="inlineStr"/>
-      <c r="JL5" t="inlineStr"/>
       <c r="JM5" t="inlineStr">
         <is>
           <t>.9</t>
@@ -4619,136 +4443,2666 @@
           <t>.15</t>
         </is>
       </c>
-      <c r="JS5" t="inlineStr"/>
-      <c r="JT5" t="inlineStr"/>
-      <c r="JU5" t="inlineStr"/>
-      <c r="JV5" t="inlineStr"/>
-      <c r="JW5" t="inlineStr"/>
-      <c r="JX5" t="inlineStr"/>
-      <c r="JY5" t="inlineStr"/>
-      <c r="JZ5" t="inlineStr"/>
-      <c r="KA5" t="inlineStr"/>
-      <c r="KB5" t="inlineStr"/>
-      <c r="KC5" t="inlineStr"/>
-      <c r="KD5" t="inlineStr"/>
-      <c r="KE5" t="inlineStr"/>
-      <c r="KF5" t="inlineStr"/>
-      <c r="KG5" t="inlineStr"/>
-      <c r="KH5" t="inlineStr"/>
-      <c r="KI5" t="inlineStr"/>
-      <c r="KJ5" t="inlineStr"/>
-      <c r="KK5" t="inlineStr"/>
-      <c r="KL5" t="inlineStr"/>
-      <c r="KM5" t="inlineStr"/>
-      <c r="KN5" t="inlineStr"/>
-      <c r="KO5" t="inlineStr"/>
-      <c r="KP5" t="inlineStr"/>
-      <c r="KQ5" t="inlineStr"/>
-      <c r="KR5" t="inlineStr"/>
-      <c r="KS5" t="inlineStr"/>
-      <c r="KT5" t="inlineStr"/>
-      <c r="KU5" t="inlineStr"/>
-      <c r="KV5" t="inlineStr"/>
-      <c r="KW5" t="inlineStr"/>
-      <c r="KX5" t="inlineStr"/>
-      <c r="KY5" t="inlineStr"/>
-      <c r="KZ5" t="inlineStr"/>
-      <c r="LA5" t="inlineStr"/>
-      <c r="LB5" t="inlineStr"/>
-      <c r="LC5" t="inlineStr"/>
-      <c r="LD5" t="inlineStr"/>
-      <c r="LE5" t="inlineStr"/>
-      <c r="LF5" t="inlineStr"/>
-      <c r="LG5" t="inlineStr"/>
-      <c r="LH5" t="inlineStr"/>
-      <c r="LI5" t="inlineStr"/>
-      <c r="LJ5" t="inlineStr"/>
-      <c r="LK5" t="inlineStr"/>
-      <c r="LL5" t="inlineStr"/>
-      <c r="LM5" t="inlineStr"/>
-      <c r="LN5" t="inlineStr"/>
-      <c r="LO5" t="inlineStr"/>
-      <c r="LP5" t="inlineStr"/>
-      <c r="LQ5" t="inlineStr"/>
-      <c r="LR5" t="inlineStr"/>
-      <c r="LS5" t="inlineStr"/>
-      <c r="LT5" t="inlineStr"/>
-      <c r="LU5" t="inlineStr"/>
-      <c r="LV5" t="inlineStr"/>
-      <c r="LW5" t="inlineStr"/>
-      <c r="LX5" t="inlineStr"/>
-      <c r="LY5" t="inlineStr"/>
-      <c r="LZ5" t="inlineStr"/>
-      <c r="MA5" t="inlineStr"/>
-      <c r="MB5" t="inlineStr"/>
-      <c r="MC5" t="inlineStr"/>
-      <c r="MD5" t="inlineStr"/>
-      <c r="ME5" t="inlineStr"/>
-      <c r="MF5" t="inlineStr"/>
-      <c r="MG5" t="inlineStr"/>
-      <c r="MH5" t="inlineStr"/>
-      <c r="MI5" t="inlineStr"/>
-      <c r="MJ5" t="inlineStr"/>
-      <c r="MK5" t="inlineStr"/>
-      <c r="ML5" t="inlineStr"/>
-      <c r="MM5" t="inlineStr"/>
-      <c r="MN5" t="inlineStr"/>
-      <c r="MO5" t="inlineStr"/>
-      <c r="MP5" t="inlineStr"/>
-      <c r="MQ5" t="inlineStr"/>
-      <c r="MR5" t="inlineStr"/>
-      <c r="MS5" t="inlineStr"/>
-      <c r="MT5" t="inlineStr"/>
-      <c r="MU5" t="inlineStr"/>
-      <c r="MV5" t="inlineStr"/>
-      <c r="MW5" t="inlineStr"/>
-      <c r="MX5" t="inlineStr"/>
-      <c r="MY5" t="inlineStr"/>
-      <c r="MZ5" t="inlineStr"/>
-      <c r="NA5" t="inlineStr"/>
-      <c r="NB5" t="inlineStr"/>
-      <c r="NC5" t="inlineStr"/>
-      <c r="ND5" t="inlineStr"/>
-      <c r="NE5" t="inlineStr"/>
-      <c r="NF5" t="inlineStr"/>
-      <c r="NG5" t="inlineStr"/>
-      <c r="NH5" t="inlineStr"/>
-      <c r="NI5" t="inlineStr"/>
-      <c r="NJ5" t="inlineStr"/>
-      <c r="NK5" t="inlineStr"/>
-      <c r="NL5" t="inlineStr"/>
-      <c r="NM5" t="inlineStr"/>
-      <c r="NN5" t="inlineStr"/>
-      <c r="NO5" t="inlineStr"/>
-      <c r="NP5" t="inlineStr"/>
-      <c r="NQ5" t="inlineStr"/>
-      <c r="NR5" t="inlineStr"/>
-      <c r="NS5" t="inlineStr"/>
-      <c r="NT5" t="inlineStr"/>
-      <c r="NU5" t="inlineStr"/>
-      <c r="NV5" t="inlineStr"/>
-      <c r="NW5" t="inlineStr"/>
-      <c r="NX5" t="inlineStr"/>
-      <c r="NY5" t="inlineStr"/>
-      <c r="NZ5" t="inlineStr"/>
-      <c r="OA5" t="inlineStr"/>
-      <c r="OB5" t="inlineStr"/>
-      <c r="OC5" t="inlineStr"/>
-      <c r="OD5" t="inlineStr"/>
-      <c r="OE5" t="inlineStr"/>
-      <c r="OF5" t="inlineStr"/>
-      <c r="OG5" t="inlineStr"/>
-      <c r="OH5" t="inlineStr"/>
-      <c r="OI5" t="inlineStr"/>
-      <c r="OJ5" t="inlineStr"/>
-      <c r="OK5" t="inlineStr"/>
-      <c r="OL5" t="inlineStr"/>
-      <c r="OM5" t="inlineStr"/>
-      <c r="ON5" t="inlineStr"/>
-      <c r="OO5" t="inlineStr"/>
-      <c r="OP5" t="inlineStr"/>
-      <c r="OQ5" t="inlineStr"/>
-      <c r="OR5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>type01</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>16.0</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>3.22</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>3.03</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>3.00</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>2.97</t>
+        </is>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>3.01</t>
+        </is>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>2.93</t>
+        </is>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>2.31</t>
+        </is>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t>2.75</t>
+        </is>
+      </c>
+      <c r="AK6" t="inlineStr">
+        <is>
+          <t>94</t>
+        </is>
+      </c>
+      <c r="AM6" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="AN6" t="inlineStr">
+        <is>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="AO6" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="AP6" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="AQ6" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="AR6" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="AW6" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="AX6" t="inlineStr">
+        <is>
+          <t>.2</t>
+        </is>
+      </c>
+      <c r="AY6" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="AZ6" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="BA6" t="inlineStr">
+        <is>
+          <t>.7</t>
+        </is>
+      </c>
+      <c r="BB6" t="inlineStr">
+        <is>
+          <t>.9</t>
+        </is>
+      </c>
+      <c r="BO6" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="BP6" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="BQ6" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="BR6" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="BS6" t="inlineStr">
+        <is>
+          <t>15.0</t>
+        </is>
+      </c>
+      <c r="BT6" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="BX6" t="inlineStr">
+        <is>
+          <t>2.51</t>
+        </is>
+      </c>
+      <c r="BY6" t="inlineStr">
+        <is>
+          <t>2.20</t>
+        </is>
+      </c>
+      <c r="CA6" t="inlineStr">
+        <is>
+          <t>2.23</t>
+        </is>
+      </c>
+      <c r="CB6" t="inlineStr">
+        <is>
+          <t>2.25</t>
+        </is>
+      </c>
+      <c r="CC6" t="inlineStr">
+        <is>
+          <t>2.27</t>
+        </is>
+      </c>
+      <c r="CD6" t="inlineStr">
+        <is>
+          <t>2.20</t>
+        </is>
+      </c>
+      <c r="CE6" t="inlineStr">
+        <is>
+          <t>2.10</t>
+        </is>
+      </c>
+      <c r="CF6" t="inlineStr">
+        <is>
+          <t>1.99</t>
+        </is>
+      </c>
+      <c r="CR6" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="CT6" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="CU6" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="CV6" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="CW6" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="CX6" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="CY6" t="inlineStr">
+        <is>
+          <t>79</t>
+        </is>
+      </c>
+      <c r="DD6" t="inlineStr">
+        <is>
+          <t>.2</t>
+        </is>
+      </c>
+      <c r="DE6" t="inlineStr">
+        <is>
+          <t>.2</t>
+        </is>
+      </c>
+      <c r="DF6" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="DG6" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="DH6" t="inlineStr">
+        <is>
+          <t>.3</t>
+        </is>
+      </c>
+      <c r="DI6" t="inlineStr">
+        <is>
+          <t>.13</t>
+        </is>
+      </c>
+      <c r="DP6" t="inlineStr">
+        <is>
+          <t>220</t>
+        </is>
+      </c>
+      <c r="EJ6" t="inlineStr">
+        <is>
+          <t>2.57</t>
+        </is>
+      </c>
+      <c r="EK6" t="inlineStr">
+        <is>
+          <t>1.75</t>
+        </is>
+      </c>
+      <c r="EL6" t="inlineStr">
+        <is>
+          <t>1.67</t>
+        </is>
+      </c>
+      <c r="EM6" t="inlineStr">
+        <is>
+          <t>1.69</t>
+        </is>
+      </c>
+      <c r="EN6" t="inlineStr">
+        <is>
+          <t>1.73</t>
+        </is>
+      </c>
+      <c r="EO6" t="inlineStr">
+        <is>
+          <t>1.69</t>
+        </is>
+      </c>
+      <c r="ET6" t="inlineStr">
+        <is>
+          <t>68</t>
+        </is>
+      </c>
+      <c r="EV6" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="EW6" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="EX6" t="inlineStr">
+        <is>
+          <t>63</t>
+        </is>
+      </c>
+      <c r="EY6" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="EZ6" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="FA6" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="FY6" t="inlineStr">
+        <is>
+          <t>.4</t>
+        </is>
+      </c>
+      <c r="FZ6" t="inlineStr">
+        <is>
+          <t>.3</t>
+        </is>
+      </c>
+      <c r="GA6" t="inlineStr">
+        <is>
+          <t>.0</t>
+        </is>
+      </c>
+      <c r="GB6" t="inlineStr">
+        <is>
+          <t>.3</t>
+        </is>
+      </c>
+      <c r="GC6" t="inlineStr">
+        <is>
+          <t>.11</t>
+        </is>
+      </c>
+      <c r="GD6" t="inlineStr">
+        <is>
+          <t>.24</t>
+        </is>
+      </c>
+      <c r="HX6" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="HY6" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="HZ6" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="IA6" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="IB6" t="inlineStr">
+        <is>
+          <t>16.0</t>
+        </is>
+      </c>
+      <c r="IC6" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="IG6" t="inlineStr">
+        <is>
+          <t>5.45</t>
+        </is>
+      </c>
+      <c r="IH6" t="inlineStr">
+        <is>
+          <t>9.33</t>
+        </is>
+      </c>
+      <c r="IJ6" t="inlineStr">
+        <is>
+          <t>7.32</t>
+        </is>
+      </c>
+      <c r="IK6" t="inlineStr">
+        <is>
+          <t>0.47</t>
+        </is>
+      </c>
+      <c r="IL6" t="inlineStr">
+        <is>
+          <t>7.99</t>
+        </is>
+      </c>
+      <c r="IM6" t="inlineStr">
+        <is>
+          <t>7.64</t>
+        </is>
+      </c>
+      <c r="IN6" t="inlineStr">
+        <is>
+          <t>3.12</t>
+        </is>
+      </c>
+      <c r="IO6" t="inlineStr">
+        <is>
+          <t>7.31</t>
+        </is>
+      </c>
+      <c r="JA6" t="inlineStr">
+        <is>
+          <t>153</t>
+        </is>
+      </c>
+      <c r="JC6" t="inlineStr">
+        <is>
+          <t>143</t>
+        </is>
+      </c>
+      <c r="JD6" t="inlineStr">
+        <is>
+          <t>155</t>
+        </is>
+      </c>
+      <c r="JE6" t="inlineStr">
+        <is>
+          <t>147</t>
+        </is>
+      </c>
+      <c r="JF6" t="inlineStr">
+        <is>
+          <t>140</t>
+        </is>
+      </c>
+      <c r="JG6" t="inlineStr">
+        <is>
+          <t>149</t>
+        </is>
+      </c>
+      <c r="JH6" t="inlineStr">
+        <is>
+          <t>134</t>
+        </is>
+      </c>
+      <c r="JM6" t="inlineStr">
+        <is>
+          <t>.9</t>
+        </is>
+      </c>
+      <c r="JN6" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="JO6" t="inlineStr">
+        <is>
+          <t>.7</t>
+        </is>
+      </c>
+      <c r="JP6" t="inlineStr">
+        <is>
+          <t>.11</t>
+        </is>
+      </c>
+      <c r="JQ6" t="inlineStr">
+        <is>
+          <t>.5</t>
+        </is>
+      </c>
+      <c r="JR6" t="inlineStr">
+        <is>
+          <t>.15</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>type01</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>16.0</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>3.22</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>3.03</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>3.00</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>2.97</t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>3.01</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>2.93</t>
+        </is>
+      </c>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>2.31</t>
+        </is>
+      </c>
+      <c r="Y7" t="inlineStr">
+        <is>
+          <t>2.75</t>
+        </is>
+      </c>
+      <c r="AK7" t="inlineStr">
+        <is>
+          <t>94</t>
+        </is>
+      </c>
+      <c r="AM7" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="AN7" t="inlineStr">
+        <is>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="AO7" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="AP7" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="AQ7" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="AR7" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="AW7" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="AX7" t="inlineStr">
+        <is>
+          <t>.2</t>
+        </is>
+      </c>
+      <c r="AY7" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="AZ7" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="BA7" t="inlineStr">
+        <is>
+          <t>.7</t>
+        </is>
+      </c>
+      <c r="BB7" t="inlineStr">
+        <is>
+          <t>.9</t>
+        </is>
+      </c>
+      <c r="BO7" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="BP7" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="BQ7" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="BR7" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="BS7" t="inlineStr">
+        <is>
+          <t>15.0</t>
+        </is>
+      </c>
+      <c r="BT7" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="BX7" t="inlineStr">
+        <is>
+          <t>2.51</t>
+        </is>
+      </c>
+      <c r="BY7" t="inlineStr">
+        <is>
+          <t>2.20</t>
+        </is>
+      </c>
+      <c r="CA7" t="inlineStr">
+        <is>
+          <t>2.23</t>
+        </is>
+      </c>
+      <c r="CB7" t="inlineStr">
+        <is>
+          <t>2.25</t>
+        </is>
+      </c>
+      <c r="CC7" t="inlineStr">
+        <is>
+          <t>2.27</t>
+        </is>
+      </c>
+      <c r="CD7" t="inlineStr">
+        <is>
+          <t>2.20</t>
+        </is>
+      </c>
+      <c r="CE7" t="inlineStr">
+        <is>
+          <t>2.10</t>
+        </is>
+      </c>
+      <c r="CF7" t="inlineStr">
+        <is>
+          <t>1.99</t>
+        </is>
+      </c>
+      <c r="CR7" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="CT7" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="CU7" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="CV7" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="CW7" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="CX7" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="CY7" t="inlineStr">
+        <is>
+          <t>79</t>
+        </is>
+      </c>
+      <c r="DD7" t="inlineStr">
+        <is>
+          <t>.2</t>
+        </is>
+      </c>
+      <c r="DE7" t="inlineStr">
+        <is>
+          <t>.2</t>
+        </is>
+      </c>
+      <c r="DF7" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="DG7" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="DH7" t="inlineStr">
+        <is>
+          <t>.3</t>
+        </is>
+      </c>
+      <c r="DI7" t="inlineStr">
+        <is>
+          <t>.13</t>
+        </is>
+      </c>
+      <c r="DP7" t="inlineStr">
+        <is>
+          <t>220</t>
+        </is>
+      </c>
+      <c r="EJ7" t="inlineStr">
+        <is>
+          <t>2.57</t>
+        </is>
+      </c>
+      <c r="EK7" t="inlineStr">
+        <is>
+          <t>1.75</t>
+        </is>
+      </c>
+      <c r="EL7" t="inlineStr">
+        <is>
+          <t>1.67</t>
+        </is>
+      </c>
+      <c r="EM7" t="inlineStr">
+        <is>
+          <t>1.69</t>
+        </is>
+      </c>
+      <c r="EN7" t="inlineStr">
+        <is>
+          <t>1.73</t>
+        </is>
+      </c>
+      <c r="EO7" t="inlineStr">
+        <is>
+          <t>1.69</t>
+        </is>
+      </c>
+      <c r="ET7" t="inlineStr">
+        <is>
+          <t>68</t>
+        </is>
+      </c>
+      <c r="EV7" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="EW7" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="EX7" t="inlineStr">
+        <is>
+          <t>63</t>
+        </is>
+      </c>
+      <c r="EY7" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="EZ7" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="FA7" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="FY7" t="inlineStr">
+        <is>
+          <t>.4</t>
+        </is>
+      </c>
+      <c r="FZ7" t="inlineStr">
+        <is>
+          <t>.3</t>
+        </is>
+      </c>
+      <c r="GA7" t="inlineStr">
+        <is>
+          <t>.0</t>
+        </is>
+      </c>
+      <c r="GB7" t="inlineStr">
+        <is>
+          <t>.3</t>
+        </is>
+      </c>
+      <c r="GC7" t="inlineStr">
+        <is>
+          <t>.11</t>
+        </is>
+      </c>
+      <c r="GD7" t="inlineStr">
+        <is>
+          <t>.24</t>
+        </is>
+      </c>
+      <c r="HX7" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="HY7" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="HZ7" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="IA7" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="IB7" t="inlineStr">
+        <is>
+          <t>16.0</t>
+        </is>
+      </c>
+      <c r="IC7" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="IG7" t="inlineStr">
+        <is>
+          <t>5.45</t>
+        </is>
+      </c>
+      <c r="IH7" t="inlineStr">
+        <is>
+          <t>9.33</t>
+        </is>
+      </c>
+      <c r="IJ7" t="inlineStr">
+        <is>
+          <t>7.32</t>
+        </is>
+      </c>
+      <c r="IK7" t="inlineStr">
+        <is>
+          <t>0.47</t>
+        </is>
+      </c>
+      <c r="IL7" t="inlineStr">
+        <is>
+          <t>7.99</t>
+        </is>
+      </c>
+      <c r="IM7" t="inlineStr">
+        <is>
+          <t>7.64</t>
+        </is>
+      </c>
+      <c r="IN7" t="inlineStr">
+        <is>
+          <t>3.12</t>
+        </is>
+      </c>
+      <c r="IO7" t="inlineStr">
+        <is>
+          <t>7.31</t>
+        </is>
+      </c>
+      <c r="JA7" t="inlineStr">
+        <is>
+          <t>153</t>
+        </is>
+      </c>
+      <c r="JC7" t="inlineStr">
+        <is>
+          <t>143</t>
+        </is>
+      </c>
+      <c r="JD7" t="inlineStr">
+        <is>
+          <t>155</t>
+        </is>
+      </c>
+      <c r="JE7" t="inlineStr">
+        <is>
+          <t>147</t>
+        </is>
+      </c>
+      <c r="JF7" t="inlineStr">
+        <is>
+          <t>140</t>
+        </is>
+      </c>
+      <c r="JG7" t="inlineStr">
+        <is>
+          <t>149</t>
+        </is>
+      </c>
+      <c r="JH7" t="inlineStr">
+        <is>
+          <t>134</t>
+        </is>
+      </c>
+      <c r="JM7" t="inlineStr">
+        <is>
+          <t>.9</t>
+        </is>
+      </c>
+      <c r="JN7" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="JO7" t="inlineStr">
+        <is>
+          <t>.7</t>
+        </is>
+      </c>
+      <c r="JP7" t="inlineStr">
+        <is>
+          <t>.11</t>
+        </is>
+      </c>
+      <c r="JQ7" t="inlineStr">
+        <is>
+          <t>.5</t>
+        </is>
+      </c>
+      <c r="JR7" t="inlineStr">
+        <is>
+          <t>.15</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>type01</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>16.0</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>3.22</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>3.03</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr"/>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>3.00</t>
+        </is>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>2.97</t>
+        </is>
+      </c>
+      <c r="V8" t="inlineStr">
+        <is>
+          <t>3.01</t>
+        </is>
+      </c>
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>2.93</t>
+        </is>
+      </c>
+      <c r="X8" t="inlineStr">
+        <is>
+          <t>2.31</t>
+        </is>
+      </c>
+      <c r="Y8" t="inlineStr">
+        <is>
+          <t>2.75</t>
+        </is>
+      </c>
+      <c r="Z8" t="inlineStr"/>
+      <c r="AA8" t="inlineStr"/>
+      <c r="AB8" t="inlineStr"/>
+      <c r="AC8" t="inlineStr"/>
+      <c r="AD8" t="inlineStr"/>
+      <c r="AE8" t="inlineStr"/>
+      <c r="AF8" t="inlineStr"/>
+      <c r="AG8" t="inlineStr"/>
+      <c r="AH8" t="inlineStr"/>
+      <c r="AI8" t="inlineStr"/>
+      <c r="AJ8" t="inlineStr"/>
+      <c r="AK8" t="inlineStr">
+        <is>
+          <t>94</t>
+        </is>
+      </c>
+      <c r="AL8" t="inlineStr"/>
+      <c r="AM8" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="AN8" t="inlineStr">
+        <is>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="AO8" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="AP8" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="AQ8" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="AR8" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="AS8" t="inlineStr"/>
+      <c r="AT8" t="inlineStr"/>
+      <c r="AU8" t="inlineStr"/>
+      <c r="AV8" t="inlineStr"/>
+      <c r="AW8" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="AX8" t="inlineStr">
+        <is>
+          <t>.2</t>
+        </is>
+      </c>
+      <c r="AY8" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="AZ8" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="BA8" t="inlineStr">
+        <is>
+          <t>.7</t>
+        </is>
+      </c>
+      <c r="BB8" t="inlineStr">
+        <is>
+          <t>.9</t>
+        </is>
+      </c>
+      <c r="BC8" t="inlineStr"/>
+      <c r="BD8" t="inlineStr"/>
+      <c r="BE8" t="inlineStr"/>
+      <c r="BF8" t="inlineStr"/>
+      <c r="BG8" t="inlineStr"/>
+      <c r="BH8" t="inlineStr"/>
+      <c r="BI8" t="inlineStr"/>
+      <c r="BJ8" t="inlineStr"/>
+      <c r="BK8" t="inlineStr"/>
+      <c r="BL8" t="inlineStr"/>
+      <c r="BM8" t="inlineStr"/>
+      <c r="BN8" t="inlineStr"/>
+      <c r="BO8" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="BP8" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="BQ8" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="BR8" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="BS8" t="inlineStr">
+        <is>
+          <t>15.0</t>
+        </is>
+      </c>
+      <c r="BT8" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="BU8" t="inlineStr"/>
+      <c r="BV8" t="inlineStr"/>
+      <c r="BW8" t="inlineStr"/>
+      <c r="BX8" t="inlineStr">
+        <is>
+          <t>2.51</t>
+        </is>
+      </c>
+      <c r="BY8" t="inlineStr">
+        <is>
+          <t>2.20</t>
+        </is>
+      </c>
+      <c r="BZ8" t="inlineStr"/>
+      <c r="CA8" t="inlineStr">
+        <is>
+          <t>2.23</t>
+        </is>
+      </c>
+      <c r="CB8" t="inlineStr">
+        <is>
+          <t>2.25</t>
+        </is>
+      </c>
+      <c r="CC8" t="inlineStr">
+        <is>
+          <t>2.27</t>
+        </is>
+      </c>
+      <c r="CD8" t="inlineStr">
+        <is>
+          <t>2.20</t>
+        </is>
+      </c>
+      <c r="CE8" t="inlineStr">
+        <is>
+          <t>2.10</t>
+        </is>
+      </c>
+      <c r="CF8" t="inlineStr">
+        <is>
+          <t>1.99</t>
+        </is>
+      </c>
+      <c r="CG8" t="inlineStr"/>
+      <c r="CH8" t="inlineStr"/>
+      <c r="CI8" t="inlineStr"/>
+      <c r="CJ8" t="inlineStr"/>
+      <c r="CK8" t="inlineStr"/>
+      <c r="CL8" t="inlineStr"/>
+      <c r="CM8" t="inlineStr"/>
+      <c r="CN8" t="inlineStr"/>
+      <c r="CO8" t="inlineStr"/>
+      <c r="CP8" t="inlineStr"/>
+      <c r="CQ8" t="inlineStr"/>
+      <c r="CR8" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="CS8" t="inlineStr"/>
+      <c r="CT8" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="CU8" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="CV8" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="CW8" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="CX8" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="CY8" t="inlineStr">
+        <is>
+          <t>79</t>
+        </is>
+      </c>
+      <c r="CZ8" t="inlineStr"/>
+      <c r="DA8" t="inlineStr"/>
+      <c r="DB8" t="inlineStr"/>
+      <c r="DC8" t="inlineStr"/>
+      <c r="DD8" t="inlineStr">
+        <is>
+          <t>.2</t>
+        </is>
+      </c>
+      <c r="DE8" t="inlineStr">
+        <is>
+          <t>.2</t>
+        </is>
+      </c>
+      <c r="DF8" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="DG8" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="DH8" t="inlineStr">
+        <is>
+          <t>.3</t>
+        </is>
+      </c>
+      <c r="DI8" t="inlineStr">
+        <is>
+          <t>.13</t>
+        </is>
+      </c>
+      <c r="DJ8" t="inlineStr"/>
+      <c r="DK8" t="inlineStr"/>
+      <c r="DL8" t="inlineStr"/>
+      <c r="DM8" t="inlineStr"/>
+      <c r="DN8" t="inlineStr"/>
+      <c r="DO8" t="inlineStr"/>
+      <c r="DP8" t="inlineStr">
+        <is>
+          <t>220</t>
+        </is>
+      </c>
+      <c r="DQ8" t="inlineStr"/>
+      <c r="DR8" t="inlineStr"/>
+      <c r="DS8" t="inlineStr"/>
+      <c r="DT8" t="inlineStr"/>
+      <c r="DU8" t="inlineStr"/>
+      <c r="DV8" t="inlineStr"/>
+      <c r="DW8" t="inlineStr"/>
+      <c r="DX8" t="inlineStr"/>
+      <c r="DY8" t="inlineStr"/>
+      <c r="DZ8" t="inlineStr"/>
+      <c r="EA8" t="inlineStr"/>
+      <c r="EB8" t="inlineStr"/>
+      <c r="EC8" t="inlineStr"/>
+      <c r="ED8" t="inlineStr"/>
+      <c r="EE8" t="inlineStr"/>
+      <c r="EF8" t="inlineStr"/>
+      <c r="EG8" t="inlineStr"/>
+      <c r="EH8" t="inlineStr"/>
+      <c r="EI8" t="inlineStr"/>
+      <c r="EJ8" t="inlineStr">
+        <is>
+          <t>2.57</t>
+        </is>
+      </c>
+      <c r="EK8" t="inlineStr">
+        <is>
+          <t>1.75</t>
+        </is>
+      </c>
+      <c r="EL8" t="inlineStr">
+        <is>
+          <t>1.67</t>
+        </is>
+      </c>
+      <c r="EM8" t="inlineStr">
+        <is>
+          <t>1.69</t>
+        </is>
+      </c>
+      <c r="EN8" t="inlineStr">
+        <is>
+          <t>1.73</t>
+        </is>
+      </c>
+      <c r="EO8" t="inlineStr">
+        <is>
+          <t>1.69</t>
+        </is>
+      </c>
+      <c r="EP8" t="inlineStr"/>
+      <c r="EQ8" t="inlineStr"/>
+      <c r="ER8" t="inlineStr"/>
+      <c r="ES8" t="inlineStr"/>
+      <c r="ET8" t="inlineStr">
+        <is>
+          <t>68</t>
+        </is>
+      </c>
+      <c r="EU8" t="inlineStr"/>
+      <c r="EV8" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="EW8" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="EX8" t="inlineStr">
+        <is>
+          <t>63</t>
+        </is>
+      </c>
+      <c r="EY8" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="EZ8" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="FA8" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="FB8" t="inlineStr"/>
+      <c r="FC8" t="inlineStr"/>
+      <c r="FD8" t="inlineStr"/>
+      <c r="FE8" t="inlineStr"/>
+      <c r="FF8" t="inlineStr"/>
+      <c r="FG8" t="inlineStr"/>
+      <c r="FH8" t="inlineStr"/>
+      <c r="FI8" t="inlineStr"/>
+      <c r="FJ8" t="inlineStr"/>
+      <c r="FK8" t="inlineStr"/>
+      <c r="FL8" t="inlineStr"/>
+      <c r="FM8" t="inlineStr"/>
+      <c r="FN8" t="inlineStr"/>
+      <c r="FO8" t="inlineStr"/>
+      <c r="FP8" t="inlineStr"/>
+      <c r="FQ8" t="inlineStr"/>
+      <c r="FR8" t="inlineStr"/>
+      <c r="FS8" t="inlineStr"/>
+      <c r="FT8" t="inlineStr"/>
+      <c r="FU8" t="inlineStr"/>
+      <c r="FV8" t="inlineStr"/>
+      <c r="FW8" t="inlineStr"/>
+      <c r="FX8" t="inlineStr"/>
+      <c r="FY8" t="inlineStr">
+        <is>
+          <t>.4</t>
+        </is>
+      </c>
+      <c r="FZ8" t="inlineStr">
+        <is>
+          <t>.3</t>
+        </is>
+      </c>
+      <c r="GA8" t="inlineStr">
+        <is>
+          <t>.0</t>
+        </is>
+      </c>
+      <c r="GB8" t="inlineStr">
+        <is>
+          <t>.3</t>
+        </is>
+      </c>
+      <c r="GC8" t="inlineStr">
+        <is>
+          <t>.11</t>
+        </is>
+      </c>
+      <c r="GD8" t="inlineStr">
+        <is>
+          <t>.24</t>
+        </is>
+      </c>
+      <c r="GE8" t="inlineStr"/>
+      <c r="GF8" t="inlineStr"/>
+      <c r="GG8" t="inlineStr"/>
+      <c r="GH8" t="inlineStr"/>
+      <c r="GI8" t="inlineStr"/>
+      <c r="GJ8" t="inlineStr"/>
+      <c r="GK8" t="inlineStr"/>
+      <c r="GL8" t="inlineStr"/>
+      <c r="GM8" t="inlineStr"/>
+      <c r="GN8" t="inlineStr"/>
+      <c r="GO8" t="inlineStr"/>
+      <c r="GP8" t="inlineStr"/>
+      <c r="GQ8" t="inlineStr"/>
+      <c r="GR8" t="inlineStr"/>
+      <c r="GS8" t="inlineStr"/>
+      <c r="GT8" t="inlineStr"/>
+      <c r="GU8" t="inlineStr"/>
+      <c r="GV8" t="inlineStr"/>
+      <c r="GW8" t="inlineStr"/>
+      <c r="GX8" t="inlineStr"/>
+      <c r="GY8" t="inlineStr"/>
+      <c r="GZ8" t="inlineStr"/>
+      <c r="HA8" t="inlineStr"/>
+      <c r="HB8" t="inlineStr"/>
+      <c r="HC8" t="inlineStr"/>
+      <c r="HD8" t="inlineStr"/>
+      <c r="HE8" t="inlineStr"/>
+      <c r="HF8" t="inlineStr"/>
+      <c r="HG8" t="inlineStr"/>
+      <c r="HH8" t="inlineStr"/>
+      <c r="HI8" t="inlineStr"/>
+      <c r="HJ8" t="inlineStr"/>
+      <c r="HK8" t="inlineStr"/>
+      <c r="HL8" t="inlineStr"/>
+      <c r="HM8" t="inlineStr"/>
+      <c r="HN8" t="inlineStr"/>
+      <c r="HO8" t="inlineStr"/>
+      <c r="HP8" t="inlineStr"/>
+      <c r="HQ8" t="inlineStr"/>
+      <c r="HR8" t="inlineStr"/>
+      <c r="HS8" t="inlineStr"/>
+      <c r="HT8" t="inlineStr"/>
+      <c r="HU8" t="inlineStr"/>
+      <c r="HV8" t="inlineStr"/>
+      <c r="HW8" t="inlineStr"/>
+      <c r="HX8" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="HY8" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="HZ8" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="IA8" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="IB8" t="inlineStr">
+        <is>
+          <t>16.0</t>
+        </is>
+      </c>
+      <c r="IC8" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="ID8" t="inlineStr"/>
+      <c r="IE8" t="inlineStr"/>
+      <c r="IF8" t="inlineStr"/>
+      <c r="IG8" t="inlineStr">
+        <is>
+          <t>5.45</t>
+        </is>
+      </c>
+      <c r="IH8" t="inlineStr">
+        <is>
+          <t>9.33</t>
+        </is>
+      </c>
+      <c r="II8" t="inlineStr"/>
+      <c r="IJ8" t="inlineStr">
+        <is>
+          <t>7.32</t>
+        </is>
+      </c>
+      <c r="IK8" t="inlineStr">
+        <is>
+          <t>0.47</t>
+        </is>
+      </c>
+      <c r="IL8" t="inlineStr">
+        <is>
+          <t>7.99</t>
+        </is>
+      </c>
+      <c r="IM8" t="inlineStr">
+        <is>
+          <t>7.64</t>
+        </is>
+      </c>
+      <c r="IN8" t="inlineStr">
+        <is>
+          <t>3.12</t>
+        </is>
+      </c>
+      <c r="IO8" t="inlineStr">
+        <is>
+          <t>7.31</t>
+        </is>
+      </c>
+      <c r="IP8" t="inlineStr"/>
+      <c r="IQ8" t="inlineStr"/>
+      <c r="IR8" t="inlineStr"/>
+      <c r="IS8" t="inlineStr"/>
+      <c r="IT8" t="inlineStr"/>
+      <c r="IU8" t="inlineStr"/>
+      <c r="IV8" t="inlineStr"/>
+      <c r="IW8" t="inlineStr"/>
+      <c r="IX8" t="inlineStr"/>
+      <c r="IY8" t="inlineStr"/>
+      <c r="IZ8" t="inlineStr"/>
+      <c r="JA8" t="inlineStr">
+        <is>
+          <t>153</t>
+        </is>
+      </c>
+      <c r="JB8" t="inlineStr"/>
+      <c r="JC8" t="inlineStr">
+        <is>
+          <t>143</t>
+        </is>
+      </c>
+      <c r="JD8" t="inlineStr">
+        <is>
+          <t>155</t>
+        </is>
+      </c>
+      <c r="JE8" t="inlineStr">
+        <is>
+          <t>147</t>
+        </is>
+      </c>
+      <c r="JF8" t="inlineStr">
+        <is>
+          <t>140</t>
+        </is>
+      </c>
+      <c r="JG8" t="inlineStr">
+        <is>
+          <t>149</t>
+        </is>
+      </c>
+      <c r="JH8" t="inlineStr">
+        <is>
+          <t>134</t>
+        </is>
+      </c>
+      <c r="JI8" t="inlineStr"/>
+      <c r="JJ8" t="inlineStr"/>
+      <c r="JK8" t="inlineStr"/>
+      <c r="JL8" t="inlineStr"/>
+      <c r="JM8" t="inlineStr">
+        <is>
+          <t>.9</t>
+        </is>
+      </c>
+      <c r="JN8" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="JO8" t="inlineStr">
+        <is>
+          <t>.7</t>
+        </is>
+      </c>
+      <c r="JP8" t="inlineStr">
+        <is>
+          <t>.11</t>
+        </is>
+      </c>
+      <c r="JQ8" t="inlineStr">
+        <is>
+          <t>.5</t>
+        </is>
+      </c>
+      <c r="JR8" t="inlineStr">
+        <is>
+          <t>.15</t>
+        </is>
+      </c>
+      <c r="JS8" t="inlineStr"/>
+      <c r="JT8" t="inlineStr"/>
+      <c r="JU8" t="inlineStr"/>
+      <c r="JV8" t="inlineStr"/>
+      <c r="JW8" t="inlineStr"/>
+      <c r="JX8" t="inlineStr"/>
+      <c r="JY8" t="inlineStr"/>
+      <c r="JZ8" t="inlineStr"/>
+      <c r="KA8" t="inlineStr"/>
+      <c r="KB8" t="inlineStr"/>
+      <c r="KC8" t="inlineStr"/>
+      <c r="KD8" t="inlineStr"/>
+      <c r="KE8" t="inlineStr"/>
+      <c r="KF8" t="inlineStr"/>
+      <c r="KG8" t="inlineStr"/>
+      <c r="KH8" t="inlineStr"/>
+      <c r="KI8" t="inlineStr"/>
+      <c r="KJ8" t="inlineStr"/>
+      <c r="KK8" t="inlineStr"/>
+      <c r="KL8" t="inlineStr"/>
+      <c r="KM8" t="inlineStr"/>
+      <c r="KN8" t="inlineStr"/>
+      <c r="KO8" t="inlineStr"/>
+      <c r="KP8" t="inlineStr"/>
+      <c r="KQ8" t="inlineStr"/>
+      <c r="KR8" t="inlineStr"/>
+      <c r="KS8" t="inlineStr"/>
+      <c r="KT8" t="inlineStr"/>
+      <c r="KU8" t="inlineStr"/>
+      <c r="KV8" t="inlineStr"/>
+      <c r="KW8" t="inlineStr"/>
+      <c r="KX8" t="inlineStr"/>
+      <c r="KY8" t="inlineStr"/>
+      <c r="KZ8" t="inlineStr"/>
+      <c r="LA8" t="inlineStr"/>
+      <c r="LB8" t="inlineStr"/>
+      <c r="LC8" t="inlineStr"/>
+      <c r="LD8" t="inlineStr"/>
+      <c r="LE8" t="inlineStr"/>
+      <c r="LF8" t="inlineStr"/>
+      <c r="LG8" t="inlineStr"/>
+      <c r="LH8" t="inlineStr"/>
+      <c r="LI8" t="inlineStr"/>
+      <c r="LJ8" t="inlineStr"/>
+      <c r="LK8" t="inlineStr"/>
+      <c r="LL8" t="inlineStr"/>
+      <c r="LM8" t="inlineStr"/>
+      <c r="LN8" t="inlineStr"/>
+      <c r="LO8" t="inlineStr"/>
+      <c r="LP8" t="inlineStr"/>
+      <c r="LQ8" t="inlineStr"/>
+      <c r="LR8" t="inlineStr"/>
+      <c r="LS8" t="inlineStr"/>
+      <c r="LT8" t="inlineStr"/>
+      <c r="LU8" t="inlineStr"/>
+      <c r="LV8" t="inlineStr"/>
+      <c r="LW8" t="inlineStr"/>
+      <c r="LX8" t="inlineStr"/>
+      <c r="LY8" t="inlineStr"/>
+      <c r="LZ8" t="inlineStr"/>
+      <c r="MA8" t="inlineStr"/>
+      <c r="MB8" t="inlineStr"/>
+      <c r="MC8" t="inlineStr"/>
+      <c r="MD8" t="inlineStr"/>
+      <c r="ME8" t="inlineStr"/>
+      <c r="MF8" t="inlineStr"/>
+      <c r="MG8" t="inlineStr"/>
+      <c r="MH8" t="inlineStr"/>
+      <c r="MI8" t="inlineStr"/>
+      <c r="MJ8" t="inlineStr"/>
+      <c r="MK8" t="inlineStr"/>
+      <c r="ML8" t="inlineStr"/>
+      <c r="MM8" t="inlineStr"/>
+      <c r="MN8" t="inlineStr"/>
+      <c r="MO8" t="inlineStr"/>
+      <c r="MP8" t="inlineStr"/>
+      <c r="MQ8" t="inlineStr"/>
+      <c r="MR8" t="inlineStr"/>
+      <c r="MS8" t="inlineStr"/>
+      <c r="MT8" t="inlineStr"/>
+      <c r="MU8" t="inlineStr"/>
+      <c r="MV8" t="inlineStr"/>
+      <c r="MW8" t="inlineStr"/>
+      <c r="MX8" t="inlineStr"/>
+      <c r="MY8" t="inlineStr"/>
+      <c r="MZ8" t="inlineStr"/>
+      <c r="NA8" t="inlineStr"/>
+      <c r="NB8" t="inlineStr"/>
+      <c r="NC8" t="inlineStr"/>
+      <c r="ND8" t="inlineStr"/>
+      <c r="NE8" t="inlineStr"/>
+      <c r="NF8" t="inlineStr"/>
+      <c r="NG8" t="inlineStr"/>
+      <c r="NH8" t="inlineStr"/>
+      <c r="NI8" t="inlineStr"/>
+      <c r="NJ8" t="inlineStr"/>
+      <c r="NK8" t="inlineStr"/>
+      <c r="NL8" t="inlineStr"/>
+      <c r="NM8" t="inlineStr"/>
+      <c r="NN8" t="inlineStr"/>
+      <c r="NO8" t="inlineStr"/>
+      <c r="NP8" t="inlineStr"/>
+      <c r="NQ8" t="inlineStr"/>
+      <c r="NR8" t="inlineStr"/>
+      <c r="NS8" t="inlineStr"/>
+      <c r="NT8" t="inlineStr"/>
+      <c r="NU8" t="inlineStr"/>
+      <c r="NV8" t="inlineStr"/>
+      <c r="NW8" t="inlineStr"/>
+      <c r="NX8" t="inlineStr"/>
+      <c r="NY8" t="inlineStr"/>
+      <c r="NZ8" t="inlineStr"/>
+      <c r="OA8" t="inlineStr"/>
+      <c r="OB8" t="inlineStr"/>
+      <c r="OC8" t="inlineStr"/>
+      <c r="OD8" t="inlineStr"/>
+      <c r="OE8" t="inlineStr"/>
+      <c r="OF8" t="inlineStr"/>
+      <c r="OG8" t="inlineStr"/>
+      <c r="OH8" t="inlineStr"/>
+      <c r="OI8" t="inlineStr"/>
+      <c r="OJ8" t="inlineStr"/>
+      <c r="OK8" t="inlineStr"/>
+      <c r="OL8" t="inlineStr"/>
+      <c r="OM8" t="inlineStr"/>
+      <c r="ON8" t="inlineStr"/>
+      <c r="OO8" t="inlineStr"/>
+      <c r="OP8" t="inlineStr"/>
+      <c r="OQ8" t="inlineStr"/>
+      <c r="OR8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>type01</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>16.0</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>4.39</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>2.88</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr"/>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>2.92</t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>2.90</t>
+        </is>
+      </c>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>2.89</t>
+        </is>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>2.99</t>
+        </is>
+      </c>
+      <c r="X9" t="inlineStr">
+        <is>
+          <t>2.89</t>
+        </is>
+      </c>
+      <c r="Y9" t="inlineStr">
+        <is>
+          <t>2.90</t>
+        </is>
+      </c>
+      <c r="Z9" t="inlineStr"/>
+      <c r="AA9" t="inlineStr"/>
+      <c r="AB9" t="inlineStr"/>
+      <c r="AC9" t="inlineStr"/>
+      <c r="AD9" t="inlineStr"/>
+      <c r="AE9" t="inlineStr"/>
+      <c r="AF9" t="inlineStr"/>
+      <c r="AG9" t="inlineStr"/>
+      <c r="AH9" t="inlineStr"/>
+      <c r="AI9" t="inlineStr"/>
+      <c r="AJ9" t="inlineStr"/>
+      <c r="AK9" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="AL9" t="inlineStr"/>
+      <c r="AM9" t="inlineStr">
+        <is>
+          <t>67</t>
+        </is>
+      </c>
+      <c r="AN9" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="AO9" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="AP9" t="inlineStr">
+        <is>
+          <t>68</t>
+        </is>
+      </c>
+      <c r="AQ9" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="AR9" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="AS9" t="inlineStr"/>
+      <c r="AT9" t="inlineStr"/>
+      <c r="AU9" t="inlineStr"/>
+      <c r="AV9" t="inlineStr"/>
+      <c r="AW9" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="AX9" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="AY9" t="inlineStr">
+        <is>
+          <t>-2</t>
+        </is>
+      </c>
+      <c r="AZ9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="BA9" t="inlineStr">
+        <is>
+          <t>-2</t>
+        </is>
+      </c>
+      <c r="BB9" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="BC9" t="inlineStr"/>
+      <c r="BD9" t="inlineStr"/>
+      <c r="BE9" t="inlineStr"/>
+      <c r="BF9" t="inlineStr"/>
+      <c r="BG9" t="inlineStr"/>
+      <c r="BH9" t="inlineStr"/>
+      <c r="BI9" t="inlineStr"/>
+      <c r="BJ9" t="inlineStr"/>
+      <c r="BK9" t="inlineStr"/>
+      <c r="BL9" t="inlineStr"/>
+      <c r="BM9" t="inlineStr"/>
+      <c r="BN9" t="inlineStr"/>
+      <c r="BO9" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="BP9" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="BQ9" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="BR9" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="BS9" t="inlineStr">
+        <is>
+          <t>16.0</t>
+        </is>
+      </c>
+      <c r="BT9" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="BU9" t="inlineStr"/>
+      <c r="BV9" t="inlineStr"/>
+      <c r="BW9" t="inlineStr"/>
+      <c r="BX9" t="inlineStr">
+        <is>
+          <t>3.06</t>
+        </is>
+      </c>
+      <c r="BY9" t="inlineStr">
+        <is>
+          <t>2.17</t>
+        </is>
+      </c>
+      <c r="BZ9" t="inlineStr"/>
+      <c r="CA9" t="inlineStr">
+        <is>
+          <t>225</t>
+        </is>
+      </c>
+      <c r="CB9" t="inlineStr">
+        <is>
+          <t>2.18</t>
+        </is>
+      </c>
+      <c r="CC9" t="inlineStr">
+        <is>
+          <t>2.24</t>
+        </is>
+      </c>
+      <c r="CD9" t="inlineStr">
+        <is>
+          <t>2.27</t>
+        </is>
+      </c>
+      <c r="CE9" t="inlineStr">
+        <is>
+          <t>2.26</t>
+        </is>
+      </c>
+      <c r="CF9" t="inlineStr">
+        <is>
+          <t>2.16</t>
+        </is>
+      </c>
+      <c r="CG9" t="inlineStr"/>
+      <c r="CH9" t="inlineStr"/>
+      <c r="CI9" t="inlineStr"/>
+      <c r="CJ9" t="inlineStr"/>
+      <c r="CK9" t="inlineStr"/>
+      <c r="CL9" t="inlineStr"/>
+      <c r="CM9" t="inlineStr"/>
+      <c r="CN9" t="inlineStr"/>
+      <c r="CO9" t="inlineStr"/>
+      <c r="CP9" t="inlineStr"/>
+      <c r="CQ9" t="inlineStr"/>
+      <c r="CR9" t="inlineStr">
+        <is>
+          <t>71</t>
+        </is>
+      </c>
+      <c r="CS9" t="inlineStr"/>
+      <c r="CT9" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
+      </c>
+      <c r="CU9" t="inlineStr">
+        <is>
+          <t>71</t>
+        </is>
+      </c>
+      <c r="CV9" t="inlineStr">
+        <is>
+          <t>73</t>
+        </is>
+      </c>
+      <c r="CW9" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
+      </c>
+      <c r="CX9" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
+      </c>
+      <c r="CY9" t="inlineStr">
+        <is>
+          <t>71</t>
+        </is>
+      </c>
+      <c r="CZ9" t="inlineStr"/>
+      <c r="DA9" t="inlineStr"/>
+      <c r="DB9" t="inlineStr"/>
+      <c r="DC9" t="inlineStr"/>
+      <c r="DD9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="DE9" t="inlineStr">
+        <is>
+          <t>-3</t>
+        </is>
+      </c>
+      <c r="DF9" t="inlineStr">
+        <is>
+          <t>-0</t>
+        </is>
+      </c>
+      <c r="DG9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="DH9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="DI9" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="DJ9" t="inlineStr"/>
+      <c r="DK9" t="inlineStr"/>
+      <c r="DL9" t="inlineStr"/>
+      <c r="DM9" t="inlineStr"/>
+      <c r="DN9" t="inlineStr"/>
+      <c r="DO9" t="inlineStr"/>
+      <c r="DP9" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="DQ9" t="inlineStr"/>
+      <c r="DR9" t="inlineStr"/>
+      <c r="DS9" t="inlineStr"/>
+      <c r="DT9" t="inlineStr"/>
+      <c r="DU9" t="inlineStr"/>
+      <c r="DV9" t="inlineStr"/>
+      <c r="DW9" t="inlineStr"/>
+      <c r="DX9" t="inlineStr"/>
+      <c r="DY9" t="inlineStr"/>
+      <c r="DZ9" t="inlineStr"/>
+      <c r="EA9" t="inlineStr"/>
+      <c r="EB9" t="inlineStr"/>
+      <c r="EC9" t="inlineStr"/>
+      <c r="ED9" t="inlineStr"/>
+      <c r="EE9" t="inlineStr"/>
+      <c r="EF9" t="inlineStr"/>
+      <c r="EG9" t="inlineStr"/>
+      <c r="EH9" t="inlineStr"/>
+      <c r="EI9" t="inlineStr"/>
+      <c r="EJ9" t="inlineStr">
+        <is>
+          <t>2.60</t>
+        </is>
+      </c>
+      <c r="EK9" t="inlineStr">
+        <is>
+          <t>1.71</t>
+        </is>
+      </c>
+      <c r="EL9" t="inlineStr">
+        <is>
+          <t>1.90</t>
+        </is>
+      </c>
+      <c r="EM9" t="inlineStr">
+        <is>
+          <t>1.63</t>
+        </is>
+      </c>
+      <c r="EN9" t="inlineStr">
+        <is>
+          <t>1.97</t>
+        </is>
+      </c>
+      <c r="EO9" t="inlineStr">
+        <is>
+          <t>1.75</t>
+        </is>
+      </c>
+      <c r="EP9" t="inlineStr"/>
+      <c r="EQ9" t="inlineStr"/>
+      <c r="ER9" t="inlineStr"/>
+      <c r="ES9" t="inlineStr"/>
+      <c r="ET9" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="EU9" t="inlineStr"/>
+      <c r="EV9" t="inlineStr">
+        <is>
+          <t>73</t>
+        </is>
+      </c>
+      <c r="EW9" t="inlineStr">
+        <is>
+          <t>63</t>
+        </is>
+      </c>
+      <c r="EX9" t="inlineStr">
+        <is>
+          <t>76</t>
+        </is>
+      </c>
+      <c r="EY9" t="inlineStr">
+        <is>
+          <t>67</t>
+        </is>
+      </c>
+      <c r="EZ9" t="inlineStr">
+        <is>
+          <t>76</t>
+        </is>
+      </c>
+      <c r="FA9" t="inlineStr">
+        <is>
+          <t>61</t>
+        </is>
+      </c>
+      <c r="FB9" t="inlineStr"/>
+      <c r="FC9" t="inlineStr"/>
+      <c r="FD9" t="inlineStr"/>
+      <c r="FE9" t="inlineStr"/>
+      <c r="FF9" t="inlineStr"/>
+      <c r="FG9" t="inlineStr"/>
+      <c r="FH9" t="inlineStr"/>
+      <c r="FI9" t="inlineStr"/>
+      <c r="FJ9" t="inlineStr"/>
+      <c r="FK9" t="inlineStr"/>
+      <c r="FL9" t="inlineStr"/>
+      <c r="FM9" t="inlineStr"/>
+      <c r="FN9" t="inlineStr"/>
+      <c r="FO9" t="inlineStr"/>
+      <c r="FP9" t="inlineStr"/>
+      <c r="FQ9" t="inlineStr"/>
+      <c r="FR9" t="inlineStr"/>
+      <c r="FS9" t="inlineStr"/>
+      <c r="FT9" t="inlineStr"/>
+      <c r="FU9" t="inlineStr"/>
+      <c r="FV9" t="inlineStr"/>
+      <c r="FW9" t="inlineStr"/>
+      <c r="FX9" t="inlineStr"/>
+      <c r="FY9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="FZ9" t="inlineStr">
+        <is>
+          <t>-12</t>
+        </is>
+      </c>
+      <c r="GA9" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="GB9" t="inlineStr">
+        <is>
+          <t>-6</t>
+        </is>
+      </c>
+      <c r="GC9" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="GD9" t="inlineStr">
+        <is>
+          <t>-15</t>
+        </is>
+      </c>
+      <c r="GE9" t="inlineStr"/>
+      <c r="GF9" t="inlineStr"/>
+      <c r="GG9" t="inlineStr"/>
+      <c r="GH9" t="inlineStr"/>
+      <c r="GI9" t="inlineStr"/>
+      <c r="GJ9" t="inlineStr"/>
+      <c r="GK9" t="inlineStr"/>
+      <c r="GL9" t="inlineStr"/>
+      <c r="GM9" t="inlineStr"/>
+      <c r="GN9" t="inlineStr"/>
+      <c r="GO9" t="inlineStr"/>
+      <c r="GP9" t="inlineStr"/>
+      <c r="GQ9" t="inlineStr"/>
+      <c r="GR9" t="inlineStr"/>
+      <c r="GS9" t="inlineStr"/>
+      <c r="GT9" t="inlineStr"/>
+      <c r="GU9" t="inlineStr"/>
+      <c r="GV9" t="inlineStr"/>
+      <c r="GW9" t="inlineStr"/>
+      <c r="GX9" t="inlineStr"/>
+      <c r="GY9" t="inlineStr"/>
+      <c r="GZ9" t="inlineStr"/>
+      <c r="HA9" t="inlineStr"/>
+      <c r="HB9" t="inlineStr"/>
+      <c r="HC9" t="inlineStr"/>
+      <c r="HD9" t="inlineStr"/>
+      <c r="HE9" t="inlineStr"/>
+      <c r="HF9" t="inlineStr"/>
+      <c r="HG9" t="inlineStr"/>
+      <c r="HH9" t="inlineStr"/>
+      <c r="HI9" t="inlineStr"/>
+      <c r="HJ9" t="inlineStr"/>
+      <c r="HK9" t="inlineStr"/>
+      <c r="HL9" t="inlineStr"/>
+      <c r="HM9" t="inlineStr"/>
+      <c r="HN9" t="inlineStr"/>
+      <c r="HO9" t="inlineStr"/>
+      <c r="HP9" t="inlineStr"/>
+      <c r="HQ9" t="inlineStr"/>
+      <c r="HR9" t="inlineStr"/>
+      <c r="HS9" t="inlineStr"/>
+      <c r="HT9" t="inlineStr"/>
+      <c r="HU9" t="inlineStr"/>
+      <c r="HV9" t="inlineStr"/>
+      <c r="HW9" t="inlineStr"/>
+      <c r="HX9" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="HY9" t="inlineStr">
+        <is>
+          <t>025</t>
+        </is>
+      </c>
+      <c r="HZ9" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="IA9" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="IB9" t="inlineStr">
+        <is>
+          <t>16.0</t>
+        </is>
+      </c>
+      <c r="IC9" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="ID9" t="inlineStr"/>
+      <c r="IE9" t="inlineStr"/>
+      <c r="IF9" t="inlineStr"/>
+      <c r="IG9" t="inlineStr">
+        <is>
+          <t>7.21</t>
+        </is>
+      </c>
+      <c r="IH9" t="inlineStr">
+        <is>
+          <t>7.63</t>
+        </is>
+      </c>
+      <c r="II9" t="inlineStr"/>
+      <c r="IJ9" t="inlineStr">
+        <is>
+          <t>8.01</t>
+        </is>
+      </c>
+      <c r="IK9" t="inlineStr">
+        <is>
+          <t>8.92</t>
+        </is>
+      </c>
+      <c r="IL9" t="inlineStr">
+        <is>
+          <t>8.23</t>
+        </is>
+      </c>
+      <c r="IM9" t="inlineStr">
+        <is>
+          <t>9.00</t>
+        </is>
+      </c>
+      <c r="IN9" t="inlineStr">
+        <is>
+          <t>7.80</t>
+        </is>
+      </c>
+      <c r="IO9" t="inlineStr">
+        <is>
+          <t>8.58</t>
+        </is>
+      </c>
+      <c r="IP9" t="inlineStr"/>
+      <c r="IQ9" t="inlineStr"/>
+      <c r="IR9" t="inlineStr"/>
+      <c r="IS9" t="inlineStr"/>
+      <c r="IT9" t="inlineStr"/>
+      <c r="IU9" t="inlineStr"/>
+      <c r="IV9" t="inlineStr"/>
+      <c r="IW9" t="inlineStr"/>
+      <c r="IX9" t="inlineStr"/>
+      <c r="IY9" t="inlineStr"/>
+      <c r="IZ9" t="inlineStr"/>
+      <c r="JA9" t="inlineStr">
+        <is>
+          <t>106</t>
+        </is>
+      </c>
+      <c r="JB9" t="inlineStr"/>
+      <c r="JC9" t="inlineStr">
+        <is>
+          <t>111</t>
+        </is>
+      </c>
+      <c r="JD9" t="inlineStr">
+        <is>
+          <t>124</t>
+        </is>
+      </c>
+      <c r="JE9" t="inlineStr">
+        <is>
+          <t>114</t>
+        </is>
+      </c>
+      <c r="JF9" t="inlineStr">
+        <is>
+          <t>125</t>
+        </is>
+      </c>
+      <c r="JG9" t="inlineStr">
+        <is>
+          <t>108</t>
+        </is>
+      </c>
+      <c r="JH9" t="inlineStr">
+        <is>
+          <t>119</t>
+        </is>
+      </c>
+      <c r="JI9" t="inlineStr"/>
+      <c r="JJ9" t="inlineStr"/>
+      <c r="JK9" t="inlineStr"/>
+      <c r="JL9" t="inlineStr"/>
+      <c r="JM9" t="inlineStr">
+        <is>
+          <t>-3</t>
+        </is>
+      </c>
+      <c r="JN9" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="JO9" t="inlineStr">
+        <is>
+          <t>-0</t>
+        </is>
+      </c>
+      <c r="JP9" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="JQ9" t="inlineStr">
+        <is>
+          <t>-6</t>
+        </is>
+      </c>
+      <c r="JR9" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="JS9" t="inlineStr"/>
+      <c r="JT9" t="inlineStr"/>
+      <c r="JU9" t="inlineStr"/>
+      <c r="JV9" t="inlineStr"/>
+      <c r="JW9" t="inlineStr"/>
+      <c r="JX9" t="inlineStr"/>
+      <c r="JY9" t="inlineStr"/>
+      <c r="JZ9" t="inlineStr"/>
+      <c r="KA9" t="inlineStr"/>
+      <c r="KB9" t="inlineStr"/>
+      <c r="KC9" t="inlineStr"/>
+      <c r="KD9" t="inlineStr"/>
+      <c r="KE9" t="inlineStr"/>
+      <c r="KF9" t="inlineStr"/>
+      <c r="KG9" t="inlineStr"/>
+      <c r="KH9" t="inlineStr"/>
+      <c r="KI9" t="inlineStr"/>
+      <c r="KJ9" t="inlineStr"/>
+      <c r="KK9" t="inlineStr"/>
+      <c r="KL9" t="inlineStr"/>
+      <c r="KM9" t="inlineStr"/>
+      <c r="KN9" t="inlineStr"/>
+      <c r="KO9" t="inlineStr"/>
+      <c r="KP9" t="inlineStr"/>
+      <c r="KQ9" t="inlineStr"/>
+      <c r="KR9" t="inlineStr"/>
+      <c r="KS9" t="inlineStr"/>
+      <c r="KT9" t="inlineStr"/>
+      <c r="KU9" t="inlineStr"/>
+      <c r="KV9" t="inlineStr"/>
+      <c r="KW9" t="inlineStr"/>
+      <c r="KX9" t="inlineStr"/>
+      <c r="KY9" t="inlineStr"/>
+      <c r="KZ9" t="inlineStr"/>
+      <c r="LA9" t="inlineStr"/>
+      <c r="LB9" t="inlineStr"/>
+      <c r="LC9" t="inlineStr"/>
+      <c r="LD9" t="inlineStr"/>
+      <c r="LE9" t="inlineStr"/>
+      <c r="LF9" t="inlineStr"/>
+      <c r="LG9" t="inlineStr"/>
+      <c r="LH9" t="inlineStr"/>
+      <c r="LI9" t="inlineStr"/>
+      <c r="LJ9" t="inlineStr"/>
+      <c r="LK9" t="inlineStr"/>
+      <c r="LL9" t="inlineStr"/>
+      <c r="LM9" t="inlineStr"/>
+      <c r="LN9" t="inlineStr"/>
+      <c r="LO9" t="inlineStr"/>
+      <c r="LP9" t="inlineStr"/>
+      <c r="LQ9" t="inlineStr"/>
+      <c r="LR9" t="inlineStr"/>
+      <c r="LS9" t="inlineStr"/>
+      <c r="LT9" t="inlineStr"/>
+      <c r="LU9" t="inlineStr"/>
+      <c r="LV9" t="inlineStr"/>
+      <c r="LW9" t="inlineStr"/>
+      <c r="LX9" t="inlineStr"/>
+      <c r="LY9" t="inlineStr"/>
+      <c r="LZ9" t="inlineStr"/>
+      <c r="MA9" t="inlineStr"/>
+      <c r="MB9" t="inlineStr"/>
+      <c r="MC9" t="inlineStr"/>
+      <c r="MD9" t="inlineStr"/>
+      <c r="ME9" t="inlineStr"/>
+      <c r="MF9" t="inlineStr"/>
+      <c r="MG9" t="inlineStr"/>
+      <c r="MH9" t="inlineStr"/>
+      <c r="MI9" t="inlineStr"/>
+      <c r="MJ9" t="inlineStr"/>
+      <c r="MK9" t="inlineStr"/>
+      <c r="ML9" t="inlineStr"/>
+      <c r="MM9" t="inlineStr"/>
+      <c r="MN9" t="inlineStr"/>
+      <c r="MO9" t="inlineStr"/>
+      <c r="MP9" t="inlineStr"/>
+      <c r="MQ9" t="inlineStr"/>
+      <c r="MR9" t="inlineStr"/>
+      <c r="MS9" t="inlineStr"/>
+      <c r="MT9" t="inlineStr"/>
+      <c r="MU9" t="inlineStr"/>
+      <c r="MV9" t="inlineStr"/>
+      <c r="MW9" t="inlineStr"/>
+      <c r="MX9" t="inlineStr"/>
+      <c r="MY9" t="inlineStr"/>
+      <c r="MZ9" t="inlineStr"/>
+      <c r="NA9" t="inlineStr"/>
+      <c r="NB9" t="inlineStr"/>
+      <c r="NC9" t="inlineStr"/>
+      <c r="ND9" t="inlineStr"/>
+      <c r="NE9" t="inlineStr"/>
+      <c r="NF9" t="inlineStr"/>
+      <c r="NG9" t="inlineStr"/>
+      <c r="NH9" t="inlineStr"/>
+      <c r="NI9" t="inlineStr"/>
+      <c r="NJ9" t="inlineStr"/>
+      <c r="NK9" t="inlineStr"/>
+      <c r="NL9" t="inlineStr"/>
+      <c r="NM9" t="inlineStr"/>
+      <c r="NN9" t="inlineStr"/>
+      <c r="NO9" t="inlineStr"/>
+      <c r="NP9" t="inlineStr"/>
+      <c r="NQ9" t="inlineStr"/>
+      <c r="NR9" t="inlineStr"/>
+      <c r="NS9" t="inlineStr"/>
+      <c r="NT9" t="inlineStr"/>
+      <c r="NU9" t="inlineStr"/>
+      <c r="NV9" t="inlineStr"/>
+      <c r="NW9" t="inlineStr"/>
+      <c r="NX9" t="inlineStr"/>
+      <c r="NY9" t="inlineStr"/>
+      <c r="NZ9" t="inlineStr"/>
+      <c r="OA9" t="inlineStr"/>
+      <c r="OB9" t="inlineStr"/>
+      <c r="OC9" t="inlineStr"/>
+      <c r="OD9" t="inlineStr"/>
+      <c r="OE9" t="inlineStr"/>
+      <c r="OF9" t="inlineStr"/>
+      <c r="OG9" t="inlineStr"/>
+      <c r="OH9" t="inlineStr"/>
+      <c r="OI9" t="inlineStr"/>
+      <c r="OJ9" t="inlineStr"/>
+      <c r="OK9" t="inlineStr"/>
+      <c r="OL9" t="inlineStr"/>
+      <c r="OM9" t="inlineStr"/>
+      <c r="ON9" t="inlineStr"/>
+      <c r="OO9" t="inlineStr"/>
+      <c r="OP9" t="inlineStr"/>
+      <c r="OQ9" t="inlineStr"/>
+      <c r="OR9" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
c: progress dir progressing
</commit_message>
<xml_diff>
--- a/OOMII.xlsx
+++ b/OOMII.xlsx
@@ -346,7 +346,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:OR9"/>
+  <dimension ref="A1:OR13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5474,12 +5474,6 @@
           <t>type01</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr">
         <is>
           <t>0.0625</t>
@@ -5510,9 +5504,6 @@
           <t>25.0</t>
         </is>
       </c>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
-      <c r="P8" t="inlineStr"/>
       <c r="Q8" t="inlineStr">
         <is>
           <t>3.22</t>
@@ -5523,7 +5514,6 @@
           <t>3.03</t>
         </is>
       </c>
-      <c r="S8" t="inlineStr"/>
       <c r="T8" t="inlineStr">
         <is>
           <t>3.00</t>
@@ -5554,23 +5544,11 @@
           <t>2.75</t>
         </is>
       </c>
-      <c r="Z8" t="inlineStr"/>
-      <c r="AA8" t="inlineStr"/>
-      <c r="AB8" t="inlineStr"/>
-      <c r="AC8" t="inlineStr"/>
-      <c r="AD8" t="inlineStr"/>
-      <c r="AE8" t="inlineStr"/>
-      <c r="AF8" t="inlineStr"/>
-      <c r="AG8" t="inlineStr"/>
-      <c r="AH8" t="inlineStr"/>
-      <c r="AI8" t="inlineStr"/>
-      <c r="AJ8" t="inlineStr"/>
       <c r="AK8" t="inlineStr">
         <is>
           <t>94</t>
         </is>
       </c>
-      <c r="AL8" t="inlineStr"/>
       <c r="AM8" t="inlineStr">
         <is>
           <t>93</t>
@@ -5601,10 +5579,6 @@
           <t>35</t>
         </is>
       </c>
-      <c r="AS8" t="inlineStr"/>
-      <c r="AT8" t="inlineStr"/>
-      <c r="AU8" t="inlineStr"/>
-      <c r="AV8" t="inlineStr"/>
       <c r="AW8" t="inlineStr">
         <is>
           <t>.1</t>
@@ -5635,18 +5609,6 @@
           <t>.9</t>
         </is>
       </c>
-      <c r="BC8" t="inlineStr"/>
-      <c r="BD8" t="inlineStr"/>
-      <c r="BE8" t="inlineStr"/>
-      <c r="BF8" t="inlineStr"/>
-      <c r="BG8" t="inlineStr"/>
-      <c r="BH8" t="inlineStr"/>
-      <c r="BI8" t="inlineStr"/>
-      <c r="BJ8" t="inlineStr"/>
-      <c r="BK8" t="inlineStr"/>
-      <c r="BL8" t="inlineStr"/>
-      <c r="BM8" t="inlineStr"/>
-      <c r="BN8" t="inlineStr"/>
       <c r="BO8" t="inlineStr">
         <is>
           <t>0.0625</t>
@@ -5677,9 +5639,6 @@
           <t>25.0</t>
         </is>
       </c>
-      <c r="BU8" t="inlineStr"/>
-      <c r="BV8" t="inlineStr"/>
-      <c r="BW8" t="inlineStr"/>
       <c r="BX8" t="inlineStr">
         <is>
           <t>2.51</t>
@@ -5690,7 +5649,6 @@
           <t>2.20</t>
         </is>
       </c>
-      <c r="BZ8" t="inlineStr"/>
       <c r="CA8" t="inlineStr">
         <is>
           <t>2.23</t>
@@ -5721,23 +5679,11 @@
           <t>1.99</t>
         </is>
       </c>
-      <c r="CG8" t="inlineStr"/>
-      <c r="CH8" t="inlineStr"/>
-      <c r="CI8" t="inlineStr"/>
-      <c r="CJ8" t="inlineStr"/>
-      <c r="CK8" t="inlineStr"/>
-      <c r="CL8" t="inlineStr"/>
-      <c r="CM8" t="inlineStr"/>
-      <c r="CN8" t="inlineStr"/>
-      <c r="CO8" t="inlineStr"/>
-      <c r="CP8" t="inlineStr"/>
-      <c r="CQ8" t="inlineStr"/>
       <c r="CR8" t="inlineStr">
         <is>
           <t>91</t>
         </is>
       </c>
-      <c r="CS8" t="inlineStr"/>
       <c r="CT8" t="inlineStr">
         <is>
           <t>39</t>
@@ -5768,10 +5714,6 @@
           <t>79</t>
         </is>
       </c>
-      <c r="CZ8" t="inlineStr"/>
-      <c r="DA8" t="inlineStr"/>
-      <c r="DB8" t="inlineStr"/>
-      <c r="DC8" t="inlineStr"/>
       <c r="DD8" t="inlineStr">
         <is>
           <t>.2</t>
@@ -5802,36 +5744,11 @@
           <t>.13</t>
         </is>
       </c>
-      <c r="DJ8" t="inlineStr"/>
-      <c r="DK8" t="inlineStr"/>
-      <c r="DL8" t="inlineStr"/>
-      <c r="DM8" t="inlineStr"/>
-      <c r="DN8" t="inlineStr"/>
-      <c r="DO8" t="inlineStr"/>
       <c r="DP8" t="inlineStr">
         <is>
           <t>220</t>
         </is>
       </c>
-      <c r="DQ8" t="inlineStr"/>
-      <c r="DR8" t="inlineStr"/>
-      <c r="DS8" t="inlineStr"/>
-      <c r="DT8" t="inlineStr"/>
-      <c r="DU8" t="inlineStr"/>
-      <c r="DV8" t="inlineStr"/>
-      <c r="DW8" t="inlineStr"/>
-      <c r="DX8" t="inlineStr"/>
-      <c r="DY8" t="inlineStr"/>
-      <c r="DZ8" t="inlineStr"/>
-      <c r="EA8" t="inlineStr"/>
-      <c r="EB8" t="inlineStr"/>
-      <c r="EC8" t="inlineStr"/>
-      <c r="ED8" t="inlineStr"/>
-      <c r="EE8" t="inlineStr"/>
-      <c r="EF8" t="inlineStr"/>
-      <c r="EG8" t="inlineStr"/>
-      <c r="EH8" t="inlineStr"/>
-      <c r="EI8" t="inlineStr"/>
       <c r="EJ8" t="inlineStr">
         <is>
           <t>2.57</t>
@@ -5862,16 +5779,11 @@
           <t>1.69</t>
         </is>
       </c>
-      <c r="EP8" t="inlineStr"/>
-      <c r="EQ8" t="inlineStr"/>
-      <c r="ER8" t="inlineStr"/>
-      <c r="ES8" t="inlineStr"/>
       <c r="ET8" t="inlineStr">
         <is>
           <t>68</t>
         </is>
       </c>
-      <c r="EU8" t="inlineStr"/>
       <c r="EV8" t="inlineStr">
         <is>
           <t>55</t>
@@ -5902,29 +5814,6 @@
           <t>51</t>
         </is>
       </c>
-      <c r="FB8" t="inlineStr"/>
-      <c r="FC8" t="inlineStr"/>
-      <c r="FD8" t="inlineStr"/>
-      <c r="FE8" t="inlineStr"/>
-      <c r="FF8" t="inlineStr"/>
-      <c r="FG8" t="inlineStr"/>
-      <c r="FH8" t="inlineStr"/>
-      <c r="FI8" t="inlineStr"/>
-      <c r="FJ8" t="inlineStr"/>
-      <c r="FK8" t="inlineStr"/>
-      <c r="FL8" t="inlineStr"/>
-      <c r="FM8" t="inlineStr"/>
-      <c r="FN8" t="inlineStr"/>
-      <c r="FO8" t="inlineStr"/>
-      <c r="FP8" t="inlineStr"/>
-      <c r="FQ8" t="inlineStr"/>
-      <c r="FR8" t="inlineStr"/>
-      <c r="FS8" t="inlineStr"/>
-      <c r="FT8" t="inlineStr"/>
-      <c r="FU8" t="inlineStr"/>
-      <c r="FV8" t="inlineStr"/>
-      <c r="FW8" t="inlineStr"/>
-      <c r="FX8" t="inlineStr"/>
       <c r="FY8" t="inlineStr">
         <is>
           <t>.4</t>
@@ -5955,51 +5844,6 @@
           <t>.24</t>
         </is>
       </c>
-      <c r="GE8" t="inlineStr"/>
-      <c r="GF8" t="inlineStr"/>
-      <c r="GG8" t="inlineStr"/>
-      <c r="GH8" t="inlineStr"/>
-      <c r="GI8" t="inlineStr"/>
-      <c r="GJ8" t="inlineStr"/>
-      <c r="GK8" t="inlineStr"/>
-      <c r="GL8" t="inlineStr"/>
-      <c r="GM8" t="inlineStr"/>
-      <c r="GN8" t="inlineStr"/>
-      <c r="GO8" t="inlineStr"/>
-      <c r="GP8" t="inlineStr"/>
-      <c r="GQ8" t="inlineStr"/>
-      <c r="GR8" t="inlineStr"/>
-      <c r="GS8" t="inlineStr"/>
-      <c r="GT8" t="inlineStr"/>
-      <c r="GU8" t="inlineStr"/>
-      <c r="GV8" t="inlineStr"/>
-      <c r="GW8" t="inlineStr"/>
-      <c r="GX8" t="inlineStr"/>
-      <c r="GY8" t="inlineStr"/>
-      <c r="GZ8" t="inlineStr"/>
-      <c r="HA8" t="inlineStr"/>
-      <c r="HB8" t="inlineStr"/>
-      <c r="HC8" t="inlineStr"/>
-      <c r="HD8" t="inlineStr"/>
-      <c r="HE8" t="inlineStr"/>
-      <c r="HF8" t="inlineStr"/>
-      <c r="HG8" t="inlineStr"/>
-      <c r="HH8" t="inlineStr"/>
-      <c r="HI8" t="inlineStr"/>
-      <c r="HJ8" t="inlineStr"/>
-      <c r="HK8" t="inlineStr"/>
-      <c r="HL8" t="inlineStr"/>
-      <c r="HM8" t="inlineStr"/>
-      <c r="HN8" t="inlineStr"/>
-      <c r="HO8" t="inlineStr"/>
-      <c r="HP8" t="inlineStr"/>
-      <c r="HQ8" t="inlineStr"/>
-      <c r="HR8" t="inlineStr"/>
-      <c r="HS8" t="inlineStr"/>
-      <c r="HT8" t="inlineStr"/>
-      <c r="HU8" t="inlineStr"/>
-      <c r="HV8" t="inlineStr"/>
-      <c r="HW8" t="inlineStr"/>
       <c r="HX8" t="inlineStr">
         <is>
           <t>0.0625</t>
@@ -6030,9 +5874,6 @@
           <t>25.0</t>
         </is>
       </c>
-      <c r="ID8" t="inlineStr"/>
-      <c r="IE8" t="inlineStr"/>
-      <c r="IF8" t="inlineStr"/>
       <c r="IG8" t="inlineStr">
         <is>
           <t>5.45</t>
@@ -6043,7 +5884,6 @@
           <t>9.33</t>
         </is>
       </c>
-      <c r="II8" t="inlineStr"/>
       <c r="IJ8" t="inlineStr">
         <is>
           <t>7.32</t>
@@ -6074,23 +5914,11 @@
           <t>7.31</t>
         </is>
       </c>
-      <c r="IP8" t="inlineStr"/>
-      <c r="IQ8" t="inlineStr"/>
-      <c r="IR8" t="inlineStr"/>
-      <c r="IS8" t="inlineStr"/>
-      <c r="IT8" t="inlineStr"/>
-      <c r="IU8" t="inlineStr"/>
-      <c r="IV8" t="inlineStr"/>
-      <c r="IW8" t="inlineStr"/>
-      <c r="IX8" t="inlineStr"/>
-      <c r="IY8" t="inlineStr"/>
-      <c r="IZ8" t="inlineStr"/>
       <c r="JA8" t="inlineStr">
         <is>
           <t>153</t>
         </is>
       </c>
-      <c r="JB8" t="inlineStr"/>
       <c r="JC8" t="inlineStr">
         <is>
           <t>143</t>
@@ -6121,10 +5949,6 @@
           <t>134</t>
         </is>
       </c>
-      <c r="JI8" t="inlineStr"/>
-      <c r="JJ8" t="inlineStr"/>
-      <c r="JK8" t="inlineStr"/>
-      <c r="JL8" t="inlineStr"/>
       <c r="JM8" t="inlineStr">
         <is>
           <t>.9</t>
@@ -6155,136 +5979,6 @@
           <t>.15</t>
         </is>
       </c>
-      <c r="JS8" t="inlineStr"/>
-      <c r="JT8" t="inlineStr"/>
-      <c r="JU8" t="inlineStr"/>
-      <c r="JV8" t="inlineStr"/>
-      <c r="JW8" t="inlineStr"/>
-      <c r="JX8" t="inlineStr"/>
-      <c r="JY8" t="inlineStr"/>
-      <c r="JZ8" t="inlineStr"/>
-      <c r="KA8" t="inlineStr"/>
-      <c r="KB8" t="inlineStr"/>
-      <c r="KC8" t="inlineStr"/>
-      <c r="KD8" t="inlineStr"/>
-      <c r="KE8" t="inlineStr"/>
-      <c r="KF8" t="inlineStr"/>
-      <c r="KG8" t="inlineStr"/>
-      <c r="KH8" t="inlineStr"/>
-      <c r="KI8" t="inlineStr"/>
-      <c r="KJ8" t="inlineStr"/>
-      <c r="KK8" t="inlineStr"/>
-      <c r="KL8" t="inlineStr"/>
-      <c r="KM8" t="inlineStr"/>
-      <c r="KN8" t="inlineStr"/>
-      <c r="KO8" t="inlineStr"/>
-      <c r="KP8" t="inlineStr"/>
-      <c r="KQ8" t="inlineStr"/>
-      <c r="KR8" t="inlineStr"/>
-      <c r="KS8" t="inlineStr"/>
-      <c r="KT8" t="inlineStr"/>
-      <c r="KU8" t="inlineStr"/>
-      <c r="KV8" t="inlineStr"/>
-      <c r="KW8" t="inlineStr"/>
-      <c r="KX8" t="inlineStr"/>
-      <c r="KY8" t="inlineStr"/>
-      <c r="KZ8" t="inlineStr"/>
-      <c r="LA8" t="inlineStr"/>
-      <c r="LB8" t="inlineStr"/>
-      <c r="LC8" t="inlineStr"/>
-      <c r="LD8" t="inlineStr"/>
-      <c r="LE8" t="inlineStr"/>
-      <c r="LF8" t="inlineStr"/>
-      <c r="LG8" t="inlineStr"/>
-      <c r="LH8" t="inlineStr"/>
-      <c r="LI8" t="inlineStr"/>
-      <c r="LJ8" t="inlineStr"/>
-      <c r="LK8" t="inlineStr"/>
-      <c r="LL8" t="inlineStr"/>
-      <c r="LM8" t="inlineStr"/>
-      <c r="LN8" t="inlineStr"/>
-      <c r="LO8" t="inlineStr"/>
-      <c r="LP8" t="inlineStr"/>
-      <c r="LQ8" t="inlineStr"/>
-      <c r="LR8" t="inlineStr"/>
-      <c r="LS8" t="inlineStr"/>
-      <c r="LT8" t="inlineStr"/>
-      <c r="LU8" t="inlineStr"/>
-      <c r="LV8" t="inlineStr"/>
-      <c r="LW8" t="inlineStr"/>
-      <c r="LX8" t="inlineStr"/>
-      <c r="LY8" t="inlineStr"/>
-      <c r="LZ8" t="inlineStr"/>
-      <c r="MA8" t="inlineStr"/>
-      <c r="MB8" t="inlineStr"/>
-      <c r="MC8" t="inlineStr"/>
-      <c r="MD8" t="inlineStr"/>
-      <c r="ME8" t="inlineStr"/>
-      <c r="MF8" t="inlineStr"/>
-      <c r="MG8" t="inlineStr"/>
-      <c r="MH8" t="inlineStr"/>
-      <c r="MI8" t="inlineStr"/>
-      <c r="MJ8" t="inlineStr"/>
-      <c r="MK8" t="inlineStr"/>
-      <c r="ML8" t="inlineStr"/>
-      <c r="MM8" t="inlineStr"/>
-      <c r="MN8" t="inlineStr"/>
-      <c r="MO8" t="inlineStr"/>
-      <c r="MP8" t="inlineStr"/>
-      <c r="MQ8" t="inlineStr"/>
-      <c r="MR8" t="inlineStr"/>
-      <c r="MS8" t="inlineStr"/>
-      <c r="MT8" t="inlineStr"/>
-      <c r="MU8" t="inlineStr"/>
-      <c r="MV8" t="inlineStr"/>
-      <c r="MW8" t="inlineStr"/>
-      <c r="MX8" t="inlineStr"/>
-      <c r="MY8" t="inlineStr"/>
-      <c r="MZ8" t="inlineStr"/>
-      <c r="NA8" t="inlineStr"/>
-      <c r="NB8" t="inlineStr"/>
-      <c r="NC8" t="inlineStr"/>
-      <c r="ND8" t="inlineStr"/>
-      <c r="NE8" t="inlineStr"/>
-      <c r="NF8" t="inlineStr"/>
-      <c r="NG8" t="inlineStr"/>
-      <c r="NH8" t="inlineStr"/>
-      <c r="NI8" t="inlineStr"/>
-      <c r="NJ8" t="inlineStr"/>
-      <c r="NK8" t="inlineStr"/>
-      <c r="NL8" t="inlineStr"/>
-      <c r="NM8" t="inlineStr"/>
-      <c r="NN8" t="inlineStr"/>
-      <c r="NO8" t="inlineStr"/>
-      <c r="NP8" t="inlineStr"/>
-      <c r="NQ8" t="inlineStr"/>
-      <c r="NR8" t="inlineStr"/>
-      <c r="NS8" t="inlineStr"/>
-      <c r="NT8" t="inlineStr"/>
-      <c r="NU8" t="inlineStr"/>
-      <c r="NV8" t="inlineStr"/>
-      <c r="NW8" t="inlineStr"/>
-      <c r="NX8" t="inlineStr"/>
-      <c r="NY8" t="inlineStr"/>
-      <c r="NZ8" t="inlineStr"/>
-      <c r="OA8" t="inlineStr"/>
-      <c r="OB8" t="inlineStr"/>
-      <c r="OC8" t="inlineStr"/>
-      <c r="OD8" t="inlineStr"/>
-      <c r="OE8" t="inlineStr"/>
-      <c r="OF8" t="inlineStr"/>
-      <c r="OG8" t="inlineStr"/>
-      <c r="OH8" t="inlineStr"/>
-      <c r="OI8" t="inlineStr"/>
-      <c r="OJ8" t="inlineStr"/>
-      <c r="OK8" t="inlineStr"/>
-      <c r="OL8" t="inlineStr"/>
-      <c r="OM8" t="inlineStr"/>
-      <c r="ON8" t="inlineStr"/>
-      <c r="OO8" t="inlineStr"/>
-      <c r="OP8" t="inlineStr"/>
-      <c r="OQ8" t="inlineStr"/>
-      <c r="OR8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -6292,12 +5986,6 @@
           <t>type01</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr">
         <is>
           <t>0.0625</t>
@@ -6328,9 +6016,6 @@
           <t>25.0</t>
         </is>
       </c>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
-      <c r="P9" t="inlineStr"/>
       <c r="Q9" t="inlineStr">
         <is>
           <t>4.39</t>
@@ -6341,7 +6026,6 @@
           <t>2.88</t>
         </is>
       </c>
-      <c r="S9" t="inlineStr"/>
       <c r="T9" t="inlineStr">
         <is>
           <t>2.92</t>
@@ -6372,23 +6056,11 @@
           <t>2.90</t>
         </is>
       </c>
-      <c r="Z9" t="inlineStr"/>
-      <c r="AA9" t="inlineStr"/>
-      <c r="AB9" t="inlineStr"/>
-      <c r="AC9" t="inlineStr"/>
-      <c r="AD9" t="inlineStr"/>
-      <c r="AE9" t="inlineStr"/>
-      <c r="AF9" t="inlineStr"/>
-      <c r="AG9" t="inlineStr"/>
-      <c r="AH9" t="inlineStr"/>
-      <c r="AI9" t="inlineStr"/>
-      <c r="AJ9" t="inlineStr"/>
       <c r="AK9" t="inlineStr">
         <is>
           <t>6</t>
         </is>
       </c>
-      <c r="AL9" t="inlineStr"/>
       <c r="AM9" t="inlineStr">
         <is>
           <t>67</t>
@@ -6419,10 +6091,6 @@
           <t>66</t>
         </is>
       </c>
-      <c r="AS9" t="inlineStr"/>
-      <c r="AT9" t="inlineStr"/>
-      <c r="AU9" t="inlineStr"/>
-      <c r="AV9" t="inlineStr"/>
       <c r="AW9" t="inlineStr">
         <is>
           <t>-1</t>
@@ -6453,18 +6121,6 @@
           <t>-1</t>
         </is>
       </c>
-      <c r="BC9" t="inlineStr"/>
-      <c r="BD9" t="inlineStr"/>
-      <c r="BE9" t="inlineStr"/>
-      <c r="BF9" t="inlineStr"/>
-      <c r="BG9" t="inlineStr"/>
-      <c r="BH9" t="inlineStr"/>
-      <c r="BI9" t="inlineStr"/>
-      <c r="BJ9" t="inlineStr"/>
-      <c r="BK9" t="inlineStr"/>
-      <c r="BL9" t="inlineStr"/>
-      <c r="BM9" t="inlineStr"/>
-      <c r="BN9" t="inlineStr"/>
       <c r="BO9" t="inlineStr">
         <is>
           <t>0.0625</t>
@@ -6495,9 +6151,6 @@
           <t>25.0</t>
         </is>
       </c>
-      <c r="BU9" t="inlineStr"/>
-      <c r="BV9" t="inlineStr"/>
-      <c r="BW9" t="inlineStr"/>
       <c r="BX9" t="inlineStr">
         <is>
           <t>3.06</t>
@@ -6508,7 +6161,6 @@
           <t>2.17</t>
         </is>
       </c>
-      <c r="BZ9" t="inlineStr"/>
       <c r="CA9" t="inlineStr">
         <is>
           <t>225</t>
@@ -6539,23 +6191,11 @@
           <t>2.16</t>
         </is>
       </c>
-      <c r="CG9" t="inlineStr"/>
-      <c r="CH9" t="inlineStr"/>
-      <c r="CI9" t="inlineStr"/>
-      <c r="CJ9" t="inlineStr"/>
-      <c r="CK9" t="inlineStr"/>
-      <c r="CL9" t="inlineStr"/>
-      <c r="CM9" t="inlineStr"/>
-      <c r="CN9" t="inlineStr"/>
-      <c r="CO9" t="inlineStr"/>
-      <c r="CP9" t="inlineStr"/>
-      <c r="CQ9" t="inlineStr"/>
       <c r="CR9" t="inlineStr">
         <is>
           <t>71</t>
         </is>
       </c>
-      <c r="CS9" t="inlineStr"/>
       <c r="CT9" t="inlineStr">
         <is>
           <t>74</t>
@@ -6586,10 +6226,6 @@
           <t>71</t>
         </is>
       </c>
-      <c r="CZ9" t="inlineStr"/>
-      <c r="DA9" t="inlineStr"/>
-      <c r="DB9" t="inlineStr"/>
-      <c r="DC9" t="inlineStr"/>
       <c r="DD9" t="inlineStr">
         <is>
           <t>0</t>
@@ -6620,36 +6256,11 @@
           <t>4</t>
         </is>
       </c>
-      <c r="DJ9" t="inlineStr"/>
-      <c r="DK9" t="inlineStr"/>
-      <c r="DL9" t="inlineStr"/>
-      <c r="DM9" t="inlineStr"/>
-      <c r="DN9" t="inlineStr"/>
-      <c r="DO9" t="inlineStr"/>
       <c r="DP9" t="inlineStr">
         <is>
           <t>20</t>
         </is>
       </c>
-      <c r="DQ9" t="inlineStr"/>
-      <c r="DR9" t="inlineStr"/>
-      <c r="DS9" t="inlineStr"/>
-      <c r="DT9" t="inlineStr"/>
-      <c r="DU9" t="inlineStr"/>
-      <c r="DV9" t="inlineStr"/>
-      <c r="DW9" t="inlineStr"/>
-      <c r="DX9" t="inlineStr"/>
-      <c r="DY9" t="inlineStr"/>
-      <c r="DZ9" t="inlineStr"/>
-      <c r="EA9" t="inlineStr"/>
-      <c r="EB9" t="inlineStr"/>
-      <c r="EC9" t="inlineStr"/>
-      <c r="ED9" t="inlineStr"/>
-      <c r="EE9" t="inlineStr"/>
-      <c r="EF9" t="inlineStr"/>
-      <c r="EG9" t="inlineStr"/>
-      <c r="EH9" t="inlineStr"/>
-      <c r="EI9" t="inlineStr"/>
       <c r="EJ9" t="inlineStr">
         <is>
           <t>2.60</t>
@@ -6680,16 +6291,11 @@
           <t>1.75</t>
         </is>
       </c>
-      <c r="EP9" t="inlineStr"/>
-      <c r="EQ9" t="inlineStr"/>
-      <c r="ER9" t="inlineStr"/>
-      <c r="ES9" t="inlineStr"/>
       <c r="ET9" t="inlineStr">
         <is>
           <t>66</t>
         </is>
       </c>
-      <c r="EU9" t="inlineStr"/>
       <c r="EV9" t="inlineStr">
         <is>
           <t>73</t>
@@ -6720,29 +6326,6 @@
           <t>61</t>
         </is>
       </c>
-      <c r="FB9" t="inlineStr"/>
-      <c r="FC9" t="inlineStr"/>
-      <c r="FD9" t="inlineStr"/>
-      <c r="FE9" t="inlineStr"/>
-      <c r="FF9" t="inlineStr"/>
-      <c r="FG9" t="inlineStr"/>
-      <c r="FH9" t="inlineStr"/>
-      <c r="FI9" t="inlineStr"/>
-      <c r="FJ9" t="inlineStr"/>
-      <c r="FK9" t="inlineStr"/>
-      <c r="FL9" t="inlineStr"/>
-      <c r="FM9" t="inlineStr"/>
-      <c r="FN9" t="inlineStr"/>
-      <c r="FO9" t="inlineStr"/>
-      <c r="FP9" t="inlineStr"/>
-      <c r="FQ9" t="inlineStr"/>
-      <c r="FR9" t="inlineStr"/>
-      <c r="FS9" t="inlineStr"/>
-      <c r="FT9" t="inlineStr"/>
-      <c r="FU9" t="inlineStr"/>
-      <c r="FV9" t="inlineStr"/>
-      <c r="FW9" t="inlineStr"/>
-      <c r="FX9" t="inlineStr"/>
       <c r="FY9" t="inlineStr">
         <is>
           <t>2</t>
@@ -6773,51 +6356,6 @@
           <t>-15</t>
         </is>
       </c>
-      <c r="GE9" t="inlineStr"/>
-      <c r="GF9" t="inlineStr"/>
-      <c r="GG9" t="inlineStr"/>
-      <c r="GH9" t="inlineStr"/>
-      <c r="GI9" t="inlineStr"/>
-      <c r="GJ9" t="inlineStr"/>
-      <c r="GK9" t="inlineStr"/>
-      <c r="GL9" t="inlineStr"/>
-      <c r="GM9" t="inlineStr"/>
-      <c r="GN9" t="inlineStr"/>
-      <c r="GO9" t="inlineStr"/>
-      <c r="GP9" t="inlineStr"/>
-      <c r="GQ9" t="inlineStr"/>
-      <c r="GR9" t="inlineStr"/>
-      <c r="GS9" t="inlineStr"/>
-      <c r="GT9" t="inlineStr"/>
-      <c r="GU9" t="inlineStr"/>
-      <c r="GV9" t="inlineStr"/>
-      <c r="GW9" t="inlineStr"/>
-      <c r="GX9" t="inlineStr"/>
-      <c r="GY9" t="inlineStr"/>
-      <c r="GZ9" t="inlineStr"/>
-      <c r="HA9" t="inlineStr"/>
-      <c r="HB9" t="inlineStr"/>
-      <c r="HC9" t="inlineStr"/>
-      <c r="HD9" t="inlineStr"/>
-      <c r="HE9" t="inlineStr"/>
-      <c r="HF9" t="inlineStr"/>
-      <c r="HG9" t="inlineStr"/>
-      <c r="HH9" t="inlineStr"/>
-      <c r="HI9" t="inlineStr"/>
-      <c r="HJ9" t="inlineStr"/>
-      <c r="HK9" t="inlineStr"/>
-      <c r="HL9" t="inlineStr"/>
-      <c r="HM9" t="inlineStr"/>
-      <c r="HN9" t="inlineStr"/>
-      <c r="HO9" t="inlineStr"/>
-      <c r="HP9" t="inlineStr"/>
-      <c r="HQ9" t="inlineStr"/>
-      <c r="HR9" t="inlineStr"/>
-      <c r="HS9" t="inlineStr"/>
-      <c r="HT9" t="inlineStr"/>
-      <c r="HU9" t="inlineStr"/>
-      <c r="HV9" t="inlineStr"/>
-      <c r="HW9" t="inlineStr"/>
       <c r="HX9" t="inlineStr">
         <is>
           <t>0.0625</t>
@@ -6848,9 +6386,6 @@
           <t>25.0</t>
         </is>
       </c>
-      <c r="ID9" t="inlineStr"/>
-      <c r="IE9" t="inlineStr"/>
-      <c r="IF9" t="inlineStr"/>
       <c r="IG9" t="inlineStr">
         <is>
           <t>7.21</t>
@@ -6861,7 +6396,6 @@
           <t>7.63</t>
         </is>
       </c>
-      <c r="II9" t="inlineStr"/>
       <c r="IJ9" t="inlineStr">
         <is>
           <t>8.01</t>
@@ -6892,23 +6426,11 @@
           <t>8.58</t>
         </is>
       </c>
-      <c r="IP9" t="inlineStr"/>
-      <c r="IQ9" t="inlineStr"/>
-      <c r="IR9" t="inlineStr"/>
-      <c r="IS9" t="inlineStr"/>
-      <c r="IT9" t="inlineStr"/>
-      <c r="IU9" t="inlineStr"/>
-      <c r="IV9" t="inlineStr"/>
-      <c r="IW9" t="inlineStr"/>
-      <c r="IX9" t="inlineStr"/>
-      <c r="IY9" t="inlineStr"/>
-      <c r="IZ9" t="inlineStr"/>
       <c r="JA9" t="inlineStr">
         <is>
           <t>106</t>
         </is>
       </c>
-      <c r="JB9" t="inlineStr"/>
       <c r="JC9" t="inlineStr">
         <is>
           <t>111</t>
@@ -6939,10 +6461,6 @@
           <t>119</t>
         </is>
       </c>
-      <c r="JI9" t="inlineStr"/>
-      <c r="JJ9" t="inlineStr"/>
-      <c r="JK9" t="inlineStr"/>
-      <c r="JL9" t="inlineStr"/>
       <c r="JM9" t="inlineStr">
         <is>
           <t>-3</t>
@@ -6973,136 +6491,2360 @@
           <t>4</t>
         </is>
       </c>
-      <c r="JS9" t="inlineStr"/>
-      <c r="JT9" t="inlineStr"/>
-      <c r="JU9" t="inlineStr"/>
-      <c r="JV9" t="inlineStr"/>
-      <c r="JW9" t="inlineStr"/>
-      <c r="JX9" t="inlineStr"/>
-      <c r="JY9" t="inlineStr"/>
-      <c r="JZ9" t="inlineStr"/>
-      <c r="KA9" t="inlineStr"/>
-      <c r="KB9" t="inlineStr"/>
-      <c r="KC9" t="inlineStr"/>
-      <c r="KD9" t="inlineStr"/>
-      <c r="KE9" t="inlineStr"/>
-      <c r="KF9" t="inlineStr"/>
-      <c r="KG9" t="inlineStr"/>
-      <c r="KH9" t="inlineStr"/>
-      <c r="KI9" t="inlineStr"/>
-      <c r="KJ9" t="inlineStr"/>
-      <c r="KK9" t="inlineStr"/>
-      <c r="KL9" t="inlineStr"/>
-      <c r="KM9" t="inlineStr"/>
-      <c r="KN9" t="inlineStr"/>
-      <c r="KO9" t="inlineStr"/>
-      <c r="KP9" t="inlineStr"/>
-      <c r="KQ9" t="inlineStr"/>
-      <c r="KR9" t="inlineStr"/>
-      <c r="KS9" t="inlineStr"/>
-      <c r="KT9" t="inlineStr"/>
-      <c r="KU9" t="inlineStr"/>
-      <c r="KV9" t="inlineStr"/>
-      <c r="KW9" t="inlineStr"/>
-      <c r="KX9" t="inlineStr"/>
-      <c r="KY9" t="inlineStr"/>
-      <c r="KZ9" t="inlineStr"/>
-      <c r="LA9" t="inlineStr"/>
-      <c r="LB9" t="inlineStr"/>
-      <c r="LC9" t="inlineStr"/>
-      <c r="LD9" t="inlineStr"/>
-      <c r="LE9" t="inlineStr"/>
-      <c r="LF9" t="inlineStr"/>
-      <c r="LG9" t="inlineStr"/>
-      <c r="LH9" t="inlineStr"/>
-      <c r="LI9" t="inlineStr"/>
-      <c r="LJ9" t="inlineStr"/>
-      <c r="LK9" t="inlineStr"/>
-      <c r="LL9" t="inlineStr"/>
-      <c r="LM9" t="inlineStr"/>
-      <c r="LN9" t="inlineStr"/>
-      <c r="LO9" t="inlineStr"/>
-      <c r="LP9" t="inlineStr"/>
-      <c r="LQ9" t="inlineStr"/>
-      <c r="LR9" t="inlineStr"/>
-      <c r="LS9" t="inlineStr"/>
-      <c r="LT9" t="inlineStr"/>
-      <c r="LU9" t="inlineStr"/>
-      <c r="LV9" t="inlineStr"/>
-      <c r="LW9" t="inlineStr"/>
-      <c r="LX9" t="inlineStr"/>
-      <c r="LY9" t="inlineStr"/>
-      <c r="LZ9" t="inlineStr"/>
-      <c r="MA9" t="inlineStr"/>
-      <c r="MB9" t="inlineStr"/>
-      <c r="MC9" t="inlineStr"/>
-      <c r="MD9" t="inlineStr"/>
-      <c r="ME9" t="inlineStr"/>
-      <c r="MF9" t="inlineStr"/>
-      <c r="MG9" t="inlineStr"/>
-      <c r="MH9" t="inlineStr"/>
-      <c r="MI9" t="inlineStr"/>
-      <c r="MJ9" t="inlineStr"/>
-      <c r="MK9" t="inlineStr"/>
-      <c r="ML9" t="inlineStr"/>
-      <c r="MM9" t="inlineStr"/>
-      <c r="MN9" t="inlineStr"/>
-      <c r="MO9" t="inlineStr"/>
-      <c r="MP9" t="inlineStr"/>
-      <c r="MQ9" t="inlineStr"/>
-      <c r="MR9" t="inlineStr"/>
-      <c r="MS9" t="inlineStr"/>
-      <c r="MT9" t="inlineStr"/>
-      <c r="MU9" t="inlineStr"/>
-      <c r="MV9" t="inlineStr"/>
-      <c r="MW9" t="inlineStr"/>
-      <c r="MX9" t="inlineStr"/>
-      <c r="MY9" t="inlineStr"/>
-      <c r="MZ9" t="inlineStr"/>
-      <c r="NA9" t="inlineStr"/>
-      <c r="NB9" t="inlineStr"/>
-      <c r="NC9" t="inlineStr"/>
-      <c r="ND9" t="inlineStr"/>
-      <c r="NE9" t="inlineStr"/>
-      <c r="NF9" t="inlineStr"/>
-      <c r="NG9" t="inlineStr"/>
-      <c r="NH9" t="inlineStr"/>
-      <c r="NI9" t="inlineStr"/>
-      <c r="NJ9" t="inlineStr"/>
-      <c r="NK9" t="inlineStr"/>
-      <c r="NL9" t="inlineStr"/>
-      <c r="NM9" t="inlineStr"/>
-      <c r="NN9" t="inlineStr"/>
-      <c r="NO9" t="inlineStr"/>
-      <c r="NP9" t="inlineStr"/>
-      <c r="NQ9" t="inlineStr"/>
-      <c r="NR9" t="inlineStr"/>
-      <c r="NS9" t="inlineStr"/>
-      <c r="NT9" t="inlineStr"/>
-      <c r="NU9" t="inlineStr"/>
-      <c r="NV9" t="inlineStr"/>
-      <c r="NW9" t="inlineStr"/>
-      <c r="NX9" t="inlineStr"/>
-      <c r="NY9" t="inlineStr"/>
-      <c r="NZ9" t="inlineStr"/>
-      <c r="OA9" t="inlineStr"/>
-      <c r="OB9" t="inlineStr"/>
-      <c r="OC9" t="inlineStr"/>
-      <c r="OD9" t="inlineStr"/>
-      <c r="OE9" t="inlineStr"/>
-      <c r="OF9" t="inlineStr"/>
-      <c r="OG9" t="inlineStr"/>
-      <c r="OH9" t="inlineStr"/>
-      <c r="OI9" t="inlineStr"/>
-      <c r="OJ9" t="inlineStr"/>
-      <c r="OK9" t="inlineStr"/>
-      <c r="OL9" t="inlineStr"/>
-      <c r="OM9" t="inlineStr"/>
-      <c r="ON9" t="inlineStr"/>
-      <c r="OO9" t="inlineStr"/>
-      <c r="OP9" t="inlineStr"/>
-      <c r="OQ9" t="inlineStr"/>
-      <c r="OR9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>type01</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>16.0</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>3.22</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>3.03</t>
+        </is>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>3.00</t>
+        </is>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>2.97</t>
+        </is>
+      </c>
+      <c r="V10" t="inlineStr">
+        <is>
+          <t>3.01</t>
+        </is>
+      </c>
+      <c r="W10" t="inlineStr">
+        <is>
+          <t>2.93</t>
+        </is>
+      </c>
+      <c r="X10" t="inlineStr">
+        <is>
+          <t>2.31</t>
+        </is>
+      </c>
+      <c r="Y10" t="inlineStr">
+        <is>
+          <t>2.75</t>
+        </is>
+      </c>
+      <c r="AK10" t="inlineStr">
+        <is>
+          <t>94</t>
+        </is>
+      </c>
+      <c r="AM10" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="AN10" t="inlineStr">
+        <is>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="AO10" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="AP10" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="AQ10" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="AR10" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="AW10" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="AX10" t="inlineStr">
+        <is>
+          <t>.2</t>
+        </is>
+      </c>
+      <c r="AY10" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="AZ10" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="BA10" t="inlineStr">
+        <is>
+          <t>.7</t>
+        </is>
+      </c>
+      <c r="BB10" t="inlineStr">
+        <is>
+          <t>.9</t>
+        </is>
+      </c>
+      <c r="BO10" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="BP10" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="BQ10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="BR10" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="BS10" t="inlineStr">
+        <is>
+          <t>15.0</t>
+        </is>
+      </c>
+      <c r="BT10" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="BX10" t="inlineStr">
+        <is>
+          <t>2.51</t>
+        </is>
+      </c>
+      <c r="BY10" t="inlineStr">
+        <is>
+          <t>2.20</t>
+        </is>
+      </c>
+      <c r="CA10" t="inlineStr">
+        <is>
+          <t>2.23</t>
+        </is>
+      </c>
+      <c r="CB10" t="inlineStr">
+        <is>
+          <t>2.25</t>
+        </is>
+      </c>
+      <c r="CC10" t="inlineStr">
+        <is>
+          <t>2.27</t>
+        </is>
+      </c>
+      <c r="CD10" t="inlineStr">
+        <is>
+          <t>2.20</t>
+        </is>
+      </c>
+      <c r="CE10" t="inlineStr">
+        <is>
+          <t>2.10</t>
+        </is>
+      </c>
+      <c r="CF10" t="inlineStr">
+        <is>
+          <t>1.99</t>
+        </is>
+      </c>
+      <c r="CR10" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="CT10" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="CU10" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="CV10" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="CW10" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="CX10" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="CY10" t="inlineStr">
+        <is>
+          <t>79</t>
+        </is>
+      </c>
+      <c r="DD10" t="inlineStr">
+        <is>
+          <t>.2</t>
+        </is>
+      </c>
+      <c r="DE10" t="inlineStr">
+        <is>
+          <t>.2</t>
+        </is>
+      </c>
+      <c r="DF10" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="DG10" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="DH10" t="inlineStr">
+        <is>
+          <t>.3</t>
+        </is>
+      </c>
+      <c r="DI10" t="inlineStr">
+        <is>
+          <t>.13</t>
+        </is>
+      </c>
+      <c r="DP10" t="inlineStr">
+        <is>
+          <t>220</t>
+        </is>
+      </c>
+      <c r="EJ10" t="inlineStr">
+        <is>
+          <t>2.57</t>
+        </is>
+      </c>
+      <c r="EK10" t="inlineStr">
+        <is>
+          <t>1.75</t>
+        </is>
+      </c>
+      <c r="EL10" t="inlineStr">
+        <is>
+          <t>1.67</t>
+        </is>
+      </c>
+      <c r="EM10" t="inlineStr">
+        <is>
+          <t>1.69</t>
+        </is>
+      </c>
+      <c r="EN10" t="inlineStr">
+        <is>
+          <t>1.73</t>
+        </is>
+      </c>
+      <c r="EO10" t="inlineStr">
+        <is>
+          <t>1.69</t>
+        </is>
+      </c>
+      <c r="ET10" t="inlineStr">
+        <is>
+          <t>68</t>
+        </is>
+      </c>
+      <c r="EV10" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="EW10" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="EX10" t="inlineStr">
+        <is>
+          <t>63</t>
+        </is>
+      </c>
+      <c r="EY10" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="EZ10" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="FA10" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="FY10" t="inlineStr">
+        <is>
+          <t>.4</t>
+        </is>
+      </c>
+      <c r="FZ10" t="inlineStr">
+        <is>
+          <t>.3</t>
+        </is>
+      </c>
+      <c r="GA10" t="inlineStr">
+        <is>
+          <t>.0</t>
+        </is>
+      </c>
+      <c r="GB10" t="inlineStr">
+        <is>
+          <t>.3</t>
+        </is>
+      </c>
+      <c r="GC10" t="inlineStr">
+        <is>
+          <t>.11</t>
+        </is>
+      </c>
+      <c r="GD10" t="inlineStr">
+        <is>
+          <t>.24</t>
+        </is>
+      </c>
+      <c r="HX10" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="HY10" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="HZ10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="IA10" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="IB10" t="inlineStr">
+        <is>
+          <t>16.0</t>
+        </is>
+      </c>
+      <c r="IC10" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="IG10" t="inlineStr">
+        <is>
+          <t>5.45</t>
+        </is>
+      </c>
+      <c r="IH10" t="inlineStr">
+        <is>
+          <t>9.33</t>
+        </is>
+      </c>
+      <c r="IJ10" t="inlineStr">
+        <is>
+          <t>7.32</t>
+        </is>
+      </c>
+      <c r="IK10" t="inlineStr">
+        <is>
+          <t>0.47</t>
+        </is>
+      </c>
+      <c r="IL10" t="inlineStr">
+        <is>
+          <t>7.99</t>
+        </is>
+      </c>
+      <c r="IM10" t="inlineStr">
+        <is>
+          <t>7.64</t>
+        </is>
+      </c>
+      <c r="IN10" t="inlineStr">
+        <is>
+          <t>3.12</t>
+        </is>
+      </c>
+      <c r="IO10" t="inlineStr">
+        <is>
+          <t>7.31</t>
+        </is>
+      </c>
+      <c r="JA10" t="inlineStr">
+        <is>
+          <t>153</t>
+        </is>
+      </c>
+      <c r="JC10" t="inlineStr">
+        <is>
+          <t>143</t>
+        </is>
+      </c>
+      <c r="JD10" t="inlineStr">
+        <is>
+          <t>155</t>
+        </is>
+      </c>
+      <c r="JE10" t="inlineStr">
+        <is>
+          <t>147</t>
+        </is>
+      </c>
+      <c r="JF10" t="inlineStr">
+        <is>
+          <t>140</t>
+        </is>
+      </c>
+      <c r="JG10" t="inlineStr">
+        <is>
+          <t>149</t>
+        </is>
+      </c>
+      <c r="JH10" t="inlineStr">
+        <is>
+          <t>134</t>
+        </is>
+      </c>
+      <c r="JM10" t="inlineStr">
+        <is>
+          <t>.9</t>
+        </is>
+      </c>
+      <c r="JN10" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="JO10" t="inlineStr">
+        <is>
+          <t>.7</t>
+        </is>
+      </c>
+      <c r="JP10" t="inlineStr">
+        <is>
+          <t>.11</t>
+        </is>
+      </c>
+      <c r="JQ10" t="inlineStr">
+        <is>
+          <t>.5</t>
+        </is>
+      </c>
+      <c r="JR10" t="inlineStr">
+        <is>
+          <t>.15</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>type01</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>16.0</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>3.22</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>3.03</t>
+        </is>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>3.00</t>
+        </is>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>2.97</t>
+        </is>
+      </c>
+      <c r="V11" t="inlineStr">
+        <is>
+          <t>3.01</t>
+        </is>
+      </c>
+      <c r="W11" t="inlineStr">
+        <is>
+          <t>2.93</t>
+        </is>
+      </c>
+      <c r="X11" t="inlineStr">
+        <is>
+          <t>2.31</t>
+        </is>
+      </c>
+      <c r="Y11" t="inlineStr">
+        <is>
+          <t>2.75</t>
+        </is>
+      </c>
+      <c r="AK11" t="inlineStr">
+        <is>
+          <t>94</t>
+        </is>
+      </c>
+      <c r="AM11" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="AN11" t="inlineStr">
+        <is>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="AO11" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="AP11" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="AQ11" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="AR11" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="AW11" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="AX11" t="inlineStr">
+        <is>
+          <t>.2</t>
+        </is>
+      </c>
+      <c r="AY11" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="AZ11" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="BA11" t="inlineStr">
+        <is>
+          <t>.7</t>
+        </is>
+      </c>
+      <c r="BB11" t="inlineStr">
+        <is>
+          <t>.9</t>
+        </is>
+      </c>
+      <c r="BO11" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="BP11" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="BQ11" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="BR11" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="BS11" t="inlineStr">
+        <is>
+          <t>15.0</t>
+        </is>
+      </c>
+      <c r="BT11" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="BX11" t="inlineStr">
+        <is>
+          <t>2.51</t>
+        </is>
+      </c>
+      <c r="BY11" t="inlineStr">
+        <is>
+          <t>2.20</t>
+        </is>
+      </c>
+      <c r="CA11" t="inlineStr">
+        <is>
+          <t>2.23</t>
+        </is>
+      </c>
+      <c r="CB11" t="inlineStr">
+        <is>
+          <t>2.25</t>
+        </is>
+      </c>
+      <c r="CC11" t="inlineStr">
+        <is>
+          <t>2.27</t>
+        </is>
+      </c>
+      <c r="CD11" t="inlineStr">
+        <is>
+          <t>2.20</t>
+        </is>
+      </c>
+      <c r="CE11" t="inlineStr">
+        <is>
+          <t>2.10</t>
+        </is>
+      </c>
+      <c r="CF11" t="inlineStr">
+        <is>
+          <t>1.99</t>
+        </is>
+      </c>
+      <c r="CR11" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="CT11" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="CU11" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="CV11" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="CW11" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="CX11" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="CY11" t="inlineStr">
+        <is>
+          <t>79</t>
+        </is>
+      </c>
+      <c r="DD11" t="inlineStr">
+        <is>
+          <t>.2</t>
+        </is>
+      </c>
+      <c r="DE11" t="inlineStr">
+        <is>
+          <t>.2</t>
+        </is>
+      </c>
+      <c r="DF11" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="DG11" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="DH11" t="inlineStr">
+        <is>
+          <t>.3</t>
+        </is>
+      </c>
+      <c r="DI11" t="inlineStr">
+        <is>
+          <t>.13</t>
+        </is>
+      </c>
+      <c r="DP11" t="inlineStr">
+        <is>
+          <t>220</t>
+        </is>
+      </c>
+      <c r="EJ11" t="inlineStr">
+        <is>
+          <t>2.57</t>
+        </is>
+      </c>
+      <c r="EK11" t="inlineStr">
+        <is>
+          <t>1.75</t>
+        </is>
+      </c>
+      <c r="EL11" t="inlineStr">
+        <is>
+          <t>1.67</t>
+        </is>
+      </c>
+      <c r="EM11" t="inlineStr">
+        <is>
+          <t>1.69</t>
+        </is>
+      </c>
+      <c r="EN11" t="inlineStr">
+        <is>
+          <t>1.73</t>
+        </is>
+      </c>
+      <c r="EO11" t="inlineStr">
+        <is>
+          <t>1.69</t>
+        </is>
+      </c>
+      <c r="ET11" t="inlineStr">
+        <is>
+          <t>68</t>
+        </is>
+      </c>
+      <c r="EV11" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="EW11" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="EX11" t="inlineStr">
+        <is>
+          <t>63</t>
+        </is>
+      </c>
+      <c r="EY11" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="EZ11" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="FA11" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="FY11" t="inlineStr">
+        <is>
+          <t>.4</t>
+        </is>
+      </c>
+      <c r="FZ11" t="inlineStr">
+        <is>
+          <t>.3</t>
+        </is>
+      </c>
+      <c r="GA11" t="inlineStr">
+        <is>
+          <t>.0</t>
+        </is>
+      </c>
+      <c r="GB11" t="inlineStr">
+        <is>
+          <t>.3</t>
+        </is>
+      </c>
+      <c r="GC11" t="inlineStr">
+        <is>
+          <t>.11</t>
+        </is>
+      </c>
+      <c r="GD11" t="inlineStr">
+        <is>
+          <t>.24</t>
+        </is>
+      </c>
+      <c r="HX11" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="HY11" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="HZ11" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="IA11" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="IB11" t="inlineStr">
+        <is>
+          <t>16.0</t>
+        </is>
+      </c>
+      <c r="IC11" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="IG11" t="inlineStr">
+        <is>
+          <t>5.45</t>
+        </is>
+      </c>
+      <c r="IH11" t="inlineStr">
+        <is>
+          <t>9.33</t>
+        </is>
+      </c>
+      <c r="IJ11" t="inlineStr">
+        <is>
+          <t>7.32</t>
+        </is>
+      </c>
+      <c r="IK11" t="inlineStr">
+        <is>
+          <t>0.47</t>
+        </is>
+      </c>
+      <c r="IL11" t="inlineStr">
+        <is>
+          <t>7.99</t>
+        </is>
+      </c>
+      <c r="IM11" t="inlineStr">
+        <is>
+          <t>7.64</t>
+        </is>
+      </c>
+      <c r="IN11" t="inlineStr">
+        <is>
+          <t>3.12</t>
+        </is>
+      </c>
+      <c r="IO11" t="inlineStr">
+        <is>
+          <t>7.31</t>
+        </is>
+      </c>
+      <c r="JA11" t="inlineStr">
+        <is>
+          <t>153</t>
+        </is>
+      </c>
+      <c r="JC11" t="inlineStr">
+        <is>
+          <t>143</t>
+        </is>
+      </c>
+      <c r="JD11" t="inlineStr">
+        <is>
+          <t>155</t>
+        </is>
+      </c>
+      <c r="JE11" t="inlineStr">
+        <is>
+          <t>147</t>
+        </is>
+      </c>
+      <c r="JF11" t="inlineStr">
+        <is>
+          <t>140</t>
+        </is>
+      </c>
+      <c r="JG11" t="inlineStr">
+        <is>
+          <t>149</t>
+        </is>
+      </c>
+      <c r="JH11" t="inlineStr">
+        <is>
+          <t>134</t>
+        </is>
+      </c>
+      <c r="JM11" t="inlineStr">
+        <is>
+          <t>.9</t>
+        </is>
+      </c>
+      <c r="JN11" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="JO11" t="inlineStr">
+        <is>
+          <t>.7</t>
+        </is>
+      </c>
+      <c r="JP11" t="inlineStr">
+        <is>
+          <t>.11</t>
+        </is>
+      </c>
+      <c r="JQ11" t="inlineStr">
+        <is>
+          <t>.5</t>
+        </is>
+      </c>
+      <c r="JR11" t="inlineStr">
+        <is>
+          <t>.15</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>type01</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>16.0</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>3.22</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>3.03</t>
+        </is>
+      </c>
+      <c r="T12" t="inlineStr">
+        <is>
+          <t>3.00</t>
+        </is>
+      </c>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>2.97</t>
+        </is>
+      </c>
+      <c r="V12" t="inlineStr">
+        <is>
+          <t>3.01</t>
+        </is>
+      </c>
+      <c r="W12" t="inlineStr">
+        <is>
+          <t>2.93</t>
+        </is>
+      </c>
+      <c r="X12" t="inlineStr">
+        <is>
+          <t>2.31</t>
+        </is>
+      </c>
+      <c r="Y12" t="inlineStr">
+        <is>
+          <t>2.75</t>
+        </is>
+      </c>
+      <c r="AK12" t="inlineStr">
+        <is>
+          <t>94</t>
+        </is>
+      </c>
+      <c r="AM12" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="AN12" t="inlineStr">
+        <is>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="AO12" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="AP12" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="AQ12" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="AR12" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="AW12" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="AX12" t="inlineStr">
+        <is>
+          <t>.2</t>
+        </is>
+      </c>
+      <c r="AY12" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="AZ12" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="BA12" t="inlineStr">
+        <is>
+          <t>.7</t>
+        </is>
+      </c>
+      <c r="BB12" t="inlineStr">
+        <is>
+          <t>.9</t>
+        </is>
+      </c>
+      <c r="BO12" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="BP12" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="BQ12" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="BR12" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="BS12" t="inlineStr">
+        <is>
+          <t>15.0</t>
+        </is>
+      </c>
+      <c r="BT12" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="BX12" t="inlineStr">
+        <is>
+          <t>2.51</t>
+        </is>
+      </c>
+      <c r="BY12" t="inlineStr">
+        <is>
+          <t>2.20</t>
+        </is>
+      </c>
+      <c r="CA12" t="inlineStr">
+        <is>
+          <t>2.23</t>
+        </is>
+      </c>
+      <c r="CB12" t="inlineStr">
+        <is>
+          <t>2.25</t>
+        </is>
+      </c>
+      <c r="CC12" t="inlineStr">
+        <is>
+          <t>2.27</t>
+        </is>
+      </c>
+      <c r="CD12" t="inlineStr">
+        <is>
+          <t>2.20</t>
+        </is>
+      </c>
+      <c r="CE12" t="inlineStr">
+        <is>
+          <t>2.10</t>
+        </is>
+      </c>
+      <c r="CF12" t="inlineStr">
+        <is>
+          <t>1.99</t>
+        </is>
+      </c>
+      <c r="CR12" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="CT12" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="CU12" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="CV12" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="CW12" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="CX12" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="CY12" t="inlineStr">
+        <is>
+          <t>79</t>
+        </is>
+      </c>
+      <c r="DD12" t="inlineStr">
+        <is>
+          <t>.2</t>
+        </is>
+      </c>
+      <c r="DE12" t="inlineStr">
+        <is>
+          <t>.2</t>
+        </is>
+      </c>
+      <c r="DF12" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="DG12" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="DH12" t="inlineStr">
+        <is>
+          <t>.3</t>
+        </is>
+      </c>
+      <c r="DI12" t="inlineStr">
+        <is>
+          <t>.13</t>
+        </is>
+      </c>
+      <c r="DP12" t="inlineStr">
+        <is>
+          <t>220</t>
+        </is>
+      </c>
+      <c r="EJ12" t="inlineStr">
+        <is>
+          <t>2.57</t>
+        </is>
+      </c>
+      <c r="EK12" t="inlineStr">
+        <is>
+          <t>1.75</t>
+        </is>
+      </c>
+      <c r="EL12" t="inlineStr">
+        <is>
+          <t>1.67</t>
+        </is>
+      </c>
+      <c r="EM12" t="inlineStr">
+        <is>
+          <t>1.69</t>
+        </is>
+      </c>
+      <c r="EN12" t="inlineStr">
+        <is>
+          <t>1.73</t>
+        </is>
+      </c>
+      <c r="EO12" t="inlineStr">
+        <is>
+          <t>1.69</t>
+        </is>
+      </c>
+      <c r="ET12" t="inlineStr">
+        <is>
+          <t>68</t>
+        </is>
+      </c>
+      <c r="EV12" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="EW12" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="EX12" t="inlineStr">
+        <is>
+          <t>63</t>
+        </is>
+      </c>
+      <c r="EY12" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="EZ12" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="FA12" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="FY12" t="inlineStr">
+        <is>
+          <t>.4</t>
+        </is>
+      </c>
+      <c r="FZ12" t="inlineStr">
+        <is>
+          <t>.3</t>
+        </is>
+      </c>
+      <c r="GA12" t="inlineStr">
+        <is>
+          <t>.0</t>
+        </is>
+      </c>
+      <c r="GB12" t="inlineStr">
+        <is>
+          <t>.3</t>
+        </is>
+      </c>
+      <c r="GC12" t="inlineStr">
+        <is>
+          <t>.11</t>
+        </is>
+      </c>
+      <c r="GD12" t="inlineStr">
+        <is>
+          <t>.24</t>
+        </is>
+      </c>
+      <c r="HX12" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="HY12" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="HZ12" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="IA12" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="IB12" t="inlineStr">
+        <is>
+          <t>16.0</t>
+        </is>
+      </c>
+      <c r="IC12" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="IG12" t="inlineStr">
+        <is>
+          <t>5.45</t>
+        </is>
+      </c>
+      <c r="IH12" t="inlineStr">
+        <is>
+          <t>9.33</t>
+        </is>
+      </c>
+      <c r="IJ12" t="inlineStr">
+        <is>
+          <t>7.32</t>
+        </is>
+      </c>
+      <c r="IK12" t="inlineStr">
+        <is>
+          <t>0.47</t>
+        </is>
+      </c>
+      <c r="IL12" t="inlineStr">
+        <is>
+          <t>7.99</t>
+        </is>
+      </c>
+      <c r="IM12" t="inlineStr">
+        <is>
+          <t>7.64</t>
+        </is>
+      </c>
+      <c r="IN12" t="inlineStr">
+        <is>
+          <t>3.12</t>
+        </is>
+      </c>
+      <c r="IO12" t="inlineStr">
+        <is>
+          <t>7.31</t>
+        </is>
+      </c>
+      <c r="JA12" t="inlineStr">
+        <is>
+          <t>153</t>
+        </is>
+      </c>
+      <c r="JC12" t="inlineStr">
+        <is>
+          <t>143</t>
+        </is>
+      </c>
+      <c r="JD12" t="inlineStr">
+        <is>
+          <t>155</t>
+        </is>
+      </c>
+      <c r="JE12" t="inlineStr">
+        <is>
+          <t>147</t>
+        </is>
+      </c>
+      <c r="JF12" t="inlineStr">
+        <is>
+          <t>140</t>
+        </is>
+      </c>
+      <c r="JG12" t="inlineStr">
+        <is>
+          <t>149</t>
+        </is>
+      </c>
+      <c r="JH12" t="inlineStr">
+        <is>
+          <t>134</t>
+        </is>
+      </c>
+      <c r="JM12" t="inlineStr">
+        <is>
+          <t>.9</t>
+        </is>
+      </c>
+      <c r="JN12" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="JO12" t="inlineStr">
+        <is>
+          <t>.7</t>
+        </is>
+      </c>
+      <c r="JP12" t="inlineStr">
+        <is>
+          <t>.11</t>
+        </is>
+      </c>
+      <c r="JQ12" t="inlineStr">
+        <is>
+          <t>.5</t>
+        </is>
+      </c>
+      <c r="JR12" t="inlineStr">
+        <is>
+          <t>.15</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>type01</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>16.0</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
+      <c r="P13" t="inlineStr"/>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>3.22</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>3.03</t>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr"/>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>3.00</t>
+        </is>
+      </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>2.97</t>
+        </is>
+      </c>
+      <c r="V13" t="inlineStr">
+        <is>
+          <t>3.01</t>
+        </is>
+      </c>
+      <c r="W13" t="inlineStr">
+        <is>
+          <t>2.93</t>
+        </is>
+      </c>
+      <c r="X13" t="inlineStr">
+        <is>
+          <t>2.31</t>
+        </is>
+      </c>
+      <c r="Y13" t="inlineStr">
+        <is>
+          <t>2.75</t>
+        </is>
+      </c>
+      <c r="Z13" t="inlineStr"/>
+      <c r="AA13" t="inlineStr"/>
+      <c r="AB13" t="inlineStr"/>
+      <c r="AC13" t="inlineStr"/>
+      <c r="AD13" t="inlineStr"/>
+      <c r="AE13" t="inlineStr"/>
+      <c r="AF13" t="inlineStr"/>
+      <c r="AG13" t="inlineStr"/>
+      <c r="AH13" t="inlineStr"/>
+      <c r="AI13" t="inlineStr"/>
+      <c r="AJ13" t="inlineStr"/>
+      <c r="AK13" t="inlineStr">
+        <is>
+          <t>94</t>
+        </is>
+      </c>
+      <c r="AL13" t="inlineStr"/>
+      <c r="AM13" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="AN13" t="inlineStr">
+        <is>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="AO13" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="AP13" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="AQ13" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="AR13" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="AS13" t="inlineStr"/>
+      <c r="AT13" t="inlineStr"/>
+      <c r="AU13" t="inlineStr"/>
+      <c r="AV13" t="inlineStr"/>
+      <c r="AW13" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="AX13" t="inlineStr">
+        <is>
+          <t>.2</t>
+        </is>
+      </c>
+      <c r="AY13" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="AZ13" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="BA13" t="inlineStr">
+        <is>
+          <t>.7</t>
+        </is>
+      </c>
+      <c r="BB13" t="inlineStr">
+        <is>
+          <t>.9</t>
+        </is>
+      </c>
+      <c r="BC13" t="inlineStr"/>
+      <c r="BD13" t="inlineStr"/>
+      <c r="BE13" t="inlineStr"/>
+      <c r="BF13" t="inlineStr"/>
+      <c r="BG13" t="inlineStr"/>
+      <c r="BH13" t="inlineStr"/>
+      <c r="BI13" t="inlineStr"/>
+      <c r="BJ13" t="inlineStr"/>
+      <c r="BK13" t="inlineStr"/>
+      <c r="BL13" t="inlineStr"/>
+      <c r="BM13" t="inlineStr"/>
+      <c r="BN13" t="inlineStr"/>
+      <c r="BO13" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="BP13" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="BQ13" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="BR13" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="BS13" t="inlineStr">
+        <is>
+          <t>15.0</t>
+        </is>
+      </c>
+      <c r="BT13" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="BU13" t="inlineStr"/>
+      <c r="BV13" t="inlineStr"/>
+      <c r="BW13" t="inlineStr"/>
+      <c r="BX13" t="inlineStr">
+        <is>
+          <t>2.51</t>
+        </is>
+      </c>
+      <c r="BY13" t="inlineStr">
+        <is>
+          <t>2.20</t>
+        </is>
+      </c>
+      <c r="BZ13" t="inlineStr"/>
+      <c r="CA13" t="inlineStr">
+        <is>
+          <t>2.23</t>
+        </is>
+      </c>
+      <c r="CB13" t="inlineStr">
+        <is>
+          <t>2.25</t>
+        </is>
+      </c>
+      <c r="CC13" t="inlineStr">
+        <is>
+          <t>2.27</t>
+        </is>
+      </c>
+      <c r="CD13" t="inlineStr">
+        <is>
+          <t>2.20</t>
+        </is>
+      </c>
+      <c r="CE13" t="inlineStr">
+        <is>
+          <t>2.10</t>
+        </is>
+      </c>
+      <c r="CF13" t="inlineStr">
+        <is>
+          <t>1.99</t>
+        </is>
+      </c>
+      <c r="CG13" t="inlineStr"/>
+      <c r="CH13" t="inlineStr"/>
+      <c r="CI13" t="inlineStr"/>
+      <c r="CJ13" t="inlineStr"/>
+      <c r="CK13" t="inlineStr"/>
+      <c r="CL13" t="inlineStr"/>
+      <c r="CM13" t="inlineStr"/>
+      <c r="CN13" t="inlineStr"/>
+      <c r="CO13" t="inlineStr"/>
+      <c r="CP13" t="inlineStr"/>
+      <c r="CQ13" t="inlineStr"/>
+      <c r="CR13" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="CS13" t="inlineStr"/>
+      <c r="CT13" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="CU13" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="CV13" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="CW13" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="CX13" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="CY13" t="inlineStr">
+        <is>
+          <t>79</t>
+        </is>
+      </c>
+      <c r="CZ13" t="inlineStr"/>
+      <c r="DA13" t="inlineStr"/>
+      <c r="DB13" t="inlineStr"/>
+      <c r="DC13" t="inlineStr"/>
+      <c r="DD13" t="inlineStr">
+        <is>
+          <t>.2</t>
+        </is>
+      </c>
+      <c r="DE13" t="inlineStr">
+        <is>
+          <t>.2</t>
+        </is>
+      </c>
+      <c r="DF13" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="DG13" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="DH13" t="inlineStr">
+        <is>
+          <t>.3</t>
+        </is>
+      </c>
+      <c r="DI13" t="inlineStr">
+        <is>
+          <t>.13</t>
+        </is>
+      </c>
+      <c r="DJ13" t="inlineStr"/>
+      <c r="DK13" t="inlineStr"/>
+      <c r="DL13" t="inlineStr"/>
+      <c r="DM13" t="inlineStr"/>
+      <c r="DN13" t="inlineStr"/>
+      <c r="DO13" t="inlineStr"/>
+      <c r="DP13" t="inlineStr">
+        <is>
+          <t>220</t>
+        </is>
+      </c>
+      <c r="DQ13" t="inlineStr"/>
+      <c r="DR13" t="inlineStr"/>
+      <c r="DS13" t="inlineStr"/>
+      <c r="DT13" t="inlineStr"/>
+      <c r="DU13" t="inlineStr"/>
+      <c r="DV13" t="inlineStr"/>
+      <c r="DW13" t="inlineStr"/>
+      <c r="DX13" t="inlineStr"/>
+      <c r="DY13" t="inlineStr"/>
+      <c r="DZ13" t="inlineStr"/>
+      <c r="EA13" t="inlineStr"/>
+      <c r="EB13" t="inlineStr"/>
+      <c r="EC13" t="inlineStr"/>
+      <c r="ED13" t="inlineStr"/>
+      <c r="EE13" t="inlineStr"/>
+      <c r="EF13" t="inlineStr"/>
+      <c r="EG13" t="inlineStr"/>
+      <c r="EH13" t="inlineStr"/>
+      <c r="EI13" t="inlineStr"/>
+      <c r="EJ13" t="inlineStr">
+        <is>
+          <t>2.57</t>
+        </is>
+      </c>
+      <c r="EK13" t="inlineStr">
+        <is>
+          <t>1.75</t>
+        </is>
+      </c>
+      <c r="EL13" t="inlineStr">
+        <is>
+          <t>1.67</t>
+        </is>
+      </c>
+      <c r="EM13" t="inlineStr">
+        <is>
+          <t>1.69</t>
+        </is>
+      </c>
+      <c r="EN13" t="inlineStr">
+        <is>
+          <t>1.73</t>
+        </is>
+      </c>
+      <c r="EO13" t="inlineStr">
+        <is>
+          <t>1.69</t>
+        </is>
+      </c>
+      <c r="EP13" t="inlineStr"/>
+      <c r="EQ13" t="inlineStr"/>
+      <c r="ER13" t="inlineStr"/>
+      <c r="ES13" t="inlineStr"/>
+      <c r="ET13" t="inlineStr">
+        <is>
+          <t>68</t>
+        </is>
+      </c>
+      <c r="EU13" t="inlineStr"/>
+      <c r="EV13" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="EW13" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="EX13" t="inlineStr">
+        <is>
+          <t>63</t>
+        </is>
+      </c>
+      <c r="EY13" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="EZ13" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="FA13" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="FB13" t="inlineStr"/>
+      <c r="FC13" t="inlineStr"/>
+      <c r="FD13" t="inlineStr"/>
+      <c r="FE13" t="inlineStr"/>
+      <c r="FF13" t="inlineStr"/>
+      <c r="FG13" t="inlineStr"/>
+      <c r="FH13" t="inlineStr"/>
+      <c r="FI13" t="inlineStr"/>
+      <c r="FJ13" t="inlineStr"/>
+      <c r="FK13" t="inlineStr"/>
+      <c r="FL13" t="inlineStr"/>
+      <c r="FM13" t="inlineStr"/>
+      <c r="FN13" t="inlineStr"/>
+      <c r="FO13" t="inlineStr"/>
+      <c r="FP13" t="inlineStr"/>
+      <c r="FQ13" t="inlineStr"/>
+      <c r="FR13" t="inlineStr"/>
+      <c r="FS13" t="inlineStr"/>
+      <c r="FT13" t="inlineStr"/>
+      <c r="FU13" t="inlineStr"/>
+      <c r="FV13" t="inlineStr"/>
+      <c r="FW13" t="inlineStr"/>
+      <c r="FX13" t="inlineStr"/>
+      <c r="FY13" t="inlineStr">
+        <is>
+          <t>.4</t>
+        </is>
+      </c>
+      <c r="FZ13" t="inlineStr">
+        <is>
+          <t>.3</t>
+        </is>
+      </c>
+      <c r="GA13" t="inlineStr">
+        <is>
+          <t>.0</t>
+        </is>
+      </c>
+      <c r="GB13" t="inlineStr">
+        <is>
+          <t>.3</t>
+        </is>
+      </c>
+      <c r="GC13" t="inlineStr">
+        <is>
+          <t>.11</t>
+        </is>
+      </c>
+      <c r="GD13" t="inlineStr">
+        <is>
+          <t>.24</t>
+        </is>
+      </c>
+      <c r="GE13" t="inlineStr"/>
+      <c r="GF13" t="inlineStr"/>
+      <c r="GG13" t="inlineStr"/>
+      <c r="GH13" t="inlineStr"/>
+      <c r="GI13" t="inlineStr"/>
+      <c r="GJ13" t="inlineStr"/>
+      <c r="GK13" t="inlineStr"/>
+      <c r="GL13" t="inlineStr"/>
+      <c r="GM13" t="inlineStr"/>
+      <c r="GN13" t="inlineStr"/>
+      <c r="GO13" t="inlineStr"/>
+      <c r="GP13" t="inlineStr"/>
+      <c r="GQ13" t="inlineStr"/>
+      <c r="GR13" t="inlineStr"/>
+      <c r="GS13" t="inlineStr"/>
+      <c r="GT13" t="inlineStr"/>
+      <c r="GU13" t="inlineStr"/>
+      <c r="GV13" t="inlineStr"/>
+      <c r="GW13" t="inlineStr"/>
+      <c r="GX13" t="inlineStr"/>
+      <c r="GY13" t="inlineStr"/>
+      <c r="GZ13" t="inlineStr"/>
+      <c r="HA13" t="inlineStr"/>
+      <c r="HB13" t="inlineStr"/>
+      <c r="HC13" t="inlineStr"/>
+      <c r="HD13" t="inlineStr"/>
+      <c r="HE13" t="inlineStr"/>
+      <c r="HF13" t="inlineStr"/>
+      <c r="HG13" t="inlineStr"/>
+      <c r="HH13" t="inlineStr"/>
+      <c r="HI13" t="inlineStr"/>
+      <c r="HJ13" t="inlineStr"/>
+      <c r="HK13" t="inlineStr"/>
+      <c r="HL13" t="inlineStr"/>
+      <c r="HM13" t="inlineStr"/>
+      <c r="HN13" t="inlineStr"/>
+      <c r="HO13" t="inlineStr"/>
+      <c r="HP13" t="inlineStr"/>
+      <c r="HQ13" t="inlineStr"/>
+      <c r="HR13" t="inlineStr"/>
+      <c r="HS13" t="inlineStr"/>
+      <c r="HT13" t="inlineStr"/>
+      <c r="HU13" t="inlineStr"/>
+      <c r="HV13" t="inlineStr"/>
+      <c r="HW13" t="inlineStr"/>
+      <c r="HX13" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="HY13" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="HZ13" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="IA13" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="IB13" t="inlineStr">
+        <is>
+          <t>16.0</t>
+        </is>
+      </c>
+      <c r="IC13" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="ID13" t="inlineStr"/>
+      <c r="IE13" t="inlineStr"/>
+      <c r="IF13" t="inlineStr"/>
+      <c r="IG13" t="inlineStr">
+        <is>
+          <t>5.45</t>
+        </is>
+      </c>
+      <c r="IH13" t="inlineStr">
+        <is>
+          <t>9.33</t>
+        </is>
+      </c>
+      <c r="II13" t="inlineStr"/>
+      <c r="IJ13" t="inlineStr">
+        <is>
+          <t>7.32</t>
+        </is>
+      </c>
+      <c r="IK13" t="inlineStr">
+        <is>
+          <t>0.47</t>
+        </is>
+      </c>
+      <c r="IL13" t="inlineStr">
+        <is>
+          <t>7.99</t>
+        </is>
+      </c>
+      <c r="IM13" t="inlineStr">
+        <is>
+          <t>7.64</t>
+        </is>
+      </c>
+      <c r="IN13" t="inlineStr">
+        <is>
+          <t>3.12</t>
+        </is>
+      </c>
+      <c r="IO13" t="inlineStr">
+        <is>
+          <t>7.31</t>
+        </is>
+      </c>
+      <c r="IP13" t="inlineStr"/>
+      <c r="IQ13" t="inlineStr"/>
+      <c r="IR13" t="inlineStr"/>
+      <c r="IS13" t="inlineStr"/>
+      <c r="IT13" t="inlineStr"/>
+      <c r="IU13" t="inlineStr"/>
+      <c r="IV13" t="inlineStr"/>
+      <c r="IW13" t="inlineStr"/>
+      <c r="IX13" t="inlineStr"/>
+      <c r="IY13" t="inlineStr"/>
+      <c r="IZ13" t="inlineStr"/>
+      <c r="JA13" t="inlineStr">
+        <is>
+          <t>153</t>
+        </is>
+      </c>
+      <c r="JB13" t="inlineStr"/>
+      <c r="JC13" t="inlineStr">
+        <is>
+          <t>143</t>
+        </is>
+      </c>
+      <c r="JD13" t="inlineStr">
+        <is>
+          <t>155</t>
+        </is>
+      </c>
+      <c r="JE13" t="inlineStr">
+        <is>
+          <t>147</t>
+        </is>
+      </c>
+      <c r="JF13" t="inlineStr">
+        <is>
+          <t>140</t>
+        </is>
+      </c>
+      <c r="JG13" t="inlineStr">
+        <is>
+          <t>149</t>
+        </is>
+      </c>
+      <c r="JH13" t="inlineStr">
+        <is>
+          <t>134</t>
+        </is>
+      </c>
+      <c r="JI13" t="inlineStr"/>
+      <c r="JJ13" t="inlineStr"/>
+      <c r="JK13" t="inlineStr"/>
+      <c r="JL13" t="inlineStr"/>
+      <c r="JM13" t="inlineStr">
+        <is>
+          <t>.9</t>
+        </is>
+      </c>
+      <c r="JN13" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="JO13" t="inlineStr">
+        <is>
+          <t>.7</t>
+        </is>
+      </c>
+      <c r="JP13" t="inlineStr">
+        <is>
+          <t>.11</t>
+        </is>
+      </c>
+      <c r="JQ13" t="inlineStr">
+        <is>
+          <t>.5</t>
+        </is>
+      </c>
+      <c r="JR13" t="inlineStr">
+        <is>
+          <t>.15</t>
+        </is>
+      </c>
+      <c r="JS13" t="inlineStr"/>
+      <c r="JT13" t="inlineStr"/>
+      <c r="JU13" t="inlineStr"/>
+      <c r="JV13" t="inlineStr"/>
+      <c r="JW13" t="inlineStr"/>
+      <c r="JX13" t="inlineStr"/>
+      <c r="JY13" t="inlineStr"/>
+      <c r="JZ13" t="inlineStr"/>
+      <c r="KA13" t="inlineStr"/>
+      <c r="KB13" t="inlineStr"/>
+      <c r="KC13" t="inlineStr"/>
+      <c r="KD13" t="inlineStr"/>
+      <c r="KE13" t="inlineStr"/>
+      <c r="KF13" t="inlineStr"/>
+      <c r="KG13" t="inlineStr"/>
+      <c r="KH13" t="inlineStr"/>
+      <c r="KI13" t="inlineStr"/>
+      <c r="KJ13" t="inlineStr"/>
+      <c r="KK13" t="inlineStr"/>
+      <c r="KL13" t="inlineStr"/>
+      <c r="KM13" t="inlineStr"/>
+      <c r="KN13" t="inlineStr"/>
+      <c r="KO13" t="inlineStr"/>
+      <c r="KP13" t="inlineStr"/>
+      <c r="KQ13" t="inlineStr"/>
+      <c r="KR13" t="inlineStr"/>
+      <c r="KS13" t="inlineStr"/>
+      <c r="KT13" t="inlineStr"/>
+      <c r="KU13" t="inlineStr"/>
+      <c r="KV13" t="inlineStr"/>
+      <c r="KW13" t="inlineStr"/>
+      <c r="KX13" t="inlineStr"/>
+      <c r="KY13" t="inlineStr"/>
+      <c r="KZ13" t="inlineStr"/>
+      <c r="LA13" t="inlineStr"/>
+      <c r="LB13" t="inlineStr"/>
+      <c r="LC13" t="inlineStr"/>
+      <c r="LD13" t="inlineStr"/>
+      <c r="LE13" t="inlineStr"/>
+      <c r="LF13" t="inlineStr"/>
+      <c r="LG13" t="inlineStr"/>
+      <c r="LH13" t="inlineStr"/>
+      <c r="LI13" t="inlineStr"/>
+      <c r="LJ13" t="inlineStr"/>
+      <c r="LK13" t="inlineStr"/>
+      <c r="LL13" t="inlineStr"/>
+      <c r="LM13" t="inlineStr"/>
+      <c r="LN13" t="inlineStr"/>
+      <c r="LO13" t="inlineStr"/>
+      <c r="LP13" t="inlineStr"/>
+      <c r="LQ13" t="inlineStr"/>
+      <c r="LR13" t="inlineStr"/>
+      <c r="LS13" t="inlineStr"/>
+      <c r="LT13" t="inlineStr"/>
+      <c r="LU13" t="inlineStr"/>
+      <c r="LV13" t="inlineStr"/>
+      <c r="LW13" t="inlineStr"/>
+      <c r="LX13" t="inlineStr"/>
+      <c r="LY13" t="inlineStr"/>
+      <c r="LZ13" t="inlineStr"/>
+      <c r="MA13" t="inlineStr"/>
+      <c r="MB13" t="inlineStr"/>
+      <c r="MC13" t="inlineStr"/>
+      <c r="MD13" t="inlineStr"/>
+      <c r="ME13" t="inlineStr"/>
+      <c r="MF13" t="inlineStr"/>
+      <c r="MG13" t="inlineStr"/>
+      <c r="MH13" t="inlineStr"/>
+      <c r="MI13" t="inlineStr"/>
+      <c r="MJ13" t="inlineStr"/>
+      <c r="MK13" t="inlineStr"/>
+      <c r="ML13" t="inlineStr"/>
+      <c r="MM13" t="inlineStr"/>
+      <c r="MN13" t="inlineStr"/>
+      <c r="MO13" t="inlineStr"/>
+      <c r="MP13" t="inlineStr"/>
+      <c r="MQ13" t="inlineStr"/>
+      <c r="MR13" t="inlineStr"/>
+      <c r="MS13" t="inlineStr"/>
+      <c r="MT13" t="inlineStr"/>
+      <c r="MU13" t="inlineStr"/>
+      <c r="MV13" t="inlineStr"/>
+      <c r="MW13" t="inlineStr"/>
+      <c r="MX13" t="inlineStr"/>
+      <c r="MY13" t="inlineStr"/>
+      <c r="MZ13" t="inlineStr"/>
+      <c r="NA13" t="inlineStr"/>
+      <c r="NB13" t="inlineStr"/>
+      <c r="NC13" t="inlineStr"/>
+      <c r="ND13" t="inlineStr"/>
+      <c r="NE13" t="inlineStr"/>
+      <c r="NF13" t="inlineStr"/>
+      <c r="NG13" t="inlineStr"/>
+      <c r="NH13" t="inlineStr"/>
+      <c r="NI13" t="inlineStr"/>
+      <c r="NJ13" t="inlineStr"/>
+      <c r="NK13" t="inlineStr"/>
+      <c r="NL13" t="inlineStr"/>
+      <c r="NM13" t="inlineStr"/>
+      <c r="NN13" t="inlineStr"/>
+      <c r="NO13" t="inlineStr"/>
+      <c r="NP13" t="inlineStr"/>
+      <c r="NQ13" t="inlineStr"/>
+      <c r="NR13" t="inlineStr"/>
+      <c r="NS13" t="inlineStr"/>
+      <c r="NT13" t="inlineStr"/>
+      <c r="NU13" t="inlineStr"/>
+      <c r="NV13" t="inlineStr"/>
+      <c r="NW13" t="inlineStr"/>
+      <c r="NX13" t="inlineStr"/>
+      <c r="NY13" t="inlineStr"/>
+      <c r="NZ13" t="inlineStr"/>
+      <c r="OA13" t="inlineStr"/>
+      <c r="OB13" t="inlineStr"/>
+      <c r="OC13" t="inlineStr"/>
+      <c r="OD13" t="inlineStr"/>
+      <c r="OE13" t="inlineStr"/>
+      <c r="OF13" t="inlineStr"/>
+      <c r="OG13" t="inlineStr"/>
+      <c r="OH13" t="inlineStr"/>
+      <c r="OI13" t="inlineStr"/>
+      <c r="OJ13" t="inlineStr"/>
+      <c r="OK13" t="inlineStr"/>
+      <c r="OL13" t="inlineStr"/>
+      <c r="OM13" t="inlineStr"/>
+      <c r="ON13" t="inlineStr"/>
+      <c r="OO13" t="inlineStr"/>
+      <c r="OP13" t="inlineStr"/>
+      <c r="OQ13" t="inlineStr"/>
+      <c r="OR13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
c: startwith . replace 1 -
</commit_message>
<xml_diff>
--- a/OOMII.xlsx
+++ b/OOMII.xlsx
@@ -346,7 +346,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:OR13"/>
+  <dimension ref="A1:OR16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8034,12 +8034,6 @@
           <t>type01</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr">
         <is>
           <t>0.0625</t>
@@ -8070,9 +8064,6 @@
           <t>25.0</t>
         </is>
       </c>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr"/>
-      <c r="P13" t="inlineStr"/>
       <c r="Q13" t="inlineStr">
         <is>
           <t>3.22</t>
@@ -8083,7 +8074,6 @@
           <t>3.03</t>
         </is>
       </c>
-      <c r="S13" t="inlineStr"/>
       <c r="T13" t="inlineStr">
         <is>
           <t>3.00</t>
@@ -8114,23 +8104,11 @@
           <t>2.75</t>
         </is>
       </c>
-      <c r="Z13" t="inlineStr"/>
-      <c r="AA13" t="inlineStr"/>
-      <c r="AB13" t="inlineStr"/>
-      <c r="AC13" t="inlineStr"/>
-      <c r="AD13" t="inlineStr"/>
-      <c r="AE13" t="inlineStr"/>
-      <c r="AF13" t="inlineStr"/>
-      <c r="AG13" t="inlineStr"/>
-      <c r="AH13" t="inlineStr"/>
-      <c r="AI13" t="inlineStr"/>
-      <c r="AJ13" t="inlineStr"/>
       <c r="AK13" t="inlineStr">
         <is>
           <t>94</t>
         </is>
       </c>
-      <c r="AL13" t="inlineStr"/>
       <c r="AM13" t="inlineStr">
         <is>
           <t>93</t>
@@ -8161,10 +8139,6 @@
           <t>35</t>
         </is>
       </c>
-      <c r="AS13" t="inlineStr"/>
-      <c r="AT13" t="inlineStr"/>
-      <c r="AU13" t="inlineStr"/>
-      <c r="AV13" t="inlineStr"/>
       <c r="AW13" t="inlineStr">
         <is>
           <t>.1</t>
@@ -8195,18 +8169,6 @@
           <t>.9</t>
         </is>
       </c>
-      <c r="BC13" t="inlineStr"/>
-      <c r="BD13" t="inlineStr"/>
-      <c r="BE13" t="inlineStr"/>
-      <c r="BF13" t="inlineStr"/>
-      <c r="BG13" t="inlineStr"/>
-      <c r="BH13" t="inlineStr"/>
-      <c r="BI13" t="inlineStr"/>
-      <c r="BJ13" t="inlineStr"/>
-      <c r="BK13" t="inlineStr"/>
-      <c r="BL13" t="inlineStr"/>
-      <c r="BM13" t="inlineStr"/>
-      <c r="BN13" t="inlineStr"/>
       <c r="BO13" t="inlineStr">
         <is>
           <t>0.0625</t>
@@ -8237,9 +8199,6 @@
           <t>25.0</t>
         </is>
       </c>
-      <c r="BU13" t="inlineStr"/>
-      <c r="BV13" t="inlineStr"/>
-      <c r="BW13" t="inlineStr"/>
       <c r="BX13" t="inlineStr">
         <is>
           <t>2.51</t>
@@ -8250,7 +8209,6 @@
           <t>2.20</t>
         </is>
       </c>
-      <c r="BZ13" t="inlineStr"/>
       <c r="CA13" t="inlineStr">
         <is>
           <t>2.23</t>
@@ -8281,23 +8239,11 @@
           <t>1.99</t>
         </is>
       </c>
-      <c r="CG13" t="inlineStr"/>
-      <c r="CH13" t="inlineStr"/>
-      <c r="CI13" t="inlineStr"/>
-      <c r="CJ13" t="inlineStr"/>
-      <c r="CK13" t="inlineStr"/>
-      <c r="CL13" t="inlineStr"/>
-      <c r="CM13" t="inlineStr"/>
-      <c r="CN13" t="inlineStr"/>
-      <c r="CO13" t="inlineStr"/>
-      <c r="CP13" t="inlineStr"/>
-      <c r="CQ13" t="inlineStr"/>
       <c r="CR13" t="inlineStr">
         <is>
           <t>91</t>
         </is>
       </c>
-      <c r="CS13" t="inlineStr"/>
       <c r="CT13" t="inlineStr">
         <is>
           <t>39</t>
@@ -8328,10 +8274,6 @@
           <t>79</t>
         </is>
       </c>
-      <c r="CZ13" t="inlineStr"/>
-      <c r="DA13" t="inlineStr"/>
-      <c r="DB13" t="inlineStr"/>
-      <c r="DC13" t="inlineStr"/>
       <c r="DD13" t="inlineStr">
         <is>
           <t>.2</t>
@@ -8362,36 +8304,11 @@
           <t>.13</t>
         </is>
       </c>
-      <c r="DJ13" t="inlineStr"/>
-      <c r="DK13" t="inlineStr"/>
-      <c r="DL13" t="inlineStr"/>
-      <c r="DM13" t="inlineStr"/>
-      <c r="DN13" t="inlineStr"/>
-      <c r="DO13" t="inlineStr"/>
       <c r="DP13" t="inlineStr">
         <is>
           <t>220</t>
         </is>
       </c>
-      <c r="DQ13" t="inlineStr"/>
-      <c r="DR13" t="inlineStr"/>
-      <c r="DS13" t="inlineStr"/>
-      <c r="DT13" t="inlineStr"/>
-      <c r="DU13" t="inlineStr"/>
-      <c r="DV13" t="inlineStr"/>
-      <c r="DW13" t="inlineStr"/>
-      <c r="DX13" t="inlineStr"/>
-      <c r="DY13" t="inlineStr"/>
-      <c r="DZ13" t="inlineStr"/>
-      <c r="EA13" t="inlineStr"/>
-      <c r="EB13" t="inlineStr"/>
-      <c r="EC13" t="inlineStr"/>
-      <c r="ED13" t="inlineStr"/>
-      <c r="EE13" t="inlineStr"/>
-      <c r="EF13" t="inlineStr"/>
-      <c r="EG13" t="inlineStr"/>
-      <c r="EH13" t="inlineStr"/>
-      <c r="EI13" t="inlineStr"/>
       <c r="EJ13" t="inlineStr">
         <is>
           <t>2.57</t>
@@ -8422,16 +8339,11 @@
           <t>1.69</t>
         </is>
       </c>
-      <c r="EP13" t="inlineStr"/>
-      <c r="EQ13" t="inlineStr"/>
-      <c r="ER13" t="inlineStr"/>
-      <c r="ES13" t="inlineStr"/>
       <c r="ET13" t="inlineStr">
         <is>
           <t>68</t>
         </is>
       </c>
-      <c r="EU13" t="inlineStr"/>
       <c r="EV13" t="inlineStr">
         <is>
           <t>55</t>
@@ -8462,29 +8374,6 @@
           <t>51</t>
         </is>
       </c>
-      <c r="FB13" t="inlineStr"/>
-      <c r="FC13" t="inlineStr"/>
-      <c r="FD13" t="inlineStr"/>
-      <c r="FE13" t="inlineStr"/>
-      <c r="FF13" t="inlineStr"/>
-      <c r="FG13" t="inlineStr"/>
-      <c r="FH13" t="inlineStr"/>
-      <c r="FI13" t="inlineStr"/>
-      <c r="FJ13" t="inlineStr"/>
-      <c r="FK13" t="inlineStr"/>
-      <c r="FL13" t="inlineStr"/>
-      <c r="FM13" t="inlineStr"/>
-      <c r="FN13" t="inlineStr"/>
-      <c r="FO13" t="inlineStr"/>
-      <c r="FP13" t="inlineStr"/>
-      <c r="FQ13" t="inlineStr"/>
-      <c r="FR13" t="inlineStr"/>
-      <c r="FS13" t="inlineStr"/>
-      <c r="FT13" t="inlineStr"/>
-      <c r="FU13" t="inlineStr"/>
-      <c r="FV13" t="inlineStr"/>
-      <c r="FW13" t="inlineStr"/>
-      <c r="FX13" t="inlineStr"/>
       <c r="FY13" t="inlineStr">
         <is>
           <t>.4</t>
@@ -8515,51 +8404,6 @@
           <t>.24</t>
         </is>
       </c>
-      <c r="GE13" t="inlineStr"/>
-      <c r="GF13" t="inlineStr"/>
-      <c r="GG13" t="inlineStr"/>
-      <c r="GH13" t="inlineStr"/>
-      <c r="GI13" t="inlineStr"/>
-      <c r="GJ13" t="inlineStr"/>
-      <c r="GK13" t="inlineStr"/>
-      <c r="GL13" t="inlineStr"/>
-      <c r="GM13" t="inlineStr"/>
-      <c r="GN13" t="inlineStr"/>
-      <c r="GO13" t="inlineStr"/>
-      <c r="GP13" t="inlineStr"/>
-      <c r="GQ13" t="inlineStr"/>
-      <c r="GR13" t="inlineStr"/>
-      <c r="GS13" t="inlineStr"/>
-      <c r="GT13" t="inlineStr"/>
-      <c r="GU13" t="inlineStr"/>
-      <c r="GV13" t="inlineStr"/>
-      <c r="GW13" t="inlineStr"/>
-      <c r="GX13" t="inlineStr"/>
-      <c r="GY13" t="inlineStr"/>
-      <c r="GZ13" t="inlineStr"/>
-      <c r="HA13" t="inlineStr"/>
-      <c r="HB13" t="inlineStr"/>
-      <c r="HC13" t="inlineStr"/>
-      <c r="HD13" t="inlineStr"/>
-      <c r="HE13" t="inlineStr"/>
-      <c r="HF13" t="inlineStr"/>
-      <c r="HG13" t="inlineStr"/>
-      <c r="HH13" t="inlineStr"/>
-      <c r="HI13" t="inlineStr"/>
-      <c r="HJ13" t="inlineStr"/>
-      <c r="HK13" t="inlineStr"/>
-      <c r="HL13" t="inlineStr"/>
-      <c r="HM13" t="inlineStr"/>
-      <c r="HN13" t="inlineStr"/>
-      <c r="HO13" t="inlineStr"/>
-      <c r="HP13" t="inlineStr"/>
-      <c r="HQ13" t="inlineStr"/>
-      <c r="HR13" t="inlineStr"/>
-      <c r="HS13" t="inlineStr"/>
-      <c r="HT13" t="inlineStr"/>
-      <c r="HU13" t="inlineStr"/>
-      <c r="HV13" t="inlineStr"/>
-      <c r="HW13" t="inlineStr"/>
       <c r="HX13" t="inlineStr">
         <is>
           <t>0.0625</t>
@@ -8590,9 +8434,6 @@
           <t>25.0</t>
         </is>
       </c>
-      <c r="ID13" t="inlineStr"/>
-      <c r="IE13" t="inlineStr"/>
-      <c r="IF13" t="inlineStr"/>
       <c r="IG13" t="inlineStr">
         <is>
           <t>5.45</t>
@@ -8603,7 +8444,6 @@
           <t>9.33</t>
         </is>
       </c>
-      <c r="II13" t="inlineStr"/>
       <c r="IJ13" t="inlineStr">
         <is>
           <t>7.32</t>
@@ -8634,23 +8474,11 @@
           <t>7.31</t>
         </is>
       </c>
-      <c r="IP13" t="inlineStr"/>
-      <c r="IQ13" t="inlineStr"/>
-      <c r="IR13" t="inlineStr"/>
-      <c r="IS13" t="inlineStr"/>
-      <c r="IT13" t="inlineStr"/>
-      <c r="IU13" t="inlineStr"/>
-      <c r="IV13" t="inlineStr"/>
-      <c r="IW13" t="inlineStr"/>
-      <c r="IX13" t="inlineStr"/>
-      <c r="IY13" t="inlineStr"/>
-      <c r="IZ13" t="inlineStr"/>
       <c r="JA13" t="inlineStr">
         <is>
           <t>153</t>
         </is>
       </c>
-      <c r="JB13" t="inlineStr"/>
       <c r="JC13" t="inlineStr">
         <is>
           <t>143</t>
@@ -8681,10 +8509,6 @@
           <t>134</t>
         </is>
       </c>
-      <c r="JI13" t="inlineStr"/>
-      <c r="JJ13" t="inlineStr"/>
-      <c r="JK13" t="inlineStr"/>
-      <c r="JL13" t="inlineStr"/>
       <c r="JM13" t="inlineStr">
         <is>
           <t>.9</t>
@@ -8715,136 +8539,1848 @@
           <t>.15</t>
         </is>
       </c>
-      <c r="JS13" t="inlineStr"/>
-      <c r="JT13" t="inlineStr"/>
-      <c r="JU13" t="inlineStr"/>
-      <c r="JV13" t="inlineStr"/>
-      <c r="JW13" t="inlineStr"/>
-      <c r="JX13" t="inlineStr"/>
-      <c r="JY13" t="inlineStr"/>
-      <c r="JZ13" t="inlineStr"/>
-      <c r="KA13" t="inlineStr"/>
-      <c r="KB13" t="inlineStr"/>
-      <c r="KC13" t="inlineStr"/>
-      <c r="KD13" t="inlineStr"/>
-      <c r="KE13" t="inlineStr"/>
-      <c r="KF13" t="inlineStr"/>
-      <c r="KG13" t="inlineStr"/>
-      <c r="KH13" t="inlineStr"/>
-      <c r="KI13" t="inlineStr"/>
-      <c r="KJ13" t="inlineStr"/>
-      <c r="KK13" t="inlineStr"/>
-      <c r="KL13" t="inlineStr"/>
-      <c r="KM13" t="inlineStr"/>
-      <c r="KN13" t="inlineStr"/>
-      <c r="KO13" t="inlineStr"/>
-      <c r="KP13" t="inlineStr"/>
-      <c r="KQ13" t="inlineStr"/>
-      <c r="KR13" t="inlineStr"/>
-      <c r="KS13" t="inlineStr"/>
-      <c r="KT13" t="inlineStr"/>
-      <c r="KU13" t="inlineStr"/>
-      <c r="KV13" t="inlineStr"/>
-      <c r="KW13" t="inlineStr"/>
-      <c r="KX13" t="inlineStr"/>
-      <c r="KY13" t="inlineStr"/>
-      <c r="KZ13" t="inlineStr"/>
-      <c r="LA13" t="inlineStr"/>
-      <c r="LB13" t="inlineStr"/>
-      <c r="LC13" t="inlineStr"/>
-      <c r="LD13" t="inlineStr"/>
-      <c r="LE13" t="inlineStr"/>
-      <c r="LF13" t="inlineStr"/>
-      <c r="LG13" t="inlineStr"/>
-      <c r="LH13" t="inlineStr"/>
-      <c r="LI13" t="inlineStr"/>
-      <c r="LJ13" t="inlineStr"/>
-      <c r="LK13" t="inlineStr"/>
-      <c r="LL13" t="inlineStr"/>
-      <c r="LM13" t="inlineStr"/>
-      <c r="LN13" t="inlineStr"/>
-      <c r="LO13" t="inlineStr"/>
-      <c r="LP13" t="inlineStr"/>
-      <c r="LQ13" t="inlineStr"/>
-      <c r="LR13" t="inlineStr"/>
-      <c r="LS13" t="inlineStr"/>
-      <c r="LT13" t="inlineStr"/>
-      <c r="LU13" t="inlineStr"/>
-      <c r="LV13" t="inlineStr"/>
-      <c r="LW13" t="inlineStr"/>
-      <c r="LX13" t="inlineStr"/>
-      <c r="LY13" t="inlineStr"/>
-      <c r="LZ13" t="inlineStr"/>
-      <c r="MA13" t="inlineStr"/>
-      <c r="MB13" t="inlineStr"/>
-      <c r="MC13" t="inlineStr"/>
-      <c r="MD13" t="inlineStr"/>
-      <c r="ME13" t="inlineStr"/>
-      <c r="MF13" t="inlineStr"/>
-      <c r="MG13" t="inlineStr"/>
-      <c r="MH13" t="inlineStr"/>
-      <c r="MI13" t="inlineStr"/>
-      <c r="MJ13" t="inlineStr"/>
-      <c r="MK13" t="inlineStr"/>
-      <c r="ML13" t="inlineStr"/>
-      <c r="MM13" t="inlineStr"/>
-      <c r="MN13" t="inlineStr"/>
-      <c r="MO13" t="inlineStr"/>
-      <c r="MP13" t="inlineStr"/>
-      <c r="MQ13" t="inlineStr"/>
-      <c r="MR13" t="inlineStr"/>
-      <c r="MS13" t="inlineStr"/>
-      <c r="MT13" t="inlineStr"/>
-      <c r="MU13" t="inlineStr"/>
-      <c r="MV13" t="inlineStr"/>
-      <c r="MW13" t="inlineStr"/>
-      <c r="MX13" t="inlineStr"/>
-      <c r="MY13" t="inlineStr"/>
-      <c r="MZ13" t="inlineStr"/>
-      <c r="NA13" t="inlineStr"/>
-      <c r="NB13" t="inlineStr"/>
-      <c r="NC13" t="inlineStr"/>
-      <c r="ND13" t="inlineStr"/>
-      <c r="NE13" t="inlineStr"/>
-      <c r="NF13" t="inlineStr"/>
-      <c r="NG13" t="inlineStr"/>
-      <c r="NH13" t="inlineStr"/>
-      <c r="NI13" t="inlineStr"/>
-      <c r="NJ13" t="inlineStr"/>
-      <c r="NK13" t="inlineStr"/>
-      <c r="NL13" t="inlineStr"/>
-      <c r="NM13" t="inlineStr"/>
-      <c r="NN13" t="inlineStr"/>
-      <c r="NO13" t="inlineStr"/>
-      <c r="NP13" t="inlineStr"/>
-      <c r="NQ13" t="inlineStr"/>
-      <c r="NR13" t="inlineStr"/>
-      <c r="NS13" t="inlineStr"/>
-      <c r="NT13" t="inlineStr"/>
-      <c r="NU13" t="inlineStr"/>
-      <c r="NV13" t="inlineStr"/>
-      <c r="NW13" t="inlineStr"/>
-      <c r="NX13" t="inlineStr"/>
-      <c r="NY13" t="inlineStr"/>
-      <c r="NZ13" t="inlineStr"/>
-      <c r="OA13" t="inlineStr"/>
-      <c r="OB13" t="inlineStr"/>
-      <c r="OC13" t="inlineStr"/>
-      <c r="OD13" t="inlineStr"/>
-      <c r="OE13" t="inlineStr"/>
-      <c r="OF13" t="inlineStr"/>
-      <c r="OG13" t="inlineStr"/>
-      <c r="OH13" t="inlineStr"/>
-      <c r="OI13" t="inlineStr"/>
-      <c r="OJ13" t="inlineStr"/>
-      <c r="OK13" t="inlineStr"/>
-      <c r="OL13" t="inlineStr"/>
-      <c r="OM13" t="inlineStr"/>
-      <c r="ON13" t="inlineStr"/>
-      <c r="OO13" t="inlineStr"/>
-      <c r="OP13" t="inlineStr"/>
-      <c r="OQ13" t="inlineStr"/>
-      <c r="OR13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>type01</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>16.0</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>3.22</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>3.03</t>
+        </is>
+      </c>
+      <c r="T14" t="inlineStr">
+        <is>
+          <t>3.00</t>
+        </is>
+      </c>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>2.97</t>
+        </is>
+      </c>
+      <c r="V14" t="inlineStr">
+        <is>
+          <t>3.01</t>
+        </is>
+      </c>
+      <c r="W14" t="inlineStr">
+        <is>
+          <t>2.93</t>
+        </is>
+      </c>
+      <c r="X14" t="inlineStr">
+        <is>
+          <t>2.31</t>
+        </is>
+      </c>
+      <c r="Y14" t="inlineStr">
+        <is>
+          <t>2.75</t>
+        </is>
+      </c>
+      <c r="AK14" t="inlineStr">
+        <is>
+          <t>94</t>
+        </is>
+      </c>
+      <c r="AM14" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="AN14" t="inlineStr">
+        <is>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="AO14" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="AP14" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="AQ14" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="AR14" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="AW14" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="AX14" t="inlineStr">
+        <is>
+          <t>.2</t>
+        </is>
+      </c>
+      <c r="AY14" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="AZ14" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="BA14" t="inlineStr">
+        <is>
+          <t>.7</t>
+        </is>
+      </c>
+      <c r="BB14" t="inlineStr">
+        <is>
+          <t>.9</t>
+        </is>
+      </c>
+      <c r="BO14" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="BP14" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="BQ14" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="BR14" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="BS14" t="inlineStr">
+        <is>
+          <t>15.0</t>
+        </is>
+      </c>
+      <c r="BT14" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="BX14" t="inlineStr">
+        <is>
+          <t>2.51</t>
+        </is>
+      </c>
+      <c r="BY14" t="inlineStr">
+        <is>
+          <t>2.20</t>
+        </is>
+      </c>
+      <c r="CA14" t="inlineStr">
+        <is>
+          <t>2.23</t>
+        </is>
+      </c>
+      <c r="CB14" t="inlineStr">
+        <is>
+          <t>2.25</t>
+        </is>
+      </c>
+      <c r="CC14" t="inlineStr">
+        <is>
+          <t>2.27</t>
+        </is>
+      </c>
+      <c r="CD14" t="inlineStr">
+        <is>
+          <t>2.20</t>
+        </is>
+      </c>
+      <c r="CE14" t="inlineStr">
+        <is>
+          <t>2.10</t>
+        </is>
+      </c>
+      <c r="CF14" t="inlineStr">
+        <is>
+          <t>1.99</t>
+        </is>
+      </c>
+      <c r="CR14" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="CT14" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="CU14" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="CV14" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="CW14" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="CX14" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="CY14" t="inlineStr">
+        <is>
+          <t>79</t>
+        </is>
+      </c>
+      <c r="DD14" t="inlineStr">
+        <is>
+          <t>.2</t>
+        </is>
+      </c>
+      <c r="DE14" t="inlineStr">
+        <is>
+          <t>.2</t>
+        </is>
+      </c>
+      <c r="DF14" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="DG14" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="DH14" t="inlineStr">
+        <is>
+          <t>.3</t>
+        </is>
+      </c>
+      <c r="DI14" t="inlineStr">
+        <is>
+          <t>.13</t>
+        </is>
+      </c>
+      <c r="DP14" t="inlineStr">
+        <is>
+          <t>220</t>
+        </is>
+      </c>
+      <c r="EJ14" t="inlineStr">
+        <is>
+          <t>2.57</t>
+        </is>
+      </c>
+      <c r="EK14" t="inlineStr">
+        <is>
+          <t>1.75</t>
+        </is>
+      </c>
+      <c r="EL14" t="inlineStr">
+        <is>
+          <t>1.67</t>
+        </is>
+      </c>
+      <c r="EM14" t="inlineStr">
+        <is>
+          <t>1.69</t>
+        </is>
+      </c>
+      <c r="EN14" t="inlineStr">
+        <is>
+          <t>1.73</t>
+        </is>
+      </c>
+      <c r="EO14" t="inlineStr">
+        <is>
+          <t>1.69</t>
+        </is>
+      </c>
+      <c r="ET14" t="inlineStr">
+        <is>
+          <t>68</t>
+        </is>
+      </c>
+      <c r="EV14" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="EW14" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="EX14" t="inlineStr">
+        <is>
+          <t>63</t>
+        </is>
+      </c>
+      <c r="EY14" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="EZ14" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="FA14" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="FY14" t="inlineStr">
+        <is>
+          <t>.4</t>
+        </is>
+      </c>
+      <c r="FZ14" t="inlineStr">
+        <is>
+          <t>.3</t>
+        </is>
+      </c>
+      <c r="GA14" t="inlineStr">
+        <is>
+          <t>.0</t>
+        </is>
+      </c>
+      <c r="GB14" t="inlineStr">
+        <is>
+          <t>.3</t>
+        </is>
+      </c>
+      <c r="GC14" t="inlineStr">
+        <is>
+          <t>.11</t>
+        </is>
+      </c>
+      <c r="GD14" t="inlineStr">
+        <is>
+          <t>.24</t>
+        </is>
+      </c>
+      <c r="HX14" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="HY14" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="HZ14" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="IA14" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="IB14" t="inlineStr">
+        <is>
+          <t>16.0</t>
+        </is>
+      </c>
+      <c r="IC14" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="IG14" t="inlineStr">
+        <is>
+          <t>5.45</t>
+        </is>
+      </c>
+      <c r="IH14" t="inlineStr">
+        <is>
+          <t>9.33</t>
+        </is>
+      </c>
+      <c r="IJ14" t="inlineStr">
+        <is>
+          <t>7.32</t>
+        </is>
+      </c>
+      <c r="IK14" t="inlineStr">
+        <is>
+          <t>0.47</t>
+        </is>
+      </c>
+      <c r="IL14" t="inlineStr">
+        <is>
+          <t>7.99</t>
+        </is>
+      </c>
+      <c r="IM14" t="inlineStr">
+        <is>
+          <t>7.64</t>
+        </is>
+      </c>
+      <c r="IN14" t="inlineStr">
+        <is>
+          <t>3.12</t>
+        </is>
+      </c>
+      <c r="IO14" t="inlineStr">
+        <is>
+          <t>7.31</t>
+        </is>
+      </c>
+      <c r="JA14" t="inlineStr">
+        <is>
+          <t>153</t>
+        </is>
+      </c>
+      <c r="JC14" t="inlineStr">
+        <is>
+          <t>143</t>
+        </is>
+      </c>
+      <c r="JD14" t="inlineStr">
+        <is>
+          <t>155</t>
+        </is>
+      </c>
+      <c r="JE14" t="inlineStr">
+        <is>
+          <t>147</t>
+        </is>
+      </c>
+      <c r="JF14" t="inlineStr">
+        <is>
+          <t>140</t>
+        </is>
+      </c>
+      <c r="JG14" t="inlineStr">
+        <is>
+          <t>149</t>
+        </is>
+      </c>
+      <c r="JH14" t="inlineStr">
+        <is>
+          <t>134</t>
+        </is>
+      </c>
+      <c r="JM14" t="inlineStr">
+        <is>
+          <t>.9</t>
+        </is>
+      </c>
+      <c r="JN14" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="JO14" t="inlineStr">
+        <is>
+          <t>.7</t>
+        </is>
+      </c>
+      <c r="JP14" t="inlineStr">
+        <is>
+          <t>.11</t>
+        </is>
+      </c>
+      <c r="JQ14" t="inlineStr">
+        <is>
+          <t>.5</t>
+        </is>
+      </c>
+      <c r="JR14" t="inlineStr">
+        <is>
+          <t>.15</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>type01</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>16.0</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>3.22</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>3.03</t>
+        </is>
+      </c>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>3.00</t>
+        </is>
+      </c>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>2.97</t>
+        </is>
+      </c>
+      <c r="V15" t="inlineStr">
+        <is>
+          <t>3.01</t>
+        </is>
+      </c>
+      <c r="W15" t="inlineStr">
+        <is>
+          <t>2.93</t>
+        </is>
+      </c>
+      <c r="X15" t="inlineStr">
+        <is>
+          <t>2.31</t>
+        </is>
+      </c>
+      <c r="Y15" t="inlineStr">
+        <is>
+          <t>2.75</t>
+        </is>
+      </c>
+      <c r="AK15" t="inlineStr">
+        <is>
+          <t>94</t>
+        </is>
+      </c>
+      <c r="AM15" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="AN15" t="inlineStr">
+        <is>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="AO15" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="AP15" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="AQ15" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="AR15" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="AW15" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="AX15" t="inlineStr">
+        <is>
+          <t>.2</t>
+        </is>
+      </c>
+      <c r="AY15" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="AZ15" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="BA15" t="inlineStr">
+        <is>
+          <t>.7</t>
+        </is>
+      </c>
+      <c r="BB15" t="inlineStr">
+        <is>
+          <t>.9</t>
+        </is>
+      </c>
+      <c r="BO15" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="BP15" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="BQ15" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="BR15" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="BS15" t="inlineStr">
+        <is>
+          <t>15.0</t>
+        </is>
+      </c>
+      <c r="BT15" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="BX15" t="inlineStr">
+        <is>
+          <t>2.51</t>
+        </is>
+      </c>
+      <c r="BY15" t="inlineStr">
+        <is>
+          <t>2.20</t>
+        </is>
+      </c>
+      <c r="CA15" t="inlineStr">
+        <is>
+          <t>2.23</t>
+        </is>
+      </c>
+      <c r="CB15" t="inlineStr">
+        <is>
+          <t>2.25</t>
+        </is>
+      </c>
+      <c r="CC15" t="inlineStr">
+        <is>
+          <t>2.27</t>
+        </is>
+      </c>
+      <c r="CD15" t="inlineStr">
+        <is>
+          <t>2.20</t>
+        </is>
+      </c>
+      <c r="CE15" t="inlineStr">
+        <is>
+          <t>2.10</t>
+        </is>
+      </c>
+      <c r="CF15" t="inlineStr">
+        <is>
+          <t>1.99</t>
+        </is>
+      </c>
+      <c r="CR15" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="CT15" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="CU15" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="CV15" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="CW15" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="CX15" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="CY15" t="inlineStr">
+        <is>
+          <t>79</t>
+        </is>
+      </c>
+      <c r="DD15" t="inlineStr">
+        <is>
+          <t>.2</t>
+        </is>
+      </c>
+      <c r="DE15" t="inlineStr">
+        <is>
+          <t>.2</t>
+        </is>
+      </c>
+      <c r="DF15" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="DG15" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="DH15" t="inlineStr">
+        <is>
+          <t>.3</t>
+        </is>
+      </c>
+      <c r="DI15" t="inlineStr">
+        <is>
+          <t>.13</t>
+        </is>
+      </c>
+      <c r="DP15" t="inlineStr">
+        <is>
+          <t>220</t>
+        </is>
+      </c>
+      <c r="EJ15" t="inlineStr">
+        <is>
+          <t>2.57</t>
+        </is>
+      </c>
+      <c r="EK15" t="inlineStr">
+        <is>
+          <t>1.75</t>
+        </is>
+      </c>
+      <c r="EL15" t="inlineStr">
+        <is>
+          <t>1.67</t>
+        </is>
+      </c>
+      <c r="EM15" t="inlineStr">
+        <is>
+          <t>1.69</t>
+        </is>
+      </c>
+      <c r="EN15" t="inlineStr">
+        <is>
+          <t>1.73</t>
+        </is>
+      </c>
+      <c r="EO15" t="inlineStr">
+        <is>
+          <t>1.69</t>
+        </is>
+      </c>
+      <c r="ET15" t="inlineStr">
+        <is>
+          <t>68</t>
+        </is>
+      </c>
+      <c r="EV15" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="EW15" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="EX15" t="inlineStr">
+        <is>
+          <t>63</t>
+        </is>
+      </c>
+      <c r="EY15" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="EZ15" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="FA15" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="FY15" t="inlineStr">
+        <is>
+          <t>.4</t>
+        </is>
+      </c>
+      <c r="FZ15" t="inlineStr">
+        <is>
+          <t>.3</t>
+        </is>
+      </c>
+      <c r="GA15" t="inlineStr">
+        <is>
+          <t>.0</t>
+        </is>
+      </c>
+      <c r="GB15" t="inlineStr">
+        <is>
+          <t>.3</t>
+        </is>
+      </c>
+      <c r="GC15" t="inlineStr">
+        <is>
+          <t>.11</t>
+        </is>
+      </c>
+      <c r="GD15" t="inlineStr">
+        <is>
+          <t>.24</t>
+        </is>
+      </c>
+      <c r="HX15" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="HY15" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="HZ15" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="IA15" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="IB15" t="inlineStr">
+        <is>
+          <t>16.0</t>
+        </is>
+      </c>
+      <c r="IC15" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="IG15" t="inlineStr">
+        <is>
+          <t>5.45</t>
+        </is>
+      </c>
+      <c r="IH15" t="inlineStr">
+        <is>
+          <t>9.33</t>
+        </is>
+      </c>
+      <c r="IJ15" t="inlineStr">
+        <is>
+          <t>7.32</t>
+        </is>
+      </c>
+      <c r="IK15" t="inlineStr">
+        <is>
+          <t>0.47</t>
+        </is>
+      </c>
+      <c r="IL15" t="inlineStr">
+        <is>
+          <t>7.99</t>
+        </is>
+      </c>
+      <c r="IM15" t="inlineStr">
+        <is>
+          <t>7.64</t>
+        </is>
+      </c>
+      <c r="IN15" t="inlineStr">
+        <is>
+          <t>3.12</t>
+        </is>
+      </c>
+      <c r="IO15" t="inlineStr">
+        <is>
+          <t>7.31</t>
+        </is>
+      </c>
+      <c r="JA15" t="inlineStr">
+        <is>
+          <t>153</t>
+        </is>
+      </c>
+      <c r="JC15" t="inlineStr">
+        <is>
+          <t>143</t>
+        </is>
+      </c>
+      <c r="JD15" t="inlineStr">
+        <is>
+          <t>155</t>
+        </is>
+      </c>
+      <c r="JE15" t="inlineStr">
+        <is>
+          <t>147</t>
+        </is>
+      </c>
+      <c r="JF15" t="inlineStr">
+        <is>
+          <t>140</t>
+        </is>
+      </c>
+      <c r="JG15" t="inlineStr">
+        <is>
+          <t>149</t>
+        </is>
+      </c>
+      <c r="JH15" t="inlineStr">
+        <is>
+          <t>134</t>
+        </is>
+      </c>
+      <c r="JM15" t="inlineStr">
+        <is>
+          <t>.9</t>
+        </is>
+      </c>
+      <c r="JN15" t="inlineStr">
+        <is>
+          <t>.1</t>
+        </is>
+      </c>
+      <c r="JO15" t="inlineStr">
+        <is>
+          <t>.7</t>
+        </is>
+      </c>
+      <c r="JP15" t="inlineStr">
+        <is>
+          <t>.11</t>
+        </is>
+      </c>
+      <c r="JQ15" t="inlineStr">
+        <is>
+          <t>.5</t>
+        </is>
+      </c>
+      <c r="JR15" t="inlineStr">
+        <is>
+          <t>.15</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>type01</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>16.0</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr"/>
+      <c r="O16" t="inlineStr"/>
+      <c r="P16" t="inlineStr"/>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>3.22</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>3.03</t>
+        </is>
+      </c>
+      <c r="S16" t="inlineStr"/>
+      <c r="T16" t="inlineStr">
+        <is>
+          <t>3.00</t>
+        </is>
+      </c>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>2.97</t>
+        </is>
+      </c>
+      <c r="V16" t="inlineStr">
+        <is>
+          <t>3.01</t>
+        </is>
+      </c>
+      <c r="W16" t="inlineStr">
+        <is>
+          <t>2.93</t>
+        </is>
+      </c>
+      <c r="X16" t="inlineStr">
+        <is>
+          <t>2.31</t>
+        </is>
+      </c>
+      <c r="Y16" t="inlineStr">
+        <is>
+          <t>2.75</t>
+        </is>
+      </c>
+      <c r="Z16" t="inlineStr"/>
+      <c r="AA16" t="inlineStr"/>
+      <c r="AB16" t="inlineStr"/>
+      <c r="AC16" t="inlineStr"/>
+      <c r="AD16" t="inlineStr"/>
+      <c r="AE16" t="inlineStr"/>
+      <c r="AF16" t="inlineStr"/>
+      <c r="AG16" t="inlineStr"/>
+      <c r="AH16" t="inlineStr"/>
+      <c r="AI16" t="inlineStr"/>
+      <c r="AJ16" t="inlineStr"/>
+      <c r="AK16" t="inlineStr">
+        <is>
+          <t>94</t>
+        </is>
+      </c>
+      <c r="AL16" t="inlineStr"/>
+      <c r="AM16" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="AN16" t="inlineStr">
+        <is>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="AO16" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="AP16" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="AQ16" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="AR16" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="AS16" t="inlineStr"/>
+      <c r="AT16" t="inlineStr"/>
+      <c r="AU16" t="inlineStr"/>
+      <c r="AV16" t="inlineStr"/>
+      <c r="AW16" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="AX16" t="inlineStr">
+        <is>
+          <t>-2</t>
+        </is>
+      </c>
+      <c r="AY16" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="AZ16" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="BA16" t="inlineStr">
+        <is>
+          <t>-7</t>
+        </is>
+      </c>
+      <c r="BB16" t="inlineStr">
+        <is>
+          <t>-9</t>
+        </is>
+      </c>
+      <c r="BC16" t="inlineStr"/>
+      <c r="BD16" t="inlineStr"/>
+      <c r="BE16" t="inlineStr"/>
+      <c r="BF16" t="inlineStr"/>
+      <c r="BG16" t="inlineStr"/>
+      <c r="BH16" t="inlineStr"/>
+      <c r="BI16" t="inlineStr"/>
+      <c r="BJ16" t="inlineStr"/>
+      <c r="BK16" t="inlineStr"/>
+      <c r="BL16" t="inlineStr"/>
+      <c r="BM16" t="inlineStr"/>
+      <c r="BN16" t="inlineStr"/>
+      <c r="BO16" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="BP16" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="BQ16" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="BR16" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="BS16" t="inlineStr">
+        <is>
+          <t>15.0</t>
+        </is>
+      </c>
+      <c r="BT16" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="BU16" t="inlineStr"/>
+      <c r="BV16" t="inlineStr"/>
+      <c r="BW16" t="inlineStr"/>
+      <c r="BX16" t="inlineStr">
+        <is>
+          <t>2.51</t>
+        </is>
+      </c>
+      <c r="BY16" t="inlineStr">
+        <is>
+          <t>2.20</t>
+        </is>
+      </c>
+      <c r="BZ16" t="inlineStr"/>
+      <c r="CA16" t="inlineStr">
+        <is>
+          <t>2.23</t>
+        </is>
+      </c>
+      <c r="CB16" t="inlineStr">
+        <is>
+          <t>2.25</t>
+        </is>
+      </c>
+      <c r="CC16" t="inlineStr">
+        <is>
+          <t>2.27</t>
+        </is>
+      </c>
+      <c r="CD16" t="inlineStr">
+        <is>
+          <t>2.20</t>
+        </is>
+      </c>
+      <c r="CE16" t="inlineStr">
+        <is>
+          <t>2.10</t>
+        </is>
+      </c>
+      <c r="CF16" t="inlineStr">
+        <is>
+          <t>1.99</t>
+        </is>
+      </c>
+      <c r="CG16" t="inlineStr"/>
+      <c r="CH16" t="inlineStr"/>
+      <c r="CI16" t="inlineStr"/>
+      <c r="CJ16" t="inlineStr"/>
+      <c r="CK16" t="inlineStr"/>
+      <c r="CL16" t="inlineStr"/>
+      <c r="CM16" t="inlineStr"/>
+      <c r="CN16" t="inlineStr"/>
+      <c r="CO16" t="inlineStr"/>
+      <c r="CP16" t="inlineStr"/>
+      <c r="CQ16" t="inlineStr"/>
+      <c r="CR16" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="CS16" t="inlineStr"/>
+      <c r="CT16" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="CU16" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="CV16" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="CW16" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="CX16" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="CY16" t="inlineStr">
+        <is>
+          <t>79</t>
+        </is>
+      </c>
+      <c r="CZ16" t="inlineStr"/>
+      <c r="DA16" t="inlineStr"/>
+      <c r="DB16" t="inlineStr"/>
+      <c r="DC16" t="inlineStr"/>
+      <c r="DD16" t="inlineStr">
+        <is>
+          <t>-2</t>
+        </is>
+      </c>
+      <c r="DE16" t="inlineStr">
+        <is>
+          <t>-2</t>
+        </is>
+      </c>
+      <c r="DF16" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="DG16" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="DH16" t="inlineStr">
+        <is>
+          <t>-3</t>
+        </is>
+      </c>
+      <c r="DI16" t="inlineStr">
+        <is>
+          <t>-13</t>
+        </is>
+      </c>
+      <c r="DJ16" t="inlineStr"/>
+      <c r="DK16" t="inlineStr"/>
+      <c r="DL16" t="inlineStr"/>
+      <c r="DM16" t="inlineStr"/>
+      <c r="DN16" t="inlineStr"/>
+      <c r="DO16" t="inlineStr"/>
+      <c r="DP16" t="inlineStr">
+        <is>
+          <t>220</t>
+        </is>
+      </c>
+      <c r="DQ16" t="inlineStr"/>
+      <c r="DR16" t="inlineStr"/>
+      <c r="DS16" t="inlineStr"/>
+      <c r="DT16" t="inlineStr"/>
+      <c r="DU16" t="inlineStr"/>
+      <c r="DV16" t="inlineStr"/>
+      <c r="DW16" t="inlineStr"/>
+      <c r="DX16" t="inlineStr"/>
+      <c r="DY16" t="inlineStr"/>
+      <c r="DZ16" t="inlineStr"/>
+      <c r="EA16" t="inlineStr"/>
+      <c r="EB16" t="inlineStr"/>
+      <c r="EC16" t="inlineStr"/>
+      <c r="ED16" t="inlineStr"/>
+      <c r="EE16" t="inlineStr"/>
+      <c r="EF16" t="inlineStr"/>
+      <c r="EG16" t="inlineStr"/>
+      <c r="EH16" t="inlineStr"/>
+      <c r="EI16" t="inlineStr"/>
+      <c r="EJ16" t="inlineStr">
+        <is>
+          <t>2.57</t>
+        </is>
+      </c>
+      <c r="EK16" t="inlineStr">
+        <is>
+          <t>1.75</t>
+        </is>
+      </c>
+      <c r="EL16" t="inlineStr">
+        <is>
+          <t>1.67</t>
+        </is>
+      </c>
+      <c r="EM16" t="inlineStr">
+        <is>
+          <t>1.69</t>
+        </is>
+      </c>
+      <c r="EN16" t="inlineStr">
+        <is>
+          <t>1.73</t>
+        </is>
+      </c>
+      <c r="EO16" t="inlineStr">
+        <is>
+          <t>1.69</t>
+        </is>
+      </c>
+      <c r="EP16" t="inlineStr"/>
+      <c r="EQ16" t="inlineStr"/>
+      <c r="ER16" t="inlineStr"/>
+      <c r="ES16" t="inlineStr"/>
+      <c r="ET16" t="inlineStr">
+        <is>
+          <t>68</t>
+        </is>
+      </c>
+      <c r="EU16" t="inlineStr"/>
+      <c r="EV16" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="EW16" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="EX16" t="inlineStr">
+        <is>
+          <t>63</t>
+        </is>
+      </c>
+      <c r="EY16" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="EZ16" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="FA16" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="FB16" t="inlineStr"/>
+      <c r="FC16" t="inlineStr"/>
+      <c r="FD16" t="inlineStr"/>
+      <c r="FE16" t="inlineStr"/>
+      <c r="FF16" t="inlineStr"/>
+      <c r="FG16" t="inlineStr"/>
+      <c r="FH16" t="inlineStr"/>
+      <c r="FI16" t="inlineStr"/>
+      <c r="FJ16" t="inlineStr"/>
+      <c r="FK16" t="inlineStr"/>
+      <c r="FL16" t="inlineStr"/>
+      <c r="FM16" t="inlineStr"/>
+      <c r="FN16" t="inlineStr"/>
+      <c r="FO16" t="inlineStr"/>
+      <c r="FP16" t="inlineStr"/>
+      <c r="FQ16" t="inlineStr"/>
+      <c r="FR16" t="inlineStr"/>
+      <c r="FS16" t="inlineStr"/>
+      <c r="FT16" t="inlineStr"/>
+      <c r="FU16" t="inlineStr"/>
+      <c r="FV16" t="inlineStr"/>
+      <c r="FW16" t="inlineStr"/>
+      <c r="FX16" t="inlineStr"/>
+      <c r="FY16" t="inlineStr">
+        <is>
+          <t>-4</t>
+        </is>
+      </c>
+      <c r="FZ16" t="inlineStr">
+        <is>
+          <t>-3</t>
+        </is>
+      </c>
+      <c r="GA16" t="inlineStr">
+        <is>
+          <t>-0</t>
+        </is>
+      </c>
+      <c r="GB16" t="inlineStr">
+        <is>
+          <t>-3</t>
+        </is>
+      </c>
+      <c r="GC16" t="inlineStr">
+        <is>
+          <t>-11</t>
+        </is>
+      </c>
+      <c r="GD16" t="inlineStr">
+        <is>
+          <t>-24</t>
+        </is>
+      </c>
+      <c r="GE16" t="inlineStr"/>
+      <c r="GF16" t="inlineStr"/>
+      <c r="GG16" t="inlineStr"/>
+      <c r="GH16" t="inlineStr"/>
+      <c r="GI16" t="inlineStr"/>
+      <c r="GJ16" t="inlineStr"/>
+      <c r="GK16" t="inlineStr"/>
+      <c r="GL16" t="inlineStr"/>
+      <c r="GM16" t="inlineStr"/>
+      <c r="GN16" t="inlineStr"/>
+      <c r="GO16" t="inlineStr"/>
+      <c r="GP16" t="inlineStr"/>
+      <c r="GQ16" t="inlineStr"/>
+      <c r="GR16" t="inlineStr"/>
+      <c r="GS16" t="inlineStr"/>
+      <c r="GT16" t="inlineStr"/>
+      <c r="GU16" t="inlineStr"/>
+      <c r="GV16" t="inlineStr"/>
+      <c r="GW16" t="inlineStr"/>
+      <c r="GX16" t="inlineStr"/>
+      <c r="GY16" t="inlineStr"/>
+      <c r="GZ16" t="inlineStr"/>
+      <c r="HA16" t="inlineStr"/>
+      <c r="HB16" t="inlineStr"/>
+      <c r="HC16" t="inlineStr"/>
+      <c r="HD16" t="inlineStr"/>
+      <c r="HE16" t="inlineStr"/>
+      <c r="HF16" t="inlineStr"/>
+      <c r="HG16" t="inlineStr"/>
+      <c r="HH16" t="inlineStr"/>
+      <c r="HI16" t="inlineStr"/>
+      <c r="HJ16" t="inlineStr"/>
+      <c r="HK16" t="inlineStr"/>
+      <c r="HL16" t="inlineStr"/>
+      <c r="HM16" t="inlineStr"/>
+      <c r="HN16" t="inlineStr"/>
+      <c r="HO16" t="inlineStr"/>
+      <c r="HP16" t="inlineStr"/>
+      <c r="HQ16" t="inlineStr"/>
+      <c r="HR16" t="inlineStr"/>
+      <c r="HS16" t="inlineStr"/>
+      <c r="HT16" t="inlineStr"/>
+      <c r="HU16" t="inlineStr"/>
+      <c r="HV16" t="inlineStr"/>
+      <c r="HW16" t="inlineStr"/>
+      <c r="HX16" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="HY16" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="HZ16" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="IA16" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="IB16" t="inlineStr">
+        <is>
+          <t>16.0</t>
+        </is>
+      </c>
+      <c r="IC16" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="ID16" t="inlineStr"/>
+      <c r="IE16" t="inlineStr"/>
+      <c r="IF16" t="inlineStr"/>
+      <c r="IG16" t="inlineStr">
+        <is>
+          <t>5.45</t>
+        </is>
+      </c>
+      <c r="IH16" t="inlineStr">
+        <is>
+          <t>9.33</t>
+        </is>
+      </c>
+      <c r="II16" t="inlineStr"/>
+      <c r="IJ16" t="inlineStr">
+        <is>
+          <t>7.32</t>
+        </is>
+      </c>
+      <c r="IK16" t="inlineStr">
+        <is>
+          <t>0.47</t>
+        </is>
+      </c>
+      <c r="IL16" t="inlineStr">
+        <is>
+          <t>7.99</t>
+        </is>
+      </c>
+      <c r="IM16" t="inlineStr">
+        <is>
+          <t>7.64</t>
+        </is>
+      </c>
+      <c r="IN16" t="inlineStr">
+        <is>
+          <t>3.12</t>
+        </is>
+      </c>
+      <c r="IO16" t="inlineStr">
+        <is>
+          <t>7.31</t>
+        </is>
+      </c>
+      <c r="IP16" t="inlineStr"/>
+      <c r="IQ16" t="inlineStr"/>
+      <c r="IR16" t="inlineStr"/>
+      <c r="IS16" t="inlineStr"/>
+      <c r="IT16" t="inlineStr"/>
+      <c r="IU16" t="inlineStr"/>
+      <c r="IV16" t="inlineStr"/>
+      <c r="IW16" t="inlineStr"/>
+      <c r="IX16" t="inlineStr"/>
+      <c r="IY16" t="inlineStr"/>
+      <c r="IZ16" t="inlineStr"/>
+      <c r="JA16" t="inlineStr">
+        <is>
+          <t>153</t>
+        </is>
+      </c>
+      <c r="JB16" t="inlineStr"/>
+      <c r="JC16" t="inlineStr">
+        <is>
+          <t>143</t>
+        </is>
+      </c>
+      <c r="JD16" t="inlineStr">
+        <is>
+          <t>155</t>
+        </is>
+      </c>
+      <c r="JE16" t="inlineStr">
+        <is>
+          <t>147</t>
+        </is>
+      </c>
+      <c r="JF16" t="inlineStr">
+        <is>
+          <t>140</t>
+        </is>
+      </c>
+      <c r="JG16" t="inlineStr">
+        <is>
+          <t>149</t>
+        </is>
+      </c>
+      <c r="JH16" t="inlineStr">
+        <is>
+          <t>134</t>
+        </is>
+      </c>
+      <c r="JI16" t="inlineStr"/>
+      <c r="JJ16" t="inlineStr"/>
+      <c r="JK16" t="inlineStr"/>
+      <c r="JL16" t="inlineStr"/>
+      <c r="JM16" t="inlineStr">
+        <is>
+          <t>-9</t>
+        </is>
+      </c>
+      <c r="JN16" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="JO16" t="inlineStr">
+        <is>
+          <t>-7</t>
+        </is>
+      </c>
+      <c r="JP16" t="inlineStr">
+        <is>
+          <t>-11</t>
+        </is>
+      </c>
+      <c r="JQ16" t="inlineStr">
+        <is>
+          <t>-5</t>
+        </is>
+      </c>
+      <c r="JR16" t="inlineStr">
+        <is>
+          <t>-15</t>
+        </is>
+      </c>
+      <c r="JS16" t="inlineStr"/>
+      <c r="JT16" t="inlineStr"/>
+      <c r="JU16" t="inlineStr"/>
+      <c r="JV16" t="inlineStr"/>
+      <c r="JW16" t="inlineStr"/>
+      <c r="JX16" t="inlineStr"/>
+      <c r="JY16" t="inlineStr"/>
+      <c r="JZ16" t="inlineStr"/>
+      <c r="KA16" t="inlineStr"/>
+      <c r="KB16" t="inlineStr"/>
+      <c r="KC16" t="inlineStr"/>
+      <c r="KD16" t="inlineStr"/>
+      <c r="KE16" t="inlineStr"/>
+      <c r="KF16" t="inlineStr"/>
+      <c r="KG16" t="inlineStr"/>
+      <c r="KH16" t="inlineStr"/>
+      <c r="KI16" t="inlineStr"/>
+      <c r="KJ16" t="inlineStr"/>
+      <c r="KK16" t="inlineStr"/>
+      <c r="KL16" t="inlineStr"/>
+      <c r="KM16" t="inlineStr"/>
+      <c r="KN16" t="inlineStr"/>
+      <c r="KO16" t="inlineStr"/>
+      <c r="KP16" t="inlineStr"/>
+      <c r="KQ16" t="inlineStr"/>
+      <c r="KR16" t="inlineStr"/>
+      <c r="KS16" t="inlineStr"/>
+      <c r="KT16" t="inlineStr"/>
+      <c r="KU16" t="inlineStr"/>
+      <c r="KV16" t="inlineStr"/>
+      <c r="KW16" t="inlineStr"/>
+      <c r="KX16" t="inlineStr"/>
+      <c r="KY16" t="inlineStr"/>
+      <c r="KZ16" t="inlineStr"/>
+      <c r="LA16" t="inlineStr"/>
+      <c r="LB16" t="inlineStr"/>
+      <c r="LC16" t="inlineStr"/>
+      <c r="LD16" t="inlineStr"/>
+      <c r="LE16" t="inlineStr"/>
+      <c r="LF16" t="inlineStr"/>
+      <c r="LG16" t="inlineStr"/>
+      <c r="LH16" t="inlineStr"/>
+      <c r="LI16" t="inlineStr"/>
+      <c r="LJ16" t="inlineStr"/>
+      <c r="LK16" t="inlineStr"/>
+      <c r="LL16" t="inlineStr"/>
+      <c r="LM16" t="inlineStr"/>
+      <c r="LN16" t="inlineStr"/>
+      <c r="LO16" t="inlineStr"/>
+      <c r="LP16" t="inlineStr"/>
+      <c r="LQ16" t="inlineStr"/>
+      <c r="LR16" t="inlineStr"/>
+      <c r="LS16" t="inlineStr"/>
+      <c r="LT16" t="inlineStr"/>
+      <c r="LU16" t="inlineStr"/>
+      <c r="LV16" t="inlineStr"/>
+      <c r="LW16" t="inlineStr"/>
+      <c r="LX16" t="inlineStr"/>
+      <c r="LY16" t="inlineStr"/>
+      <c r="LZ16" t="inlineStr"/>
+      <c r="MA16" t="inlineStr"/>
+      <c r="MB16" t="inlineStr"/>
+      <c r="MC16" t="inlineStr"/>
+      <c r="MD16" t="inlineStr"/>
+      <c r="ME16" t="inlineStr"/>
+      <c r="MF16" t="inlineStr"/>
+      <c r="MG16" t="inlineStr"/>
+      <c r="MH16" t="inlineStr"/>
+      <c r="MI16" t="inlineStr"/>
+      <c r="MJ16" t="inlineStr"/>
+      <c r="MK16" t="inlineStr"/>
+      <c r="ML16" t="inlineStr"/>
+      <c r="MM16" t="inlineStr"/>
+      <c r="MN16" t="inlineStr"/>
+      <c r="MO16" t="inlineStr"/>
+      <c r="MP16" t="inlineStr"/>
+      <c r="MQ16" t="inlineStr"/>
+      <c r="MR16" t="inlineStr"/>
+      <c r="MS16" t="inlineStr"/>
+      <c r="MT16" t="inlineStr"/>
+      <c r="MU16" t="inlineStr"/>
+      <c r="MV16" t="inlineStr"/>
+      <c r="MW16" t="inlineStr"/>
+      <c r="MX16" t="inlineStr"/>
+      <c r="MY16" t="inlineStr"/>
+      <c r="MZ16" t="inlineStr"/>
+      <c r="NA16" t="inlineStr"/>
+      <c r="NB16" t="inlineStr"/>
+      <c r="NC16" t="inlineStr"/>
+      <c r="ND16" t="inlineStr"/>
+      <c r="NE16" t="inlineStr"/>
+      <c r="NF16" t="inlineStr"/>
+      <c r="NG16" t="inlineStr"/>
+      <c r="NH16" t="inlineStr"/>
+      <c r="NI16" t="inlineStr"/>
+      <c r="NJ16" t="inlineStr"/>
+      <c r="NK16" t="inlineStr"/>
+      <c r="NL16" t="inlineStr"/>
+      <c r="NM16" t="inlineStr"/>
+      <c r="NN16" t="inlineStr"/>
+      <c r="NO16" t="inlineStr"/>
+      <c r="NP16" t="inlineStr"/>
+      <c r="NQ16" t="inlineStr"/>
+      <c r="NR16" t="inlineStr"/>
+      <c r="NS16" t="inlineStr"/>
+      <c r="NT16" t="inlineStr"/>
+      <c r="NU16" t="inlineStr"/>
+      <c r="NV16" t="inlineStr"/>
+      <c r="NW16" t="inlineStr"/>
+      <c r="NX16" t="inlineStr"/>
+      <c r="NY16" t="inlineStr"/>
+      <c r="NZ16" t="inlineStr"/>
+      <c r="OA16" t="inlineStr"/>
+      <c r="OB16" t="inlineStr"/>
+      <c r="OC16" t="inlineStr"/>
+      <c r="OD16" t="inlineStr"/>
+      <c r="OE16" t="inlineStr"/>
+      <c r="OF16" t="inlineStr"/>
+      <c r="OG16" t="inlineStr"/>
+      <c r="OH16" t="inlineStr"/>
+      <c r="OI16" t="inlineStr"/>
+      <c r="OJ16" t="inlineStr"/>
+      <c r="OK16" t="inlineStr"/>
+      <c r="OL16" t="inlineStr"/>
+      <c r="OM16" t="inlineStr"/>
+      <c r="ON16" t="inlineStr"/>
+      <c r="OO16" t="inlineStr"/>
+      <c r="OP16" t="inlineStr"/>
+      <c r="OQ16" t="inlineStr"/>
+      <c r="OR16" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
c: result txt result 1 0 "
</commit_message>
<xml_diff>
--- a/OOMII.xlsx
+++ b/OOMII.xlsx
@@ -346,7 +346,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:OR16"/>
+  <dimension ref="A1:OR18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9570,12 +9570,6 @@
           <t>type01</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr">
         <is>
           <t>0.0625</t>
@@ -9606,9 +9600,6 @@
           <t>25.0</t>
         </is>
       </c>
-      <c r="N16" t="inlineStr"/>
-      <c r="O16" t="inlineStr"/>
-      <c r="P16" t="inlineStr"/>
       <c r="Q16" t="inlineStr">
         <is>
           <t>3.22</t>
@@ -9619,7 +9610,6 @@
           <t>3.03</t>
         </is>
       </c>
-      <c r="S16" t="inlineStr"/>
       <c r="T16" t="inlineStr">
         <is>
           <t>3.00</t>
@@ -9650,23 +9640,11 @@
           <t>2.75</t>
         </is>
       </c>
-      <c r="Z16" t="inlineStr"/>
-      <c r="AA16" t="inlineStr"/>
-      <c r="AB16" t="inlineStr"/>
-      <c r="AC16" t="inlineStr"/>
-      <c r="AD16" t="inlineStr"/>
-      <c r="AE16" t="inlineStr"/>
-      <c r="AF16" t="inlineStr"/>
-      <c r="AG16" t="inlineStr"/>
-      <c r="AH16" t="inlineStr"/>
-      <c r="AI16" t="inlineStr"/>
-      <c r="AJ16" t="inlineStr"/>
       <c r="AK16" t="inlineStr">
         <is>
           <t>94</t>
         </is>
       </c>
-      <c r="AL16" t="inlineStr"/>
       <c r="AM16" t="inlineStr">
         <is>
           <t>93</t>
@@ -9697,10 +9675,6 @@
           <t>35</t>
         </is>
       </c>
-      <c r="AS16" t="inlineStr"/>
-      <c r="AT16" t="inlineStr"/>
-      <c r="AU16" t="inlineStr"/>
-      <c r="AV16" t="inlineStr"/>
       <c r="AW16" t="inlineStr">
         <is>
           <t>-1</t>
@@ -9731,18 +9705,6 @@
           <t>-9</t>
         </is>
       </c>
-      <c r="BC16" t="inlineStr"/>
-      <c r="BD16" t="inlineStr"/>
-      <c r="BE16" t="inlineStr"/>
-      <c r="BF16" t="inlineStr"/>
-      <c r="BG16" t="inlineStr"/>
-      <c r="BH16" t="inlineStr"/>
-      <c r="BI16" t="inlineStr"/>
-      <c r="BJ16" t="inlineStr"/>
-      <c r="BK16" t="inlineStr"/>
-      <c r="BL16" t="inlineStr"/>
-      <c r="BM16" t="inlineStr"/>
-      <c r="BN16" t="inlineStr"/>
       <c r="BO16" t="inlineStr">
         <is>
           <t>0.0625</t>
@@ -9773,9 +9735,6 @@
           <t>25.0</t>
         </is>
       </c>
-      <c r="BU16" t="inlineStr"/>
-      <c r="BV16" t="inlineStr"/>
-      <c r="BW16" t="inlineStr"/>
       <c r="BX16" t="inlineStr">
         <is>
           <t>2.51</t>
@@ -9786,7 +9745,6 @@
           <t>2.20</t>
         </is>
       </c>
-      <c r="BZ16" t="inlineStr"/>
       <c r="CA16" t="inlineStr">
         <is>
           <t>2.23</t>
@@ -9817,23 +9775,11 @@
           <t>1.99</t>
         </is>
       </c>
-      <c r="CG16" t="inlineStr"/>
-      <c r="CH16" t="inlineStr"/>
-      <c r="CI16" t="inlineStr"/>
-      <c r="CJ16" t="inlineStr"/>
-      <c r="CK16" t="inlineStr"/>
-      <c r="CL16" t="inlineStr"/>
-      <c r="CM16" t="inlineStr"/>
-      <c r="CN16" t="inlineStr"/>
-      <c r="CO16" t="inlineStr"/>
-      <c r="CP16" t="inlineStr"/>
-      <c r="CQ16" t="inlineStr"/>
       <c r="CR16" t="inlineStr">
         <is>
           <t>91</t>
         </is>
       </c>
-      <c r="CS16" t="inlineStr"/>
       <c r="CT16" t="inlineStr">
         <is>
           <t>39</t>
@@ -9864,10 +9810,6 @@
           <t>79</t>
         </is>
       </c>
-      <c r="CZ16" t="inlineStr"/>
-      <c r="DA16" t="inlineStr"/>
-      <c r="DB16" t="inlineStr"/>
-      <c r="DC16" t="inlineStr"/>
       <c r="DD16" t="inlineStr">
         <is>
           <t>-2</t>
@@ -9898,36 +9840,11 @@
           <t>-13</t>
         </is>
       </c>
-      <c r="DJ16" t="inlineStr"/>
-      <c r="DK16" t="inlineStr"/>
-      <c r="DL16" t="inlineStr"/>
-      <c r="DM16" t="inlineStr"/>
-      <c r="DN16" t="inlineStr"/>
-      <c r="DO16" t="inlineStr"/>
       <c r="DP16" t="inlineStr">
         <is>
           <t>220</t>
         </is>
       </c>
-      <c r="DQ16" t="inlineStr"/>
-      <c r="DR16" t="inlineStr"/>
-      <c r="DS16" t="inlineStr"/>
-      <c r="DT16" t="inlineStr"/>
-      <c r="DU16" t="inlineStr"/>
-      <c r="DV16" t="inlineStr"/>
-      <c r="DW16" t="inlineStr"/>
-      <c r="DX16" t="inlineStr"/>
-      <c r="DY16" t="inlineStr"/>
-      <c r="DZ16" t="inlineStr"/>
-      <c r="EA16" t="inlineStr"/>
-      <c r="EB16" t="inlineStr"/>
-      <c r="EC16" t="inlineStr"/>
-      <c r="ED16" t="inlineStr"/>
-      <c r="EE16" t="inlineStr"/>
-      <c r="EF16" t="inlineStr"/>
-      <c r="EG16" t="inlineStr"/>
-      <c r="EH16" t="inlineStr"/>
-      <c r="EI16" t="inlineStr"/>
       <c r="EJ16" t="inlineStr">
         <is>
           <t>2.57</t>
@@ -9958,16 +9875,11 @@
           <t>1.69</t>
         </is>
       </c>
-      <c r="EP16" t="inlineStr"/>
-      <c r="EQ16" t="inlineStr"/>
-      <c r="ER16" t="inlineStr"/>
-      <c r="ES16" t="inlineStr"/>
       <c r="ET16" t="inlineStr">
         <is>
           <t>68</t>
         </is>
       </c>
-      <c r="EU16" t="inlineStr"/>
       <c r="EV16" t="inlineStr">
         <is>
           <t>55</t>
@@ -9998,29 +9910,6 @@
           <t>51</t>
         </is>
       </c>
-      <c r="FB16" t="inlineStr"/>
-      <c r="FC16" t="inlineStr"/>
-      <c r="FD16" t="inlineStr"/>
-      <c r="FE16" t="inlineStr"/>
-      <c r="FF16" t="inlineStr"/>
-      <c r="FG16" t="inlineStr"/>
-      <c r="FH16" t="inlineStr"/>
-      <c r="FI16" t="inlineStr"/>
-      <c r="FJ16" t="inlineStr"/>
-      <c r="FK16" t="inlineStr"/>
-      <c r="FL16" t="inlineStr"/>
-      <c r="FM16" t="inlineStr"/>
-      <c r="FN16" t="inlineStr"/>
-      <c r="FO16" t="inlineStr"/>
-      <c r="FP16" t="inlineStr"/>
-      <c r="FQ16" t="inlineStr"/>
-      <c r="FR16" t="inlineStr"/>
-      <c r="FS16" t="inlineStr"/>
-      <c r="FT16" t="inlineStr"/>
-      <c r="FU16" t="inlineStr"/>
-      <c r="FV16" t="inlineStr"/>
-      <c r="FW16" t="inlineStr"/>
-      <c r="FX16" t="inlineStr"/>
       <c r="FY16" t="inlineStr">
         <is>
           <t>-4</t>
@@ -10051,51 +9940,6 @@
           <t>-24</t>
         </is>
       </c>
-      <c r="GE16" t="inlineStr"/>
-      <c r="GF16" t="inlineStr"/>
-      <c r="GG16" t="inlineStr"/>
-      <c r="GH16" t="inlineStr"/>
-      <c r="GI16" t="inlineStr"/>
-      <c r="GJ16" t="inlineStr"/>
-      <c r="GK16" t="inlineStr"/>
-      <c r="GL16" t="inlineStr"/>
-      <c r="GM16" t="inlineStr"/>
-      <c r="GN16" t="inlineStr"/>
-      <c r="GO16" t="inlineStr"/>
-      <c r="GP16" t="inlineStr"/>
-      <c r="GQ16" t="inlineStr"/>
-      <c r="GR16" t="inlineStr"/>
-      <c r="GS16" t="inlineStr"/>
-      <c r="GT16" t="inlineStr"/>
-      <c r="GU16" t="inlineStr"/>
-      <c r="GV16" t="inlineStr"/>
-      <c r="GW16" t="inlineStr"/>
-      <c r="GX16" t="inlineStr"/>
-      <c r="GY16" t="inlineStr"/>
-      <c r="GZ16" t="inlineStr"/>
-      <c r="HA16" t="inlineStr"/>
-      <c r="HB16" t="inlineStr"/>
-      <c r="HC16" t="inlineStr"/>
-      <c r="HD16" t="inlineStr"/>
-      <c r="HE16" t="inlineStr"/>
-      <c r="HF16" t="inlineStr"/>
-      <c r="HG16" t="inlineStr"/>
-      <c r="HH16" t="inlineStr"/>
-      <c r="HI16" t="inlineStr"/>
-      <c r="HJ16" t="inlineStr"/>
-      <c r="HK16" t="inlineStr"/>
-      <c r="HL16" t="inlineStr"/>
-      <c r="HM16" t="inlineStr"/>
-      <c r="HN16" t="inlineStr"/>
-      <c r="HO16" t="inlineStr"/>
-      <c r="HP16" t="inlineStr"/>
-      <c r="HQ16" t="inlineStr"/>
-      <c r="HR16" t="inlineStr"/>
-      <c r="HS16" t="inlineStr"/>
-      <c r="HT16" t="inlineStr"/>
-      <c r="HU16" t="inlineStr"/>
-      <c r="HV16" t="inlineStr"/>
-      <c r="HW16" t="inlineStr"/>
       <c r="HX16" t="inlineStr">
         <is>
           <t>0.0625</t>
@@ -10126,9 +9970,6 @@
           <t>25.0</t>
         </is>
       </c>
-      <c r="ID16" t="inlineStr"/>
-      <c r="IE16" t="inlineStr"/>
-      <c r="IF16" t="inlineStr"/>
       <c r="IG16" t="inlineStr">
         <is>
           <t>5.45</t>
@@ -10139,7 +9980,6 @@
           <t>9.33</t>
         </is>
       </c>
-      <c r="II16" t="inlineStr"/>
       <c r="IJ16" t="inlineStr">
         <is>
           <t>7.32</t>
@@ -10170,23 +10010,11 @@
           <t>7.31</t>
         </is>
       </c>
-      <c r="IP16" t="inlineStr"/>
-      <c r="IQ16" t="inlineStr"/>
-      <c r="IR16" t="inlineStr"/>
-      <c r="IS16" t="inlineStr"/>
-      <c r="IT16" t="inlineStr"/>
-      <c r="IU16" t="inlineStr"/>
-      <c r="IV16" t="inlineStr"/>
-      <c r="IW16" t="inlineStr"/>
-      <c r="IX16" t="inlineStr"/>
-      <c r="IY16" t="inlineStr"/>
-      <c r="IZ16" t="inlineStr"/>
       <c r="JA16" t="inlineStr">
         <is>
           <t>153</t>
         </is>
       </c>
-      <c r="JB16" t="inlineStr"/>
       <c r="JC16" t="inlineStr">
         <is>
           <t>143</t>
@@ -10217,10 +10045,6 @@
           <t>134</t>
         </is>
       </c>
-      <c r="JI16" t="inlineStr"/>
-      <c r="JJ16" t="inlineStr"/>
-      <c r="JK16" t="inlineStr"/>
-      <c r="JL16" t="inlineStr"/>
       <c r="JM16" t="inlineStr">
         <is>
           <t>-9</t>
@@ -10251,136 +10075,1336 @@
           <t>-15</t>
         </is>
       </c>
-      <c r="JS16" t="inlineStr"/>
-      <c r="JT16" t="inlineStr"/>
-      <c r="JU16" t="inlineStr"/>
-      <c r="JV16" t="inlineStr"/>
-      <c r="JW16" t="inlineStr"/>
-      <c r="JX16" t="inlineStr"/>
-      <c r="JY16" t="inlineStr"/>
-      <c r="JZ16" t="inlineStr"/>
-      <c r="KA16" t="inlineStr"/>
-      <c r="KB16" t="inlineStr"/>
-      <c r="KC16" t="inlineStr"/>
-      <c r="KD16" t="inlineStr"/>
-      <c r="KE16" t="inlineStr"/>
-      <c r="KF16" t="inlineStr"/>
-      <c r="KG16" t="inlineStr"/>
-      <c r="KH16" t="inlineStr"/>
-      <c r="KI16" t="inlineStr"/>
-      <c r="KJ16" t="inlineStr"/>
-      <c r="KK16" t="inlineStr"/>
-      <c r="KL16" t="inlineStr"/>
-      <c r="KM16" t="inlineStr"/>
-      <c r="KN16" t="inlineStr"/>
-      <c r="KO16" t="inlineStr"/>
-      <c r="KP16" t="inlineStr"/>
-      <c r="KQ16" t="inlineStr"/>
-      <c r="KR16" t="inlineStr"/>
-      <c r="KS16" t="inlineStr"/>
-      <c r="KT16" t="inlineStr"/>
-      <c r="KU16" t="inlineStr"/>
-      <c r="KV16" t="inlineStr"/>
-      <c r="KW16" t="inlineStr"/>
-      <c r="KX16" t="inlineStr"/>
-      <c r="KY16" t="inlineStr"/>
-      <c r="KZ16" t="inlineStr"/>
-      <c r="LA16" t="inlineStr"/>
-      <c r="LB16" t="inlineStr"/>
-      <c r="LC16" t="inlineStr"/>
-      <c r="LD16" t="inlineStr"/>
-      <c r="LE16" t="inlineStr"/>
-      <c r="LF16" t="inlineStr"/>
-      <c r="LG16" t="inlineStr"/>
-      <c r="LH16" t="inlineStr"/>
-      <c r="LI16" t="inlineStr"/>
-      <c r="LJ16" t="inlineStr"/>
-      <c r="LK16" t="inlineStr"/>
-      <c r="LL16" t="inlineStr"/>
-      <c r="LM16" t="inlineStr"/>
-      <c r="LN16" t="inlineStr"/>
-      <c r="LO16" t="inlineStr"/>
-      <c r="LP16" t="inlineStr"/>
-      <c r="LQ16" t="inlineStr"/>
-      <c r="LR16" t="inlineStr"/>
-      <c r="LS16" t="inlineStr"/>
-      <c r="LT16" t="inlineStr"/>
-      <c r="LU16" t="inlineStr"/>
-      <c r="LV16" t="inlineStr"/>
-      <c r="LW16" t="inlineStr"/>
-      <c r="LX16" t="inlineStr"/>
-      <c r="LY16" t="inlineStr"/>
-      <c r="LZ16" t="inlineStr"/>
-      <c r="MA16" t="inlineStr"/>
-      <c r="MB16" t="inlineStr"/>
-      <c r="MC16" t="inlineStr"/>
-      <c r="MD16" t="inlineStr"/>
-      <c r="ME16" t="inlineStr"/>
-      <c r="MF16" t="inlineStr"/>
-      <c r="MG16" t="inlineStr"/>
-      <c r="MH16" t="inlineStr"/>
-      <c r="MI16" t="inlineStr"/>
-      <c r="MJ16" t="inlineStr"/>
-      <c r="MK16" t="inlineStr"/>
-      <c r="ML16" t="inlineStr"/>
-      <c r="MM16" t="inlineStr"/>
-      <c r="MN16" t="inlineStr"/>
-      <c r="MO16" t="inlineStr"/>
-      <c r="MP16" t="inlineStr"/>
-      <c r="MQ16" t="inlineStr"/>
-      <c r="MR16" t="inlineStr"/>
-      <c r="MS16" t="inlineStr"/>
-      <c r="MT16" t="inlineStr"/>
-      <c r="MU16" t="inlineStr"/>
-      <c r="MV16" t="inlineStr"/>
-      <c r="MW16" t="inlineStr"/>
-      <c r="MX16" t="inlineStr"/>
-      <c r="MY16" t="inlineStr"/>
-      <c r="MZ16" t="inlineStr"/>
-      <c r="NA16" t="inlineStr"/>
-      <c r="NB16" t="inlineStr"/>
-      <c r="NC16" t="inlineStr"/>
-      <c r="ND16" t="inlineStr"/>
-      <c r="NE16" t="inlineStr"/>
-      <c r="NF16" t="inlineStr"/>
-      <c r="NG16" t="inlineStr"/>
-      <c r="NH16" t="inlineStr"/>
-      <c r="NI16" t="inlineStr"/>
-      <c r="NJ16" t="inlineStr"/>
-      <c r="NK16" t="inlineStr"/>
-      <c r="NL16" t="inlineStr"/>
-      <c r="NM16" t="inlineStr"/>
-      <c r="NN16" t="inlineStr"/>
-      <c r="NO16" t="inlineStr"/>
-      <c r="NP16" t="inlineStr"/>
-      <c r="NQ16" t="inlineStr"/>
-      <c r="NR16" t="inlineStr"/>
-      <c r="NS16" t="inlineStr"/>
-      <c r="NT16" t="inlineStr"/>
-      <c r="NU16" t="inlineStr"/>
-      <c r="NV16" t="inlineStr"/>
-      <c r="NW16" t="inlineStr"/>
-      <c r="NX16" t="inlineStr"/>
-      <c r="NY16" t="inlineStr"/>
-      <c r="NZ16" t="inlineStr"/>
-      <c r="OA16" t="inlineStr"/>
-      <c r="OB16" t="inlineStr"/>
-      <c r="OC16" t="inlineStr"/>
-      <c r="OD16" t="inlineStr"/>
-      <c r="OE16" t="inlineStr"/>
-      <c r="OF16" t="inlineStr"/>
-      <c r="OG16" t="inlineStr"/>
-      <c r="OH16" t="inlineStr"/>
-      <c r="OI16" t="inlineStr"/>
-      <c r="OJ16" t="inlineStr"/>
-      <c r="OK16" t="inlineStr"/>
-      <c r="OL16" t="inlineStr"/>
-      <c r="OM16" t="inlineStr"/>
-      <c r="ON16" t="inlineStr"/>
-      <c r="OO16" t="inlineStr"/>
-      <c r="OP16" t="inlineStr"/>
-      <c r="OQ16" t="inlineStr"/>
-      <c r="OR16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>type01</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>16.0</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>3.22</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>3.03</t>
+        </is>
+      </c>
+      <c r="T17" t="inlineStr">
+        <is>
+          <t>3.00</t>
+        </is>
+      </c>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>2.97</t>
+        </is>
+      </c>
+      <c r="V17" t="inlineStr">
+        <is>
+          <t>3.01</t>
+        </is>
+      </c>
+      <c r="W17" t="inlineStr">
+        <is>
+          <t>2.93</t>
+        </is>
+      </c>
+      <c r="X17" t="inlineStr">
+        <is>
+          <t>2.31</t>
+        </is>
+      </c>
+      <c r="Y17" t="inlineStr">
+        <is>
+          <t>2.75</t>
+        </is>
+      </c>
+      <c r="AK17" t="inlineStr">
+        <is>
+          <t>94</t>
+        </is>
+      </c>
+      <c r="AM17" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="AN17" t="inlineStr">
+        <is>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="AO17" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="AP17" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="AQ17" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="AR17" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="AW17" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="AX17" t="inlineStr">
+        <is>
+          <t>-2</t>
+        </is>
+      </c>
+      <c r="AY17" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="AZ17" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="BA17" t="inlineStr">
+        <is>
+          <t>-7</t>
+        </is>
+      </c>
+      <c r="BB17" t="inlineStr">
+        <is>
+          <t>-9</t>
+        </is>
+      </c>
+      <c r="BO17" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="BP17" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="BQ17" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="BR17" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="BS17" t="inlineStr">
+        <is>
+          <t>15.0</t>
+        </is>
+      </c>
+      <c r="BT17" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="BX17" t="inlineStr">
+        <is>
+          <t>2.51</t>
+        </is>
+      </c>
+      <c r="BY17" t="inlineStr">
+        <is>
+          <t>2.20</t>
+        </is>
+      </c>
+      <c r="CA17" t="inlineStr">
+        <is>
+          <t>2.23</t>
+        </is>
+      </c>
+      <c r="CB17" t="inlineStr">
+        <is>
+          <t>2.25</t>
+        </is>
+      </c>
+      <c r="CC17" t="inlineStr">
+        <is>
+          <t>2.27</t>
+        </is>
+      </c>
+      <c r="CD17" t="inlineStr">
+        <is>
+          <t>2.20</t>
+        </is>
+      </c>
+      <c r="CE17" t="inlineStr">
+        <is>
+          <t>2.10</t>
+        </is>
+      </c>
+      <c r="CF17" t="inlineStr">
+        <is>
+          <t>1.99</t>
+        </is>
+      </c>
+      <c r="CR17" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="CT17" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="CU17" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="CV17" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="CW17" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="CX17" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="CY17" t="inlineStr">
+        <is>
+          <t>79</t>
+        </is>
+      </c>
+      <c r="DD17" t="inlineStr">
+        <is>
+          <t>-2</t>
+        </is>
+      </c>
+      <c r="DE17" t="inlineStr">
+        <is>
+          <t>-2</t>
+        </is>
+      </c>
+      <c r="DF17" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="DG17" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="DH17" t="inlineStr">
+        <is>
+          <t>-3</t>
+        </is>
+      </c>
+      <c r="DI17" t="inlineStr">
+        <is>
+          <t>-13</t>
+        </is>
+      </c>
+      <c r="DP17" t="inlineStr">
+        <is>
+          <t>220</t>
+        </is>
+      </c>
+      <c r="EJ17" t="inlineStr">
+        <is>
+          <t>2.57</t>
+        </is>
+      </c>
+      <c r="EK17" t="inlineStr">
+        <is>
+          <t>1.75</t>
+        </is>
+      </c>
+      <c r="EL17" t="inlineStr">
+        <is>
+          <t>1.67</t>
+        </is>
+      </c>
+      <c r="EM17" t="inlineStr">
+        <is>
+          <t>1.69</t>
+        </is>
+      </c>
+      <c r="EN17" t="inlineStr">
+        <is>
+          <t>1.73</t>
+        </is>
+      </c>
+      <c r="EO17" t="inlineStr">
+        <is>
+          <t>1.69</t>
+        </is>
+      </c>
+      <c r="ET17" t="inlineStr">
+        <is>
+          <t>68</t>
+        </is>
+      </c>
+      <c r="EV17" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="EW17" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="EX17" t="inlineStr">
+        <is>
+          <t>63</t>
+        </is>
+      </c>
+      <c r="EY17" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="EZ17" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="FA17" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="FY17" t="inlineStr">
+        <is>
+          <t>-4</t>
+        </is>
+      </c>
+      <c r="FZ17" t="inlineStr">
+        <is>
+          <t>-3</t>
+        </is>
+      </c>
+      <c r="GA17" t="inlineStr">
+        <is>
+          <t>-0</t>
+        </is>
+      </c>
+      <c r="GB17" t="inlineStr">
+        <is>
+          <t>-3</t>
+        </is>
+      </c>
+      <c r="GC17" t="inlineStr">
+        <is>
+          <t>-11</t>
+        </is>
+      </c>
+      <c r="GD17" t="inlineStr">
+        <is>
+          <t>-24</t>
+        </is>
+      </c>
+      <c r="HX17" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="HY17" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="HZ17" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="IA17" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="IB17" t="inlineStr">
+        <is>
+          <t>16.0</t>
+        </is>
+      </c>
+      <c r="IC17" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="IG17" t="inlineStr">
+        <is>
+          <t>5.45</t>
+        </is>
+      </c>
+      <c r="IH17" t="inlineStr">
+        <is>
+          <t>9.33</t>
+        </is>
+      </c>
+      <c r="IJ17" t="inlineStr">
+        <is>
+          <t>7.32</t>
+        </is>
+      </c>
+      <c r="IK17" t="inlineStr">
+        <is>
+          <t>0.47</t>
+        </is>
+      </c>
+      <c r="IL17" t="inlineStr">
+        <is>
+          <t>7.99</t>
+        </is>
+      </c>
+      <c r="IM17" t="inlineStr">
+        <is>
+          <t>7.64</t>
+        </is>
+      </c>
+      <c r="IN17" t="inlineStr">
+        <is>
+          <t>3.12</t>
+        </is>
+      </c>
+      <c r="IO17" t="inlineStr">
+        <is>
+          <t>7.31</t>
+        </is>
+      </c>
+      <c r="JA17" t="inlineStr">
+        <is>
+          <t>153</t>
+        </is>
+      </c>
+      <c r="JC17" t="inlineStr">
+        <is>
+          <t>143</t>
+        </is>
+      </c>
+      <c r="JD17" t="inlineStr">
+        <is>
+          <t>155</t>
+        </is>
+      </c>
+      <c r="JE17" t="inlineStr">
+        <is>
+          <t>147</t>
+        </is>
+      </c>
+      <c r="JF17" t="inlineStr">
+        <is>
+          <t>140</t>
+        </is>
+      </c>
+      <c r="JG17" t="inlineStr">
+        <is>
+          <t>149</t>
+        </is>
+      </c>
+      <c r="JH17" t="inlineStr">
+        <is>
+          <t>134</t>
+        </is>
+      </c>
+      <c r="JM17" t="inlineStr">
+        <is>
+          <t>-9</t>
+        </is>
+      </c>
+      <c r="JN17" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="JO17" t="inlineStr">
+        <is>
+          <t>-7</t>
+        </is>
+      </c>
+      <c r="JP17" t="inlineStr">
+        <is>
+          <t>-11</t>
+        </is>
+      </c>
+      <c r="JQ17" t="inlineStr">
+        <is>
+          <t>-5</t>
+        </is>
+      </c>
+      <c r="JR17" t="inlineStr">
+        <is>
+          <t>-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>type01</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>16.0</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr"/>
+      <c r="O18" t="inlineStr"/>
+      <c r="P18" t="inlineStr"/>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>3.22</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>3.03</t>
+        </is>
+      </c>
+      <c r="S18" t="inlineStr"/>
+      <c r="T18" t="inlineStr">
+        <is>
+          <t>3.00</t>
+        </is>
+      </c>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>2.97</t>
+        </is>
+      </c>
+      <c r="V18" t="inlineStr">
+        <is>
+          <t>3.01</t>
+        </is>
+      </c>
+      <c r="W18" t="inlineStr">
+        <is>
+          <t>2.93</t>
+        </is>
+      </c>
+      <c r="X18" t="inlineStr">
+        <is>
+          <t>2.31</t>
+        </is>
+      </c>
+      <c r="Y18" t="inlineStr">
+        <is>
+          <t>2.75</t>
+        </is>
+      </c>
+      <c r="Z18" t="inlineStr"/>
+      <c r="AA18" t="inlineStr"/>
+      <c r="AB18" t="inlineStr"/>
+      <c r="AC18" t="inlineStr"/>
+      <c r="AD18" t="inlineStr"/>
+      <c r="AE18" t="inlineStr"/>
+      <c r="AF18" t="inlineStr"/>
+      <c r="AG18" t="inlineStr"/>
+      <c r="AH18" t="inlineStr"/>
+      <c r="AI18" t="inlineStr"/>
+      <c r="AJ18" t="inlineStr"/>
+      <c r="AK18" t="inlineStr">
+        <is>
+          <t>94</t>
+        </is>
+      </c>
+      <c r="AL18" t="inlineStr"/>
+      <c r="AM18" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="AN18" t="inlineStr">
+        <is>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="AO18" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="AP18" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="AQ18" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="AR18" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="AS18" t="inlineStr"/>
+      <c r="AT18" t="inlineStr"/>
+      <c r="AU18" t="inlineStr"/>
+      <c r="AV18" t="inlineStr"/>
+      <c r="AW18" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="AX18" t="inlineStr">
+        <is>
+          <t>-2</t>
+        </is>
+      </c>
+      <c r="AY18" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="AZ18" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="BA18" t="inlineStr">
+        <is>
+          <t>-7</t>
+        </is>
+      </c>
+      <c r="BB18" t="inlineStr">
+        <is>
+          <t>-9</t>
+        </is>
+      </c>
+      <c r="BC18" t="inlineStr"/>
+      <c r="BD18" t="inlineStr"/>
+      <c r="BE18" t="inlineStr"/>
+      <c r="BF18" t="inlineStr"/>
+      <c r="BG18" t="inlineStr"/>
+      <c r="BH18" t="inlineStr"/>
+      <c r="BI18" t="inlineStr"/>
+      <c r="BJ18" t="inlineStr"/>
+      <c r="BK18" t="inlineStr"/>
+      <c r="BL18" t="inlineStr"/>
+      <c r="BM18" t="inlineStr"/>
+      <c r="BN18" t="inlineStr"/>
+      <c r="BO18" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="BP18" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="BQ18" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="BR18" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="BS18" t="inlineStr">
+        <is>
+          <t>15.0</t>
+        </is>
+      </c>
+      <c r="BT18" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="BU18" t="inlineStr"/>
+      <c r="BV18" t="inlineStr"/>
+      <c r="BW18" t="inlineStr"/>
+      <c r="BX18" t="inlineStr">
+        <is>
+          <t>2.51</t>
+        </is>
+      </c>
+      <c r="BY18" t="inlineStr">
+        <is>
+          <t>2.20</t>
+        </is>
+      </c>
+      <c r="BZ18" t="inlineStr"/>
+      <c r="CA18" t="inlineStr">
+        <is>
+          <t>2.23</t>
+        </is>
+      </c>
+      <c r="CB18" t="inlineStr">
+        <is>
+          <t>2.25</t>
+        </is>
+      </c>
+      <c r="CC18" t="inlineStr">
+        <is>
+          <t>2.27</t>
+        </is>
+      </c>
+      <c r="CD18" t="inlineStr">
+        <is>
+          <t>2.20</t>
+        </is>
+      </c>
+      <c r="CE18" t="inlineStr">
+        <is>
+          <t>2.10</t>
+        </is>
+      </c>
+      <c r="CF18" t="inlineStr">
+        <is>
+          <t>1.99</t>
+        </is>
+      </c>
+      <c r="CG18" t="inlineStr"/>
+      <c r="CH18" t="inlineStr"/>
+      <c r="CI18" t="inlineStr"/>
+      <c r="CJ18" t="inlineStr"/>
+      <c r="CK18" t="inlineStr"/>
+      <c r="CL18" t="inlineStr"/>
+      <c r="CM18" t="inlineStr"/>
+      <c r="CN18" t="inlineStr"/>
+      <c r="CO18" t="inlineStr"/>
+      <c r="CP18" t="inlineStr"/>
+      <c r="CQ18" t="inlineStr"/>
+      <c r="CR18" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="CS18" t="inlineStr"/>
+      <c r="CT18" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="CU18" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="CV18" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="CW18" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="CX18" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="CY18" t="inlineStr">
+        <is>
+          <t>79</t>
+        </is>
+      </c>
+      <c r="CZ18" t="inlineStr"/>
+      <c r="DA18" t="inlineStr"/>
+      <c r="DB18" t="inlineStr"/>
+      <c r="DC18" t="inlineStr"/>
+      <c r="DD18" t="inlineStr">
+        <is>
+          <t>-2</t>
+        </is>
+      </c>
+      <c r="DE18" t="inlineStr">
+        <is>
+          <t>-2</t>
+        </is>
+      </c>
+      <c r="DF18" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="DG18" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="DH18" t="inlineStr">
+        <is>
+          <t>-3</t>
+        </is>
+      </c>
+      <c r="DI18" t="inlineStr">
+        <is>
+          <t>-13</t>
+        </is>
+      </c>
+      <c r="DJ18" t="inlineStr"/>
+      <c r="DK18" t="inlineStr"/>
+      <c r="DL18" t="inlineStr"/>
+      <c r="DM18" t="inlineStr"/>
+      <c r="DN18" t="inlineStr"/>
+      <c r="DO18" t="inlineStr"/>
+      <c r="DP18" t="inlineStr">
+        <is>
+          <t>220</t>
+        </is>
+      </c>
+      <c r="DQ18" t="inlineStr"/>
+      <c r="DR18" t="inlineStr"/>
+      <c r="DS18" t="inlineStr"/>
+      <c r="DT18" t="inlineStr"/>
+      <c r="DU18" t="inlineStr"/>
+      <c r="DV18" t="inlineStr"/>
+      <c r="DW18" t="inlineStr"/>
+      <c r="DX18" t="inlineStr"/>
+      <c r="DY18" t="inlineStr"/>
+      <c r="DZ18" t="inlineStr"/>
+      <c r="EA18" t="inlineStr"/>
+      <c r="EB18" t="inlineStr"/>
+      <c r="EC18" t="inlineStr"/>
+      <c r="ED18" t="inlineStr"/>
+      <c r="EE18" t="inlineStr"/>
+      <c r="EF18" t="inlineStr"/>
+      <c r="EG18" t="inlineStr"/>
+      <c r="EH18" t="inlineStr"/>
+      <c r="EI18" t="inlineStr"/>
+      <c r="EJ18" t="inlineStr">
+        <is>
+          <t>2.57</t>
+        </is>
+      </c>
+      <c r="EK18" t="inlineStr">
+        <is>
+          <t>1.75</t>
+        </is>
+      </c>
+      <c r="EL18" t="inlineStr">
+        <is>
+          <t>1.67</t>
+        </is>
+      </c>
+      <c r="EM18" t="inlineStr">
+        <is>
+          <t>1.69</t>
+        </is>
+      </c>
+      <c r="EN18" t="inlineStr">
+        <is>
+          <t>1.73</t>
+        </is>
+      </c>
+      <c r="EO18" t="inlineStr">
+        <is>
+          <t>1.69</t>
+        </is>
+      </c>
+      <c r="EP18" t="inlineStr"/>
+      <c r="EQ18" t="inlineStr"/>
+      <c r="ER18" t="inlineStr"/>
+      <c r="ES18" t="inlineStr"/>
+      <c r="ET18" t="inlineStr">
+        <is>
+          <t>68</t>
+        </is>
+      </c>
+      <c r="EU18" t="inlineStr"/>
+      <c r="EV18" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="EW18" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="EX18" t="inlineStr">
+        <is>
+          <t>63</t>
+        </is>
+      </c>
+      <c r="EY18" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="EZ18" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="FA18" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="FB18" t="inlineStr"/>
+      <c r="FC18" t="inlineStr"/>
+      <c r="FD18" t="inlineStr"/>
+      <c r="FE18" t="inlineStr"/>
+      <c r="FF18" t="inlineStr"/>
+      <c r="FG18" t="inlineStr"/>
+      <c r="FH18" t="inlineStr"/>
+      <c r="FI18" t="inlineStr"/>
+      <c r="FJ18" t="inlineStr"/>
+      <c r="FK18" t="inlineStr"/>
+      <c r="FL18" t="inlineStr"/>
+      <c r="FM18" t="inlineStr"/>
+      <c r="FN18" t="inlineStr"/>
+      <c r="FO18" t="inlineStr"/>
+      <c r="FP18" t="inlineStr"/>
+      <c r="FQ18" t="inlineStr"/>
+      <c r="FR18" t="inlineStr"/>
+      <c r="FS18" t="inlineStr"/>
+      <c r="FT18" t="inlineStr"/>
+      <c r="FU18" t="inlineStr"/>
+      <c r="FV18" t="inlineStr"/>
+      <c r="FW18" t="inlineStr"/>
+      <c r="FX18" t="inlineStr"/>
+      <c r="FY18" t="inlineStr">
+        <is>
+          <t>-4</t>
+        </is>
+      </c>
+      <c r="FZ18" t="inlineStr">
+        <is>
+          <t>-3</t>
+        </is>
+      </c>
+      <c r="GA18" t="inlineStr">
+        <is>
+          <t>-0</t>
+        </is>
+      </c>
+      <c r="GB18" t="inlineStr">
+        <is>
+          <t>-3</t>
+        </is>
+      </c>
+      <c r="GC18" t="inlineStr">
+        <is>
+          <t>-11</t>
+        </is>
+      </c>
+      <c r="GD18" t="inlineStr">
+        <is>
+          <t>-24</t>
+        </is>
+      </c>
+      <c r="GE18" t="inlineStr"/>
+      <c r="GF18" t="inlineStr"/>
+      <c r="GG18" t="inlineStr"/>
+      <c r="GH18" t="inlineStr"/>
+      <c r="GI18" t="inlineStr"/>
+      <c r="GJ18" t="inlineStr"/>
+      <c r="GK18" t="inlineStr"/>
+      <c r="GL18" t="inlineStr"/>
+      <c r="GM18" t="inlineStr"/>
+      <c r="GN18" t="inlineStr"/>
+      <c r="GO18" t="inlineStr"/>
+      <c r="GP18" t="inlineStr"/>
+      <c r="GQ18" t="inlineStr"/>
+      <c r="GR18" t="inlineStr"/>
+      <c r="GS18" t="inlineStr"/>
+      <c r="GT18" t="inlineStr"/>
+      <c r="GU18" t="inlineStr"/>
+      <c r="GV18" t="inlineStr"/>
+      <c r="GW18" t="inlineStr"/>
+      <c r="GX18" t="inlineStr"/>
+      <c r="GY18" t="inlineStr"/>
+      <c r="GZ18" t="inlineStr"/>
+      <c r="HA18" t="inlineStr"/>
+      <c r="HB18" t="inlineStr"/>
+      <c r="HC18" t="inlineStr"/>
+      <c r="HD18" t="inlineStr"/>
+      <c r="HE18" t="inlineStr"/>
+      <c r="HF18" t="inlineStr"/>
+      <c r="HG18" t="inlineStr"/>
+      <c r="HH18" t="inlineStr"/>
+      <c r="HI18" t="inlineStr"/>
+      <c r="HJ18" t="inlineStr"/>
+      <c r="HK18" t="inlineStr"/>
+      <c r="HL18" t="inlineStr"/>
+      <c r="HM18" t="inlineStr"/>
+      <c r="HN18" t="inlineStr"/>
+      <c r="HO18" t="inlineStr"/>
+      <c r="HP18" t="inlineStr"/>
+      <c r="HQ18" t="inlineStr"/>
+      <c r="HR18" t="inlineStr"/>
+      <c r="HS18" t="inlineStr"/>
+      <c r="HT18" t="inlineStr"/>
+      <c r="HU18" t="inlineStr"/>
+      <c r="HV18" t="inlineStr"/>
+      <c r="HW18" t="inlineStr"/>
+      <c r="HX18" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="HY18" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="HZ18" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="IA18" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="IB18" t="inlineStr">
+        <is>
+          <t>16.0</t>
+        </is>
+      </c>
+      <c r="IC18" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="ID18" t="inlineStr"/>
+      <c r="IE18" t="inlineStr"/>
+      <c r="IF18" t="inlineStr"/>
+      <c r="IG18" t="inlineStr">
+        <is>
+          <t>5.45</t>
+        </is>
+      </c>
+      <c r="IH18" t="inlineStr">
+        <is>
+          <t>9.33</t>
+        </is>
+      </c>
+      <c r="II18" t="inlineStr"/>
+      <c r="IJ18" t="inlineStr">
+        <is>
+          <t>7.32</t>
+        </is>
+      </c>
+      <c r="IK18" t="inlineStr">
+        <is>
+          <t>0.47</t>
+        </is>
+      </c>
+      <c r="IL18" t="inlineStr">
+        <is>
+          <t>7.99</t>
+        </is>
+      </c>
+      <c r="IM18" t="inlineStr">
+        <is>
+          <t>7.64</t>
+        </is>
+      </c>
+      <c r="IN18" t="inlineStr">
+        <is>
+          <t>3.12</t>
+        </is>
+      </c>
+      <c r="IO18" t="inlineStr">
+        <is>
+          <t>7.31</t>
+        </is>
+      </c>
+      <c r="IP18" t="inlineStr"/>
+      <c r="IQ18" t="inlineStr"/>
+      <c r="IR18" t="inlineStr"/>
+      <c r="IS18" t="inlineStr"/>
+      <c r="IT18" t="inlineStr"/>
+      <c r="IU18" t="inlineStr"/>
+      <c r="IV18" t="inlineStr"/>
+      <c r="IW18" t="inlineStr"/>
+      <c r="IX18" t="inlineStr"/>
+      <c r="IY18" t="inlineStr"/>
+      <c r="IZ18" t="inlineStr"/>
+      <c r="JA18" t="inlineStr">
+        <is>
+          <t>153</t>
+        </is>
+      </c>
+      <c r="JB18" t="inlineStr"/>
+      <c r="JC18" t="inlineStr">
+        <is>
+          <t>143</t>
+        </is>
+      </c>
+      <c r="JD18" t="inlineStr">
+        <is>
+          <t>155</t>
+        </is>
+      </c>
+      <c r="JE18" t="inlineStr">
+        <is>
+          <t>147</t>
+        </is>
+      </c>
+      <c r="JF18" t="inlineStr">
+        <is>
+          <t>140</t>
+        </is>
+      </c>
+      <c r="JG18" t="inlineStr">
+        <is>
+          <t>149</t>
+        </is>
+      </c>
+      <c r="JH18" t="inlineStr">
+        <is>
+          <t>134</t>
+        </is>
+      </c>
+      <c r="JI18" t="inlineStr"/>
+      <c r="JJ18" t="inlineStr"/>
+      <c r="JK18" t="inlineStr"/>
+      <c r="JL18" t="inlineStr"/>
+      <c r="JM18" t="inlineStr">
+        <is>
+          <t>-9</t>
+        </is>
+      </c>
+      <c r="JN18" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="JO18" t="inlineStr">
+        <is>
+          <t>-7</t>
+        </is>
+      </c>
+      <c r="JP18" t="inlineStr">
+        <is>
+          <t>-11</t>
+        </is>
+      </c>
+      <c r="JQ18" t="inlineStr">
+        <is>
+          <t>-5</t>
+        </is>
+      </c>
+      <c r="JR18" t="inlineStr">
+        <is>
+          <t>-15</t>
+        </is>
+      </c>
+      <c r="JS18" t="inlineStr"/>
+      <c r="JT18" t="inlineStr"/>
+      <c r="JU18" t="inlineStr"/>
+      <c r="JV18" t="inlineStr"/>
+      <c r="JW18" t="inlineStr"/>
+      <c r="JX18" t="inlineStr"/>
+      <c r="JY18" t="inlineStr"/>
+      <c r="JZ18" t="inlineStr"/>
+      <c r="KA18" t="inlineStr"/>
+      <c r="KB18" t="inlineStr"/>
+      <c r="KC18" t="inlineStr"/>
+      <c r="KD18" t="inlineStr"/>
+      <c r="KE18" t="inlineStr"/>
+      <c r="KF18" t="inlineStr"/>
+      <c r="KG18" t="inlineStr"/>
+      <c r="KH18" t="inlineStr"/>
+      <c r="KI18" t="inlineStr"/>
+      <c r="KJ18" t="inlineStr"/>
+      <c r="KK18" t="inlineStr"/>
+      <c r="KL18" t="inlineStr"/>
+      <c r="KM18" t="inlineStr"/>
+      <c r="KN18" t="inlineStr"/>
+      <c r="KO18" t="inlineStr"/>
+      <c r="KP18" t="inlineStr"/>
+      <c r="KQ18" t="inlineStr"/>
+      <c r="KR18" t="inlineStr"/>
+      <c r="KS18" t="inlineStr"/>
+      <c r="KT18" t="inlineStr"/>
+      <c r="KU18" t="inlineStr"/>
+      <c r="KV18" t="inlineStr"/>
+      <c r="KW18" t="inlineStr"/>
+      <c r="KX18" t="inlineStr"/>
+      <c r="KY18" t="inlineStr"/>
+      <c r="KZ18" t="inlineStr"/>
+      <c r="LA18" t="inlineStr"/>
+      <c r="LB18" t="inlineStr"/>
+      <c r="LC18" t="inlineStr"/>
+      <c r="LD18" t="inlineStr"/>
+      <c r="LE18" t="inlineStr"/>
+      <c r="LF18" t="inlineStr"/>
+      <c r="LG18" t="inlineStr"/>
+      <c r="LH18" t="inlineStr"/>
+      <c r="LI18" t="inlineStr"/>
+      <c r="LJ18" t="inlineStr"/>
+      <c r="LK18" t="inlineStr"/>
+      <c r="LL18" t="inlineStr"/>
+      <c r="LM18" t="inlineStr"/>
+      <c r="LN18" t="inlineStr"/>
+      <c r="LO18" t="inlineStr"/>
+      <c r="LP18" t="inlineStr"/>
+      <c r="LQ18" t="inlineStr"/>
+      <c r="LR18" t="inlineStr"/>
+      <c r="LS18" t="inlineStr"/>
+      <c r="LT18" t="inlineStr"/>
+      <c r="LU18" t="inlineStr"/>
+      <c r="LV18" t="inlineStr"/>
+      <c r="LW18" t="inlineStr"/>
+      <c r="LX18" t="inlineStr"/>
+      <c r="LY18" t="inlineStr"/>
+      <c r="LZ18" t="inlineStr"/>
+      <c r="MA18" t="inlineStr"/>
+      <c r="MB18" t="inlineStr"/>
+      <c r="MC18" t="inlineStr"/>
+      <c r="MD18" t="inlineStr"/>
+      <c r="ME18" t="inlineStr"/>
+      <c r="MF18" t="inlineStr"/>
+      <c r="MG18" t="inlineStr"/>
+      <c r="MH18" t="inlineStr"/>
+      <c r="MI18" t="inlineStr"/>
+      <c r="MJ18" t="inlineStr"/>
+      <c r="MK18" t="inlineStr"/>
+      <c r="ML18" t="inlineStr"/>
+      <c r="MM18" t="inlineStr"/>
+      <c r="MN18" t="inlineStr"/>
+      <c r="MO18" t="inlineStr"/>
+      <c r="MP18" t="inlineStr"/>
+      <c r="MQ18" t="inlineStr"/>
+      <c r="MR18" t="inlineStr"/>
+      <c r="MS18" t="inlineStr"/>
+      <c r="MT18" t="inlineStr"/>
+      <c r="MU18" t="inlineStr"/>
+      <c r="MV18" t="inlineStr"/>
+      <c r="MW18" t="inlineStr"/>
+      <c r="MX18" t="inlineStr"/>
+      <c r="MY18" t="inlineStr"/>
+      <c r="MZ18" t="inlineStr"/>
+      <c r="NA18" t="inlineStr"/>
+      <c r="NB18" t="inlineStr"/>
+      <c r="NC18" t="inlineStr"/>
+      <c r="ND18" t="inlineStr"/>
+      <c r="NE18" t="inlineStr"/>
+      <c r="NF18" t="inlineStr"/>
+      <c r="NG18" t="inlineStr"/>
+      <c r="NH18" t="inlineStr"/>
+      <c r="NI18" t="inlineStr"/>
+      <c r="NJ18" t="inlineStr"/>
+      <c r="NK18" t="inlineStr"/>
+      <c r="NL18" t="inlineStr"/>
+      <c r="NM18" t="inlineStr"/>
+      <c r="NN18" t="inlineStr"/>
+      <c r="NO18" t="inlineStr"/>
+      <c r="NP18" t="inlineStr"/>
+      <c r="NQ18" t="inlineStr"/>
+      <c r="NR18" t="inlineStr"/>
+      <c r="NS18" t="inlineStr"/>
+      <c r="NT18" t="inlineStr"/>
+      <c r="NU18" t="inlineStr"/>
+      <c r="NV18" t="inlineStr"/>
+      <c r="NW18" t="inlineStr"/>
+      <c r="NX18" t="inlineStr"/>
+      <c r="NY18" t="inlineStr"/>
+      <c r="NZ18" t="inlineStr"/>
+      <c r="OA18" t="inlineStr"/>
+      <c r="OB18" t="inlineStr"/>
+      <c r="OC18" t="inlineStr"/>
+      <c r="OD18" t="inlineStr"/>
+      <c r="OE18" t="inlineStr"/>
+      <c r="OF18" t="inlineStr"/>
+      <c r="OG18" t="inlineStr"/>
+      <c r="OH18" t="inlineStr"/>
+      <c r="OI18" t="inlineStr"/>
+      <c r="OJ18" t="inlineStr"/>
+      <c r="OK18" t="inlineStr"/>
+      <c r="OL18" t="inlineStr"/>
+      <c r="OM18" t="inlineStr"/>
+      <c r="ON18" t="inlineStr"/>
+      <c r="OO18" t="inlineStr"/>
+      <c r="OP18" t="inlineStr"/>
+      <c r="OQ18" t="inlineStr"/>
+      <c r="OR18" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
c: version1, 2, 3 file add
</commit_message>
<xml_diff>
--- a/OOMII.xlsx
+++ b/OOMII.xlsx
@@ -346,7 +346,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:OR24"/>
+  <dimension ref="A1:OR27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13666,12 +13666,6 @@
           <t>type01</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr"/>
-      <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr"/>
-      <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr">
         <is>
           <t>0.0625</t>
@@ -13702,9 +13696,6 @@
           <t>25.0</t>
         </is>
       </c>
-      <c r="N24" t="inlineStr"/>
-      <c r="O24" t="inlineStr"/>
-      <c r="P24" t="inlineStr"/>
       <c r="Q24" t="inlineStr">
         <is>
           <t>3.22</t>
@@ -13715,7 +13706,6 @@
           <t>3.03</t>
         </is>
       </c>
-      <c r="S24" t="inlineStr"/>
       <c r="T24" t="inlineStr">
         <is>
           <t>3.00</t>
@@ -13746,23 +13736,11 @@
           <t>2.75</t>
         </is>
       </c>
-      <c r="Z24" t="inlineStr"/>
-      <c r="AA24" t="inlineStr"/>
-      <c r="AB24" t="inlineStr"/>
-      <c r="AC24" t="inlineStr"/>
-      <c r="AD24" t="inlineStr"/>
-      <c r="AE24" t="inlineStr"/>
-      <c r="AF24" t="inlineStr"/>
-      <c r="AG24" t="inlineStr"/>
-      <c r="AH24" t="inlineStr"/>
-      <c r="AI24" t="inlineStr"/>
-      <c r="AJ24" t="inlineStr"/>
       <c r="AK24" t="inlineStr">
         <is>
           <t>94</t>
         </is>
       </c>
-      <c r="AL24" t="inlineStr"/>
       <c r="AM24" t="inlineStr">
         <is>
           <t>93</t>
@@ -13793,10 +13771,6 @@
           <t>35</t>
         </is>
       </c>
-      <c r="AS24" t="inlineStr"/>
-      <c r="AT24" t="inlineStr"/>
-      <c r="AU24" t="inlineStr"/>
-      <c r="AV24" t="inlineStr"/>
       <c r="AW24" t="inlineStr">
         <is>
           <t>-1</t>
@@ -13827,18 +13801,6 @@
           <t>-9</t>
         </is>
       </c>
-      <c r="BC24" t="inlineStr"/>
-      <c r="BD24" t="inlineStr"/>
-      <c r="BE24" t="inlineStr"/>
-      <c r="BF24" t="inlineStr"/>
-      <c r="BG24" t="inlineStr"/>
-      <c r="BH24" t="inlineStr"/>
-      <c r="BI24" t="inlineStr"/>
-      <c r="BJ24" t="inlineStr"/>
-      <c r="BK24" t="inlineStr"/>
-      <c r="BL24" t="inlineStr"/>
-      <c r="BM24" t="inlineStr"/>
-      <c r="BN24" t="inlineStr"/>
       <c r="BO24" t="inlineStr">
         <is>
           <t>0.0625</t>
@@ -13869,9 +13831,6 @@
           <t>25.0</t>
         </is>
       </c>
-      <c r="BU24" t="inlineStr"/>
-      <c r="BV24" t="inlineStr"/>
-      <c r="BW24" t="inlineStr"/>
       <c r="BX24" t="inlineStr">
         <is>
           <t>2.51</t>
@@ -13882,7 +13841,6 @@
           <t>2.20</t>
         </is>
       </c>
-      <c r="BZ24" t="inlineStr"/>
       <c r="CA24" t="inlineStr">
         <is>
           <t>2.23</t>
@@ -13913,23 +13871,11 @@
           <t>1.99</t>
         </is>
       </c>
-      <c r="CG24" t="inlineStr"/>
-      <c r="CH24" t="inlineStr"/>
-      <c r="CI24" t="inlineStr"/>
-      <c r="CJ24" t="inlineStr"/>
-      <c r="CK24" t="inlineStr"/>
-      <c r="CL24" t="inlineStr"/>
-      <c r="CM24" t="inlineStr"/>
-      <c r="CN24" t="inlineStr"/>
-      <c r="CO24" t="inlineStr"/>
-      <c r="CP24" t="inlineStr"/>
-      <c r="CQ24" t="inlineStr"/>
       <c r="CR24" t="inlineStr">
         <is>
           <t>91</t>
         </is>
       </c>
-      <c r="CS24" t="inlineStr"/>
       <c r="CT24" t="inlineStr">
         <is>
           <t>39</t>
@@ -13960,10 +13906,6 @@
           <t>79</t>
         </is>
       </c>
-      <c r="CZ24" t="inlineStr"/>
-      <c r="DA24" t="inlineStr"/>
-      <c r="DB24" t="inlineStr"/>
-      <c r="DC24" t="inlineStr"/>
       <c r="DD24" t="inlineStr">
         <is>
           <t>-2</t>
@@ -13994,36 +13936,11 @@
           <t>-13</t>
         </is>
       </c>
-      <c r="DJ24" t="inlineStr"/>
-      <c r="DK24" t="inlineStr"/>
-      <c r="DL24" t="inlineStr"/>
-      <c r="DM24" t="inlineStr"/>
-      <c r="DN24" t="inlineStr"/>
-      <c r="DO24" t="inlineStr"/>
       <c r="DP24" t="inlineStr">
         <is>
           <t>220</t>
         </is>
       </c>
-      <c r="DQ24" t="inlineStr"/>
-      <c r="DR24" t="inlineStr"/>
-      <c r="DS24" t="inlineStr"/>
-      <c r="DT24" t="inlineStr"/>
-      <c r="DU24" t="inlineStr"/>
-      <c r="DV24" t="inlineStr"/>
-      <c r="DW24" t="inlineStr"/>
-      <c r="DX24" t="inlineStr"/>
-      <c r="DY24" t="inlineStr"/>
-      <c r="DZ24" t="inlineStr"/>
-      <c r="EA24" t="inlineStr"/>
-      <c r="EB24" t="inlineStr"/>
-      <c r="EC24" t="inlineStr"/>
-      <c r="ED24" t="inlineStr"/>
-      <c r="EE24" t="inlineStr"/>
-      <c r="EF24" t="inlineStr"/>
-      <c r="EG24" t="inlineStr"/>
-      <c r="EH24" t="inlineStr"/>
-      <c r="EI24" t="inlineStr"/>
       <c r="EJ24" t="inlineStr">
         <is>
           <t>2.57</t>
@@ -14054,16 +13971,11 @@
           <t>1.69</t>
         </is>
       </c>
-      <c r="EP24" t="inlineStr"/>
-      <c r="EQ24" t="inlineStr"/>
-      <c r="ER24" t="inlineStr"/>
-      <c r="ES24" t="inlineStr"/>
       <c r="ET24" t="inlineStr">
         <is>
           <t>68</t>
         </is>
       </c>
-      <c r="EU24" t="inlineStr"/>
       <c r="EV24" t="inlineStr">
         <is>
           <t>55</t>
@@ -14094,29 +14006,6 @@
           <t>51</t>
         </is>
       </c>
-      <c r="FB24" t="inlineStr"/>
-      <c r="FC24" t="inlineStr"/>
-      <c r="FD24" t="inlineStr"/>
-      <c r="FE24" t="inlineStr"/>
-      <c r="FF24" t="inlineStr"/>
-      <c r="FG24" t="inlineStr"/>
-      <c r="FH24" t="inlineStr"/>
-      <c r="FI24" t="inlineStr"/>
-      <c r="FJ24" t="inlineStr"/>
-      <c r="FK24" t="inlineStr"/>
-      <c r="FL24" t="inlineStr"/>
-      <c r="FM24" t="inlineStr"/>
-      <c r="FN24" t="inlineStr"/>
-      <c r="FO24" t="inlineStr"/>
-      <c r="FP24" t="inlineStr"/>
-      <c r="FQ24" t="inlineStr"/>
-      <c r="FR24" t="inlineStr"/>
-      <c r="FS24" t="inlineStr"/>
-      <c r="FT24" t="inlineStr"/>
-      <c r="FU24" t="inlineStr"/>
-      <c r="FV24" t="inlineStr"/>
-      <c r="FW24" t="inlineStr"/>
-      <c r="FX24" t="inlineStr"/>
       <c r="FY24" t="inlineStr">
         <is>
           <t>-4</t>
@@ -14147,51 +14036,6 @@
           <t>-24</t>
         </is>
       </c>
-      <c r="GE24" t="inlineStr"/>
-      <c r="GF24" t="inlineStr"/>
-      <c r="GG24" t="inlineStr"/>
-      <c r="GH24" t="inlineStr"/>
-      <c r="GI24" t="inlineStr"/>
-      <c r="GJ24" t="inlineStr"/>
-      <c r="GK24" t="inlineStr"/>
-      <c r="GL24" t="inlineStr"/>
-      <c r="GM24" t="inlineStr"/>
-      <c r="GN24" t="inlineStr"/>
-      <c r="GO24" t="inlineStr"/>
-      <c r="GP24" t="inlineStr"/>
-      <c r="GQ24" t="inlineStr"/>
-      <c r="GR24" t="inlineStr"/>
-      <c r="GS24" t="inlineStr"/>
-      <c r="GT24" t="inlineStr"/>
-      <c r="GU24" t="inlineStr"/>
-      <c r="GV24" t="inlineStr"/>
-      <c r="GW24" t="inlineStr"/>
-      <c r="GX24" t="inlineStr"/>
-      <c r="GY24" t="inlineStr"/>
-      <c r="GZ24" t="inlineStr"/>
-      <c r="HA24" t="inlineStr"/>
-      <c r="HB24" t="inlineStr"/>
-      <c r="HC24" t="inlineStr"/>
-      <c r="HD24" t="inlineStr"/>
-      <c r="HE24" t="inlineStr"/>
-      <c r="HF24" t="inlineStr"/>
-      <c r="HG24" t="inlineStr"/>
-      <c r="HH24" t="inlineStr"/>
-      <c r="HI24" t="inlineStr"/>
-      <c r="HJ24" t="inlineStr"/>
-      <c r="HK24" t="inlineStr"/>
-      <c r="HL24" t="inlineStr"/>
-      <c r="HM24" t="inlineStr"/>
-      <c r="HN24" t="inlineStr"/>
-      <c r="HO24" t="inlineStr"/>
-      <c r="HP24" t="inlineStr"/>
-      <c r="HQ24" t="inlineStr"/>
-      <c r="HR24" t="inlineStr"/>
-      <c r="HS24" t="inlineStr"/>
-      <c r="HT24" t="inlineStr"/>
-      <c r="HU24" t="inlineStr"/>
-      <c r="HV24" t="inlineStr"/>
-      <c r="HW24" t="inlineStr"/>
       <c r="HX24" t="inlineStr">
         <is>
           <t>0.0625</t>
@@ -14222,9 +14066,6 @@
           <t>25.0</t>
         </is>
       </c>
-      <c r="ID24" t="inlineStr"/>
-      <c r="IE24" t="inlineStr"/>
-      <c r="IF24" t="inlineStr"/>
       <c r="IG24" t="inlineStr">
         <is>
           <t>5.45</t>
@@ -14235,7 +14076,6 @@
           <t>9.33</t>
         </is>
       </c>
-      <c r="II24" t="inlineStr"/>
       <c r="IJ24" t="inlineStr">
         <is>
           <t>7.32</t>
@@ -14266,23 +14106,11 @@
           <t>7.31</t>
         </is>
       </c>
-      <c r="IP24" t="inlineStr"/>
-      <c r="IQ24" t="inlineStr"/>
-      <c r="IR24" t="inlineStr"/>
-      <c r="IS24" t="inlineStr"/>
-      <c r="IT24" t="inlineStr"/>
-      <c r="IU24" t="inlineStr"/>
-      <c r="IV24" t="inlineStr"/>
-      <c r="IW24" t="inlineStr"/>
-      <c r="IX24" t="inlineStr"/>
-      <c r="IY24" t="inlineStr"/>
-      <c r="IZ24" t="inlineStr"/>
       <c r="JA24" t="inlineStr">
         <is>
           <t>153</t>
         </is>
       </c>
-      <c r="JB24" t="inlineStr"/>
       <c r="JC24" t="inlineStr">
         <is>
           <t>143</t>
@@ -14313,10 +14141,6 @@
           <t>134</t>
         </is>
       </c>
-      <c r="JI24" t="inlineStr"/>
-      <c r="JJ24" t="inlineStr"/>
-      <c r="JK24" t="inlineStr"/>
-      <c r="JL24" t="inlineStr"/>
       <c r="JM24" t="inlineStr">
         <is>
           <t>-9</t>
@@ -14347,136 +14171,1848 @@
           <t>-15</t>
         </is>
       </c>
-      <c r="JS24" t="inlineStr"/>
-      <c r="JT24" t="inlineStr"/>
-      <c r="JU24" t="inlineStr"/>
-      <c r="JV24" t="inlineStr"/>
-      <c r="JW24" t="inlineStr"/>
-      <c r="JX24" t="inlineStr"/>
-      <c r="JY24" t="inlineStr"/>
-      <c r="JZ24" t="inlineStr"/>
-      <c r="KA24" t="inlineStr"/>
-      <c r="KB24" t="inlineStr"/>
-      <c r="KC24" t="inlineStr"/>
-      <c r="KD24" t="inlineStr"/>
-      <c r="KE24" t="inlineStr"/>
-      <c r="KF24" t="inlineStr"/>
-      <c r="KG24" t="inlineStr"/>
-      <c r="KH24" t="inlineStr"/>
-      <c r="KI24" t="inlineStr"/>
-      <c r="KJ24" t="inlineStr"/>
-      <c r="KK24" t="inlineStr"/>
-      <c r="KL24" t="inlineStr"/>
-      <c r="KM24" t="inlineStr"/>
-      <c r="KN24" t="inlineStr"/>
-      <c r="KO24" t="inlineStr"/>
-      <c r="KP24" t="inlineStr"/>
-      <c r="KQ24" t="inlineStr"/>
-      <c r="KR24" t="inlineStr"/>
-      <c r="KS24" t="inlineStr"/>
-      <c r="KT24" t="inlineStr"/>
-      <c r="KU24" t="inlineStr"/>
-      <c r="KV24" t="inlineStr"/>
-      <c r="KW24" t="inlineStr"/>
-      <c r="KX24" t="inlineStr"/>
-      <c r="KY24" t="inlineStr"/>
-      <c r="KZ24" t="inlineStr"/>
-      <c r="LA24" t="inlineStr"/>
-      <c r="LB24" t="inlineStr"/>
-      <c r="LC24" t="inlineStr"/>
-      <c r="LD24" t="inlineStr"/>
-      <c r="LE24" t="inlineStr"/>
-      <c r="LF24" t="inlineStr"/>
-      <c r="LG24" t="inlineStr"/>
-      <c r="LH24" t="inlineStr"/>
-      <c r="LI24" t="inlineStr"/>
-      <c r="LJ24" t="inlineStr"/>
-      <c r="LK24" t="inlineStr"/>
-      <c r="LL24" t="inlineStr"/>
-      <c r="LM24" t="inlineStr"/>
-      <c r="LN24" t="inlineStr"/>
-      <c r="LO24" t="inlineStr"/>
-      <c r="LP24" t="inlineStr"/>
-      <c r="LQ24" t="inlineStr"/>
-      <c r="LR24" t="inlineStr"/>
-      <c r="LS24" t="inlineStr"/>
-      <c r="LT24" t="inlineStr"/>
-      <c r="LU24" t="inlineStr"/>
-      <c r="LV24" t="inlineStr"/>
-      <c r="LW24" t="inlineStr"/>
-      <c r="LX24" t="inlineStr"/>
-      <c r="LY24" t="inlineStr"/>
-      <c r="LZ24" t="inlineStr"/>
-      <c r="MA24" t="inlineStr"/>
-      <c r="MB24" t="inlineStr"/>
-      <c r="MC24" t="inlineStr"/>
-      <c r="MD24" t="inlineStr"/>
-      <c r="ME24" t="inlineStr"/>
-      <c r="MF24" t="inlineStr"/>
-      <c r="MG24" t="inlineStr"/>
-      <c r="MH24" t="inlineStr"/>
-      <c r="MI24" t="inlineStr"/>
-      <c r="MJ24" t="inlineStr"/>
-      <c r="MK24" t="inlineStr"/>
-      <c r="ML24" t="inlineStr"/>
-      <c r="MM24" t="inlineStr"/>
-      <c r="MN24" t="inlineStr"/>
-      <c r="MO24" t="inlineStr"/>
-      <c r="MP24" t="inlineStr"/>
-      <c r="MQ24" t="inlineStr"/>
-      <c r="MR24" t="inlineStr"/>
-      <c r="MS24" t="inlineStr"/>
-      <c r="MT24" t="inlineStr"/>
-      <c r="MU24" t="inlineStr"/>
-      <c r="MV24" t="inlineStr"/>
-      <c r="MW24" t="inlineStr"/>
-      <c r="MX24" t="inlineStr"/>
-      <c r="MY24" t="inlineStr"/>
-      <c r="MZ24" t="inlineStr"/>
-      <c r="NA24" t="inlineStr"/>
-      <c r="NB24" t="inlineStr"/>
-      <c r="NC24" t="inlineStr"/>
-      <c r="ND24" t="inlineStr"/>
-      <c r="NE24" t="inlineStr"/>
-      <c r="NF24" t="inlineStr"/>
-      <c r="NG24" t="inlineStr"/>
-      <c r="NH24" t="inlineStr"/>
-      <c r="NI24" t="inlineStr"/>
-      <c r="NJ24" t="inlineStr"/>
-      <c r="NK24" t="inlineStr"/>
-      <c r="NL24" t="inlineStr"/>
-      <c r="NM24" t="inlineStr"/>
-      <c r="NN24" t="inlineStr"/>
-      <c r="NO24" t="inlineStr"/>
-      <c r="NP24" t="inlineStr"/>
-      <c r="NQ24" t="inlineStr"/>
-      <c r="NR24" t="inlineStr"/>
-      <c r="NS24" t="inlineStr"/>
-      <c r="NT24" t="inlineStr"/>
-      <c r="NU24" t="inlineStr"/>
-      <c r="NV24" t="inlineStr"/>
-      <c r="NW24" t="inlineStr"/>
-      <c r="NX24" t="inlineStr"/>
-      <c r="NY24" t="inlineStr"/>
-      <c r="NZ24" t="inlineStr"/>
-      <c r="OA24" t="inlineStr"/>
-      <c r="OB24" t="inlineStr"/>
-      <c r="OC24" t="inlineStr"/>
-      <c r="OD24" t="inlineStr"/>
-      <c r="OE24" t="inlineStr"/>
-      <c r="OF24" t="inlineStr"/>
-      <c r="OG24" t="inlineStr"/>
-      <c r="OH24" t="inlineStr"/>
-      <c r="OI24" t="inlineStr"/>
-      <c r="OJ24" t="inlineStr"/>
-      <c r="OK24" t="inlineStr"/>
-      <c r="OL24" t="inlineStr"/>
-      <c r="OM24" t="inlineStr"/>
-      <c r="ON24" t="inlineStr"/>
-      <c r="OO24" t="inlineStr"/>
-      <c r="OP24" t="inlineStr"/>
-      <c r="OQ24" t="inlineStr"/>
-      <c r="OR24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>type01</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>16.0</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>3.22</t>
+        </is>
+      </c>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>3.03</t>
+        </is>
+      </c>
+      <c r="T25" t="inlineStr">
+        <is>
+          <t>3.00</t>
+        </is>
+      </c>
+      <c r="U25" t="inlineStr">
+        <is>
+          <t>2.97</t>
+        </is>
+      </c>
+      <c r="V25" t="inlineStr">
+        <is>
+          <t>3.01</t>
+        </is>
+      </c>
+      <c r="W25" t="inlineStr">
+        <is>
+          <t>2.93</t>
+        </is>
+      </c>
+      <c r="X25" t="inlineStr">
+        <is>
+          <t>2.31</t>
+        </is>
+      </c>
+      <c r="Y25" t="inlineStr">
+        <is>
+          <t>2.75</t>
+        </is>
+      </c>
+      <c r="AK25" t="inlineStr">
+        <is>
+          <t>94</t>
+        </is>
+      </c>
+      <c r="AM25" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="AN25" t="inlineStr">
+        <is>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="AO25" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="AP25" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="AQ25" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="AR25" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="AW25" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="AX25" t="inlineStr">
+        <is>
+          <t>-2</t>
+        </is>
+      </c>
+      <c r="AY25" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="AZ25" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="BA25" t="inlineStr">
+        <is>
+          <t>-7</t>
+        </is>
+      </c>
+      <c r="BB25" t="inlineStr">
+        <is>
+          <t>-9</t>
+        </is>
+      </c>
+      <c r="BO25" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="BP25" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="BQ25" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="BR25" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="BS25" t="inlineStr">
+        <is>
+          <t>15.0</t>
+        </is>
+      </c>
+      <c r="BT25" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="BX25" t="inlineStr">
+        <is>
+          <t>2.51</t>
+        </is>
+      </c>
+      <c r="BY25" t="inlineStr">
+        <is>
+          <t>2.20</t>
+        </is>
+      </c>
+      <c r="CA25" t="inlineStr">
+        <is>
+          <t>2.23</t>
+        </is>
+      </c>
+      <c r="CB25" t="inlineStr">
+        <is>
+          <t>2.25</t>
+        </is>
+      </c>
+      <c r="CC25" t="inlineStr">
+        <is>
+          <t>2.27</t>
+        </is>
+      </c>
+      <c r="CD25" t="inlineStr">
+        <is>
+          <t>2.20</t>
+        </is>
+      </c>
+      <c r="CE25" t="inlineStr">
+        <is>
+          <t>2.10</t>
+        </is>
+      </c>
+      <c r="CF25" t="inlineStr">
+        <is>
+          <t>1.99</t>
+        </is>
+      </c>
+      <c r="CR25" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="CT25" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="CU25" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="CV25" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="CW25" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="CX25" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="CY25" t="inlineStr">
+        <is>
+          <t>79</t>
+        </is>
+      </c>
+      <c r="DD25" t="inlineStr">
+        <is>
+          <t>-2</t>
+        </is>
+      </c>
+      <c r="DE25" t="inlineStr">
+        <is>
+          <t>-2</t>
+        </is>
+      </c>
+      <c r="DF25" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="DG25" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="DH25" t="inlineStr">
+        <is>
+          <t>-3</t>
+        </is>
+      </c>
+      <c r="DI25" t="inlineStr">
+        <is>
+          <t>-13</t>
+        </is>
+      </c>
+      <c r="DP25" t="inlineStr">
+        <is>
+          <t>220</t>
+        </is>
+      </c>
+      <c r="EJ25" t="inlineStr">
+        <is>
+          <t>2.57</t>
+        </is>
+      </c>
+      <c r="EK25" t="inlineStr">
+        <is>
+          <t>1.75</t>
+        </is>
+      </c>
+      <c r="EL25" t="inlineStr">
+        <is>
+          <t>1.67</t>
+        </is>
+      </c>
+      <c r="EM25" t="inlineStr">
+        <is>
+          <t>1.69</t>
+        </is>
+      </c>
+      <c r="EN25" t="inlineStr">
+        <is>
+          <t>1.73</t>
+        </is>
+      </c>
+      <c r="EO25" t="inlineStr">
+        <is>
+          <t>1.69</t>
+        </is>
+      </c>
+      <c r="ET25" t="inlineStr">
+        <is>
+          <t>68</t>
+        </is>
+      </c>
+      <c r="EV25" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="EW25" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="EX25" t="inlineStr">
+        <is>
+          <t>63</t>
+        </is>
+      </c>
+      <c r="EY25" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="EZ25" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="FA25" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="FY25" t="inlineStr">
+        <is>
+          <t>-4</t>
+        </is>
+      </c>
+      <c r="FZ25" t="inlineStr">
+        <is>
+          <t>-3</t>
+        </is>
+      </c>
+      <c r="GA25" t="inlineStr">
+        <is>
+          <t>-0</t>
+        </is>
+      </c>
+      <c r="GB25" t="inlineStr">
+        <is>
+          <t>-3</t>
+        </is>
+      </c>
+      <c r="GC25" t="inlineStr">
+        <is>
+          <t>-11</t>
+        </is>
+      </c>
+      <c r="GD25" t="inlineStr">
+        <is>
+          <t>-24</t>
+        </is>
+      </c>
+      <c r="HX25" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="HY25" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="HZ25" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="IA25" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="IB25" t="inlineStr">
+        <is>
+          <t>16.0</t>
+        </is>
+      </c>
+      <c r="IC25" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="IG25" t="inlineStr">
+        <is>
+          <t>5.45</t>
+        </is>
+      </c>
+      <c r="IH25" t="inlineStr">
+        <is>
+          <t>9.33</t>
+        </is>
+      </c>
+      <c r="IJ25" t="inlineStr">
+        <is>
+          <t>7.32</t>
+        </is>
+      </c>
+      <c r="IK25" t="inlineStr">
+        <is>
+          <t>0.47</t>
+        </is>
+      </c>
+      <c r="IL25" t="inlineStr">
+        <is>
+          <t>7.99</t>
+        </is>
+      </c>
+      <c r="IM25" t="inlineStr">
+        <is>
+          <t>7.64</t>
+        </is>
+      </c>
+      <c r="IN25" t="inlineStr">
+        <is>
+          <t>3.12</t>
+        </is>
+      </c>
+      <c r="IO25" t="inlineStr">
+        <is>
+          <t>7.31</t>
+        </is>
+      </c>
+      <c r="JA25" t="inlineStr">
+        <is>
+          <t>153</t>
+        </is>
+      </c>
+      <c r="JC25" t="inlineStr">
+        <is>
+          <t>143</t>
+        </is>
+      </c>
+      <c r="JD25" t="inlineStr">
+        <is>
+          <t>155</t>
+        </is>
+      </c>
+      <c r="JE25" t="inlineStr">
+        <is>
+          <t>147</t>
+        </is>
+      </c>
+      <c r="JF25" t="inlineStr">
+        <is>
+          <t>140</t>
+        </is>
+      </c>
+      <c r="JG25" t="inlineStr">
+        <is>
+          <t>149</t>
+        </is>
+      </c>
+      <c r="JH25" t="inlineStr">
+        <is>
+          <t>134</t>
+        </is>
+      </c>
+      <c r="JM25" t="inlineStr">
+        <is>
+          <t>-9</t>
+        </is>
+      </c>
+      <c r="JN25" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="JO25" t="inlineStr">
+        <is>
+          <t>-7</t>
+        </is>
+      </c>
+      <c r="JP25" t="inlineStr">
+        <is>
+          <t>-11</t>
+        </is>
+      </c>
+      <c r="JQ25" t="inlineStr">
+        <is>
+          <t>-5</t>
+        </is>
+      </c>
+      <c r="JR25" t="inlineStr">
+        <is>
+          <t>-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>type01</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>16.0</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>3.22</t>
+        </is>
+      </c>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>3.03</t>
+        </is>
+      </c>
+      <c r="T26" t="inlineStr">
+        <is>
+          <t>3.00</t>
+        </is>
+      </c>
+      <c r="U26" t="inlineStr">
+        <is>
+          <t>2.97</t>
+        </is>
+      </c>
+      <c r="V26" t="inlineStr">
+        <is>
+          <t>3.01</t>
+        </is>
+      </c>
+      <c r="W26" t="inlineStr">
+        <is>
+          <t>2.93</t>
+        </is>
+      </c>
+      <c r="X26" t="inlineStr">
+        <is>
+          <t>2.31</t>
+        </is>
+      </c>
+      <c r="Y26" t="inlineStr">
+        <is>
+          <t>2.75</t>
+        </is>
+      </c>
+      <c r="AK26" t="inlineStr">
+        <is>
+          <t>94</t>
+        </is>
+      </c>
+      <c r="AM26" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="AN26" t="inlineStr">
+        <is>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="AO26" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="AP26" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="AQ26" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="AR26" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="AW26" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="AX26" t="inlineStr">
+        <is>
+          <t>-2</t>
+        </is>
+      </c>
+      <c r="AY26" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="AZ26" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="BA26" t="inlineStr">
+        <is>
+          <t>-7</t>
+        </is>
+      </c>
+      <c r="BB26" t="inlineStr">
+        <is>
+          <t>-9</t>
+        </is>
+      </c>
+      <c r="BO26" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="BP26" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="BQ26" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="BR26" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="BS26" t="inlineStr">
+        <is>
+          <t>15.0</t>
+        </is>
+      </c>
+      <c r="BT26" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="BX26" t="inlineStr">
+        <is>
+          <t>2.51</t>
+        </is>
+      </c>
+      <c r="BY26" t="inlineStr">
+        <is>
+          <t>2.20</t>
+        </is>
+      </c>
+      <c r="CA26" t="inlineStr">
+        <is>
+          <t>2.23</t>
+        </is>
+      </c>
+      <c r="CB26" t="inlineStr">
+        <is>
+          <t>2.25</t>
+        </is>
+      </c>
+      <c r="CC26" t="inlineStr">
+        <is>
+          <t>2.27</t>
+        </is>
+      </c>
+      <c r="CD26" t="inlineStr">
+        <is>
+          <t>2.20</t>
+        </is>
+      </c>
+      <c r="CE26" t="inlineStr">
+        <is>
+          <t>2.10</t>
+        </is>
+      </c>
+      <c r="CF26" t="inlineStr">
+        <is>
+          <t>1.99</t>
+        </is>
+      </c>
+      <c r="CR26" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="CT26" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="CU26" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="CV26" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="CW26" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="CX26" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="CY26" t="inlineStr">
+        <is>
+          <t>79</t>
+        </is>
+      </c>
+      <c r="DD26" t="inlineStr">
+        <is>
+          <t>-2</t>
+        </is>
+      </c>
+      <c r="DE26" t="inlineStr">
+        <is>
+          <t>-2</t>
+        </is>
+      </c>
+      <c r="DF26" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="DG26" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="DH26" t="inlineStr">
+        <is>
+          <t>-3</t>
+        </is>
+      </c>
+      <c r="DI26" t="inlineStr">
+        <is>
+          <t>-13</t>
+        </is>
+      </c>
+      <c r="DP26" t="inlineStr">
+        <is>
+          <t>220</t>
+        </is>
+      </c>
+      <c r="EJ26" t="inlineStr">
+        <is>
+          <t>2.57</t>
+        </is>
+      </c>
+      <c r="EK26" t="inlineStr">
+        <is>
+          <t>1.75</t>
+        </is>
+      </c>
+      <c r="EL26" t="inlineStr">
+        <is>
+          <t>1.67</t>
+        </is>
+      </c>
+      <c r="EM26" t="inlineStr">
+        <is>
+          <t>1.69</t>
+        </is>
+      </c>
+      <c r="EN26" t="inlineStr">
+        <is>
+          <t>1.73</t>
+        </is>
+      </c>
+      <c r="EO26" t="inlineStr">
+        <is>
+          <t>1.69</t>
+        </is>
+      </c>
+      <c r="ET26" t="inlineStr">
+        <is>
+          <t>68</t>
+        </is>
+      </c>
+      <c r="EV26" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="EW26" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="EX26" t="inlineStr">
+        <is>
+          <t>63</t>
+        </is>
+      </c>
+      <c r="EY26" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="EZ26" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="FA26" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="FY26" t="inlineStr">
+        <is>
+          <t>-4</t>
+        </is>
+      </c>
+      <c r="FZ26" t="inlineStr">
+        <is>
+          <t>-3</t>
+        </is>
+      </c>
+      <c r="GA26" t="inlineStr">
+        <is>
+          <t>-0</t>
+        </is>
+      </c>
+      <c r="GB26" t="inlineStr">
+        <is>
+          <t>-3</t>
+        </is>
+      </c>
+      <c r="GC26" t="inlineStr">
+        <is>
+          <t>-11</t>
+        </is>
+      </c>
+      <c r="GD26" t="inlineStr">
+        <is>
+          <t>-24</t>
+        </is>
+      </c>
+      <c r="HX26" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="HY26" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="HZ26" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="IA26" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="IB26" t="inlineStr">
+        <is>
+          <t>16.0</t>
+        </is>
+      </c>
+      <c r="IC26" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="IG26" t="inlineStr">
+        <is>
+          <t>5.45</t>
+        </is>
+      </c>
+      <c r="IH26" t="inlineStr">
+        <is>
+          <t>9.33</t>
+        </is>
+      </c>
+      <c r="IJ26" t="inlineStr">
+        <is>
+          <t>7.32</t>
+        </is>
+      </c>
+      <c r="IK26" t="inlineStr">
+        <is>
+          <t>0.47</t>
+        </is>
+      </c>
+      <c r="IL26" t="inlineStr">
+        <is>
+          <t>7.99</t>
+        </is>
+      </c>
+      <c r="IM26" t="inlineStr">
+        <is>
+          <t>7.64</t>
+        </is>
+      </c>
+      <c r="IN26" t="inlineStr">
+        <is>
+          <t>3.12</t>
+        </is>
+      </c>
+      <c r="IO26" t="inlineStr">
+        <is>
+          <t>7.31</t>
+        </is>
+      </c>
+      <c r="JA26" t="inlineStr">
+        <is>
+          <t>153</t>
+        </is>
+      </c>
+      <c r="JC26" t="inlineStr">
+        <is>
+          <t>143</t>
+        </is>
+      </c>
+      <c r="JD26" t="inlineStr">
+        <is>
+          <t>155</t>
+        </is>
+      </c>
+      <c r="JE26" t="inlineStr">
+        <is>
+          <t>147</t>
+        </is>
+      </c>
+      <c r="JF26" t="inlineStr">
+        <is>
+          <t>140</t>
+        </is>
+      </c>
+      <c r="JG26" t="inlineStr">
+        <is>
+          <t>149</t>
+        </is>
+      </c>
+      <c r="JH26" t="inlineStr">
+        <is>
+          <t>134</t>
+        </is>
+      </c>
+      <c r="JM26" t="inlineStr">
+        <is>
+          <t>-9</t>
+        </is>
+      </c>
+      <c r="JN26" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="JO26" t="inlineStr">
+        <is>
+          <t>-7</t>
+        </is>
+      </c>
+      <c r="JP26" t="inlineStr">
+        <is>
+          <t>-11</t>
+        </is>
+      </c>
+      <c r="JQ26" t="inlineStr">
+        <is>
+          <t>-5</t>
+        </is>
+      </c>
+      <c r="JR26" t="inlineStr">
+        <is>
+          <t>-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>type01</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr"/>
+      <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>16.0</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr"/>
+      <c r="O27" t="inlineStr"/>
+      <c r="P27" t="inlineStr"/>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>3.22</t>
+        </is>
+      </c>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>3.03</t>
+        </is>
+      </c>
+      <c r="S27" t="inlineStr"/>
+      <c r="T27" t="inlineStr">
+        <is>
+          <t>3.00</t>
+        </is>
+      </c>
+      <c r="U27" t="inlineStr">
+        <is>
+          <t>2.97</t>
+        </is>
+      </c>
+      <c r="V27" t="inlineStr">
+        <is>
+          <t>3.01</t>
+        </is>
+      </c>
+      <c r="W27" t="inlineStr">
+        <is>
+          <t>2.93</t>
+        </is>
+      </c>
+      <c r="X27" t="inlineStr">
+        <is>
+          <t>2.31</t>
+        </is>
+      </c>
+      <c r="Y27" t="inlineStr">
+        <is>
+          <t>2.75</t>
+        </is>
+      </c>
+      <c r="Z27" t="inlineStr"/>
+      <c r="AA27" t="inlineStr"/>
+      <c r="AB27" t="inlineStr"/>
+      <c r="AC27" t="inlineStr"/>
+      <c r="AD27" t="inlineStr"/>
+      <c r="AE27" t="inlineStr"/>
+      <c r="AF27" t="inlineStr"/>
+      <c r="AG27" t="inlineStr"/>
+      <c r="AH27" t="inlineStr"/>
+      <c r="AI27" t="inlineStr"/>
+      <c r="AJ27" t="inlineStr"/>
+      <c r="AK27" t="inlineStr">
+        <is>
+          <t>94</t>
+        </is>
+      </c>
+      <c r="AL27" t="inlineStr"/>
+      <c r="AM27" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="AN27" t="inlineStr">
+        <is>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="AO27" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="AP27" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="AQ27" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="AR27" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="AS27" t="inlineStr"/>
+      <c r="AT27" t="inlineStr"/>
+      <c r="AU27" t="inlineStr"/>
+      <c r="AV27" t="inlineStr"/>
+      <c r="AW27" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="AX27" t="inlineStr">
+        <is>
+          <t>-2</t>
+        </is>
+      </c>
+      <c r="AY27" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="AZ27" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="BA27" t="inlineStr">
+        <is>
+          <t>-7</t>
+        </is>
+      </c>
+      <c r="BB27" t="inlineStr">
+        <is>
+          <t>-9</t>
+        </is>
+      </c>
+      <c r="BC27" t="inlineStr"/>
+      <c r="BD27" t="inlineStr"/>
+      <c r="BE27" t="inlineStr"/>
+      <c r="BF27" t="inlineStr"/>
+      <c r="BG27" t="inlineStr"/>
+      <c r="BH27" t="inlineStr"/>
+      <c r="BI27" t="inlineStr"/>
+      <c r="BJ27" t="inlineStr"/>
+      <c r="BK27" t="inlineStr"/>
+      <c r="BL27" t="inlineStr"/>
+      <c r="BM27" t="inlineStr"/>
+      <c r="BN27" t="inlineStr"/>
+      <c r="BO27" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="BP27" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="BQ27" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="BR27" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="BS27" t="inlineStr">
+        <is>
+          <t>15.0</t>
+        </is>
+      </c>
+      <c r="BT27" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="BU27" t="inlineStr"/>
+      <c r="BV27" t="inlineStr"/>
+      <c r="BW27" t="inlineStr"/>
+      <c r="BX27" t="inlineStr">
+        <is>
+          <t>2.51</t>
+        </is>
+      </c>
+      <c r="BY27" t="inlineStr">
+        <is>
+          <t>2.20</t>
+        </is>
+      </c>
+      <c r="BZ27" t="inlineStr"/>
+      <c r="CA27" t="inlineStr">
+        <is>
+          <t>2.23</t>
+        </is>
+      </c>
+      <c r="CB27" t="inlineStr">
+        <is>
+          <t>2.25</t>
+        </is>
+      </c>
+      <c r="CC27" t="inlineStr">
+        <is>
+          <t>2.27</t>
+        </is>
+      </c>
+      <c r="CD27" t="inlineStr">
+        <is>
+          <t>2.20</t>
+        </is>
+      </c>
+      <c r="CE27" t="inlineStr">
+        <is>
+          <t>2.10</t>
+        </is>
+      </c>
+      <c r="CF27" t="inlineStr">
+        <is>
+          <t>1.99</t>
+        </is>
+      </c>
+      <c r="CG27" t="inlineStr"/>
+      <c r="CH27" t="inlineStr"/>
+      <c r="CI27" t="inlineStr"/>
+      <c r="CJ27" t="inlineStr"/>
+      <c r="CK27" t="inlineStr"/>
+      <c r="CL27" t="inlineStr"/>
+      <c r="CM27" t="inlineStr"/>
+      <c r="CN27" t="inlineStr"/>
+      <c r="CO27" t="inlineStr"/>
+      <c r="CP27" t="inlineStr"/>
+      <c r="CQ27" t="inlineStr"/>
+      <c r="CR27" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="CS27" t="inlineStr"/>
+      <c r="CT27" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="CU27" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="CV27" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="CW27" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="CX27" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="CY27" t="inlineStr">
+        <is>
+          <t>79</t>
+        </is>
+      </c>
+      <c r="CZ27" t="inlineStr"/>
+      <c r="DA27" t="inlineStr"/>
+      <c r="DB27" t="inlineStr"/>
+      <c r="DC27" t="inlineStr"/>
+      <c r="DD27" t="inlineStr">
+        <is>
+          <t>-2</t>
+        </is>
+      </c>
+      <c r="DE27" t="inlineStr">
+        <is>
+          <t>-2</t>
+        </is>
+      </c>
+      <c r="DF27" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="DG27" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="DH27" t="inlineStr">
+        <is>
+          <t>-3</t>
+        </is>
+      </c>
+      <c r="DI27" t="inlineStr">
+        <is>
+          <t>-13</t>
+        </is>
+      </c>
+      <c r="DJ27" t="inlineStr"/>
+      <c r="DK27" t="inlineStr"/>
+      <c r="DL27" t="inlineStr"/>
+      <c r="DM27" t="inlineStr"/>
+      <c r="DN27" t="inlineStr"/>
+      <c r="DO27" t="inlineStr"/>
+      <c r="DP27" t="inlineStr">
+        <is>
+          <t>220</t>
+        </is>
+      </c>
+      <c r="DQ27" t="inlineStr"/>
+      <c r="DR27" t="inlineStr"/>
+      <c r="DS27" t="inlineStr"/>
+      <c r="DT27" t="inlineStr"/>
+      <c r="DU27" t="inlineStr"/>
+      <c r="DV27" t="inlineStr"/>
+      <c r="DW27" t="inlineStr"/>
+      <c r="DX27" t="inlineStr"/>
+      <c r="DY27" t="inlineStr"/>
+      <c r="DZ27" t="inlineStr"/>
+      <c r="EA27" t="inlineStr"/>
+      <c r="EB27" t="inlineStr"/>
+      <c r="EC27" t="inlineStr"/>
+      <c r="ED27" t="inlineStr"/>
+      <c r="EE27" t="inlineStr"/>
+      <c r="EF27" t="inlineStr"/>
+      <c r="EG27" t="inlineStr"/>
+      <c r="EH27" t="inlineStr"/>
+      <c r="EI27" t="inlineStr"/>
+      <c r="EJ27" t="inlineStr">
+        <is>
+          <t>2.57</t>
+        </is>
+      </c>
+      <c r="EK27" t="inlineStr">
+        <is>
+          <t>1.75</t>
+        </is>
+      </c>
+      <c r="EL27" t="inlineStr">
+        <is>
+          <t>1.67</t>
+        </is>
+      </c>
+      <c r="EM27" t="inlineStr">
+        <is>
+          <t>1.69</t>
+        </is>
+      </c>
+      <c r="EN27" t="inlineStr">
+        <is>
+          <t>1.73</t>
+        </is>
+      </c>
+      <c r="EO27" t="inlineStr">
+        <is>
+          <t>1.69</t>
+        </is>
+      </c>
+      <c r="EP27" t="inlineStr"/>
+      <c r="EQ27" t="inlineStr"/>
+      <c r="ER27" t="inlineStr"/>
+      <c r="ES27" t="inlineStr"/>
+      <c r="ET27" t="inlineStr">
+        <is>
+          <t>68</t>
+        </is>
+      </c>
+      <c r="EU27" t="inlineStr"/>
+      <c r="EV27" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="EW27" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="EX27" t="inlineStr">
+        <is>
+          <t>63</t>
+        </is>
+      </c>
+      <c r="EY27" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="EZ27" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="FA27" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="FB27" t="inlineStr"/>
+      <c r="FC27" t="inlineStr"/>
+      <c r="FD27" t="inlineStr"/>
+      <c r="FE27" t="inlineStr"/>
+      <c r="FF27" t="inlineStr"/>
+      <c r="FG27" t="inlineStr"/>
+      <c r="FH27" t="inlineStr"/>
+      <c r="FI27" t="inlineStr"/>
+      <c r="FJ27" t="inlineStr"/>
+      <c r="FK27" t="inlineStr"/>
+      <c r="FL27" t="inlineStr"/>
+      <c r="FM27" t="inlineStr"/>
+      <c r="FN27" t="inlineStr"/>
+      <c r="FO27" t="inlineStr"/>
+      <c r="FP27" t="inlineStr"/>
+      <c r="FQ27" t="inlineStr"/>
+      <c r="FR27" t="inlineStr"/>
+      <c r="FS27" t="inlineStr"/>
+      <c r="FT27" t="inlineStr"/>
+      <c r="FU27" t="inlineStr"/>
+      <c r="FV27" t="inlineStr"/>
+      <c r="FW27" t="inlineStr"/>
+      <c r="FX27" t="inlineStr"/>
+      <c r="FY27" t="inlineStr">
+        <is>
+          <t>-4</t>
+        </is>
+      </c>
+      <c r="FZ27" t="inlineStr">
+        <is>
+          <t>-3</t>
+        </is>
+      </c>
+      <c r="GA27" t="inlineStr">
+        <is>
+          <t>-0</t>
+        </is>
+      </c>
+      <c r="GB27" t="inlineStr">
+        <is>
+          <t>-3</t>
+        </is>
+      </c>
+      <c r="GC27" t="inlineStr">
+        <is>
+          <t>-11</t>
+        </is>
+      </c>
+      <c r="GD27" t="inlineStr">
+        <is>
+          <t>-24</t>
+        </is>
+      </c>
+      <c r="GE27" t="inlineStr"/>
+      <c r="GF27" t="inlineStr"/>
+      <c r="GG27" t="inlineStr"/>
+      <c r="GH27" t="inlineStr"/>
+      <c r="GI27" t="inlineStr"/>
+      <c r="GJ27" t="inlineStr"/>
+      <c r="GK27" t="inlineStr"/>
+      <c r="GL27" t="inlineStr"/>
+      <c r="GM27" t="inlineStr"/>
+      <c r="GN27" t="inlineStr"/>
+      <c r="GO27" t="inlineStr"/>
+      <c r="GP27" t="inlineStr"/>
+      <c r="GQ27" t="inlineStr"/>
+      <c r="GR27" t="inlineStr"/>
+      <c r="GS27" t="inlineStr"/>
+      <c r="GT27" t="inlineStr"/>
+      <c r="GU27" t="inlineStr"/>
+      <c r="GV27" t="inlineStr"/>
+      <c r="GW27" t="inlineStr"/>
+      <c r="GX27" t="inlineStr"/>
+      <c r="GY27" t="inlineStr"/>
+      <c r="GZ27" t="inlineStr"/>
+      <c r="HA27" t="inlineStr"/>
+      <c r="HB27" t="inlineStr"/>
+      <c r="HC27" t="inlineStr"/>
+      <c r="HD27" t="inlineStr"/>
+      <c r="HE27" t="inlineStr"/>
+      <c r="HF27" t="inlineStr"/>
+      <c r="HG27" t="inlineStr"/>
+      <c r="HH27" t="inlineStr"/>
+      <c r="HI27" t="inlineStr"/>
+      <c r="HJ27" t="inlineStr"/>
+      <c r="HK27" t="inlineStr"/>
+      <c r="HL27" t="inlineStr"/>
+      <c r="HM27" t="inlineStr"/>
+      <c r="HN27" t="inlineStr"/>
+      <c r="HO27" t="inlineStr"/>
+      <c r="HP27" t="inlineStr"/>
+      <c r="HQ27" t="inlineStr"/>
+      <c r="HR27" t="inlineStr"/>
+      <c r="HS27" t="inlineStr"/>
+      <c r="HT27" t="inlineStr"/>
+      <c r="HU27" t="inlineStr"/>
+      <c r="HV27" t="inlineStr"/>
+      <c r="HW27" t="inlineStr"/>
+      <c r="HX27" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="HY27" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="HZ27" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="IA27" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="IB27" t="inlineStr">
+        <is>
+          <t>16.0</t>
+        </is>
+      </c>
+      <c r="IC27" t="inlineStr">
+        <is>
+          <t>25.0</t>
+        </is>
+      </c>
+      <c r="ID27" t="inlineStr"/>
+      <c r="IE27" t="inlineStr"/>
+      <c r="IF27" t="inlineStr"/>
+      <c r="IG27" t="inlineStr">
+        <is>
+          <t>5.45</t>
+        </is>
+      </c>
+      <c r="IH27" t="inlineStr">
+        <is>
+          <t>9.33</t>
+        </is>
+      </c>
+      <c r="II27" t="inlineStr"/>
+      <c r="IJ27" t="inlineStr">
+        <is>
+          <t>7.32</t>
+        </is>
+      </c>
+      <c r="IK27" t="inlineStr">
+        <is>
+          <t>0.47</t>
+        </is>
+      </c>
+      <c r="IL27" t="inlineStr">
+        <is>
+          <t>7.99</t>
+        </is>
+      </c>
+      <c r="IM27" t="inlineStr">
+        <is>
+          <t>7.64</t>
+        </is>
+      </c>
+      <c r="IN27" t="inlineStr">
+        <is>
+          <t>3.12</t>
+        </is>
+      </c>
+      <c r="IO27" t="inlineStr">
+        <is>
+          <t>7.31</t>
+        </is>
+      </c>
+      <c r="IP27" t="inlineStr"/>
+      <c r="IQ27" t="inlineStr"/>
+      <c r="IR27" t="inlineStr"/>
+      <c r="IS27" t="inlineStr"/>
+      <c r="IT27" t="inlineStr"/>
+      <c r="IU27" t="inlineStr"/>
+      <c r="IV27" t="inlineStr"/>
+      <c r="IW27" t="inlineStr"/>
+      <c r="IX27" t="inlineStr"/>
+      <c r="IY27" t="inlineStr"/>
+      <c r="IZ27" t="inlineStr"/>
+      <c r="JA27" t="inlineStr">
+        <is>
+          <t>153</t>
+        </is>
+      </c>
+      <c r="JB27" t="inlineStr"/>
+      <c r="JC27" t="inlineStr">
+        <is>
+          <t>143</t>
+        </is>
+      </c>
+      <c r="JD27" t="inlineStr">
+        <is>
+          <t>155</t>
+        </is>
+      </c>
+      <c r="JE27" t="inlineStr">
+        <is>
+          <t>147</t>
+        </is>
+      </c>
+      <c r="JF27" t="inlineStr">
+        <is>
+          <t>140</t>
+        </is>
+      </c>
+      <c r="JG27" t="inlineStr">
+        <is>
+          <t>149</t>
+        </is>
+      </c>
+      <c r="JH27" t="inlineStr">
+        <is>
+          <t>134</t>
+        </is>
+      </c>
+      <c r="JI27" t="inlineStr"/>
+      <c r="JJ27" t="inlineStr"/>
+      <c r="JK27" t="inlineStr"/>
+      <c r="JL27" t="inlineStr"/>
+      <c r="JM27" t="inlineStr">
+        <is>
+          <t>-9</t>
+        </is>
+      </c>
+      <c r="JN27" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="JO27" t="inlineStr">
+        <is>
+          <t>-7</t>
+        </is>
+      </c>
+      <c r="JP27" t="inlineStr">
+        <is>
+          <t>-11</t>
+        </is>
+      </c>
+      <c r="JQ27" t="inlineStr">
+        <is>
+          <t>-5</t>
+        </is>
+      </c>
+      <c r="JR27" t="inlineStr">
+        <is>
+          <t>-15</t>
+        </is>
+      </c>
+      <c r="JS27" t="inlineStr"/>
+      <c r="JT27" t="inlineStr"/>
+      <c r="JU27" t="inlineStr"/>
+      <c r="JV27" t="inlineStr"/>
+      <c r="JW27" t="inlineStr"/>
+      <c r="JX27" t="inlineStr"/>
+      <c r="JY27" t="inlineStr"/>
+      <c r="JZ27" t="inlineStr"/>
+      <c r="KA27" t="inlineStr"/>
+      <c r="KB27" t="inlineStr"/>
+      <c r="KC27" t="inlineStr"/>
+      <c r="KD27" t="inlineStr"/>
+      <c r="KE27" t="inlineStr"/>
+      <c r="KF27" t="inlineStr"/>
+      <c r="KG27" t="inlineStr"/>
+      <c r="KH27" t="inlineStr"/>
+      <c r="KI27" t="inlineStr"/>
+      <c r="KJ27" t="inlineStr"/>
+      <c r="KK27" t="inlineStr"/>
+      <c r="KL27" t="inlineStr"/>
+      <c r="KM27" t="inlineStr"/>
+      <c r="KN27" t="inlineStr"/>
+      <c r="KO27" t="inlineStr"/>
+      <c r="KP27" t="inlineStr"/>
+      <c r="KQ27" t="inlineStr"/>
+      <c r="KR27" t="inlineStr"/>
+      <c r="KS27" t="inlineStr"/>
+      <c r="KT27" t="inlineStr"/>
+      <c r="KU27" t="inlineStr"/>
+      <c r="KV27" t="inlineStr"/>
+      <c r="KW27" t="inlineStr"/>
+      <c r="KX27" t="inlineStr"/>
+      <c r="KY27" t="inlineStr"/>
+      <c r="KZ27" t="inlineStr"/>
+      <c r="LA27" t="inlineStr"/>
+      <c r="LB27" t="inlineStr"/>
+      <c r="LC27" t="inlineStr"/>
+      <c r="LD27" t="inlineStr"/>
+      <c r="LE27" t="inlineStr"/>
+      <c r="LF27" t="inlineStr"/>
+      <c r="LG27" t="inlineStr"/>
+      <c r="LH27" t="inlineStr"/>
+      <c r="LI27" t="inlineStr"/>
+      <c r="LJ27" t="inlineStr"/>
+      <c r="LK27" t="inlineStr"/>
+      <c r="LL27" t="inlineStr"/>
+      <c r="LM27" t="inlineStr"/>
+      <c r="LN27" t="inlineStr"/>
+      <c r="LO27" t="inlineStr"/>
+      <c r="LP27" t="inlineStr"/>
+      <c r="LQ27" t="inlineStr"/>
+      <c r="LR27" t="inlineStr"/>
+      <c r="LS27" t="inlineStr"/>
+      <c r="LT27" t="inlineStr"/>
+      <c r="LU27" t="inlineStr"/>
+      <c r="LV27" t="inlineStr"/>
+      <c r="LW27" t="inlineStr"/>
+      <c r="LX27" t="inlineStr"/>
+      <c r="LY27" t="inlineStr"/>
+      <c r="LZ27" t="inlineStr"/>
+      <c r="MA27" t="inlineStr"/>
+      <c r="MB27" t="inlineStr"/>
+      <c r="MC27" t="inlineStr"/>
+      <c r="MD27" t="inlineStr"/>
+      <c r="ME27" t="inlineStr"/>
+      <c r="MF27" t="inlineStr"/>
+      <c r="MG27" t="inlineStr"/>
+      <c r="MH27" t="inlineStr"/>
+      <c r="MI27" t="inlineStr"/>
+      <c r="MJ27" t="inlineStr"/>
+      <c r="MK27" t="inlineStr"/>
+      <c r="ML27" t="inlineStr"/>
+      <c r="MM27" t="inlineStr"/>
+      <c r="MN27" t="inlineStr"/>
+      <c r="MO27" t="inlineStr"/>
+      <c r="MP27" t="inlineStr"/>
+      <c r="MQ27" t="inlineStr"/>
+      <c r="MR27" t="inlineStr"/>
+      <c r="MS27" t="inlineStr"/>
+      <c r="MT27" t="inlineStr"/>
+      <c r="MU27" t="inlineStr"/>
+      <c r="MV27" t="inlineStr"/>
+      <c r="MW27" t="inlineStr"/>
+      <c r="MX27" t="inlineStr"/>
+      <c r="MY27" t="inlineStr"/>
+      <c r="MZ27" t="inlineStr"/>
+      <c r="NA27" t="inlineStr"/>
+      <c r="NB27" t="inlineStr"/>
+      <c r="NC27" t="inlineStr"/>
+      <c r="ND27" t="inlineStr"/>
+      <c r="NE27" t="inlineStr"/>
+      <c r="NF27" t="inlineStr"/>
+      <c r="NG27" t="inlineStr"/>
+      <c r="NH27" t="inlineStr"/>
+      <c r="NI27" t="inlineStr"/>
+      <c r="NJ27" t="inlineStr"/>
+      <c r="NK27" t="inlineStr"/>
+      <c r="NL27" t="inlineStr"/>
+      <c r="NM27" t="inlineStr"/>
+      <c r="NN27" t="inlineStr"/>
+      <c r="NO27" t="inlineStr"/>
+      <c r="NP27" t="inlineStr"/>
+      <c r="NQ27" t="inlineStr"/>
+      <c r="NR27" t="inlineStr"/>
+      <c r="NS27" t="inlineStr"/>
+      <c r="NT27" t="inlineStr"/>
+      <c r="NU27" t="inlineStr"/>
+      <c r="NV27" t="inlineStr"/>
+      <c r="NW27" t="inlineStr"/>
+      <c r="NX27" t="inlineStr"/>
+      <c r="NY27" t="inlineStr"/>
+      <c r="NZ27" t="inlineStr"/>
+      <c r="OA27" t="inlineStr"/>
+      <c r="OB27" t="inlineStr"/>
+      <c r="OC27" t="inlineStr"/>
+      <c r="OD27" t="inlineStr"/>
+      <c r="OE27" t="inlineStr"/>
+      <c r="OF27" t="inlineStr"/>
+      <c r="OG27" t="inlineStr"/>
+      <c r="OH27" t="inlineStr"/>
+      <c r="OI27" t="inlineStr"/>
+      <c r="OJ27" t="inlineStr"/>
+      <c r="OK27" t="inlineStr"/>
+      <c r="OL27" t="inlineStr"/>
+      <c r="OM27" t="inlineStr"/>
+      <c r="ON27" t="inlineStr"/>
+      <c r="OO27" t="inlineStr"/>
+      <c r="OP27" t="inlineStr"/>
+      <c r="OQ27" t="inlineStr"/>
+      <c r="OR27" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
remove unused val: get_max_matched_res function
</commit_message>
<xml_diff>
--- a/OOMII.xlsx
+++ b/OOMII.xlsx
@@ -346,7 +346,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:OR27"/>
+  <dimension ref="A1:OR30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15202,12 +15202,6 @@
           <t>type01</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr"/>
-      <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr"/>
-      <c r="E27" t="inlineStr"/>
-      <c r="F27" t="inlineStr"/>
-      <c r="G27" t="inlineStr"/>
       <c r="H27" t="inlineStr">
         <is>
           <t>0.0625</t>
@@ -15238,9 +15232,6 @@
           <t>25.0</t>
         </is>
       </c>
-      <c r="N27" t="inlineStr"/>
-      <c r="O27" t="inlineStr"/>
-      <c r="P27" t="inlineStr"/>
       <c r="Q27" t="inlineStr">
         <is>
           <t>3.22</t>
@@ -15251,7 +15242,6 @@
           <t>3.03</t>
         </is>
       </c>
-      <c r="S27" t="inlineStr"/>
       <c r="T27" t="inlineStr">
         <is>
           <t>3.00</t>
@@ -15282,23 +15272,11 @@
           <t>2.75</t>
         </is>
       </c>
-      <c r="Z27" t="inlineStr"/>
-      <c r="AA27" t="inlineStr"/>
-      <c r="AB27" t="inlineStr"/>
-      <c r="AC27" t="inlineStr"/>
-      <c r="AD27" t="inlineStr"/>
-      <c r="AE27" t="inlineStr"/>
-      <c r="AF27" t="inlineStr"/>
-      <c r="AG27" t="inlineStr"/>
-      <c r="AH27" t="inlineStr"/>
-      <c r="AI27" t="inlineStr"/>
-      <c r="AJ27" t="inlineStr"/>
       <c r="AK27" t="inlineStr">
         <is>
           <t>94</t>
         </is>
       </c>
-      <c r="AL27" t="inlineStr"/>
       <c r="AM27" t="inlineStr">
         <is>
           <t>93</t>
@@ -15329,10 +15307,6 @@
           <t>35</t>
         </is>
       </c>
-      <c r="AS27" t="inlineStr"/>
-      <c r="AT27" t="inlineStr"/>
-      <c r="AU27" t="inlineStr"/>
-      <c r="AV27" t="inlineStr"/>
       <c r="AW27" t="inlineStr">
         <is>
           <t>-1</t>
@@ -15363,18 +15337,6 @@
           <t>-9</t>
         </is>
       </c>
-      <c r="BC27" t="inlineStr"/>
-      <c r="BD27" t="inlineStr"/>
-      <c r="BE27" t="inlineStr"/>
-      <c r="BF27" t="inlineStr"/>
-      <c r="BG27" t="inlineStr"/>
-      <c r="BH27" t="inlineStr"/>
-      <c r="BI27" t="inlineStr"/>
-      <c r="BJ27" t="inlineStr"/>
-      <c r="BK27" t="inlineStr"/>
-      <c r="BL27" t="inlineStr"/>
-      <c r="BM27" t="inlineStr"/>
-      <c r="BN27" t="inlineStr"/>
       <c r="BO27" t="inlineStr">
         <is>
           <t>0.0625</t>
@@ -15405,9 +15367,6 @@
           <t>25.0</t>
         </is>
       </c>
-      <c r="BU27" t="inlineStr"/>
-      <c r="BV27" t="inlineStr"/>
-      <c r="BW27" t="inlineStr"/>
       <c r="BX27" t="inlineStr">
         <is>
           <t>2.51</t>
@@ -15418,7 +15377,6 @@
           <t>2.20</t>
         </is>
       </c>
-      <c r="BZ27" t="inlineStr"/>
       <c r="CA27" t="inlineStr">
         <is>
           <t>2.23</t>
@@ -15449,23 +15407,11 @@
           <t>1.99</t>
         </is>
       </c>
-      <c r="CG27" t="inlineStr"/>
-      <c r="CH27" t="inlineStr"/>
-      <c r="CI27" t="inlineStr"/>
-      <c r="CJ27" t="inlineStr"/>
-      <c r="CK27" t="inlineStr"/>
-      <c r="CL27" t="inlineStr"/>
-      <c r="CM27" t="inlineStr"/>
-      <c r="CN27" t="inlineStr"/>
-      <c r="CO27" t="inlineStr"/>
-      <c r="CP27" t="inlineStr"/>
-      <c r="CQ27" t="inlineStr"/>
       <c r="CR27" t="inlineStr">
         <is>
           <t>91</t>
         </is>
       </c>
-      <c r="CS27" t="inlineStr"/>
       <c r="CT27" t="inlineStr">
         <is>
           <t>39</t>
@@ -15496,10 +15442,6 @@
           <t>79</t>
         </is>
       </c>
-      <c r="CZ27" t="inlineStr"/>
-      <c r="DA27" t="inlineStr"/>
-      <c r="DB27" t="inlineStr"/>
-      <c r="DC27" t="inlineStr"/>
       <c r="DD27" t="inlineStr">
         <is>
           <t>-2</t>
@@ -15530,36 +15472,11 @@
           <t>-13</t>
         </is>
       </c>
-      <c r="DJ27" t="inlineStr"/>
-      <c r="DK27" t="inlineStr"/>
-      <c r="DL27" t="inlineStr"/>
-      <c r="DM27" t="inlineStr"/>
-      <c r="DN27" t="inlineStr"/>
-      <c r="DO27" t="inlineStr"/>
       <c r="DP27" t="inlineStr">
         <is>
           <t>220</t>
         </is>
       </c>
-      <c r="DQ27" t="inlineStr"/>
-      <c r="DR27" t="inlineStr"/>
-      <c r="DS27" t="inlineStr"/>
-      <c r="DT27" t="inlineStr"/>
-      <c r="DU27" t="inlineStr"/>
-      <c r="DV27" t="inlineStr"/>
-      <c r="DW27" t="inlineStr"/>
-      <c r="DX27" t="inlineStr"/>
-      <c r="DY27" t="inlineStr"/>
-      <c r="DZ27" t="inlineStr"/>
-      <c r="EA27" t="inlineStr"/>
-      <c r="EB27" t="inlineStr"/>
-      <c r="EC27" t="inlineStr"/>
-      <c r="ED27" t="inlineStr"/>
-      <c r="EE27" t="inlineStr"/>
-      <c r="EF27" t="inlineStr"/>
-      <c r="EG27" t="inlineStr"/>
-      <c r="EH27" t="inlineStr"/>
-      <c r="EI27" t="inlineStr"/>
       <c r="EJ27" t="inlineStr">
         <is>
           <t>2.57</t>
@@ -15590,16 +15507,11 @@
           <t>1.69</t>
         </is>
       </c>
-      <c r="EP27" t="inlineStr"/>
-      <c r="EQ27" t="inlineStr"/>
-      <c r="ER27" t="inlineStr"/>
-      <c r="ES27" t="inlineStr"/>
       <c r="ET27" t="inlineStr">
         <is>
           <t>68</t>
         </is>
       </c>
-      <c r="EU27" t="inlineStr"/>
       <c r="EV27" t="inlineStr">
         <is>
           <t>55</t>
@@ -15630,29 +15542,6 @@
           <t>51</t>
         </is>
       </c>
-      <c r="FB27" t="inlineStr"/>
-      <c r="FC27" t="inlineStr"/>
-      <c r="FD27" t="inlineStr"/>
-      <c r="FE27" t="inlineStr"/>
-      <c r="FF27" t="inlineStr"/>
-      <c r="FG27" t="inlineStr"/>
-      <c r="FH27" t="inlineStr"/>
-      <c r="FI27" t="inlineStr"/>
-      <c r="FJ27" t="inlineStr"/>
-      <c r="FK27" t="inlineStr"/>
-      <c r="FL27" t="inlineStr"/>
-      <c r="FM27" t="inlineStr"/>
-      <c r="FN27" t="inlineStr"/>
-      <c r="FO27" t="inlineStr"/>
-      <c r="FP27" t="inlineStr"/>
-      <c r="FQ27" t="inlineStr"/>
-      <c r="FR27" t="inlineStr"/>
-      <c r="FS27" t="inlineStr"/>
-      <c r="FT27" t="inlineStr"/>
-      <c r="FU27" t="inlineStr"/>
-      <c r="FV27" t="inlineStr"/>
-      <c r="FW27" t="inlineStr"/>
-      <c r="FX27" t="inlineStr"/>
       <c r="FY27" t="inlineStr">
         <is>
           <t>-4</t>
@@ -15683,51 +15572,6 @@
           <t>-24</t>
         </is>
       </c>
-      <c r="GE27" t="inlineStr"/>
-      <c r="GF27" t="inlineStr"/>
-      <c r="GG27" t="inlineStr"/>
-      <c r="GH27" t="inlineStr"/>
-      <c r="GI27" t="inlineStr"/>
-      <c r="GJ27" t="inlineStr"/>
-      <c r="GK27" t="inlineStr"/>
-      <c r="GL27" t="inlineStr"/>
-      <c r="GM27" t="inlineStr"/>
-      <c r="GN27" t="inlineStr"/>
-      <c r="GO27" t="inlineStr"/>
-      <c r="GP27" t="inlineStr"/>
-      <c r="GQ27" t="inlineStr"/>
-      <c r="GR27" t="inlineStr"/>
-      <c r="GS27" t="inlineStr"/>
-      <c r="GT27" t="inlineStr"/>
-      <c r="GU27" t="inlineStr"/>
-      <c r="GV27" t="inlineStr"/>
-      <c r="GW27" t="inlineStr"/>
-      <c r="GX27" t="inlineStr"/>
-      <c r="GY27" t="inlineStr"/>
-      <c r="GZ27" t="inlineStr"/>
-      <c r="HA27" t="inlineStr"/>
-      <c r="HB27" t="inlineStr"/>
-      <c r="HC27" t="inlineStr"/>
-      <c r="HD27" t="inlineStr"/>
-      <c r="HE27" t="inlineStr"/>
-      <c r="HF27" t="inlineStr"/>
-      <c r="HG27" t="inlineStr"/>
-      <c r="HH27" t="inlineStr"/>
-      <c r="HI27" t="inlineStr"/>
-      <c r="HJ27" t="inlineStr"/>
-      <c r="HK27" t="inlineStr"/>
-      <c r="HL27" t="inlineStr"/>
-      <c r="HM27" t="inlineStr"/>
-      <c r="HN27" t="inlineStr"/>
-      <c r="HO27" t="inlineStr"/>
-      <c r="HP27" t="inlineStr"/>
-      <c r="HQ27" t="inlineStr"/>
-      <c r="HR27" t="inlineStr"/>
-      <c r="HS27" t="inlineStr"/>
-      <c r="HT27" t="inlineStr"/>
-      <c r="HU27" t="inlineStr"/>
-      <c r="HV27" t="inlineStr"/>
-      <c r="HW27" t="inlineStr"/>
       <c r="HX27" t="inlineStr">
         <is>
           <t>0.0625</t>
@@ -15758,9 +15602,6 @@
           <t>25.0</t>
         </is>
       </c>
-      <c r="ID27" t="inlineStr"/>
-      <c r="IE27" t="inlineStr"/>
-      <c r="IF27" t="inlineStr"/>
       <c r="IG27" t="inlineStr">
         <is>
           <t>5.45</t>
@@ -15771,7 +15612,6 @@
           <t>9.33</t>
         </is>
       </c>
-      <c r="II27" t="inlineStr"/>
       <c r="IJ27" t="inlineStr">
         <is>
           <t>7.32</t>
@@ -15802,23 +15642,11 @@
           <t>7.31</t>
         </is>
       </c>
-      <c r="IP27" t="inlineStr"/>
-      <c r="IQ27" t="inlineStr"/>
-      <c r="IR27" t="inlineStr"/>
-      <c r="IS27" t="inlineStr"/>
-      <c r="IT27" t="inlineStr"/>
-      <c r="IU27" t="inlineStr"/>
-      <c r="IV27" t="inlineStr"/>
-      <c r="IW27" t="inlineStr"/>
-      <c r="IX27" t="inlineStr"/>
-      <c r="IY27" t="inlineStr"/>
-      <c r="IZ27" t="inlineStr"/>
       <c r="JA27" t="inlineStr">
         <is>
           <t>153</t>
         </is>
       </c>
-      <c r="JB27" t="inlineStr"/>
       <c r="JC27" t="inlineStr">
         <is>
           <t>143</t>
@@ -15849,10 +15677,6 @@
           <t>134</t>
         </is>
       </c>
-      <c r="JI27" t="inlineStr"/>
-      <c r="JJ27" t="inlineStr"/>
-      <c r="JK27" t="inlineStr"/>
-      <c r="JL27" t="inlineStr"/>
       <c r="JM27" t="inlineStr">
         <is>
           <t>-9</t>
@@ -15883,136 +15707,2464 @@
           <t>-15</t>
         </is>
       </c>
-      <c r="JS27" t="inlineStr"/>
-      <c r="JT27" t="inlineStr"/>
-      <c r="JU27" t="inlineStr"/>
-      <c r="JV27" t="inlineStr"/>
-      <c r="JW27" t="inlineStr"/>
-      <c r="JX27" t="inlineStr"/>
-      <c r="JY27" t="inlineStr"/>
-      <c r="JZ27" t="inlineStr"/>
-      <c r="KA27" t="inlineStr"/>
-      <c r="KB27" t="inlineStr"/>
-      <c r="KC27" t="inlineStr"/>
-      <c r="KD27" t="inlineStr"/>
-      <c r="KE27" t="inlineStr"/>
-      <c r="KF27" t="inlineStr"/>
-      <c r="KG27" t="inlineStr"/>
-      <c r="KH27" t="inlineStr"/>
-      <c r="KI27" t="inlineStr"/>
-      <c r="KJ27" t="inlineStr"/>
-      <c r="KK27" t="inlineStr"/>
-      <c r="KL27" t="inlineStr"/>
-      <c r="KM27" t="inlineStr"/>
-      <c r="KN27" t="inlineStr"/>
-      <c r="KO27" t="inlineStr"/>
-      <c r="KP27" t="inlineStr"/>
-      <c r="KQ27" t="inlineStr"/>
-      <c r="KR27" t="inlineStr"/>
-      <c r="KS27" t="inlineStr"/>
-      <c r="KT27" t="inlineStr"/>
-      <c r="KU27" t="inlineStr"/>
-      <c r="KV27" t="inlineStr"/>
-      <c r="KW27" t="inlineStr"/>
-      <c r="KX27" t="inlineStr"/>
-      <c r="KY27" t="inlineStr"/>
-      <c r="KZ27" t="inlineStr"/>
-      <c r="LA27" t="inlineStr"/>
-      <c r="LB27" t="inlineStr"/>
-      <c r="LC27" t="inlineStr"/>
-      <c r="LD27" t="inlineStr"/>
-      <c r="LE27" t="inlineStr"/>
-      <c r="LF27" t="inlineStr"/>
-      <c r="LG27" t="inlineStr"/>
-      <c r="LH27" t="inlineStr"/>
-      <c r="LI27" t="inlineStr"/>
-      <c r="LJ27" t="inlineStr"/>
-      <c r="LK27" t="inlineStr"/>
-      <c r="LL27" t="inlineStr"/>
-      <c r="LM27" t="inlineStr"/>
-      <c r="LN27" t="inlineStr"/>
-      <c r="LO27" t="inlineStr"/>
-      <c r="LP27" t="inlineStr"/>
-      <c r="LQ27" t="inlineStr"/>
-      <c r="LR27" t="inlineStr"/>
-      <c r="LS27" t="inlineStr"/>
-      <c r="LT27" t="inlineStr"/>
-      <c r="LU27" t="inlineStr"/>
-      <c r="LV27" t="inlineStr"/>
-      <c r="LW27" t="inlineStr"/>
-      <c r="LX27" t="inlineStr"/>
-      <c r="LY27" t="inlineStr"/>
-      <c r="LZ27" t="inlineStr"/>
-      <c r="MA27" t="inlineStr"/>
-      <c r="MB27" t="inlineStr"/>
-      <c r="MC27" t="inlineStr"/>
-      <c r="MD27" t="inlineStr"/>
-      <c r="ME27" t="inlineStr"/>
-      <c r="MF27" t="inlineStr"/>
-      <c r="MG27" t="inlineStr"/>
-      <c r="MH27" t="inlineStr"/>
-      <c r="MI27" t="inlineStr"/>
-      <c r="MJ27" t="inlineStr"/>
-      <c r="MK27" t="inlineStr"/>
-      <c r="ML27" t="inlineStr"/>
-      <c r="MM27" t="inlineStr"/>
-      <c r="MN27" t="inlineStr"/>
-      <c r="MO27" t="inlineStr"/>
-      <c r="MP27" t="inlineStr"/>
-      <c r="MQ27" t="inlineStr"/>
-      <c r="MR27" t="inlineStr"/>
-      <c r="MS27" t="inlineStr"/>
-      <c r="MT27" t="inlineStr"/>
-      <c r="MU27" t="inlineStr"/>
-      <c r="MV27" t="inlineStr"/>
-      <c r="MW27" t="inlineStr"/>
-      <c r="MX27" t="inlineStr"/>
-      <c r="MY27" t="inlineStr"/>
-      <c r="MZ27" t="inlineStr"/>
-      <c r="NA27" t="inlineStr"/>
-      <c r="NB27" t="inlineStr"/>
-      <c r="NC27" t="inlineStr"/>
-      <c r="ND27" t="inlineStr"/>
-      <c r="NE27" t="inlineStr"/>
-      <c r="NF27" t="inlineStr"/>
-      <c r="NG27" t="inlineStr"/>
-      <c r="NH27" t="inlineStr"/>
-      <c r="NI27" t="inlineStr"/>
-      <c r="NJ27" t="inlineStr"/>
-      <c r="NK27" t="inlineStr"/>
-      <c r="NL27" t="inlineStr"/>
-      <c r="NM27" t="inlineStr"/>
-      <c r="NN27" t="inlineStr"/>
-      <c r="NO27" t="inlineStr"/>
-      <c r="NP27" t="inlineStr"/>
-      <c r="NQ27" t="inlineStr"/>
-      <c r="NR27" t="inlineStr"/>
-      <c r="NS27" t="inlineStr"/>
-      <c r="NT27" t="inlineStr"/>
-      <c r="NU27" t="inlineStr"/>
-      <c r="NV27" t="inlineStr"/>
-      <c r="NW27" t="inlineStr"/>
-      <c r="NX27" t="inlineStr"/>
-      <c r="NY27" t="inlineStr"/>
-      <c r="NZ27" t="inlineStr"/>
-      <c r="OA27" t="inlineStr"/>
-      <c r="OB27" t="inlineStr"/>
-      <c r="OC27" t="inlineStr"/>
-      <c r="OD27" t="inlineStr"/>
-      <c r="OE27" t="inlineStr"/>
-      <c r="OF27" t="inlineStr"/>
-      <c r="OG27" t="inlineStr"/>
-      <c r="OH27" t="inlineStr"/>
-      <c r="OI27" t="inlineStr"/>
-      <c r="OJ27" t="inlineStr"/>
-      <c r="OK27" t="inlineStr"/>
-      <c r="OL27" t="inlineStr"/>
-      <c r="OM27" t="inlineStr"/>
-      <c r="ON27" t="inlineStr"/>
-      <c r="OO27" t="inlineStr"/>
-      <c r="OP27" t="inlineStr"/>
-      <c r="OQ27" t="inlineStr"/>
-      <c r="OR27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>type02</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>155</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>315</t>
+        </is>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>475</t>
+        </is>
+      </c>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>635</t>
+        </is>
+      </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>3.73</t>
+        </is>
+      </c>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>3.21</t>
+        </is>
+      </c>
+      <c r="T28" t="inlineStr">
+        <is>
+          <t>3.11</t>
+        </is>
+      </c>
+      <c r="U28" t="inlineStr">
+        <is>
+          <t>3.26</t>
+        </is>
+      </c>
+      <c r="V28" t="inlineStr">
+        <is>
+          <t>3.23</t>
+        </is>
+      </c>
+      <c r="W28" t="inlineStr">
+        <is>
+          <t>3.25</t>
+        </is>
+      </c>
+      <c r="X28" t="inlineStr">
+        <is>
+          <t>3.21</t>
+        </is>
+      </c>
+      <c r="Y28" t="inlineStr">
+        <is>
+          <t>3.16</t>
+        </is>
+      </c>
+      <c r="Z28" t="inlineStr">
+        <is>
+          <t>3.09</t>
+        </is>
+      </c>
+      <c r="AA28" t="inlineStr">
+        <is>
+          <t>3.16</t>
+        </is>
+      </c>
+      <c r="AB28" t="inlineStr">
+        <is>
+          <t>3.00</t>
+        </is>
+      </c>
+      <c r="AK28" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="AM28" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="AN28" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="AO28" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="AP28" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="AQ28" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="AR28" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="AS28" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="AT28" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="AU28" t="inlineStr">
+        <is>
+          <t>79</t>
+        </is>
+      </c>
+      <c r="AW28" t="inlineStr">
+        <is>
+          <t>-3</t>
+        </is>
+      </c>
+      <c r="AX28" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AY28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AZ28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BA28" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BB28" t="inlineStr">
+        <is>
+          <t>-2</t>
+        </is>
+      </c>
+      <c r="BC28" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="BD28" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="BE28" t="inlineStr">
+        <is>
+          <t>-7</t>
+        </is>
+      </c>
+      <c r="BO28" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BP28" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="BQ28" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="BR28" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="BS28" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="BT28" t="inlineStr">
+        <is>
+          <t>155</t>
+        </is>
+      </c>
+      <c r="BU28" t="inlineStr">
+        <is>
+          <t>315</t>
+        </is>
+      </c>
+      <c r="BV28" t="inlineStr">
+        <is>
+          <t>475</t>
+        </is>
+      </c>
+      <c r="BW28" t="inlineStr">
+        <is>
+          <t>635</t>
+        </is>
+      </c>
+      <c r="BX28" t="inlineStr">
+        <is>
+          <t>3.23</t>
+        </is>
+      </c>
+      <c r="BY28" t="inlineStr">
+        <is>
+          <t>2.71</t>
+        </is>
+      </c>
+      <c r="CA28" t="inlineStr">
+        <is>
+          <t>2.65</t>
+        </is>
+      </c>
+      <c r="CB28" t="inlineStr">
+        <is>
+          <t>2.31</t>
+        </is>
+      </c>
+      <c r="CC28" t="inlineStr">
+        <is>
+          <t>2.37</t>
+        </is>
+      </c>
+      <c r="CD28" t="inlineStr">
+        <is>
+          <t>2.66</t>
+        </is>
+      </c>
+      <c r="CE28" t="inlineStr">
+        <is>
+          <t>2.79</t>
+        </is>
+      </c>
+      <c r="CF28" t="inlineStr">
+        <is>
+          <t>2.35</t>
+        </is>
+      </c>
+      <c r="CG28" t="inlineStr">
+        <is>
+          <t>2.72</t>
+        </is>
+      </c>
+      <c r="CH28" t="inlineStr">
+        <is>
+          <t>2.32</t>
+        </is>
+      </c>
+      <c r="CI28" t="inlineStr">
+        <is>
+          <t>2.74</t>
+        </is>
+      </c>
+      <c r="CR28" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="CT28" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="CU28" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="CV28" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="CW28" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="CX28" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="CY28" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="CZ28" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="DA28" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="DB28" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="DD28" t="inlineStr">
+        <is>
+          <t>-2</t>
+        </is>
+      </c>
+      <c r="DE28" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="DF28" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="DG28" t="inlineStr">
+        <is>
+          <t>-2</t>
+        </is>
+      </c>
+      <c r="DH28" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="DI28" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="DJ28" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="DK28" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="DL28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="EJ28" t="inlineStr">
+        <is>
+          <t>3.33</t>
+        </is>
+      </c>
+      <c r="EK28" t="inlineStr">
+        <is>
+          <t>2.70</t>
+        </is>
+      </c>
+      <c r="EL28" t="inlineStr">
+        <is>
+          <t>2.70</t>
+        </is>
+      </c>
+      <c r="EM28" t="inlineStr">
+        <is>
+          <t>2.94</t>
+        </is>
+      </c>
+      <c r="EN28" t="inlineStr">
+        <is>
+          <t>2.33</t>
+        </is>
+      </c>
+      <c r="EO28" t="inlineStr">
+        <is>
+          <t>2.55</t>
+        </is>
+      </c>
+      <c r="EP28" t="inlineStr">
+        <is>
+          <t>2.93</t>
+        </is>
+      </c>
+      <c r="EQ28" t="inlineStr">
+        <is>
+          <t>3.37</t>
+        </is>
+      </c>
+      <c r="ER28" t="inlineStr">
+        <is>
+          <t>3.35</t>
+        </is>
+      </c>
+      <c r="ET28" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
+      </c>
+      <c r="EV28" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="EW28" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="EX28" t="inlineStr">
+        <is>
+          <t>73</t>
+        </is>
+      </c>
+      <c r="EY28" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="EZ28" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="FA28" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="FB28" t="inlineStr">
+        <is>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="FC28" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="FD28" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="FY28" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="FZ28" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="GA28" t="inlineStr">
+        <is>
+          <t>-2</t>
+        </is>
+      </c>
+      <c r="GB28" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="GC28" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="GD28" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="GE28" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="GF28" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="GG28" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="HX28" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="HY28" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="HZ28" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="IA28" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="IB28" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="IC28" t="inlineStr">
+        <is>
+          <t>155</t>
+        </is>
+      </c>
+      <c r="ID28" t="inlineStr">
+        <is>
+          <t>315</t>
+        </is>
+      </c>
+      <c r="IE28" t="inlineStr">
+        <is>
+          <t>475</t>
+        </is>
+      </c>
+      <c r="IF28" t="inlineStr">
+        <is>
+          <t>635</t>
+        </is>
+      </c>
+      <c r="IG28" t="inlineStr">
+        <is>
+          <t>3.53</t>
+        </is>
+      </c>
+      <c r="IH28" t="inlineStr">
+        <is>
+          <t>4.35</t>
+        </is>
+      </c>
+      <c r="IJ28" t="inlineStr">
+        <is>
+          <t>4.37</t>
+        </is>
+      </c>
+      <c r="IK28" t="inlineStr">
+        <is>
+          <t>4.77</t>
+        </is>
+      </c>
+      <c r="IL28" t="inlineStr">
+        <is>
+          <t>5.32</t>
+        </is>
+      </c>
+      <c r="IM28" t="inlineStr">
+        <is>
+          <t>4.76</t>
+        </is>
+      </c>
+      <c r="IN28" t="inlineStr">
+        <is>
+          <t>5.14</t>
+        </is>
+      </c>
+      <c r="IO28" t="inlineStr">
+        <is>
+          <t>5.72</t>
+        </is>
+      </c>
+      <c r="IP28" t="inlineStr">
+        <is>
+          <t>5.33</t>
+        </is>
+      </c>
+      <c r="IQ28" t="inlineStr">
+        <is>
+          <t>5.95</t>
+        </is>
+      </c>
+      <c r="IR28" t="inlineStr">
+        <is>
+          <t>6.76</t>
+        </is>
+      </c>
+      <c r="JA28" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
+      </c>
+      <c r="JC28" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
+      </c>
+      <c r="JD28" t="inlineStr">
+        <is>
+          <t>72</t>
+        </is>
+      </c>
+      <c r="JE28" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="JF28" t="inlineStr">
+        <is>
+          <t>72</t>
+        </is>
+      </c>
+      <c r="JG28" t="inlineStr">
+        <is>
+          <t>73</t>
+        </is>
+      </c>
+      <c r="JH28" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="JI28" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="JJ28" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="JK28" t="inlineStr">
+        <is>
+          <t>103</t>
+        </is>
+      </c>
+      <c r="JM28" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="JN28" t="inlineStr">
+        <is>
+          <t>-2</t>
+        </is>
+      </c>
+      <c r="JO28" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="JP28" t="inlineStr">
+        <is>
+          <t>-2</t>
+        </is>
+      </c>
+      <c r="JQ28" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="JR28" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="JS28" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="JT28" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="JU28" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>type02</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>155</t>
+        </is>
+      </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>315</t>
+        </is>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>475</t>
+        </is>
+      </c>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t>635</t>
+        </is>
+      </c>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>3.73</t>
+        </is>
+      </c>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t>3.21</t>
+        </is>
+      </c>
+      <c r="T29" t="inlineStr">
+        <is>
+          <t>3.11</t>
+        </is>
+      </c>
+      <c r="U29" t="inlineStr">
+        <is>
+          <t>3.26</t>
+        </is>
+      </c>
+      <c r="V29" t="inlineStr">
+        <is>
+          <t>3.23</t>
+        </is>
+      </c>
+      <c r="W29" t="inlineStr">
+        <is>
+          <t>3.25</t>
+        </is>
+      </c>
+      <c r="X29" t="inlineStr">
+        <is>
+          <t>3.21</t>
+        </is>
+      </c>
+      <c r="Y29" t="inlineStr">
+        <is>
+          <t>3.16</t>
+        </is>
+      </c>
+      <c r="Z29" t="inlineStr">
+        <is>
+          <t>3.09</t>
+        </is>
+      </c>
+      <c r="AA29" t="inlineStr">
+        <is>
+          <t>3.16</t>
+        </is>
+      </c>
+      <c r="AB29" t="inlineStr">
+        <is>
+          <t>3.00</t>
+        </is>
+      </c>
+      <c r="AK29" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="AM29" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="AN29" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="AO29" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="AP29" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="AQ29" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="AR29" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="AS29" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="AT29" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="AU29" t="inlineStr">
+        <is>
+          <t>79</t>
+        </is>
+      </c>
+      <c r="AW29" t="inlineStr">
+        <is>
+          <t>-3</t>
+        </is>
+      </c>
+      <c r="AX29" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AY29" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AZ29" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BA29" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BB29" t="inlineStr">
+        <is>
+          <t>-2</t>
+        </is>
+      </c>
+      <c r="BC29" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="BD29" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="BE29" t="inlineStr">
+        <is>
+          <t>-7</t>
+        </is>
+      </c>
+      <c r="BO29" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BP29" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="BQ29" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="BR29" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="BS29" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="BT29" t="inlineStr">
+        <is>
+          <t>155</t>
+        </is>
+      </c>
+      <c r="BU29" t="inlineStr">
+        <is>
+          <t>315</t>
+        </is>
+      </c>
+      <c r="BV29" t="inlineStr">
+        <is>
+          <t>475</t>
+        </is>
+      </c>
+      <c r="BW29" t="inlineStr">
+        <is>
+          <t>635</t>
+        </is>
+      </c>
+      <c r="BX29" t="inlineStr">
+        <is>
+          <t>3.23</t>
+        </is>
+      </c>
+      <c r="BY29" t="inlineStr">
+        <is>
+          <t>2.71</t>
+        </is>
+      </c>
+      <c r="CA29" t="inlineStr">
+        <is>
+          <t>2.65</t>
+        </is>
+      </c>
+      <c r="CB29" t="inlineStr">
+        <is>
+          <t>2.31</t>
+        </is>
+      </c>
+      <c r="CC29" t="inlineStr">
+        <is>
+          <t>2.37</t>
+        </is>
+      </c>
+      <c r="CD29" t="inlineStr">
+        <is>
+          <t>2.66</t>
+        </is>
+      </c>
+      <c r="CE29" t="inlineStr">
+        <is>
+          <t>2.79</t>
+        </is>
+      </c>
+      <c r="CF29" t="inlineStr">
+        <is>
+          <t>2.35</t>
+        </is>
+      </c>
+      <c r="CG29" t="inlineStr">
+        <is>
+          <t>2.72</t>
+        </is>
+      </c>
+      <c r="CH29" t="inlineStr">
+        <is>
+          <t>2.32</t>
+        </is>
+      </c>
+      <c r="CI29" t="inlineStr">
+        <is>
+          <t>2.74</t>
+        </is>
+      </c>
+      <c r="CR29" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="CT29" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="CU29" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="CV29" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="CW29" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="CX29" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="CY29" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="CZ29" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="DA29" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="DB29" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="DD29" t="inlineStr">
+        <is>
+          <t>-2</t>
+        </is>
+      </c>
+      <c r="DE29" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="DF29" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="DG29" t="inlineStr">
+        <is>
+          <t>-2</t>
+        </is>
+      </c>
+      <c r="DH29" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="DI29" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="DJ29" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="DK29" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="DL29" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="EJ29" t="inlineStr">
+        <is>
+          <t>3.33</t>
+        </is>
+      </c>
+      <c r="EK29" t="inlineStr">
+        <is>
+          <t>2.70</t>
+        </is>
+      </c>
+      <c r="EL29" t="inlineStr">
+        <is>
+          <t>2.70</t>
+        </is>
+      </c>
+      <c r="EM29" t="inlineStr">
+        <is>
+          <t>2.94</t>
+        </is>
+      </c>
+      <c r="EN29" t="inlineStr">
+        <is>
+          <t>2.33</t>
+        </is>
+      </c>
+      <c r="EO29" t="inlineStr">
+        <is>
+          <t>2.55</t>
+        </is>
+      </c>
+      <c r="EP29" t="inlineStr">
+        <is>
+          <t>2.93</t>
+        </is>
+      </c>
+      <c r="EQ29" t="inlineStr">
+        <is>
+          <t>3.37</t>
+        </is>
+      </c>
+      <c r="ER29" t="inlineStr">
+        <is>
+          <t>3.35</t>
+        </is>
+      </c>
+      <c r="ET29" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
+      </c>
+      <c r="EV29" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="EW29" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="EX29" t="inlineStr">
+        <is>
+          <t>73</t>
+        </is>
+      </c>
+      <c r="EY29" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="EZ29" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="FA29" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="FB29" t="inlineStr">
+        <is>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="FC29" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="FD29" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="FY29" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="FZ29" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="GA29" t="inlineStr">
+        <is>
+          <t>-2</t>
+        </is>
+      </c>
+      <c r="GB29" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="GC29" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="GD29" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="GE29" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="GF29" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="GG29" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="HX29" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="HY29" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="HZ29" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="IA29" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="IB29" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="IC29" t="inlineStr">
+        <is>
+          <t>155</t>
+        </is>
+      </c>
+      <c r="ID29" t="inlineStr">
+        <is>
+          <t>315</t>
+        </is>
+      </c>
+      <c r="IE29" t="inlineStr">
+        <is>
+          <t>475</t>
+        </is>
+      </c>
+      <c r="IF29" t="inlineStr">
+        <is>
+          <t>635</t>
+        </is>
+      </c>
+      <c r="IG29" t="inlineStr">
+        <is>
+          <t>3.53</t>
+        </is>
+      </c>
+      <c r="IH29" t="inlineStr">
+        <is>
+          <t>4.35</t>
+        </is>
+      </c>
+      <c r="IJ29" t="inlineStr">
+        <is>
+          <t>4.37</t>
+        </is>
+      </c>
+      <c r="IK29" t="inlineStr">
+        <is>
+          <t>4.77</t>
+        </is>
+      </c>
+      <c r="IL29" t="inlineStr">
+        <is>
+          <t>5.32</t>
+        </is>
+      </c>
+      <c r="IM29" t="inlineStr">
+        <is>
+          <t>4.76</t>
+        </is>
+      </c>
+      <c r="IN29" t="inlineStr">
+        <is>
+          <t>5.14</t>
+        </is>
+      </c>
+      <c r="IO29" t="inlineStr">
+        <is>
+          <t>5.72</t>
+        </is>
+      </c>
+      <c r="IP29" t="inlineStr">
+        <is>
+          <t>5.33</t>
+        </is>
+      </c>
+      <c r="IQ29" t="inlineStr">
+        <is>
+          <t>5.95</t>
+        </is>
+      </c>
+      <c r="IR29" t="inlineStr">
+        <is>
+          <t>6.76</t>
+        </is>
+      </c>
+      <c r="JA29" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
+      </c>
+      <c r="JC29" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
+      </c>
+      <c r="JD29" t="inlineStr">
+        <is>
+          <t>72</t>
+        </is>
+      </c>
+      <c r="JE29" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="JF29" t="inlineStr">
+        <is>
+          <t>72</t>
+        </is>
+      </c>
+      <c r="JG29" t="inlineStr">
+        <is>
+          <t>73</t>
+        </is>
+      </c>
+      <c r="JH29" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="JI29" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="JJ29" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="JK29" t="inlineStr">
+        <is>
+          <t>103</t>
+        </is>
+      </c>
+      <c r="JM29" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="JN29" t="inlineStr">
+        <is>
+          <t>-2</t>
+        </is>
+      </c>
+      <c r="JO29" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="JP29" t="inlineStr">
+        <is>
+          <t>-2</t>
+        </is>
+      </c>
+      <c r="JQ29" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="JR29" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="JS29" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="JT29" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="JU29" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>type02</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr"/>
+      <c r="C30" t="inlineStr"/>
+      <c r="D30" t="inlineStr"/>
+      <c r="E30" t="inlineStr"/>
+      <c r="F30" t="inlineStr"/>
+      <c r="G30" t="inlineStr"/>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>155</t>
+        </is>
+      </c>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>315</t>
+        </is>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>475</t>
+        </is>
+      </c>
+      <c r="P30" t="inlineStr">
+        <is>
+          <t>635</t>
+        </is>
+      </c>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>3.73</t>
+        </is>
+      </c>
+      <c r="R30" t="inlineStr">
+        <is>
+          <t>3.21</t>
+        </is>
+      </c>
+      <c r="S30" t="inlineStr"/>
+      <c r="T30" t="inlineStr">
+        <is>
+          <t>3.11</t>
+        </is>
+      </c>
+      <c r="U30" t="inlineStr">
+        <is>
+          <t>3.26</t>
+        </is>
+      </c>
+      <c r="V30" t="inlineStr">
+        <is>
+          <t>3.23</t>
+        </is>
+      </c>
+      <c r="W30" t="inlineStr">
+        <is>
+          <t>3.25</t>
+        </is>
+      </c>
+      <c r="X30" t="inlineStr">
+        <is>
+          <t>3.21</t>
+        </is>
+      </c>
+      <c r="Y30" t="inlineStr">
+        <is>
+          <t>3.16</t>
+        </is>
+      </c>
+      <c r="Z30" t="inlineStr">
+        <is>
+          <t>3.09</t>
+        </is>
+      </c>
+      <c r="AA30" t="inlineStr">
+        <is>
+          <t>3.16</t>
+        </is>
+      </c>
+      <c r="AB30" t="inlineStr">
+        <is>
+          <t>3.00</t>
+        </is>
+      </c>
+      <c r="AC30" t="inlineStr"/>
+      <c r="AD30" t="inlineStr"/>
+      <c r="AE30" t="inlineStr"/>
+      <c r="AF30" t="inlineStr"/>
+      <c r="AG30" t="inlineStr"/>
+      <c r="AH30" t="inlineStr"/>
+      <c r="AI30" t="inlineStr"/>
+      <c r="AJ30" t="inlineStr"/>
+      <c r="AK30" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="AL30" t="inlineStr"/>
+      <c r="AM30" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="AN30" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="AO30" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="AP30" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="AQ30" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="AR30" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="AS30" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="AT30" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="AU30" t="inlineStr">
+        <is>
+          <t>79</t>
+        </is>
+      </c>
+      <c r="AV30" t="inlineStr"/>
+      <c r="AW30" t="inlineStr">
+        <is>
+          <t>-3</t>
+        </is>
+      </c>
+      <c r="AX30" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AY30" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AZ30" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BA30" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BB30" t="inlineStr">
+        <is>
+          <t>-2</t>
+        </is>
+      </c>
+      <c r="BC30" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="BD30" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="BE30" t="inlineStr">
+        <is>
+          <t>-7</t>
+        </is>
+      </c>
+      <c r="BF30" t="inlineStr"/>
+      <c r="BG30" t="inlineStr"/>
+      <c r="BH30" t="inlineStr"/>
+      <c r="BI30" t="inlineStr"/>
+      <c r="BJ30" t="inlineStr"/>
+      <c r="BK30" t="inlineStr"/>
+      <c r="BL30" t="inlineStr"/>
+      <c r="BM30" t="inlineStr"/>
+      <c r="BN30" t="inlineStr"/>
+      <c r="BO30" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BP30" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="BQ30" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="BR30" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="BS30" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="BT30" t="inlineStr">
+        <is>
+          <t>155</t>
+        </is>
+      </c>
+      <c r="BU30" t="inlineStr">
+        <is>
+          <t>315</t>
+        </is>
+      </c>
+      <c r="BV30" t="inlineStr">
+        <is>
+          <t>475</t>
+        </is>
+      </c>
+      <c r="BW30" t="inlineStr">
+        <is>
+          <t>635</t>
+        </is>
+      </c>
+      <c r="BX30" t="inlineStr">
+        <is>
+          <t>3.23</t>
+        </is>
+      </c>
+      <c r="BY30" t="inlineStr">
+        <is>
+          <t>2.71</t>
+        </is>
+      </c>
+      <c r="BZ30" t="inlineStr"/>
+      <c r="CA30" t="inlineStr">
+        <is>
+          <t>2.65</t>
+        </is>
+      </c>
+      <c r="CB30" t="inlineStr">
+        <is>
+          <t>2.31</t>
+        </is>
+      </c>
+      <c r="CC30" t="inlineStr">
+        <is>
+          <t>2.37</t>
+        </is>
+      </c>
+      <c r="CD30" t="inlineStr">
+        <is>
+          <t>2.66</t>
+        </is>
+      </c>
+      <c r="CE30" t="inlineStr">
+        <is>
+          <t>2.79</t>
+        </is>
+      </c>
+      <c r="CF30" t="inlineStr">
+        <is>
+          <t>2.35</t>
+        </is>
+      </c>
+      <c r="CG30" t="inlineStr">
+        <is>
+          <t>2.72</t>
+        </is>
+      </c>
+      <c r="CH30" t="inlineStr">
+        <is>
+          <t>2.32</t>
+        </is>
+      </c>
+      <c r="CI30" t="inlineStr">
+        <is>
+          <t>2.74</t>
+        </is>
+      </c>
+      <c r="CJ30" t="inlineStr"/>
+      <c r="CK30" t="inlineStr"/>
+      <c r="CL30" t="inlineStr"/>
+      <c r="CM30" t="inlineStr"/>
+      <c r="CN30" t="inlineStr"/>
+      <c r="CO30" t="inlineStr"/>
+      <c r="CP30" t="inlineStr"/>
+      <c r="CQ30" t="inlineStr"/>
+      <c r="CR30" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="CS30" t="inlineStr"/>
+      <c r="CT30" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="CU30" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="CV30" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="CW30" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="CX30" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="CY30" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="CZ30" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="DA30" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="DB30" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="DC30" t="inlineStr"/>
+      <c r="DD30" t="inlineStr">
+        <is>
+          <t>-2</t>
+        </is>
+      </c>
+      <c r="DE30" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="DF30" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="DG30" t="inlineStr">
+        <is>
+          <t>-2</t>
+        </is>
+      </c>
+      <c r="DH30" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="DI30" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="DJ30" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="DK30" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="DL30" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="DM30" t="inlineStr"/>
+      <c r="DN30" t="inlineStr"/>
+      <c r="DO30" t="inlineStr"/>
+      <c r="DP30" t="inlineStr"/>
+      <c r="DQ30" t="inlineStr"/>
+      <c r="DR30" t="inlineStr"/>
+      <c r="DS30" t="inlineStr"/>
+      <c r="DT30" t="inlineStr"/>
+      <c r="DU30" t="inlineStr"/>
+      <c r="DV30" t="inlineStr"/>
+      <c r="DW30" t="inlineStr"/>
+      <c r="DX30" t="inlineStr"/>
+      <c r="DY30" t="inlineStr"/>
+      <c r="DZ30" t="inlineStr"/>
+      <c r="EA30" t="inlineStr"/>
+      <c r="EB30" t="inlineStr"/>
+      <c r="EC30" t="inlineStr"/>
+      <c r="ED30" t="inlineStr"/>
+      <c r="EE30" t="inlineStr"/>
+      <c r="EF30" t="inlineStr"/>
+      <c r="EG30" t="inlineStr"/>
+      <c r="EH30" t="inlineStr"/>
+      <c r="EI30" t="inlineStr"/>
+      <c r="EJ30" t="inlineStr">
+        <is>
+          <t>3.33</t>
+        </is>
+      </c>
+      <c r="EK30" t="inlineStr">
+        <is>
+          <t>2.70</t>
+        </is>
+      </c>
+      <c r="EL30" t="inlineStr">
+        <is>
+          <t>2.70</t>
+        </is>
+      </c>
+      <c r="EM30" t="inlineStr">
+        <is>
+          <t>2.94</t>
+        </is>
+      </c>
+      <c r="EN30" t="inlineStr">
+        <is>
+          <t>2.33</t>
+        </is>
+      </c>
+      <c r="EO30" t="inlineStr">
+        <is>
+          <t>2.55</t>
+        </is>
+      </c>
+      <c r="EP30" t="inlineStr">
+        <is>
+          <t>2.93</t>
+        </is>
+      </c>
+      <c r="EQ30" t="inlineStr">
+        <is>
+          <t>3.37</t>
+        </is>
+      </c>
+      <c r="ER30" t="inlineStr">
+        <is>
+          <t>3.35</t>
+        </is>
+      </c>
+      <c r="ES30" t="inlineStr"/>
+      <c r="ET30" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
+      </c>
+      <c r="EU30" t="inlineStr"/>
+      <c r="EV30" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="EW30" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="EX30" t="inlineStr">
+        <is>
+          <t>73</t>
+        </is>
+      </c>
+      <c r="EY30" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="EZ30" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="FA30" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="FB30" t="inlineStr">
+        <is>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="FC30" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="FD30" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="FE30" t="inlineStr"/>
+      <c r="FF30" t="inlineStr"/>
+      <c r="FG30" t="inlineStr"/>
+      <c r="FH30" t="inlineStr"/>
+      <c r="FI30" t="inlineStr"/>
+      <c r="FJ30" t="inlineStr"/>
+      <c r="FK30" t="inlineStr"/>
+      <c r="FL30" t="inlineStr"/>
+      <c r="FM30" t="inlineStr"/>
+      <c r="FN30" t="inlineStr"/>
+      <c r="FO30" t="inlineStr"/>
+      <c r="FP30" t="inlineStr"/>
+      <c r="FQ30" t="inlineStr"/>
+      <c r="FR30" t="inlineStr"/>
+      <c r="FS30" t="inlineStr"/>
+      <c r="FT30" t="inlineStr"/>
+      <c r="FU30" t="inlineStr"/>
+      <c r="FV30" t="inlineStr"/>
+      <c r="FW30" t="inlineStr"/>
+      <c r="FX30" t="inlineStr"/>
+      <c r="FY30" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="FZ30" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="GA30" t="inlineStr">
+        <is>
+          <t>-2</t>
+        </is>
+      </c>
+      <c r="GB30" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="GC30" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="GD30" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="GE30" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="GF30" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="GG30" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="GH30" t="inlineStr"/>
+      <c r="GI30" t="inlineStr"/>
+      <c r="GJ30" t="inlineStr"/>
+      <c r="GK30" t="inlineStr"/>
+      <c r="GL30" t="inlineStr"/>
+      <c r="GM30" t="inlineStr"/>
+      <c r="GN30" t="inlineStr"/>
+      <c r="GO30" t="inlineStr"/>
+      <c r="GP30" t="inlineStr"/>
+      <c r="GQ30" t="inlineStr"/>
+      <c r="GR30" t="inlineStr"/>
+      <c r="GS30" t="inlineStr"/>
+      <c r="GT30" t="inlineStr"/>
+      <c r="GU30" t="inlineStr"/>
+      <c r="GV30" t="inlineStr"/>
+      <c r="GW30" t="inlineStr"/>
+      <c r="GX30" t="inlineStr"/>
+      <c r="GY30" t="inlineStr"/>
+      <c r="GZ30" t="inlineStr"/>
+      <c r="HA30" t="inlineStr"/>
+      <c r="HB30" t="inlineStr"/>
+      <c r="HC30" t="inlineStr"/>
+      <c r="HD30" t="inlineStr"/>
+      <c r="HE30" t="inlineStr"/>
+      <c r="HF30" t="inlineStr"/>
+      <c r="HG30" t="inlineStr"/>
+      <c r="HH30" t="inlineStr"/>
+      <c r="HI30" t="inlineStr"/>
+      <c r="HJ30" t="inlineStr"/>
+      <c r="HK30" t="inlineStr"/>
+      <c r="HL30" t="inlineStr"/>
+      <c r="HM30" t="inlineStr"/>
+      <c r="HN30" t="inlineStr"/>
+      <c r="HO30" t="inlineStr"/>
+      <c r="HP30" t="inlineStr"/>
+      <c r="HQ30" t="inlineStr"/>
+      <c r="HR30" t="inlineStr"/>
+      <c r="HS30" t="inlineStr"/>
+      <c r="HT30" t="inlineStr"/>
+      <c r="HU30" t="inlineStr"/>
+      <c r="HV30" t="inlineStr"/>
+      <c r="HW30" t="inlineStr"/>
+      <c r="HX30" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="HY30" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="HZ30" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="IA30" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="IB30" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="IC30" t="inlineStr">
+        <is>
+          <t>155</t>
+        </is>
+      </c>
+      <c r="ID30" t="inlineStr">
+        <is>
+          <t>315</t>
+        </is>
+      </c>
+      <c r="IE30" t="inlineStr">
+        <is>
+          <t>475</t>
+        </is>
+      </c>
+      <c r="IF30" t="inlineStr">
+        <is>
+          <t>635</t>
+        </is>
+      </c>
+      <c r="IG30" t="inlineStr">
+        <is>
+          <t>3.53</t>
+        </is>
+      </c>
+      <c r="IH30" t="inlineStr">
+        <is>
+          <t>4.35</t>
+        </is>
+      </c>
+      <c r="II30" t="inlineStr"/>
+      <c r="IJ30" t="inlineStr">
+        <is>
+          <t>4.37</t>
+        </is>
+      </c>
+      <c r="IK30" t="inlineStr">
+        <is>
+          <t>4.77</t>
+        </is>
+      </c>
+      <c r="IL30" t="inlineStr">
+        <is>
+          <t>5.32</t>
+        </is>
+      </c>
+      <c r="IM30" t="inlineStr">
+        <is>
+          <t>4.76</t>
+        </is>
+      </c>
+      <c r="IN30" t="inlineStr">
+        <is>
+          <t>5.14</t>
+        </is>
+      </c>
+      <c r="IO30" t="inlineStr">
+        <is>
+          <t>5.72</t>
+        </is>
+      </c>
+      <c r="IP30" t="inlineStr">
+        <is>
+          <t>5.33</t>
+        </is>
+      </c>
+      <c r="IQ30" t="inlineStr">
+        <is>
+          <t>5.95</t>
+        </is>
+      </c>
+      <c r="IR30" t="inlineStr">
+        <is>
+          <t>6.76</t>
+        </is>
+      </c>
+      <c r="IS30" t="inlineStr"/>
+      <c r="IT30" t="inlineStr"/>
+      <c r="IU30" t="inlineStr"/>
+      <c r="IV30" t="inlineStr"/>
+      <c r="IW30" t="inlineStr"/>
+      <c r="IX30" t="inlineStr"/>
+      <c r="IY30" t="inlineStr"/>
+      <c r="IZ30" t="inlineStr"/>
+      <c r="JA30" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
+      </c>
+      <c r="JB30" t="inlineStr"/>
+      <c r="JC30" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
+      </c>
+      <c r="JD30" t="inlineStr">
+        <is>
+          <t>72</t>
+        </is>
+      </c>
+      <c r="JE30" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="JF30" t="inlineStr">
+        <is>
+          <t>72</t>
+        </is>
+      </c>
+      <c r="JG30" t="inlineStr">
+        <is>
+          <t>73</t>
+        </is>
+      </c>
+      <c r="JH30" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="JI30" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="JJ30" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="JK30" t="inlineStr">
+        <is>
+          <t>103</t>
+        </is>
+      </c>
+      <c r="JL30" t="inlineStr"/>
+      <c r="JM30" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="JN30" t="inlineStr">
+        <is>
+          <t>-2</t>
+        </is>
+      </c>
+      <c r="JO30" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="JP30" t="inlineStr">
+        <is>
+          <t>-2</t>
+        </is>
+      </c>
+      <c r="JQ30" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="JR30" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="JS30" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="JT30" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="JU30" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="JV30" t="inlineStr"/>
+      <c r="JW30" t="inlineStr"/>
+      <c r="JX30" t="inlineStr"/>
+      <c r="JY30" t="inlineStr"/>
+      <c r="JZ30" t="inlineStr"/>
+      <c r="KA30" t="inlineStr"/>
+      <c r="KB30" t="inlineStr"/>
+      <c r="KC30" t="inlineStr"/>
+      <c r="KD30" t="inlineStr"/>
+      <c r="KE30" t="inlineStr"/>
+      <c r="KF30" t="inlineStr"/>
+      <c r="KG30" t="inlineStr"/>
+      <c r="KH30" t="inlineStr"/>
+      <c r="KI30" t="inlineStr"/>
+      <c r="KJ30" t="inlineStr"/>
+      <c r="KK30" t="inlineStr"/>
+      <c r="KL30" t="inlineStr"/>
+      <c r="KM30" t="inlineStr"/>
+      <c r="KN30" t="inlineStr"/>
+      <c r="KO30" t="inlineStr"/>
+      <c r="KP30" t="inlineStr"/>
+      <c r="KQ30" t="inlineStr"/>
+      <c r="KR30" t="inlineStr"/>
+      <c r="KS30" t="inlineStr"/>
+      <c r="KT30" t="inlineStr"/>
+      <c r="KU30" t="inlineStr"/>
+      <c r="KV30" t="inlineStr"/>
+      <c r="KW30" t="inlineStr"/>
+      <c r="KX30" t="inlineStr"/>
+      <c r="KY30" t="inlineStr"/>
+      <c r="KZ30" t="inlineStr"/>
+      <c r="LA30" t="inlineStr"/>
+      <c r="LB30" t="inlineStr"/>
+      <c r="LC30" t="inlineStr"/>
+      <c r="LD30" t="inlineStr"/>
+      <c r="LE30" t="inlineStr"/>
+      <c r="LF30" t="inlineStr"/>
+      <c r="LG30" t="inlineStr"/>
+      <c r="LH30" t="inlineStr"/>
+      <c r="LI30" t="inlineStr"/>
+      <c r="LJ30" t="inlineStr"/>
+      <c r="LK30" t="inlineStr"/>
+      <c r="LL30" t="inlineStr"/>
+      <c r="LM30" t="inlineStr"/>
+      <c r="LN30" t="inlineStr"/>
+      <c r="LO30" t="inlineStr"/>
+      <c r="LP30" t="inlineStr"/>
+      <c r="LQ30" t="inlineStr"/>
+      <c r="LR30" t="inlineStr"/>
+      <c r="LS30" t="inlineStr"/>
+      <c r="LT30" t="inlineStr"/>
+      <c r="LU30" t="inlineStr"/>
+      <c r="LV30" t="inlineStr"/>
+      <c r="LW30" t="inlineStr"/>
+      <c r="LX30" t="inlineStr"/>
+      <c r="LY30" t="inlineStr"/>
+      <c r="LZ30" t="inlineStr"/>
+      <c r="MA30" t="inlineStr"/>
+      <c r="MB30" t="inlineStr"/>
+      <c r="MC30" t="inlineStr"/>
+      <c r="MD30" t="inlineStr"/>
+      <c r="ME30" t="inlineStr"/>
+      <c r="MF30" t="inlineStr"/>
+      <c r="MG30" t="inlineStr"/>
+      <c r="MH30" t="inlineStr"/>
+      <c r="MI30" t="inlineStr"/>
+      <c r="MJ30" t="inlineStr"/>
+      <c r="MK30" t="inlineStr"/>
+      <c r="ML30" t="inlineStr"/>
+      <c r="MM30" t="inlineStr"/>
+      <c r="MN30" t="inlineStr"/>
+      <c r="MO30" t="inlineStr"/>
+      <c r="MP30" t="inlineStr"/>
+      <c r="MQ30" t="inlineStr"/>
+      <c r="MR30" t="inlineStr"/>
+      <c r="MS30" t="inlineStr"/>
+      <c r="MT30" t="inlineStr"/>
+      <c r="MU30" t="inlineStr"/>
+      <c r="MV30" t="inlineStr"/>
+      <c r="MW30" t="inlineStr"/>
+      <c r="MX30" t="inlineStr"/>
+      <c r="MY30" t="inlineStr"/>
+      <c r="MZ30" t="inlineStr"/>
+      <c r="NA30" t="inlineStr"/>
+      <c r="NB30" t="inlineStr"/>
+      <c r="NC30" t="inlineStr"/>
+      <c r="ND30" t="inlineStr"/>
+      <c r="NE30" t="inlineStr"/>
+      <c r="NF30" t="inlineStr"/>
+      <c r="NG30" t="inlineStr"/>
+      <c r="NH30" t="inlineStr"/>
+      <c r="NI30" t="inlineStr"/>
+      <c r="NJ30" t="inlineStr"/>
+      <c r="NK30" t="inlineStr"/>
+      <c r="NL30" t="inlineStr"/>
+      <c r="NM30" t="inlineStr"/>
+      <c r="NN30" t="inlineStr"/>
+      <c r="NO30" t="inlineStr"/>
+      <c r="NP30" t="inlineStr"/>
+      <c r="NQ30" t="inlineStr"/>
+      <c r="NR30" t="inlineStr"/>
+      <c r="NS30" t="inlineStr"/>
+      <c r="NT30" t="inlineStr"/>
+      <c r="NU30" t="inlineStr"/>
+      <c r="NV30" t="inlineStr"/>
+      <c r="NW30" t="inlineStr"/>
+      <c r="NX30" t="inlineStr"/>
+      <c r="NY30" t="inlineStr"/>
+      <c r="NZ30" t="inlineStr"/>
+      <c r="OA30" t="inlineStr"/>
+      <c r="OB30" t="inlineStr"/>
+      <c r="OC30" t="inlineStr"/>
+      <c r="OD30" t="inlineStr"/>
+      <c r="OE30" t="inlineStr"/>
+      <c r="OF30" t="inlineStr"/>
+      <c r="OG30" t="inlineStr"/>
+      <c r="OH30" t="inlineStr"/>
+      <c r="OI30" t="inlineStr"/>
+      <c r="OJ30" t="inlineStr"/>
+      <c r="OK30" t="inlineStr"/>
+      <c r="OL30" t="inlineStr"/>
+      <c r="OM30" t="inlineStr"/>
+      <c r="ON30" t="inlineStr"/>
+      <c r="OO30" t="inlineStr"/>
+      <c r="OP30" t="inlineStr"/>
+      <c r="OQ30" t="inlineStr"/>
+      <c r="OR30" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
function add : get_diffusing_table
</commit_message>
<xml_diff>
--- a/OOMII.xlsx
+++ b/OOMII.xlsx
@@ -346,7 +346,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:OR43"/>
+  <dimension ref="A1:OR54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15489,413 +15489,490 @@
           <t>type03</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr"/>
-      <c r="C43" t="inlineStr"/>
-      <c r="D43" t="inlineStr"/>
-      <c r="E43" t="inlineStr"/>
-      <c r="F43" t="inlineStr"/>
-      <c r="G43" t="inlineStr"/>
-      <c r="H43" t="inlineStr"/>
-      <c r="I43" t="inlineStr"/>
-      <c r="J43" t="inlineStr"/>
-      <c r="K43" t="inlineStr"/>
-      <c r="L43" t="inlineStr"/>
-      <c r="M43" t="inlineStr"/>
-      <c r="N43" t="inlineStr"/>
-      <c r="O43" t="inlineStr"/>
-      <c r="P43" t="inlineStr"/>
-      <c r="Q43" t="inlineStr"/>
-      <c r="R43" t="inlineStr"/>
-      <c r="S43" t="inlineStr"/>
-      <c r="T43" t="inlineStr"/>
-      <c r="U43" t="inlineStr"/>
-      <c r="V43" t="inlineStr"/>
-      <c r="W43" t="inlineStr"/>
-      <c r="X43" t="inlineStr"/>
-      <c r="Y43" t="inlineStr"/>
-      <c r="Z43" t="inlineStr"/>
-      <c r="AA43" t="inlineStr"/>
-      <c r="AB43" t="inlineStr"/>
-      <c r="AC43" t="inlineStr"/>
-      <c r="AD43" t="inlineStr"/>
-      <c r="AE43" t="inlineStr"/>
-      <c r="AF43" t="inlineStr"/>
-      <c r="AG43" t="inlineStr"/>
-      <c r="AH43" t="inlineStr"/>
-      <c r="AI43" t="inlineStr"/>
-      <c r="AJ43" t="inlineStr"/>
-      <c r="AK43" t="inlineStr"/>
-      <c r="AL43" t="inlineStr"/>
-      <c r="AM43" t="inlineStr"/>
-      <c r="AN43" t="inlineStr"/>
-      <c r="AO43" t="inlineStr"/>
-      <c r="AP43" t="inlineStr"/>
-      <c r="AQ43" t="inlineStr"/>
-      <c r="AR43" t="inlineStr"/>
-      <c r="AS43" t="inlineStr"/>
-      <c r="AT43" t="inlineStr"/>
-      <c r="AU43" t="inlineStr"/>
-      <c r="AV43" t="inlineStr"/>
-      <c r="AW43" t="inlineStr"/>
-      <c r="AX43" t="inlineStr"/>
-      <c r="AY43" t="inlineStr"/>
-      <c r="AZ43" t="inlineStr"/>
-      <c r="BA43" t="inlineStr"/>
-      <c r="BB43" t="inlineStr"/>
-      <c r="BC43" t="inlineStr"/>
-      <c r="BD43" t="inlineStr"/>
-      <c r="BE43" t="inlineStr"/>
-      <c r="BF43" t="inlineStr"/>
-      <c r="BG43" t="inlineStr"/>
-      <c r="BH43" t="inlineStr"/>
-      <c r="BI43" t="inlineStr"/>
-      <c r="BJ43" t="inlineStr"/>
-      <c r="BK43" t="inlineStr"/>
-      <c r="BL43" t="inlineStr"/>
-      <c r="BM43" t="inlineStr"/>
-      <c r="BN43" t="inlineStr"/>
-      <c r="BO43" t="inlineStr"/>
-      <c r="BP43" t="inlineStr"/>
-      <c r="BQ43" t="inlineStr"/>
-      <c r="BR43" t="inlineStr"/>
-      <c r="BS43" t="inlineStr"/>
-      <c r="BT43" t="inlineStr"/>
-      <c r="BU43" t="inlineStr"/>
-      <c r="BV43" t="inlineStr"/>
-      <c r="BW43" t="inlineStr"/>
-      <c r="BX43" t="inlineStr"/>
-      <c r="BY43" t="inlineStr"/>
-      <c r="BZ43" t="inlineStr"/>
-      <c r="CA43" t="inlineStr"/>
-      <c r="CB43" t="inlineStr"/>
-      <c r="CC43" t="inlineStr"/>
-      <c r="CD43" t="inlineStr"/>
-      <c r="CE43" t="inlineStr"/>
-      <c r="CF43" t="inlineStr"/>
-      <c r="CG43" t="inlineStr"/>
-      <c r="CH43" t="inlineStr"/>
-      <c r="CI43" t="inlineStr"/>
-      <c r="CJ43" t="inlineStr"/>
-      <c r="CK43" t="inlineStr"/>
-      <c r="CL43" t="inlineStr"/>
-      <c r="CM43" t="inlineStr"/>
-      <c r="CN43" t="inlineStr"/>
-      <c r="CO43" t="inlineStr"/>
-      <c r="CP43" t="inlineStr"/>
-      <c r="CQ43" t="inlineStr"/>
-      <c r="CR43" t="inlineStr"/>
-      <c r="CS43" t="inlineStr"/>
-      <c r="CT43" t="inlineStr"/>
-      <c r="CU43" t="inlineStr"/>
-      <c r="CV43" t="inlineStr"/>
-      <c r="CW43" t="inlineStr"/>
-      <c r="CX43" t="inlineStr"/>
-      <c r="CY43" t="inlineStr"/>
-      <c r="CZ43" t="inlineStr"/>
-      <c r="DA43" t="inlineStr"/>
-      <c r="DB43" t="inlineStr"/>
-      <c r="DC43" t="inlineStr"/>
-      <c r="DD43" t="inlineStr"/>
-      <c r="DE43" t="inlineStr"/>
-      <c r="DF43" t="inlineStr"/>
-      <c r="DG43" t="inlineStr"/>
-      <c r="DH43" t="inlineStr"/>
-      <c r="DI43" t="inlineStr"/>
-      <c r="DJ43" t="inlineStr"/>
-      <c r="DK43" t="inlineStr"/>
-      <c r="DL43" t="inlineStr"/>
-      <c r="DM43" t="inlineStr"/>
-      <c r="DN43" t="inlineStr"/>
-      <c r="DO43" t="inlineStr"/>
-      <c r="DP43" t="inlineStr"/>
-      <c r="DQ43" t="inlineStr"/>
-      <c r="DR43" t="inlineStr"/>
-      <c r="DS43" t="inlineStr"/>
-      <c r="DT43" t="inlineStr"/>
-      <c r="DU43" t="inlineStr"/>
-      <c r="DV43" t="inlineStr"/>
-      <c r="DW43" t="inlineStr"/>
-      <c r="DX43" t="inlineStr"/>
-      <c r="DY43" t="inlineStr"/>
-      <c r="DZ43" t="inlineStr"/>
-      <c r="EA43" t="inlineStr"/>
-      <c r="EB43" t="inlineStr"/>
-      <c r="EC43" t="inlineStr"/>
-      <c r="ED43" t="inlineStr"/>
-      <c r="EE43" t="inlineStr"/>
-      <c r="EF43" t="inlineStr"/>
-      <c r="EG43" t="inlineStr"/>
-      <c r="EH43" t="inlineStr"/>
-      <c r="EI43" t="inlineStr"/>
-      <c r="EJ43" t="inlineStr"/>
-      <c r="EK43" t="inlineStr"/>
-      <c r="EL43" t="inlineStr"/>
-      <c r="EM43" t="inlineStr"/>
-      <c r="EN43" t="inlineStr"/>
-      <c r="EO43" t="inlineStr"/>
-      <c r="EP43" t="inlineStr"/>
-      <c r="EQ43" t="inlineStr"/>
-      <c r="ER43" t="inlineStr"/>
-      <c r="ES43" t="inlineStr"/>
-      <c r="ET43" t="inlineStr"/>
-      <c r="EU43" t="inlineStr"/>
-      <c r="EV43" t="inlineStr"/>
-      <c r="EW43" t="inlineStr"/>
-      <c r="EX43" t="inlineStr"/>
-      <c r="EY43" t="inlineStr"/>
-      <c r="EZ43" t="inlineStr"/>
-      <c r="FA43" t="inlineStr"/>
-      <c r="FB43" t="inlineStr"/>
-      <c r="FC43" t="inlineStr"/>
-      <c r="FD43" t="inlineStr"/>
-      <c r="FE43" t="inlineStr"/>
-      <c r="FF43" t="inlineStr"/>
-      <c r="FG43" t="inlineStr"/>
-      <c r="FH43" t="inlineStr"/>
-      <c r="FI43" t="inlineStr"/>
-      <c r="FJ43" t="inlineStr"/>
-      <c r="FK43" t="inlineStr"/>
-      <c r="FL43" t="inlineStr"/>
-      <c r="FM43" t="inlineStr"/>
-      <c r="FN43" t="inlineStr"/>
-      <c r="FO43" t="inlineStr"/>
-      <c r="FP43" t="inlineStr"/>
-      <c r="FQ43" t="inlineStr"/>
-      <c r="FR43" t="inlineStr"/>
-      <c r="FS43" t="inlineStr"/>
-      <c r="FT43" t="inlineStr"/>
-      <c r="FU43" t="inlineStr"/>
-      <c r="FV43" t="inlineStr"/>
-      <c r="FW43" t="inlineStr"/>
-      <c r="FX43" t="inlineStr"/>
-      <c r="FY43" t="inlineStr"/>
-      <c r="FZ43" t="inlineStr"/>
-      <c r="GA43" t="inlineStr"/>
-      <c r="GB43" t="inlineStr"/>
-      <c r="GC43" t="inlineStr"/>
-      <c r="GD43" t="inlineStr"/>
-      <c r="GE43" t="inlineStr"/>
-      <c r="GF43" t="inlineStr"/>
-      <c r="GG43" t="inlineStr"/>
-      <c r="GH43" t="inlineStr"/>
-      <c r="GI43" t="inlineStr"/>
-      <c r="GJ43" t="inlineStr"/>
-      <c r="GK43" t="inlineStr"/>
-      <c r="GL43" t="inlineStr"/>
-      <c r="GM43" t="inlineStr"/>
-      <c r="GN43" t="inlineStr"/>
-      <c r="GO43" t="inlineStr"/>
-      <c r="GP43" t="inlineStr"/>
-      <c r="GQ43" t="inlineStr"/>
-      <c r="GR43" t="inlineStr"/>
-      <c r="GS43" t="inlineStr"/>
-      <c r="GT43" t="inlineStr"/>
-      <c r="GU43" t="inlineStr"/>
-      <c r="GV43" t="inlineStr"/>
-      <c r="GW43" t="inlineStr"/>
-      <c r="GX43" t="inlineStr"/>
-      <c r="GY43" t="inlineStr"/>
-      <c r="GZ43" t="inlineStr"/>
-      <c r="HA43" t="inlineStr"/>
-      <c r="HB43" t="inlineStr"/>
-      <c r="HC43" t="inlineStr"/>
-      <c r="HD43" t="inlineStr"/>
-      <c r="HE43" t="inlineStr"/>
-      <c r="HF43" t="inlineStr"/>
-      <c r="HG43" t="inlineStr"/>
-      <c r="HH43" t="inlineStr"/>
-      <c r="HI43" t="inlineStr"/>
-      <c r="HJ43" t="inlineStr"/>
-      <c r="HK43" t="inlineStr"/>
-      <c r="HL43" t="inlineStr"/>
-      <c r="HM43" t="inlineStr"/>
-      <c r="HN43" t="inlineStr"/>
-      <c r="HO43" t="inlineStr"/>
-      <c r="HP43" t="inlineStr"/>
-      <c r="HQ43" t="inlineStr"/>
-      <c r="HR43" t="inlineStr"/>
-      <c r="HS43" t="inlineStr"/>
-      <c r="HT43" t="inlineStr"/>
-      <c r="HU43" t="inlineStr"/>
-      <c r="HV43" t="inlineStr"/>
-      <c r="HW43" t="inlineStr"/>
-      <c r="HX43" t="inlineStr"/>
-      <c r="HY43" t="inlineStr"/>
-      <c r="HZ43" t="inlineStr"/>
-      <c r="IA43" t="inlineStr"/>
-      <c r="IB43" t="inlineStr"/>
-      <c r="IC43" t="inlineStr"/>
-      <c r="ID43" t="inlineStr"/>
-      <c r="IE43" t="inlineStr"/>
-      <c r="IF43" t="inlineStr"/>
-      <c r="IG43" t="inlineStr"/>
-      <c r="IH43" t="inlineStr"/>
-      <c r="II43" t="inlineStr"/>
-      <c r="IJ43" t="inlineStr"/>
-      <c r="IK43" t="inlineStr"/>
-      <c r="IL43" t="inlineStr"/>
-      <c r="IM43" t="inlineStr"/>
-      <c r="IN43" t="inlineStr"/>
-      <c r="IO43" t="inlineStr"/>
-      <c r="IP43" t="inlineStr"/>
-      <c r="IQ43" t="inlineStr"/>
-      <c r="IR43" t="inlineStr"/>
-      <c r="IS43" t="inlineStr"/>
-      <c r="IT43" t="inlineStr"/>
-      <c r="IU43" t="inlineStr"/>
-      <c r="IV43" t="inlineStr"/>
-      <c r="IW43" t="inlineStr"/>
-      <c r="IX43" t="inlineStr"/>
-      <c r="IY43" t="inlineStr"/>
-      <c r="IZ43" t="inlineStr"/>
-      <c r="JA43" t="inlineStr"/>
-      <c r="JB43" t="inlineStr"/>
-      <c r="JC43" t="inlineStr"/>
-      <c r="JD43" t="inlineStr"/>
-      <c r="JE43" t="inlineStr"/>
-      <c r="JF43" t="inlineStr"/>
-      <c r="JG43" t="inlineStr"/>
-      <c r="JH43" t="inlineStr"/>
-      <c r="JI43" t="inlineStr"/>
-      <c r="JJ43" t="inlineStr"/>
-      <c r="JK43" t="inlineStr"/>
-      <c r="JL43" t="inlineStr"/>
-      <c r="JM43" t="inlineStr"/>
-      <c r="JN43" t="inlineStr"/>
-      <c r="JO43" t="inlineStr"/>
-      <c r="JP43" t="inlineStr"/>
-      <c r="JQ43" t="inlineStr"/>
-      <c r="JR43" t="inlineStr"/>
-      <c r="JS43" t="inlineStr"/>
-      <c r="JT43" t="inlineStr"/>
-      <c r="JU43" t="inlineStr"/>
-      <c r="JV43" t="inlineStr"/>
-      <c r="JW43" t="inlineStr"/>
-      <c r="JX43" t="inlineStr"/>
-      <c r="JY43" t="inlineStr"/>
-      <c r="JZ43" t="inlineStr"/>
-      <c r="KA43" t="inlineStr"/>
-      <c r="KB43" t="inlineStr"/>
-      <c r="KC43" t="inlineStr"/>
-      <c r="KD43" t="inlineStr"/>
-      <c r="KE43" t="inlineStr"/>
-      <c r="KF43" t="inlineStr"/>
-      <c r="KG43" t="inlineStr"/>
-      <c r="KH43" t="inlineStr"/>
-      <c r="KI43" t="inlineStr"/>
-      <c r="KJ43" t="inlineStr"/>
-      <c r="KK43" t="inlineStr"/>
-      <c r="KL43" t="inlineStr"/>
-      <c r="KM43" t="inlineStr"/>
-      <c r="KN43" t="inlineStr"/>
-      <c r="KO43" t="inlineStr"/>
-      <c r="KP43" t="inlineStr"/>
-      <c r="KQ43" t="inlineStr"/>
-      <c r="KR43" t="inlineStr"/>
-      <c r="KS43" t="inlineStr"/>
-      <c r="KT43" t="inlineStr"/>
-      <c r="KU43" t="inlineStr"/>
-      <c r="KV43" t="inlineStr"/>
-      <c r="KW43" t="inlineStr"/>
-      <c r="KX43" t="inlineStr"/>
-      <c r="KY43" t="inlineStr"/>
-      <c r="KZ43" t="inlineStr"/>
-      <c r="LA43" t="inlineStr"/>
-      <c r="LB43" t="inlineStr"/>
-      <c r="LC43" t="inlineStr"/>
-      <c r="LD43" t="inlineStr"/>
-      <c r="LE43" t="inlineStr"/>
-      <c r="LF43" t="inlineStr"/>
-      <c r="LG43" t="inlineStr"/>
-      <c r="LH43" t="inlineStr"/>
-      <c r="LI43" t="inlineStr"/>
-      <c r="LJ43" t="inlineStr"/>
-      <c r="LK43" t="inlineStr"/>
-      <c r="LL43" t="inlineStr"/>
-      <c r="LM43" t="inlineStr"/>
-      <c r="LN43" t="inlineStr"/>
-      <c r="LO43" t="inlineStr"/>
-      <c r="LP43" t="inlineStr"/>
-      <c r="LQ43" t="inlineStr"/>
-      <c r="LR43" t="inlineStr"/>
-      <c r="LS43" t="inlineStr"/>
-      <c r="LT43" t="inlineStr"/>
-      <c r="LU43" t="inlineStr"/>
-      <c r="LV43" t="inlineStr"/>
-      <c r="LW43" t="inlineStr"/>
-      <c r="LX43" t="inlineStr"/>
-      <c r="LY43" t="inlineStr"/>
-      <c r="LZ43" t="inlineStr"/>
-      <c r="MA43" t="inlineStr"/>
-      <c r="MB43" t="inlineStr"/>
-      <c r="MC43" t="inlineStr"/>
-      <c r="MD43" t="inlineStr"/>
-      <c r="ME43" t="inlineStr"/>
-      <c r="MF43" t="inlineStr"/>
-      <c r="MG43" t="inlineStr"/>
-      <c r="MH43" t="inlineStr"/>
-      <c r="MI43" t="inlineStr"/>
-      <c r="MJ43" t="inlineStr"/>
-      <c r="MK43" t="inlineStr"/>
-      <c r="ML43" t="inlineStr"/>
-      <c r="MM43" t="inlineStr"/>
-      <c r="MN43" t="inlineStr"/>
-      <c r="MO43" t="inlineStr"/>
-      <c r="MP43" t="inlineStr"/>
-      <c r="MQ43" t="inlineStr"/>
-      <c r="MR43" t="inlineStr"/>
-      <c r="MS43" t="inlineStr"/>
-      <c r="MT43" t="inlineStr"/>
-      <c r="MU43" t="inlineStr"/>
-      <c r="MV43" t="inlineStr"/>
-      <c r="MW43" t="inlineStr"/>
-      <c r="MX43" t="inlineStr"/>
-      <c r="MY43" t="inlineStr"/>
-      <c r="MZ43" t="inlineStr"/>
-      <c r="NA43" t="inlineStr"/>
-      <c r="NB43" t="inlineStr"/>
-      <c r="NC43" t="inlineStr"/>
-      <c r="ND43" t="inlineStr"/>
-      <c r="NE43" t="inlineStr"/>
-      <c r="NF43" t="inlineStr"/>
-      <c r="NG43" t="inlineStr"/>
-      <c r="NH43" t="inlineStr"/>
-      <c r="NI43" t="inlineStr"/>
-      <c r="NJ43" t="inlineStr"/>
-      <c r="NK43" t="inlineStr"/>
-      <c r="NL43" t="inlineStr"/>
-      <c r="NM43" t="inlineStr"/>
-      <c r="NN43" t="inlineStr"/>
-      <c r="NO43" t="inlineStr"/>
-      <c r="NP43" t="inlineStr"/>
-      <c r="NQ43" t="inlineStr"/>
-      <c r="NR43" t="inlineStr"/>
-      <c r="NS43" t="inlineStr"/>
-      <c r="NT43" t="inlineStr"/>
-      <c r="NU43" t="inlineStr"/>
-      <c r="NV43" t="inlineStr"/>
-      <c r="NW43" t="inlineStr"/>
-      <c r="NX43" t="inlineStr"/>
-      <c r="NY43" t="inlineStr"/>
-      <c r="NZ43" t="inlineStr"/>
-      <c r="OA43" t="inlineStr"/>
-      <c r="OB43" t="inlineStr"/>
-      <c r="OC43" t="inlineStr"/>
-      <c r="OD43" t="inlineStr"/>
-      <c r="OE43" t="inlineStr"/>
-      <c r="OF43" t="inlineStr"/>
-      <c r="OG43" t="inlineStr"/>
-      <c r="OH43" t="inlineStr"/>
-      <c r="OI43" t="inlineStr"/>
-      <c r="OJ43" t="inlineStr"/>
-      <c r="OK43" t="inlineStr"/>
-      <c r="OL43" t="inlineStr"/>
-      <c r="OM43" t="inlineStr"/>
-      <c r="ON43" t="inlineStr"/>
-      <c r="OO43" t="inlineStr"/>
-      <c r="OP43" t="inlineStr"/>
-      <c r="OQ43" t="inlineStr"/>
-      <c r="OR43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>type03</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>type03</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>type03</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>type03</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>type03</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>type03</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>type03</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>type03</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>type03</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>type03</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>type03</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr"/>
+      <c r="C54" t="inlineStr"/>
+      <c r="D54" t="inlineStr"/>
+      <c r="E54" t="inlineStr"/>
+      <c r="F54" t="inlineStr"/>
+      <c r="G54" t="inlineStr"/>
+      <c r="H54" t="inlineStr"/>
+      <c r="I54" t="inlineStr"/>
+      <c r="J54" t="inlineStr"/>
+      <c r="K54" t="inlineStr"/>
+      <c r="L54" t="inlineStr"/>
+      <c r="M54" t="inlineStr"/>
+      <c r="N54" t="inlineStr"/>
+      <c r="O54" t="inlineStr"/>
+      <c r="P54" t="inlineStr"/>
+      <c r="Q54" t="inlineStr"/>
+      <c r="R54" t="inlineStr"/>
+      <c r="S54" t="inlineStr"/>
+      <c r="T54" t="inlineStr"/>
+      <c r="U54" t="inlineStr"/>
+      <c r="V54" t="inlineStr"/>
+      <c r="W54" t="inlineStr"/>
+      <c r="X54" t="inlineStr"/>
+      <c r="Y54" t="inlineStr"/>
+      <c r="Z54" t="inlineStr"/>
+      <c r="AA54" t="inlineStr"/>
+      <c r="AB54" t="inlineStr"/>
+      <c r="AC54" t="inlineStr"/>
+      <c r="AD54" t="inlineStr"/>
+      <c r="AE54" t="inlineStr"/>
+      <c r="AF54" t="inlineStr"/>
+      <c r="AG54" t="inlineStr"/>
+      <c r="AH54" t="inlineStr"/>
+      <c r="AI54" t="inlineStr"/>
+      <c r="AJ54" t="inlineStr"/>
+      <c r="AK54" t="inlineStr"/>
+      <c r="AL54" t="inlineStr"/>
+      <c r="AM54" t="inlineStr"/>
+      <c r="AN54" t="inlineStr"/>
+      <c r="AO54" t="inlineStr"/>
+      <c r="AP54" t="inlineStr"/>
+      <c r="AQ54" t="inlineStr"/>
+      <c r="AR54" t="inlineStr"/>
+      <c r="AS54" t="inlineStr"/>
+      <c r="AT54" t="inlineStr"/>
+      <c r="AU54" t="inlineStr"/>
+      <c r="AV54" t="inlineStr"/>
+      <c r="AW54" t="inlineStr"/>
+      <c r="AX54" t="inlineStr"/>
+      <c r="AY54" t="inlineStr"/>
+      <c r="AZ54" t="inlineStr"/>
+      <c r="BA54" t="inlineStr"/>
+      <c r="BB54" t="inlineStr"/>
+      <c r="BC54" t="inlineStr"/>
+      <c r="BD54" t="inlineStr"/>
+      <c r="BE54" t="inlineStr"/>
+      <c r="BF54" t="inlineStr"/>
+      <c r="BG54" t="inlineStr"/>
+      <c r="BH54" t="inlineStr"/>
+      <c r="BI54" t="inlineStr"/>
+      <c r="BJ54" t="inlineStr"/>
+      <c r="BK54" t="inlineStr"/>
+      <c r="BL54" t="inlineStr"/>
+      <c r="BM54" t="inlineStr"/>
+      <c r="BN54" t="inlineStr"/>
+      <c r="BO54" t="inlineStr"/>
+      <c r="BP54" t="inlineStr"/>
+      <c r="BQ54" t="inlineStr"/>
+      <c r="BR54" t="inlineStr"/>
+      <c r="BS54" t="inlineStr"/>
+      <c r="BT54" t="inlineStr"/>
+      <c r="BU54" t="inlineStr"/>
+      <c r="BV54" t="inlineStr"/>
+      <c r="BW54" t="inlineStr"/>
+      <c r="BX54" t="inlineStr"/>
+      <c r="BY54" t="inlineStr"/>
+      <c r="BZ54" t="inlineStr"/>
+      <c r="CA54" t="inlineStr"/>
+      <c r="CB54" t="inlineStr"/>
+      <c r="CC54" t="inlineStr"/>
+      <c r="CD54" t="inlineStr"/>
+      <c r="CE54" t="inlineStr"/>
+      <c r="CF54" t="inlineStr"/>
+      <c r="CG54" t="inlineStr"/>
+      <c r="CH54" t="inlineStr"/>
+      <c r="CI54" t="inlineStr"/>
+      <c r="CJ54" t="inlineStr"/>
+      <c r="CK54" t="inlineStr"/>
+      <c r="CL54" t="inlineStr"/>
+      <c r="CM54" t="inlineStr"/>
+      <c r="CN54" t="inlineStr"/>
+      <c r="CO54" t="inlineStr"/>
+      <c r="CP54" t="inlineStr"/>
+      <c r="CQ54" t="inlineStr"/>
+      <c r="CR54" t="inlineStr"/>
+      <c r="CS54" t="inlineStr"/>
+      <c r="CT54" t="inlineStr"/>
+      <c r="CU54" t="inlineStr"/>
+      <c r="CV54" t="inlineStr"/>
+      <c r="CW54" t="inlineStr"/>
+      <c r="CX54" t="inlineStr"/>
+      <c r="CY54" t="inlineStr"/>
+      <c r="CZ54" t="inlineStr"/>
+      <c r="DA54" t="inlineStr"/>
+      <c r="DB54" t="inlineStr"/>
+      <c r="DC54" t="inlineStr"/>
+      <c r="DD54" t="inlineStr"/>
+      <c r="DE54" t="inlineStr"/>
+      <c r="DF54" t="inlineStr"/>
+      <c r="DG54" t="inlineStr"/>
+      <c r="DH54" t="inlineStr"/>
+      <c r="DI54" t="inlineStr"/>
+      <c r="DJ54" t="inlineStr"/>
+      <c r="DK54" t="inlineStr"/>
+      <c r="DL54" t="inlineStr"/>
+      <c r="DM54" t="inlineStr"/>
+      <c r="DN54" t="inlineStr"/>
+      <c r="DO54" t="inlineStr"/>
+      <c r="DP54" t="inlineStr"/>
+      <c r="DQ54" t="inlineStr"/>
+      <c r="DR54" t="inlineStr"/>
+      <c r="DS54" t="inlineStr"/>
+      <c r="DT54" t="inlineStr"/>
+      <c r="DU54" t="inlineStr"/>
+      <c r="DV54" t="inlineStr"/>
+      <c r="DW54" t="inlineStr"/>
+      <c r="DX54" t="inlineStr"/>
+      <c r="DY54" t="inlineStr"/>
+      <c r="DZ54" t="inlineStr"/>
+      <c r="EA54" t="inlineStr"/>
+      <c r="EB54" t="inlineStr"/>
+      <c r="EC54" t="inlineStr"/>
+      <c r="ED54" t="inlineStr"/>
+      <c r="EE54" t="inlineStr"/>
+      <c r="EF54" t="inlineStr"/>
+      <c r="EG54" t="inlineStr"/>
+      <c r="EH54" t="inlineStr"/>
+      <c r="EI54" t="inlineStr"/>
+      <c r="EJ54" t="inlineStr"/>
+      <c r="EK54" t="inlineStr"/>
+      <c r="EL54" t="inlineStr"/>
+      <c r="EM54" t="inlineStr"/>
+      <c r="EN54" t="inlineStr"/>
+      <c r="EO54" t="inlineStr"/>
+      <c r="EP54" t="inlineStr"/>
+      <c r="EQ54" t="inlineStr"/>
+      <c r="ER54" t="inlineStr"/>
+      <c r="ES54" t="inlineStr"/>
+      <c r="ET54" t="inlineStr"/>
+      <c r="EU54" t="inlineStr"/>
+      <c r="EV54" t="inlineStr"/>
+      <c r="EW54" t="inlineStr"/>
+      <c r="EX54" t="inlineStr"/>
+      <c r="EY54" t="inlineStr"/>
+      <c r="EZ54" t="inlineStr"/>
+      <c r="FA54" t="inlineStr"/>
+      <c r="FB54" t="inlineStr"/>
+      <c r="FC54" t="inlineStr"/>
+      <c r="FD54" t="inlineStr"/>
+      <c r="FE54" t="inlineStr"/>
+      <c r="FF54" t="inlineStr"/>
+      <c r="FG54" t="inlineStr"/>
+      <c r="FH54" t="inlineStr"/>
+      <c r="FI54" t="inlineStr"/>
+      <c r="FJ54" t="inlineStr"/>
+      <c r="FK54" t="inlineStr"/>
+      <c r="FL54" t="inlineStr"/>
+      <c r="FM54" t="inlineStr"/>
+      <c r="FN54" t="inlineStr"/>
+      <c r="FO54" t="inlineStr"/>
+      <c r="FP54" t="inlineStr"/>
+      <c r="FQ54" t="inlineStr"/>
+      <c r="FR54" t="inlineStr"/>
+      <c r="FS54" t="inlineStr"/>
+      <c r="FT54" t="inlineStr"/>
+      <c r="FU54" t="inlineStr"/>
+      <c r="FV54" t="inlineStr"/>
+      <c r="FW54" t="inlineStr"/>
+      <c r="FX54" t="inlineStr"/>
+      <c r="FY54" t="inlineStr"/>
+      <c r="FZ54" t="inlineStr"/>
+      <c r="GA54" t="inlineStr"/>
+      <c r="GB54" t="inlineStr"/>
+      <c r="GC54" t="inlineStr"/>
+      <c r="GD54" t="inlineStr"/>
+      <c r="GE54" t="inlineStr"/>
+      <c r="GF54" t="inlineStr"/>
+      <c r="GG54" t="inlineStr"/>
+      <c r="GH54" t="inlineStr"/>
+      <c r="GI54" t="inlineStr"/>
+      <c r="GJ54" t="inlineStr"/>
+      <c r="GK54" t="inlineStr"/>
+      <c r="GL54" t="inlineStr"/>
+      <c r="GM54" t="inlineStr"/>
+      <c r="GN54" t="inlineStr"/>
+      <c r="GO54" t="inlineStr"/>
+      <c r="GP54" t="inlineStr"/>
+      <c r="GQ54" t="inlineStr"/>
+      <c r="GR54" t="inlineStr"/>
+      <c r="GS54" t="inlineStr"/>
+      <c r="GT54" t="inlineStr"/>
+      <c r="GU54" t="inlineStr"/>
+      <c r="GV54" t="inlineStr"/>
+      <c r="GW54" t="inlineStr"/>
+      <c r="GX54" t="inlineStr"/>
+      <c r="GY54" t="inlineStr"/>
+      <c r="GZ54" t="inlineStr"/>
+      <c r="HA54" t="inlineStr"/>
+      <c r="HB54" t="inlineStr"/>
+      <c r="HC54" t="inlineStr"/>
+      <c r="HD54" t="inlineStr"/>
+      <c r="HE54" t="inlineStr"/>
+      <c r="HF54" t="inlineStr"/>
+      <c r="HG54" t="inlineStr"/>
+      <c r="HH54" t="inlineStr"/>
+      <c r="HI54" t="inlineStr"/>
+      <c r="HJ54" t="inlineStr"/>
+      <c r="HK54" t="inlineStr"/>
+      <c r="HL54" t="inlineStr"/>
+      <c r="HM54" t="inlineStr"/>
+      <c r="HN54" t="inlineStr"/>
+      <c r="HO54" t="inlineStr"/>
+      <c r="HP54" t="inlineStr"/>
+      <c r="HQ54" t="inlineStr"/>
+      <c r="HR54" t="inlineStr"/>
+      <c r="HS54" t="inlineStr"/>
+      <c r="HT54" t="inlineStr"/>
+      <c r="HU54" t="inlineStr"/>
+      <c r="HV54" t="inlineStr"/>
+      <c r="HW54" t="inlineStr"/>
+      <c r="HX54" t="inlineStr"/>
+      <c r="HY54" t="inlineStr"/>
+      <c r="HZ54" t="inlineStr"/>
+      <c r="IA54" t="inlineStr"/>
+      <c r="IB54" t="inlineStr"/>
+      <c r="IC54" t="inlineStr"/>
+      <c r="ID54" t="inlineStr"/>
+      <c r="IE54" t="inlineStr"/>
+      <c r="IF54" t="inlineStr"/>
+      <c r="IG54" t="inlineStr"/>
+      <c r="IH54" t="inlineStr"/>
+      <c r="II54" t="inlineStr"/>
+      <c r="IJ54" t="inlineStr"/>
+      <c r="IK54" t="inlineStr"/>
+      <c r="IL54" t="inlineStr"/>
+      <c r="IM54" t="inlineStr"/>
+      <c r="IN54" t="inlineStr"/>
+      <c r="IO54" t="inlineStr"/>
+      <c r="IP54" t="inlineStr"/>
+      <c r="IQ54" t="inlineStr"/>
+      <c r="IR54" t="inlineStr"/>
+      <c r="IS54" t="inlineStr"/>
+      <c r="IT54" t="inlineStr"/>
+      <c r="IU54" t="inlineStr"/>
+      <c r="IV54" t="inlineStr"/>
+      <c r="IW54" t="inlineStr"/>
+      <c r="IX54" t="inlineStr"/>
+      <c r="IY54" t="inlineStr"/>
+      <c r="IZ54" t="inlineStr"/>
+      <c r="JA54" t="inlineStr"/>
+      <c r="JB54" t="inlineStr"/>
+      <c r="JC54" t="inlineStr"/>
+      <c r="JD54" t="inlineStr"/>
+      <c r="JE54" t="inlineStr"/>
+      <c r="JF54" t="inlineStr"/>
+      <c r="JG54" t="inlineStr"/>
+      <c r="JH54" t="inlineStr"/>
+      <c r="JI54" t="inlineStr"/>
+      <c r="JJ54" t="inlineStr"/>
+      <c r="JK54" t="inlineStr"/>
+      <c r="JL54" t="inlineStr"/>
+      <c r="JM54" t="inlineStr"/>
+      <c r="JN54" t="inlineStr"/>
+      <c r="JO54" t="inlineStr"/>
+      <c r="JP54" t="inlineStr"/>
+      <c r="JQ54" t="inlineStr"/>
+      <c r="JR54" t="inlineStr"/>
+      <c r="JS54" t="inlineStr"/>
+      <c r="JT54" t="inlineStr"/>
+      <c r="JU54" t="inlineStr"/>
+      <c r="JV54" t="inlineStr"/>
+      <c r="JW54" t="inlineStr"/>
+      <c r="JX54" t="inlineStr"/>
+      <c r="JY54" t="inlineStr"/>
+      <c r="JZ54" t="inlineStr"/>
+      <c r="KA54" t="inlineStr"/>
+      <c r="KB54" t="inlineStr"/>
+      <c r="KC54" t="inlineStr"/>
+      <c r="KD54" t="inlineStr"/>
+      <c r="KE54" t="inlineStr"/>
+      <c r="KF54" t="inlineStr"/>
+      <c r="KG54" t="inlineStr"/>
+      <c r="KH54" t="inlineStr"/>
+      <c r="KI54" t="inlineStr"/>
+      <c r="KJ54" t="inlineStr"/>
+      <c r="KK54" t="inlineStr"/>
+      <c r="KL54" t="inlineStr"/>
+      <c r="KM54" t="inlineStr"/>
+      <c r="KN54" t="inlineStr"/>
+      <c r="KO54" t="inlineStr"/>
+      <c r="KP54" t="inlineStr"/>
+      <c r="KQ54" t="inlineStr"/>
+      <c r="KR54" t="inlineStr"/>
+      <c r="KS54" t="inlineStr"/>
+      <c r="KT54" t="inlineStr"/>
+      <c r="KU54" t="inlineStr"/>
+      <c r="KV54" t="inlineStr"/>
+      <c r="KW54" t="inlineStr"/>
+      <c r="KX54" t="inlineStr"/>
+      <c r="KY54" t="inlineStr"/>
+      <c r="KZ54" t="inlineStr"/>
+      <c r="LA54" t="inlineStr"/>
+      <c r="LB54" t="inlineStr"/>
+      <c r="LC54" t="inlineStr"/>
+      <c r="LD54" t="inlineStr"/>
+      <c r="LE54" t="inlineStr"/>
+      <c r="LF54" t="inlineStr"/>
+      <c r="LG54" t="inlineStr"/>
+      <c r="LH54" t="inlineStr"/>
+      <c r="LI54" t="inlineStr"/>
+      <c r="LJ54" t="inlineStr"/>
+      <c r="LK54" t="inlineStr"/>
+      <c r="LL54" t="inlineStr"/>
+      <c r="LM54" t="inlineStr"/>
+      <c r="LN54" t="inlineStr"/>
+      <c r="LO54" t="inlineStr"/>
+      <c r="LP54" t="inlineStr"/>
+      <c r="LQ54" t="inlineStr"/>
+      <c r="LR54" t="inlineStr"/>
+      <c r="LS54" t="inlineStr"/>
+      <c r="LT54" t="inlineStr"/>
+      <c r="LU54" t="inlineStr"/>
+      <c r="LV54" t="inlineStr"/>
+      <c r="LW54" t="inlineStr"/>
+      <c r="LX54" t="inlineStr"/>
+      <c r="LY54" t="inlineStr"/>
+      <c r="LZ54" t="inlineStr"/>
+      <c r="MA54" t="inlineStr"/>
+      <c r="MB54" t="inlineStr"/>
+      <c r="MC54" t="inlineStr"/>
+      <c r="MD54" t="inlineStr"/>
+      <c r="ME54" t="inlineStr"/>
+      <c r="MF54" t="inlineStr"/>
+      <c r="MG54" t="inlineStr"/>
+      <c r="MH54" t="inlineStr"/>
+      <c r="MI54" t="inlineStr"/>
+      <c r="MJ54" t="inlineStr"/>
+      <c r="MK54" t="inlineStr"/>
+      <c r="ML54" t="inlineStr"/>
+      <c r="MM54" t="inlineStr"/>
+      <c r="MN54" t="inlineStr"/>
+      <c r="MO54" t="inlineStr"/>
+      <c r="MP54" t="inlineStr"/>
+      <c r="MQ54" t="inlineStr"/>
+      <c r="MR54" t="inlineStr"/>
+      <c r="MS54" t="inlineStr"/>
+      <c r="MT54" t="inlineStr"/>
+      <c r="MU54" t="inlineStr"/>
+      <c r="MV54" t="inlineStr"/>
+      <c r="MW54" t="inlineStr"/>
+      <c r="MX54" t="inlineStr"/>
+      <c r="MY54" t="inlineStr"/>
+      <c r="MZ54" t="inlineStr"/>
+      <c r="NA54" t="inlineStr"/>
+      <c r="NB54" t="inlineStr"/>
+      <c r="NC54" t="inlineStr"/>
+      <c r="ND54" t="inlineStr"/>
+      <c r="NE54" t="inlineStr"/>
+      <c r="NF54" t="inlineStr"/>
+      <c r="NG54" t="inlineStr"/>
+      <c r="NH54" t="inlineStr"/>
+      <c r="NI54" t="inlineStr"/>
+      <c r="NJ54" t="inlineStr"/>
+      <c r="NK54" t="inlineStr"/>
+      <c r="NL54" t="inlineStr"/>
+      <c r="NM54" t="inlineStr"/>
+      <c r="NN54" t="inlineStr"/>
+      <c r="NO54" t="inlineStr"/>
+      <c r="NP54" t="inlineStr"/>
+      <c r="NQ54" t="inlineStr"/>
+      <c r="NR54" t="inlineStr"/>
+      <c r="NS54" t="inlineStr"/>
+      <c r="NT54" t="inlineStr"/>
+      <c r="NU54" t="inlineStr"/>
+      <c r="NV54" t="inlineStr"/>
+      <c r="NW54" t="inlineStr"/>
+      <c r="NX54" t="inlineStr"/>
+      <c r="NY54" t="inlineStr"/>
+      <c r="NZ54" t="inlineStr"/>
+      <c r="OA54" t="inlineStr"/>
+      <c r="OB54" t="inlineStr"/>
+      <c r="OC54" t="inlineStr"/>
+      <c r="OD54" t="inlineStr"/>
+      <c r="OE54" t="inlineStr"/>
+      <c r="OF54" t="inlineStr"/>
+      <c r="OG54" t="inlineStr"/>
+      <c r="OH54" t="inlineStr"/>
+      <c r="OI54" t="inlineStr"/>
+      <c r="OJ54" t="inlineStr"/>
+      <c r="OK54" t="inlineStr"/>
+      <c r="OL54" t="inlineStr"/>
+      <c r="OM54" t="inlineStr"/>
+      <c r="ON54" t="inlineStr"/>
+      <c r="OO54" t="inlineStr"/>
+      <c r="OP54" t="inlineStr"/>
+      <c r="OQ54" t="inlineStr"/>
+      <c r="OR54" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>